<commit_message>
Changes in the following files: 1)B suite.xlsx 2)Suite
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="85">
   <si>
     <t>TCID</t>
   </si>
@@ -191,9 +191,6 @@
     <t>TestCase_B6</t>
   </si>
   <si>
-    <t>SKIP</t>
-  </si>
-  <si>
     <t>TestCase_B7</t>
   </si>
   <si>
@@ -236,18 +233,12 @@
     <t>To verify that 10 MORE button is working correctly</t>
   </si>
   <si>
-    <t>FAIL</t>
-  </si>
-  <si>
     <t>TestCase_B16</t>
   </si>
   <si>
     <t>To verify that 10 MORE button is not present in search results page if the total search results is less than or equal to 10</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
     <t>TestCase_B17</t>
   </si>
   <si>
@@ -288,6 +279,42 @@
   </si>
   <si>
     <t>To verify that user is able to collapse and expand the filters in the left navigation pane in search results page</t>
+  </si>
+  <si>
+    <t>TestCase_B13</t>
+  </si>
+  <si>
+    <t>TestCase_B14</t>
+  </si>
+  <si>
+    <t>To verify that NOT is not treated as a boolean</t>
+  </si>
+  <si>
+    <t>To verify that AND is not treated as a boolean</t>
+  </si>
+  <si>
+    <t>TestCase_B24</t>
+  </si>
+  <si>
+    <t>To verify that OR is not treated as a boolean</t>
+  </si>
+  <si>
+    <t>TestCase_B25</t>
+  </si>
+  <si>
+    <t>To verify that * provides right hand truncation</t>
+  </si>
+  <si>
+    <t>TestCase_B26</t>
+  </si>
+  <si>
+    <t>To verify that ? Is supported for a single character</t>
+  </si>
+  <si>
+    <t>TestCase_B27</t>
+  </si>
+  <si>
+    <t>To verify that * is treated as a space if user does not provide 3 characters before it</t>
   </si>
 </sst>
 </file>
@@ -668,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -706,9 +733,7 @@
       <c r="C2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
@@ -720,9 +745,7 @@
       <c r="C3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
@@ -734,9 +757,7 @@
       <c r="C4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
@@ -748,9 +769,7 @@
       <c r="C5" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
@@ -762,9 +781,7 @@
       <c r="C6" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
@@ -776,219 +793,259 @@
       <c r="C7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="C8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>47</v>
-      </c>
       <c r="C9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>49</v>
-      </c>
       <c r="C10" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>51</v>
-      </c>
       <c r="C11" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" ht="16.5" customHeight="1">
       <c r="A12" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>53</v>
-      </c>
       <c r="C12" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="A14" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="A15" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="3" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="3" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
running B suite only
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -707,7 +707,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C2" sqref="C2:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -740,7 +740,7 @@
         <v>32</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>31</v>
+        <v>86</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>85</v>
@@ -754,7 +754,7 @@
         <v>34</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>31</v>
+        <v>86</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>85</v>
@@ -768,7 +768,7 @@
         <v>36</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>31</v>
+        <v>86</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>85</v>
@@ -782,7 +782,7 @@
         <v>39</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>31</v>
+        <v>86</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>85</v>
@@ -796,7 +796,7 @@
         <v>40</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>31</v>
+        <v>86</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>85</v>
@@ -810,7 +810,7 @@
         <v>41</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>31</v>
+        <v>86</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>85</v>
@@ -824,7 +824,7 @@
         <v>44</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>31</v>
+        <v>86</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>85</v>
@@ -838,7 +838,7 @@
         <v>46</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>31</v>
+        <v>86</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>85</v>
@@ -852,7 +852,7 @@
         <v>48</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>31</v>
+        <v>86</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>85</v>
@@ -866,7 +866,7 @@
         <v>50</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>31</v>
+        <v>86</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>85</v>
@@ -880,7 +880,7 @@
         <v>52</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>31</v>
+        <v>86</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>85</v>
@@ -894,7 +894,7 @@
         <v>53</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>31</v>
+        <v>86</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>85</v>
@@ -908,7 +908,7 @@
         <v>75</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>31</v>
+        <v>86</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>85</v>
@@ -922,7 +922,7 @@
         <v>76</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>31</v>
+        <v>86</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>85</v>

</xml_diff>

<commit_message>
Running all test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="81">
   <si>
     <t>TCID</t>
   </si>
@@ -291,9 +291,6 @@
   </si>
   <si>
     <t>SKIP</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>PASS</t>
@@ -689,7 +686,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C2" sqref="C2:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -722,7 +719,7 @@
         <v>32</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>76</v>
@@ -736,7 +733,7 @@
         <v>34</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>76</v>
@@ -750,7 +747,7 @@
         <v>36</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>76</v>
@@ -764,7 +761,7 @@
         <v>39</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>76</v>
@@ -778,7 +775,7 @@
         <v>40</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>76</v>
@@ -806,7 +803,7 @@
         <v>44</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>76</v>
@@ -817,13 +814,13 @@
         <v>45</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>31</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -834,7 +831,7 @@
         <v>47</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>76</v>
@@ -848,7 +845,7 @@
         <v>49</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>76</v>
@@ -859,7 +856,7 @@
         <v>50</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>31</v>
@@ -876,7 +873,7 @@
         <v>51</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>76</v>
@@ -890,7 +887,7 @@
         <v>66</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>76</v>
@@ -904,7 +901,7 @@
         <v>67</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>76</v>
@@ -915,7 +912,7 @@
         <v>53</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>31</v>
@@ -946,7 +943,7 @@
         <v>57</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>76</v>
@@ -960,7 +957,7 @@
         <v>59</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>76</v>
@@ -974,7 +971,7 @@
         <v>61</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>76</v>
@@ -988,7 +985,7 @@
         <v>63</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>76</v>
@@ -1002,7 +999,7 @@
         <v>69</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>76</v>
@@ -1016,7 +1013,7 @@
         <v>71</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>76</v>
@@ -1030,7 +1027,7 @@
         <v>73</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>76</v>
@@ -1044,7 +1041,7 @@
         <v>75</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
Changing B suite excel file
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="80">
   <si>
     <t>TCID</t>
   </si>
@@ -155,9 +155,6 @@
     <t>TestCase_B1</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>Test to verify that MINIMUM SHOULD MATCH rule is working correctly</t>
   </si>
   <si>
@@ -303,25 +300,12 @@
   </si>
   <si>
     <t>N</t>
-  </si>
-  <si>
-    <t>TestCase_B28</t>
-  </si>
-  <si>
-    <t>Verify that user is able to sort the documents by TIMES CITED field</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -696,18 +680,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="115.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="115.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -729,349 +713,335 @@
         <v>30</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="C3" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="C4" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="C8" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>47</v>
-      </c>
       <c r="C10" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>49</v>
-      </c>
       <c r="C11" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16.5" customHeight="1">
       <c r="A12" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="C17" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="C18" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="C19" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="C20" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="C21" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>69</v>
-      </c>
       <c r="C22" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>71</v>
-      </c>
       <c r="C23" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>73</v>
-      </c>
       <c r="C24" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>75</v>
-      </c>
       <c r="C25" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1090,10 +1060,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="12.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="5" width="52.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="5" width="83.85546875" collapsed="true"/>
-    <col min="4" max="16384" style="5" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="52.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.85546875" style="5" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="35.25" customHeight="1">

</xml_diff>

<commit_message>
Changes in Suite B
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="105">
   <si>
     <t>TCID</t>
   </si>
@@ -155,66 +155,36 @@
     <t>TestCase_B1</t>
   </si>
   <si>
-    <t>Test to verify that MINIMUM SHOULD MATCH rule is working correctly</t>
-  </si>
-  <si>
     <t>TestCase_B2</t>
   </si>
   <si>
-    <t>To verify that MUST OCCUR rule is working correctly</t>
-  </si>
-  <si>
     <t>TestCase_B3</t>
   </si>
   <si>
-    <t>To verify that MUST NOT OCCUR rule is working correctly</t>
-  </si>
-  <si>
     <t>TestCase_B4</t>
   </si>
   <si>
     <t>TestCase_B5</t>
   </si>
   <si>
-    <t>To verify that NESTING WITH PARENTHESIS rule is working correctly</t>
-  </si>
-  <si>
-    <t>To verify that PHRASING WITH QUOTES rule is working correctly</t>
-  </si>
-  <si>
-    <t>To verify that type ahead functionality is working correctly</t>
-  </si>
-  <si>
     <t>TestCase_B6</t>
   </si>
   <si>
     <t>TestCase_B7</t>
   </si>
   <si>
-    <t>To verify that no search results get displayed if search engine doesn't interpret the query</t>
-  </si>
-  <si>
     <t>TestCase_B8</t>
   </si>
   <si>
     <t>TestCase_B9</t>
   </si>
   <si>
-    <t>To verify that sorting is retained when user navigates back to search results page from record view page</t>
-  </si>
-  <si>
     <t>TestCase_B10</t>
   </si>
   <si>
-    <t>To verify that filtering is retained when user navigates back to search results page from record view page</t>
-  </si>
-  <si>
     <t>TestCase_B11</t>
   </si>
   <si>
-    <t>To verify that the addition of total articles count and total profiles count is equal to total search results count</t>
-  </si>
-  <si>
     <t>TestCase_B12</t>
   </si>
   <si>
@@ -224,89 +194,193 @@
     <t>TestCase_B19</t>
   </si>
   <si>
-    <t>To verify that user is able to expand and collapse SORT BY drop down</t>
-  </si>
-  <si>
     <t>TestCase_B20</t>
   </si>
   <si>
-    <t>To verify that user is able to sort the documents by TIMES CITED field</t>
-  </si>
-  <si>
     <t>TestCase_B21</t>
   </si>
   <si>
-    <t>To verify that RESET button in the left navigation pane in search results page is working correctly</t>
-  </si>
-  <si>
     <t>TestCase_B22</t>
   </si>
   <si>
-    <t>To verify that MORE and LESS links in the left navigation pane are working correctly</t>
-  </si>
-  <si>
     <t>TestCase_B23</t>
   </si>
   <si>
-    <t>To verify that user is able to collapse and expand the filters in the left navigation pane in search results page</t>
-  </si>
-  <si>
     <t>TestCase_B13</t>
   </si>
   <si>
     <t>TestCase_B14</t>
   </si>
   <si>
-    <t>To verify that NOT is not treated as a boolean</t>
-  </si>
-  <si>
-    <t>To verify that AND is not treated as a boolean</t>
-  </si>
-  <si>
     <t>TestCase_B24</t>
   </si>
   <si>
-    <t>To verify that OR is not treated as a boolean</t>
-  </si>
-  <si>
     <t>TestCase_B25</t>
   </si>
   <si>
-    <t>To verify that * provides right hand truncation</t>
-  </si>
-  <si>
     <t>TestCase_B26</t>
   </si>
   <si>
-    <t>To verify that ? Is supported for a single character</t>
-  </si>
-  <si>
     <t>TestCase_B27</t>
   </si>
   <si>
-    <t>To verify that * is treated as a space if user does not provide 3 characters before it</t>
-  </si>
-  <si>
     <t>SKIP</t>
   </si>
   <si>
-    <t>To verify that number of displayed documents gets increased as and when user scrolls down the search results page</t>
-  </si>
-  <si>
-    <t>To verify that sorting and filtering are retained when user navigates back to search results page from record view page</t>
-  </si>
-  <si>
-    <t>To verify that Times cited and Comments fields are getting displayed for each document in search results page</t>
-  </si>
-  <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Jira id</t>
+  </si>
+  <si>
+    <t>OPQA-222</t>
+  </si>
+  <si>
+    <t>OPQA-233</t>
+  </si>
+  <si>
+    <t>OPQA-234</t>
+  </si>
+  <si>
+    <t>OPQA-235</t>
+  </si>
+  <si>
+    <t>OPQA-237</t>
+  </si>
+  <si>
+    <t>OPQA-239</t>
+  </si>
+  <si>
+    <t>OPQA-241</t>
+  </si>
+  <si>
+    <t>OPQA-243</t>
+  </si>
+  <si>
+    <t>OPQA-246</t>
+  </si>
+  <si>
+    <t>OPQA-249</t>
+  </si>
+  <si>
+    <t>OPQA-250</t>
+  </si>
+  <si>
+    <t>OPQA-252</t>
+  </si>
+  <si>
+    <t>OPQA-266</t>
+  </si>
+  <si>
+    <t>OPQA-270</t>
+  </si>
+  <si>
+    <t>OPQA-274</t>
+  </si>
+  <si>
+    <t>OPQA-279</t>
+  </si>
+  <si>
+    <t>OPQA-358</t>
+  </si>
+  <si>
+    <t>OPQA-366</t>
+  </si>
+  <si>
+    <t>OPQA-362</t>
+  </si>
+  <si>
+    <t>OPQA-368</t>
+  </si>
+  <si>
+    <t>OPQA-371</t>
+  </si>
+  <si>
+    <t>OPQA-744</t>
+  </si>
+  <si>
+    <t>Verify that no search results get displayed if search engine doesn't interpret the query and that a proper message gets displayed regarding that</t>
+  </si>
+  <si>
+    <t>OPQA-258</t>
+  </si>
+  <si>
+    <t>OPQA-283</t>
+  </si>
+  <si>
+    <t>Verify that MUST OCCUR rule is working correctly</t>
+  </si>
+  <si>
+    <t>Verify that MUST NOT OCCUR rule is working correctly</t>
+  </si>
+  <si>
+    <t>Verify that NESTING WITH PARENTHESIS rule is working correctly</t>
+  </si>
+  <si>
+    <t>Verify that PHRASING WITH QUOTES rule is working correctly</t>
+  </si>
+  <si>
+    <t>Verify that type ahead functionality is working correctly</t>
+  </si>
+  <si>
+    <t>Verify that number of displayed documents gets increased as and when user scrolls down the search results page</t>
+  </si>
+  <si>
+    <t>Verify that sorting is retained when user navigates back to search results page from record view page</t>
+  </si>
+  <si>
+    <t>Verify that filtering is retained when user navigates back to search results page from record view page</t>
+  </si>
+  <si>
+    <t>Verify that sorting and filtering are retained when user navigates back to search results page from record view page</t>
+  </si>
+  <si>
+    <t>Verify that the addition of total articles count and total profiles count is equal to total search results count</t>
+  </si>
+  <si>
+    <t>Verify that NOT is not treated as a boolean</t>
+  </si>
+  <si>
+    <t>Verify that AND is not treated as a boolean</t>
+  </si>
+  <si>
+    <t>Verify that Times cited and Comments fields are getting displayed for each document in search results page</t>
+  </si>
+  <si>
+    <t>Verify that user is able to expand and collapse SORT BY drop down</t>
+  </si>
+  <si>
+    <t>Verify that user is able to sort the documents by TIMES CITED field</t>
+  </si>
+  <si>
+    <t>Verify that RESET button in the left navigation pane in search results page is working correctly</t>
+  </si>
+  <si>
+    <t>Verify that MORE and LESS links in the left navigation pane are working correctly</t>
+  </si>
+  <si>
+    <t>Verify that user is able to collapse and expand the filters in the left navigation pane in search results page</t>
+  </si>
+  <si>
+    <t>Verify that OR is not treated as a boolean</t>
+  </si>
+  <si>
+    <t>Verify that * provides right hand truncation</t>
+  </si>
+  <si>
+    <t>Verify that ? Is supported for a single character</t>
+  </si>
+  <si>
+    <t>Verify that * is treated as a space if user does not provide 3 characters before it</t>
+  </si>
+  <si>
+    <t>Verify that MINIMUM SHOULD MATCH rule is working correctly</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -324,7 +398,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -334,6 +408,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -365,7 +445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -382,6 +462,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,368 +765,444 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="115.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="136.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="B3" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1">
+      <c r="A8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D8" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="C9" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="B10" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="3" t="s">
+      <c r="B11" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A12" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="7" t="s">
+      <c r="B13" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B16" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="7" t="s">
+      <c r="B17" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="7" t="s">
+      <c r="B18" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B19" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="7" t="s">
+      <c r="B20" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A12" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="7" t="s">
+      <c r="B21" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B15" s="6" t="s">
+      <c r="B23" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="3" t="s">
+      <c r="C23" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="3" t="s">
+      <c r="B24" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B22" s="6" t="s">
+      <c r="B25" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>75</v>
+      <c r="C25" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1061,10 +1221,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="12.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="5" width="52.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="5" width="83.85546875" collapsed="true"/>
-    <col min="4" max="16384" style="5" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="52.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.85546875" style="5" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="35.25" customHeight="1">

</xml_diff>

<commit_message>
Runnning all the test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="106">
   <si>
     <t>TCID</t>
   </si>
@@ -368,9 +368,6 @@
     <t>Verify that MINIMUM SHOULD MATCH rule is working correctly</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>PASS</t>
   </si>
   <si>
@@ -387,7 +384,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -775,15 +771,15 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D2" sqref="D2:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="136.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="2" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="136.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -817,7 +813,7 @@
         <v>52</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -831,7 +827,7 @@
         <v>79</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>51</v>
@@ -848,7 +844,7 @@
         <v>80</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>51</v>
@@ -865,7 +861,7 @@
         <v>81</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>51</v>
@@ -882,7 +878,7 @@
         <v>82</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>51</v>
@@ -899,7 +895,7 @@
         <v>83</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>51</v>
@@ -916,7 +912,7 @@
         <v>76</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>51</v>
@@ -933,7 +929,7 @@
         <v>84</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>51</v>
@@ -950,7 +946,7 @@
         <v>85</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>51</v>
@@ -967,7 +963,7 @@
         <v>86</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>51</v>
@@ -984,7 +980,7 @@
         <v>87</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>51</v>
@@ -1001,7 +997,7 @@
         <v>88</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>51</v>
@@ -1018,7 +1014,7 @@
         <v>89</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>51</v>
@@ -1035,7 +1031,7 @@
         <v>90</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>51</v>
@@ -1043,7 +1039,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>70</v>
@@ -1052,7 +1048,7 @@
         <v>91</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>51</v>
@@ -1060,7 +1056,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>69</v>
@@ -1069,7 +1065,7 @@
         <v>92</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>51</v>
@@ -1077,7 +1073,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>78</v>
@@ -1086,7 +1082,7 @@
         <v>93</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>51</v>
@@ -1103,7 +1099,7 @@
         <v>94</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>51</v>
@@ -1120,7 +1116,7 @@
         <v>95</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>51</v>
@@ -1137,7 +1133,7 @@
         <v>96</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>51</v>
@@ -1154,7 +1150,7 @@
         <v>97</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>51</v>
@@ -1171,7 +1167,7 @@
         <v>98</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>51</v>
@@ -1188,7 +1184,7 @@
         <v>99</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>51</v>
@@ -1205,7 +1201,7 @@
         <v>100</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>51</v>
@@ -1227,10 +1223,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="12.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="5" width="52.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="5" width="83.85546875" collapsed="true"/>
-    <col min="4" max="16384" style="5" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="52.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.85546875" style="5" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="35.25" customHeight="1">

</xml_diff>

<commit_message>
Making changes in Search module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="124">
   <si>
     <t>TCID</t>
   </si>
@@ -374,10 +374,68 @@
     <t>TestCase_B17</t>
   </si>
   <si>
+    <t>Verify that ALL content type count is equal to the sum of the counts of other content types</t>
+  </si>
+  <si>
+    <t>TestCase_B25</t>
+  </si>
+  <si>
+    <t>TBD-1</t>
+  </si>
+  <si>
+    <t>Verify that autocomplete feature is working correctly</t>
+  </si>
+  <si>
+    <t>TestCase_B26</t>
+  </si>
+  <si>
+    <t>TBD-2</t>
+  </si>
+  <si>
+    <t>Verify that following sections get displayed in type ahead:
+a)Categories
+b)Articles
+c)Patents
+d)People</t>
+  </si>
+  <si>
+    <t>TestCase_B27</t>
+  </si>
+  <si>
+    <t>TBD-3</t>
+  </si>
+  <si>
+    <t>Verify that 4 suggested categories get displayed in type ahead and the typed keyword is present in all the 4 categories</t>
+  </si>
+  <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>Verify that ALL content type count is equal to the sum of the counts of other content types</t>
+    <t>Verify that 4 suggested articles get displayed in type ahead and the typed keyword is present in all the 4 articles</t>
+  </si>
+  <si>
+    <t>TBD-4</t>
+  </si>
+  <si>
+    <t>TestCase_B28</t>
+  </si>
+  <si>
+    <t>TestCase_B29</t>
+  </si>
+  <si>
+    <t>TBD-5</t>
+  </si>
+  <si>
+    <t>Verify that 4 suggested patents get displayed in type ahead and the typed keyword is present in all the 4 patents</t>
+  </si>
+  <si>
+    <t>TestCase_B30</t>
+  </si>
+  <si>
+    <t>TBD-6</t>
+  </si>
+  <si>
+    <t>Verify that 4 suggested people get displayed in type ahead and the typed keyword is present in all the 4 people</t>
   </si>
 </sst>
 </file>
@@ -768,10 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D25"/>
+      <selection activeCell="D2" sqref="D2:D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -966,7 +1024,7 @@
         <v>52</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>104</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16.5" customHeight="1">
@@ -994,7 +1052,7 @@
         <v>71</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>52</v>
@@ -1205,6 +1263,108 @@
       </c>
       <c r="E25" s="3" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="75">
+      <c r="A27" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New implemented automation test cases for Search Module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="12555" windowHeight="9795"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Test Case Steps" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="136">
   <si>
     <t>TCID</t>
   </si>
@@ -408,9 +409,6 @@
     <t>Verify that 4 suggested categories get displayed in type ahead and the typed keyword is present in all the 4 categories</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
     <t>Verify that 4 suggested articles get displayed in type ahead and the typed keyword is present in all the 4 articles</t>
   </si>
   <si>
@@ -436,6 +434,53 @@
   </si>
   <si>
     <t>Verify that 4 suggested people get displayed in type ahead and the typed keyword is present in all the 4 people</t>
+  </si>
+  <si>
+    <t>TestCase_B31</t>
+  </si>
+  <si>
+    <t>OPQA-610</t>
+  </si>
+  <si>
+    <t>Verify that the following content type tabs get displayed in the left navigation pane:
+a)ALL
+b)ARTICLES
+c)PATENTS
+d)PEOPLE
+e)POSTS</t>
+  </si>
+  <si>
+    <t>TestCase_B32</t>
+  </si>
+  <si>
+    <t>Verify that the following fields get displayed in the SORT BY drop down when ALL is selected as content type in the left navigation pane:
+a)Relevance
+b)Times cited
+c)Date</t>
+  </si>
+  <si>
+    <t>TestCase_B33</t>
+  </si>
+  <si>
+    <t>Verify that the items are sorted by RELEVANCE by default in ALL content type</t>
+  </si>
+  <si>
+    <t>TestCase_B34</t>
+  </si>
+  <si>
+    <t>Verify that user is able to sort the items by TIMES CITED field in ALL content type</t>
+  </si>
+  <si>
+    <t>TBD-7</t>
+  </si>
+  <si>
+    <t>TDB-8</t>
+  </si>
+  <si>
+    <t>TBD-9</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -826,10 +871,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D31"/>
+    <sheetView tabSelected="1" topLeftCell="D21" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27:D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1143,7 +1188,7 @@
         <v>52</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>51</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1318,13 +1363,13 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>52</v>
@@ -1335,13 +1380,13 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="C30" s="3" t="s">
         <v>119</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>120</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>52</v>
@@ -1352,19 +1397,87 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="C31" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="D31" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="90">
+      <c r="A32" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D31" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>114</v>
+      <c r="B32" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="60">
+      <c r="A33" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1375,7 +1488,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>

</xml_diff>

<commit_message>
Adding 6 new test cases to Search Module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="12555" windowHeight="9795"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="14205" windowHeight="10125"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="154">
   <si>
     <t>TCID</t>
   </si>
@@ -480,14 +480,77 @@
     <t>TBD-9</t>
   </si>
   <si>
-    <t>FAIL</t>
+    <t>TestCase_B35</t>
+  </si>
+  <si>
+    <t>TBD-10</t>
+  </si>
+  <si>
+    <t>Verify that no filtering options are present in ALL content type</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>TestCase_B36</t>
+  </si>
+  <si>
+    <t>TBD-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that the following fields get displayed in the SORT BY drop down when ARTICLES is selected as content type in the left navigation pane:
+a)Relevance
+b)Times cited
+c)Publication Date(Newest)
+d)Publication Date(Oldest)
+</t>
+  </si>
+  <si>
+    <t>TestCase_B37</t>
+  </si>
+  <si>
+    <t>TBD-12</t>
+  </si>
+  <si>
+    <t>Verify that user is able to sort the articles by TIMES CITED field in ARTICLES content type</t>
+  </si>
+  <si>
+    <t>TestCase_B38</t>
+  </si>
+  <si>
+    <t>TBD-13</t>
+  </si>
+  <si>
+    <t>Verify that only articles get displayed when user chooses ARTICLES as content type</t>
+  </si>
+  <si>
+    <t>TestCase_B39</t>
+  </si>
+  <si>
+    <t>TBD-14</t>
+  </si>
+  <si>
+    <t>Verify that all articles are sorted by RELEVANCE by default in ARTICLES content type</t>
+  </si>
+  <si>
+    <t>TestCase_B40</t>
+  </si>
+  <si>
+    <t>TBD-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that following filters are present for ARTICLES content type:
+a)Document Type
+b)Authors
+c)Categories
+d)Institutions
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -872,18 +935,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D21" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27:D35"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="136.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="2" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="136.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1479,6 +1542,108 @@
       </c>
       <c r="E35" s="3" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1497,10 +1662,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="12.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="5" width="52.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="5" width="83.85546875" collapsed="true"/>
-    <col min="4" max="16384" style="5" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="52.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.85546875" style="5" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="35.25" customHeight="1">

</xml_diff>

<commit_message>
Adding new test cases for Search Module(TestCase_B41,TestCase_B42,TestCase_B43,TestCase_B44)
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="14205" windowHeight="10125"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="14715" windowHeight="8040"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="166">
   <si>
     <t>TCID</t>
   </si>
@@ -216,9 +216,6 @@
     <t>TestCase_B24</t>
   </si>
   <si>
-    <t>SKIP</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -489,9 +486,6 @@
     <t>Verify that no filtering options are present in ALL content type</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
     <t>TestCase_B36</t>
   </si>
   <si>
@@ -545,6 +539,48 @@
 c)Categories
 d)Institutions
 </t>
+  </si>
+  <si>
+    <t>TestCase_B41</t>
+  </si>
+  <si>
+    <t>TBD-16</t>
+  </si>
+  <si>
+    <t>Verify that user is able to expand and collapse the Document Type filter in ARTICLES content type</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
+    <t>TestCase_B42</t>
+  </si>
+  <si>
+    <t>TBD-17</t>
+  </si>
+  <si>
+    <t>TestCase_B43</t>
+  </si>
+  <si>
+    <t>TestCase_B44</t>
+  </si>
+  <si>
+    <t>TBD-18</t>
+  </si>
+  <si>
+    <t>TBD-19</t>
+  </si>
+  <si>
+    <t>Verify that user is able to expand and collapse the Authors filter in ARTICLES content type</t>
+  </si>
+  <si>
+    <t>Verify that user is able to expand and collapse the Categories filter in ARTICLES content type</t>
+  </si>
+  <si>
+    <t>Verify that user is able to expand and collapse the Institutions filter in ARTICLES content type</t>
   </si>
 </sst>
 </file>
@@ -935,10 +971,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -954,7 +990,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -971,16 +1007,16 @@
         <v>30</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -988,16 +1024,16 @@
         <v>31</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1005,16 +1041,16 @@
         <v>32</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1022,16 +1058,16 @@
         <v>33</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1039,16 +1075,16 @@
         <v>34</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1056,16 +1092,16 @@
         <v>35</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
@@ -1073,16 +1109,16 @@
         <v>36</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1090,16 +1126,16 @@
         <v>37</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1107,16 +1143,16 @@
         <v>38</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1124,16 +1160,16 @@
         <v>39</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16.5" customHeight="1">
@@ -1141,16 +1177,16 @@
         <v>40</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1158,16 +1194,16 @@
         <v>41</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1175,16 +1211,16 @@
         <v>48</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1192,67 +1228,67 @@
         <v>49</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1260,16 +1296,16 @@
         <v>42</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1277,16 +1313,16 @@
         <v>43</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1294,16 +1330,16 @@
         <v>44</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1311,16 +1347,16 @@
         <v>45</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1328,16 +1364,16 @@
         <v>46</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1345,16 +1381,16 @@
         <v>47</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1362,288 +1398,356 @@
         <v>50</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="C26" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>107</v>
-      </c>
       <c r="D26" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="75">
       <c r="A27" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="C27" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>110</v>
-      </c>
       <c r="D27" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="C28" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>113</v>
-      </c>
       <c r="D28" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="C30" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>119</v>
-      </c>
       <c r="D30" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="C31" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>122</v>
-      </c>
       <c r="D31" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="90">
       <c r="A32" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B32" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="C32" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="C32" s="8" t="s">
-        <v>125</v>
-      </c>
       <c r="D32" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="60">
       <c r="A33" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B33" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>127</v>
-      </c>
       <c r="D33" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C34" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="B34" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>129</v>
-      </c>
       <c r="D34" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C35" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="B35" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>131</v>
-      </c>
       <c r="D35" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="D36" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="90">
+      <c r="A37" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E36" s="3" t="s">
+      <c r="B37" s="3" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="3" t="s">
+      <c r="C37" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>52</v>
+      <c r="D37" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>52</v>
+      <c r="D38" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>52</v>
+      <c r="D39" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="D40" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="90">
+      <c r="A41" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="B41" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="3" t="s">
+      <c r="C41" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="D41" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="B42" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>138</v>
+      <c r="C42" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commiting to Local.Changes for TestCase_F5
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="14205" windowHeight="10125"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="14715" windowHeight="8040"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="166">
   <si>
     <t>TCID</t>
   </si>
@@ -216,9 +216,6 @@
     <t>TestCase_B24</t>
   </si>
   <si>
-    <t>SKIP</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -489,9 +486,6 @@
     <t>Verify that no filtering options are present in ALL content type</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
     <t>TestCase_B36</t>
   </si>
   <si>
@@ -545,6 +539,48 @@
 c)Categories
 d)Institutions
 </t>
+  </si>
+  <si>
+    <t>TestCase_B41</t>
+  </si>
+  <si>
+    <t>TBD-16</t>
+  </si>
+  <si>
+    <t>Verify that user is able to expand and collapse the Document Type filter in ARTICLES content type</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
+    <t>TestCase_B42</t>
+  </si>
+  <si>
+    <t>TBD-17</t>
+  </si>
+  <si>
+    <t>TestCase_B43</t>
+  </si>
+  <si>
+    <t>TestCase_B44</t>
+  </si>
+  <si>
+    <t>TBD-18</t>
+  </si>
+  <si>
+    <t>TBD-19</t>
+  </si>
+  <si>
+    <t>Verify that user is able to expand and collapse the Authors filter in ARTICLES content type</t>
+  </si>
+  <si>
+    <t>Verify that user is able to expand and collapse the Categories filter in ARTICLES content type</t>
+  </si>
+  <si>
+    <t>Verify that user is able to expand and collapse the Institutions filter in ARTICLES content type</t>
   </si>
 </sst>
 </file>
@@ -935,10 +971,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -954,7 +990,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -971,16 +1007,16 @@
         <v>30</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -988,16 +1024,16 @@
         <v>31</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1005,16 +1041,16 @@
         <v>32</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1022,16 +1058,16 @@
         <v>33</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1039,16 +1075,16 @@
         <v>34</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1056,16 +1092,16 @@
         <v>35</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
@@ -1073,16 +1109,16 @@
         <v>36</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1090,16 +1126,16 @@
         <v>37</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1107,16 +1143,16 @@
         <v>38</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1124,16 +1160,16 @@
         <v>39</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16.5" customHeight="1">
@@ -1141,16 +1177,16 @@
         <v>40</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1158,16 +1194,16 @@
         <v>41</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1175,16 +1211,16 @@
         <v>48</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1192,67 +1228,67 @@
         <v>49</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1260,16 +1296,16 @@
         <v>42</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1277,16 +1313,16 @@
         <v>43</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1294,16 +1330,16 @@
         <v>44</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1311,16 +1347,16 @@
         <v>45</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1328,16 +1364,16 @@
         <v>46</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1345,16 +1381,16 @@
         <v>47</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1362,288 +1398,356 @@
         <v>50</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="C26" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>107</v>
-      </c>
       <c r="D26" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="75">
       <c r="A27" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="C27" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>110</v>
-      </c>
       <c r="D27" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="C28" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>113</v>
-      </c>
       <c r="D28" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="C30" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>119</v>
-      </c>
       <c r="D30" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="C31" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>122</v>
-      </c>
       <c r="D31" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="90">
       <c r="A32" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B32" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="C32" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="C32" s="8" t="s">
-        <v>125</v>
-      </c>
       <c r="D32" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="60">
       <c r="A33" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B33" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>127</v>
-      </c>
       <c r="D33" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C34" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="B34" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>129</v>
-      </c>
       <c r="D34" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C35" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="B35" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>131</v>
-      </c>
       <c r="D35" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="D36" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="90">
+      <c r="A37" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E36" s="3" t="s">
+      <c r="B37" s="3" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="3" t="s">
+      <c r="C37" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>52</v>
+      <c r="D37" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>52</v>
+      <c r="D38" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>52</v>
+      <c r="D39" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="D40" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="90">
+      <c r="A41" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="B41" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="3" t="s">
+      <c r="C41" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="D41" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="B42" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>138</v>
+      <c r="C42" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix for Notification Test Cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -11,12 +11,11 @@
     <sheet name="Test Case Steps" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="165">
   <si>
     <t>TCID</t>
   </si>
@@ -336,9 +335,6 @@
     <t>Verify that user is able to expand and collapse SORT BY drop down</t>
   </si>
   <si>
-    <t>Verify that user is able to sort the documents by TIMES CITED field</t>
-  </si>
-  <si>
     <t>Verify that RESET button in the left navigation pane in search results page is working correctly</t>
   </si>
   <si>
@@ -550,37 +546,37 @@
     <t>Verify that user is able to expand and collapse the Document Type filter in ARTICLES content type</t>
   </si>
   <si>
+    <t>SKIP</t>
+  </si>
+  <si>
+    <t>TestCase_B42</t>
+  </si>
+  <si>
+    <t>TBD-17</t>
+  </si>
+  <si>
+    <t>TestCase_B43</t>
+  </si>
+  <si>
+    <t>TestCase_B44</t>
+  </si>
+  <si>
+    <t>TBD-18</t>
+  </si>
+  <si>
+    <t>TBD-19</t>
+  </si>
+  <si>
+    <t>Verify that user is able to expand and collapse the Authors filter in ARTICLES content type</t>
+  </si>
+  <si>
+    <t>Verify that user is able to expand and collapse the Categories filter in ARTICLES content type</t>
+  </si>
+  <si>
+    <t>Verify that user is able to expand and collapse the Institutions filter in ARTICLES content type</t>
+  </si>
+  <si>
     <t>PASS</t>
-  </si>
-  <si>
-    <t>SKIP</t>
-  </si>
-  <si>
-    <t>TestCase_B42</t>
-  </si>
-  <si>
-    <t>TBD-17</t>
-  </si>
-  <si>
-    <t>TestCase_B43</t>
-  </si>
-  <si>
-    <t>TestCase_B44</t>
-  </si>
-  <si>
-    <t>TBD-18</t>
-  </si>
-  <si>
-    <t>TBD-19</t>
-  </si>
-  <si>
-    <t>Verify that user is able to expand and collapse the Authors filter in ARTICLES content type</t>
-  </si>
-  <si>
-    <t>Verify that user is able to expand and collapse the Categories filter in ARTICLES content type</t>
-  </si>
-  <si>
-    <t>Verify that user is able to expand and collapse the Institutions filter in ARTICLES content type</t>
   </si>
 </sst>
 </file>
@@ -973,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1010,13 +1006,13 @@
         <v>53</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1033,7 +1029,7 @@
         <v>51</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1050,7 +1046,7 @@
         <v>51</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1067,7 +1063,7 @@
         <v>51</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1084,7 +1080,7 @@
         <v>51</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1101,7 +1097,7 @@
         <v>51</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
@@ -1118,7 +1114,7 @@
         <v>51</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1135,7 +1131,7 @@
         <v>51</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1152,7 +1148,7 @@
         <v>51</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1169,7 +1165,7 @@
         <v>51</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16.5" customHeight="1">
@@ -1186,7 +1182,7 @@
         <v>51</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1197,13 +1193,13 @@
         <v>70</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1220,7 +1216,7 @@
         <v>51</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1237,12 +1233,12 @@
         <v>51</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>69</v>
@@ -1254,12 +1250,12 @@
         <v>51</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>68</v>
@@ -1271,24 +1267,24 @@
         <v>51</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>77</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>91</v>
+        <v>141</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1299,13 +1295,13 @@
         <v>67</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1316,13 +1312,13 @@
         <v>66</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1333,13 +1329,13 @@
         <v>65</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1350,13 +1346,13 @@
         <v>61</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1367,13 +1363,13 @@
         <v>62</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1384,13 +1380,13 @@
         <v>63</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1401,353 +1397,353 @@
         <v>64</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="C26" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>106</v>
-      </c>
       <c r="D26" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="75">
       <c r="A27" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="C27" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>109</v>
-      </c>
       <c r="D27" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="C28" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>112</v>
-      </c>
       <c r="D28" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="C30" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>118</v>
-      </c>
       <c r="D30" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="C31" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>121</v>
-      </c>
       <c r="D31" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="90">
       <c r="A32" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B32" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="C32" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="C32" s="8" t="s">
-        <v>124</v>
-      </c>
       <c r="D32" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="60">
       <c r="A33" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="B33" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>126</v>
-      </c>
       <c r="D33" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C34" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="B34" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>128</v>
-      </c>
       <c r="D34" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C35" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="B35" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>130</v>
-      </c>
       <c r="D35" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>136</v>
-      </c>
       <c r="D36" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="90">
       <c r="A37" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="C37" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>139</v>
-      </c>
       <c r="D37" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>142</v>
-      </c>
       <c r="D38" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>145</v>
-      </c>
       <c r="D39" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="C40" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>148</v>
-      </c>
       <c r="D40" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="90">
       <c r="A41" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="C41" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>151</v>
-      </c>
       <c r="D41" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="C42" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>154</v>
-      </c>
       <c r="D42" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>161</v>
-      </c>
       <c r="C44" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>162</v>
-      </c>
       <c r="C45" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -1758,7 +1754,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>

</xml_diff>

<commit_message>
2 test cases added into seaarch module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="171">
   <si>
     <t>TCID</t>
   </si>
@@ -576,6 +576,29 @@
     <t>Verify that user is able to expand and collapse the Institutions filter in ARTICLES content type</t>
   </si>
   <si>
+    <t>Verify that following  content type options are present in the search drop down:
+a)All
+b)Articles
+c)Patents
+d)People
+e)Posts</t>
+  </si>
+  <si>
+    <t>TestCase_B45</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>Verify that ALL content type is selected in the search drop down by default</t>
+  </si>
+  <si>
+    <t>TestCase_B46</t>
+  </si>
+  <si>
     <t>PASS</t>
   </si>
 </sst>
@@ -583,6 +606,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -967,18 +991,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D45"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="136.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="136.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1009,7 +1033,7 @@
         <v>98</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>154</v>
@@ -1026,7 +1050,7 @@
         <v>78</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>154</v>
@@ -1043,7 +1067,7 @@
         <v>79</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>154</v>
@@ -1060,7 +1084,7 @@
         <v>80</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>154</v>
@@ -1077,7 +1101,7 @@
         <v>81</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>154</v>
@@ -1094,7 +1118,7 @@
         <v>82</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>154</v>
@@ -1111,7 +1135,7 @@
         <v>75</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>154</v>
@@ -1128,7 +1152,7 @@
         <v>83</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>154</v>
@@ -1145,7 +1169,7 @@
         <v>84</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>154</v>
@@ -1162,7 +1186,7 @@
         <v>85</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>154</v>
@@ -1179,7 +1203,7 @@
         <v>86</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>154</v>
@@ -1196,7 +1220,7 @@
         <v>102</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>154</v>
@@ -1213,7 +1237,7 @@
         <v>87</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>154</v>
@@ -1230,7 +1254,7 @@
         <v>88</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>154</v>
@@ -1247,7 +1271,7 @@
         <v>89</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>154</v>
@@ -1264,7 +1288,7 @@
         <v>90</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>154</v>
@@ -1281,7 +1305,7 @@
         <v>141</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>154</v>
@@ -1298,7 +1322,7 @@
         <v>91</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>154</v>
@@ -1315,7 +1339,7 @@
         <v>92</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>154</v>
@@ -1332,7 +1356,7 @@
         <v>93</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>154</v>
@@ -1349,7 +1373,7 @@
         <v>94</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>154</v>
@@ -1366,7 +1390,7 @@
         <v>95</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>154</v>
@@ -1383,7 +1407,7 @@
         <v>96</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>154</v>
@@ -1400,7 +1424,7 @@
         <v>97</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>154</v>
@@ -1417,7 +1441,7 @@
         <v>105</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>154</v>
@@ -1434,7 +1458,7 @@
         <v>108</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>154</v>
@@ -1451,7 +1475,7 @@
         <v>111</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>154</v>
@@ -1468,7 +1492,7 @@
         <v>112</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>154</v>
@@ -1485,7 +1509,7 @@
         <v>117</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>154</v>
@@ -1502,7 +1526,7 @@
         <v>120</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>154</v>
@@ -1519,7 +1543,7 @@
         <v>123</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>154</v>
@@ -1536,7 +1560,7 @@
         <v>125</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>154</v>
@@ -1553,7 +1577,7 @@
         <v>127</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>154</v>
@@ -1570,7 +1594,7 @@
         <v>129</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>154</v>
@@ -1587,7 +1611,7 @@
         <v>135</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>154</v>
@@ -1604,7 +1628,7 @@
         <v>138</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>154</v>
@@ -1621,7 +1645,7 @@
         <v>141</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>154</v>
@@ -1638,7 +1662,7 @@
         <v>144</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>154</v>
@@ -1655,7 +1679,7 @@
         <v>147</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>154</v>
@@ -1672,7 +1696,7 @@
         <v>150</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>154</v>
@@ -1689,7 +1713,7 @@
         <v>153</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>154</v>
@@ -1706,7 +1730,7 @@
         <v>161</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>154</v>
@@ -1723,7 +1747,7 @@
         <v>162</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>154</v>
@@ -1740,10 +1764,44 @@
         <v>163</v>
       </c>
       <c r="D45" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="90">
+      <c r="A46" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E45" s="3" t="s">
-        <v>164</v>
+      <c r="E47" s="3" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1762,10 +1820,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="52.5703125" style="5" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.85546875" style="5" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="12.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="5" width="52.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="5" width="83.85546875" collapsed="true"/>
+    <col min="4" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="35.25" customHeight="1">

</xml_diff>

<commit_message>
taking latest changes and adding new profile implemented scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="169">
   <si>
     <t>TCID</t>
   </si>
@@ -574,6 +574,23 @@
   </si>
   <si>
     <t>Verify that user is able to expand and collapse the Institutions filter in ARTICLES content type</t>
+  </si>
+  <si>
+    <t>Verify that following  content type options are present in the search drop down:
+a)All
+b)Articles
+c)Patents
+d)People
+e)Posts</t>
+  </si>
+  <si>
+    <t>TestCase_B45</t>
+  </si>
+  <si>
+    <t>Verify that ALL content type is selected in the search drop down by default</t>
+  </si>
+  <si>
+    <t>TestCase_B46</t>
   </si>
   <si>
     <t>PASS</t>
@@ -967,10 +984,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D45"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="D47" sqref="D2:D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1008,7 +1025,7 @@
       <c r="C2" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -1025,7 +1042,7 @@
       <c r="C3" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -1042,7 +1059,7 @@
       <c r="C4" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -1059,7 +1076,7 @@
       <c r="C5" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -1076,7 +1093,7 @@
       <c r="C6" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -1093,7 +1110,7 @@
       <c r="C7" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -1110,7 +1127,7 @@
       <c r="C8" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -1127,7 +1144,7 @@
       <c r="C9" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -1144,7 +1161,7 @@
       <c r="C10" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -1161,7 +1178,7 @@
       <c r="C11" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -1178,7 +1195,7 @@
       <c r="C12" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -1195,7 +1212,7 @@
       <c r="C13" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -1212,7 +1229,7 @@
       <c r="C14" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -1229,7 +1246,7 @@
       <c r="C15" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -1246,7 +1263,7 @@
       <c r="C16" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -1263,7 +1280,7 @@
       <c r="C17" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E17" s="3" t="s">
@@ -1280,7 +1297,7 @@
       <c r="C18" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E18" s="3" t="s">
@@ -1297,7 +1314,7 @@
       <c r="C19" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E19" s="3" t="s">
@@ -1314,7 +1331,7 @@
       <c r="C20" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E20" s="3" t="s">
@@ -1331,7 +1348,7 @@
       <c r="C21" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E21" s="3" t="s">
@@ -1348,7 +1365,7 @@
       <c r="C22" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E22" s="3" t="s">
@@ -1365,7 +1382,7 @@
       <c r="C23" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E23" s="3" t="s">
@@ -1382,7 +1399,7 @@
       <c r="C24" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E24" s="3" t="s">
@@ -1399,7 +1416,7 @@
       <c r="C25" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E25" s="3" t="s">
@@ -1416,7 +1433,7 @@
       <c r="C26" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E26" s="3" t="s">
@@ -1433,7 +1450,7 @@
       <c r="C27" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E27" s="3" t="s">
@@ -1450,7 +1467,7 @@
       <c r="C28" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E28" s="3" t="s">
@@ -1467,7 +1484,7 @@
       <c r="C29" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E29" s="3" t="s">
@@ -1484,7 +1501,7 @@
       <c r="C30" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E30" s="3" t="s">
@@ -1501,7 +1518,7 @@
       <c r="C31" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E31" s="3" t="s">
@@ -1518,7 +1535,7 @@
       <c r="C32" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E32" s="3" t="s">
@@ -1535,7 +1552,7 @@
       <c r="C33" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E33" s="3" t="s">
@@ -1552,7 +1569,7 @@
       <c r="C34" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E34" s="3" t="s">
@@ -1569,7 +1586,7 @@
       <c r="C35" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E35" s="3" t="s">
@@ -1586,7 +1603,7 @@
       <c r="C36" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E36" s="3" t="s">
@@ -1603,7 +1620,7 @@
       <c r="C37" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E37" s="3" t="s">
@@ -1620,7 +1637,7 @@
       <c r="C38" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E38" s="3" t="s">
@@ -1637,7 +1654,7 @@
       <c r="C39" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E39" s="3" t="s">
@@ -1654,7 +1671,7 @@
       <c r="C40" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E40" s="3" t="s">
@@ -1671,7 +1688,7 @@
       <c r="C41" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E41" s="3" t="s">
@@ -1688,7 +1705,7 @@
       <c r="C42" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E42" s="3" t="s">
@@ -1705,7 +1722,7 @@
       <c r="C43" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E43" s="3" t="s">
@@ -1722,7 +1739,7 @@
       <c r="C44" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E44" s="3" t="s">
@@ -1739,11 +1756,45 @@
       <c r="C45" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D45" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E45" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="90">
+      <c r="A46" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C46" s="4" t="s">
         <v>164</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding new test scripts for watch list
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="169">
   <si>
     <t>TCID</t>
   </si>
@@ -574,6 +574,23 @@
   </si>
   <si>
     <t>Verify that user is able to expand and collapse the Institutions filter in ARTICLES content type</t>
+  </si>
+  <si>
+    <t>Verify that following  content type options are present in the search drop down:
+a)All
+b)Articles
+c)Patents
+d)People
+e)Posts</t>
+  </si>
+  <si>
+    <t>TestCase_B45</t>
+  </si>
+  <si>
+    <t>Verify that ALL content type is selected in the search drop down by default</t>
+  </si>
+  <si>
+    <t>TestCase_B46</t>
   </si>
   <si>
     <t>PASS</t>
@@ -967,10 +984,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D45"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="D47" sqref="D2:D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1008,7 +1025,7 @@
       <c r="C2" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -1025,7 +1042,7 @@
       <c r="C3" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -1042,7 +1059,7 @@
       <c r="C4" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -1059,7 +1076,7 @@
       <c r="C5" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -1076,7 +1093,7 @@
       <c r="C6" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -1093,7 +1110,7 @@
       <c r="C7" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -1110,7 +1127,7 @@
       <c r="C8" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -1127,7 +1144,7 @@
       <c r="C9" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -1144,7 +1161,7 @@
       <c r="C10" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -1161,7 +1178,7 @@
       <c r="C11" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -1178,7 +1195,7 @@
       <c r="C12" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -1195,7 +1212,7 @@
       <c r="C13" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -1212,7 +1229,7 @@
       <c r="C14" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -1229,7 +1246,7 @@
       <c r="C15" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -1246,7 +1263,7 @@
       <c r="C16" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -1263,7 +1280,7 @@
       <c r="C17" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E17" s="3" t="s">
@@ -1280,7 +1297,7 @@
       <c r="C18" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E18" s="3" t="s">
@@ -1297,7 +1314,7 @@
       <c r="C19" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E19" s="3" t="s">
@@ -1314,7 +1331,7 @@
       <c r="C20" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E20" s="3" t="s">
@@ -1331,7 +1348,7 @@
       <c r="C21" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E21" s="3" t="s">
@@ -1348,7 +1365,7 @@
       <c r="C22" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E22" s="3" t="s">
@@ -1365,7 +1382,7 @@
       <c r="C23" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E23" s="3" t="s">
@@ -1382,7 +1399,7 @@
       <c r="C24" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E24" s="3" t="s">
@@ -1399,7 +1416,7 @@
       <c r="C25" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E25" s="3" t="s">
@@ -1416,7 +1433,7 @@
       <c r="C26" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E26" s="3" t="s">
@@ -1433,7 +1450,7 @@
       <c r="C27" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E27" s="3" t="s">
@@ -1450,7 +1467,7 @@
       <c r="C28" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E28" s="3" t="s">
@@ -1467,7 +1484,7 @@
       <c r="C29" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E29" s="3" t="s">
@@ -1484,7 +1501,7 @@
       <c r="C30" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E30" s="3" t="s">
@@ -1501,7 +1518,7 @@
       <c r="C31" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E31" s="3" t="s">
@@ -1518,7 +1535,7 @@
       <c r="C32" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E32" s="3" t="s">
@@ -1535,7 +1552,7 @@
       <c r="C33" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E33" s="3" t="s">
@@ -1552,7 +1569,7 @@
       <c r="C34" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E34" s="3" t="s">
@@ -1569,7 +1586,7 @@
       <c r="C35" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E35" s="3" t="s">
@@ -1586,7 +1603,7 @@
       <c r="C36" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E36" s="3" t="s">
@@ -1603,7 +1620,7 @@
       <c r="C37" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E37" s="3" t="s">
@@ -1620,7 +1637,7 @@
       <c r="C38" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E38" s="3" t="s">
@@ -1637,7 +1654,7 @@
       <c r="C39" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E39" s="3" t="s">
@@ -1654,7 +1671,7 @@
       <c r="C40" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E40" s="3" t="s">
@@ -1671,7 +1688,7 @@
       <c r="C41" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E41" s="3" t="s">
@@ -1688,7 +1705,7 @@
       <c r="C42" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E42" s="3" t="s">
@@ -1705,7 +1722,7 @@
       <c r="C43" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E43" s="3" t="s">
@@ -1722,7 +1739,7 @@
       <c r="C44" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E44" s="3" t="s">
@@ -1739,11 +1756,45 @@
       <c r="C45" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D45" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E45" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="90">
+      <c r="A46" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C46" s="4" t="s">
         <v>164</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Taking latest changes and adding new profile test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="173">
   <si>
     <t>TCID</t>
   </si>
@@ -215,9 +215,6 @@
     <t>TestCase_B24</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>Jira id</t>
   </si>
   <si>
@@ -594,6 +591,21 @@
   </si>
   <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>Verify that user is able to select any of the content types present in search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B47</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>TestCase_B48</t>
+  </si>
+  <si>
+    <t>Verify that ALL option is selected in the left navigation pane by default when user searches using ALL option in the search drop down</t>
   </si>
 </sst>
 </file>
@@ -984,10 +996,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="D47" sqref="D2:D47"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1003,7 +1015,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1020,16 +1032,16 @@
         <v>30</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>51</v>
+        <v>97</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1037,16 +1049,16 @@
         <v>31</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>51</v>
+        <v>77</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1054,16 +1066,16 @@
         <v>32</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>51</v>
+        <v>78</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1071,16 +1083,16 @@
         <v>33</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>51</v>
+        <v>79</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1088,16 +1100,16 @@
         <v>34</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>51</v>
+        <v>80</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1105,16 +1117,16 @@
         <v>35</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>51</v>
+        <v>81</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
@@ -1122,16 +1134,16 @@
         <v>36</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>51</v>
+        <v>74</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1139,16 +1151,16 @@
         <v>37</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>51</v>
+        <v>82</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1156,16 +1168,16 @@
         <v>38</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>51</v>
+        <v>83</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1173,16 +1185,16 @@
         <v>39</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>51</v>
+        <v>84</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16.5" customHeight="1">
@@ -1190,16 +1202,16 @@
         <v>40</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>51</v>
+        <v>85</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1207,16 +1219,16 @@
         <v>41</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>51</v>
+        <v>101</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1224,16 +1236,16 @@
         <v>48</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>51</v>
+        <v>86</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1241,67 +1253,67 @@
         <v>49</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>51</v>
+        <v>87</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>51</v>
+        <v>88</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>51</v>
+        <v>89</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>51</v>
+        <v>140</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1309,16 +1321,16 @@
         <v>42</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>51</v>
+        <v>90</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1326,16 +1338,16 @@
         <v>43</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>51</v>
+        <v>91</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1343,16 +1355,16 @@
         <v>44</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>51</v>
+        <v>92</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1360,16 +1372,16 @@
         <v>45</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>51</v>
+        <v>93</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1377,16 +1389,16 @@
         <v>46</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>51</v>
+        <v>94</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1394,16 +1406,16 @@
         <v>47</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>51</v>
+        <v>95</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1411,390 +1423,424 @@
         <v>50</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>51</v>
+        <v>96</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="C26" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>51</v>
+      <c r="D26" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="75">
       <c r="A27" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="C27" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>51</v>
+      <c r="D27" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="C28" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>51</v>
+      <c r="D28" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>51</v>
+        <v>111</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="C30" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>51</v>
+      <c r="D30" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="C31" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>51</v>
+      <c r="D31" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="90">
       <c r="A32" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B32" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="C32" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="C32" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>51</v>
+      <c r="D32" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="60">
       <c r="A33" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="B33" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>51</v>
+      <c r="D33" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C34" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B34" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>51</v>
+      <c r="D34" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C35" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="B35" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>51</v>
+      <c r="D35" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>51</v>
+      <c r="D36" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="90">
       <c r="A37" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="C37" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>51</v>
+      <c r="D37" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>51</v>
+      <c r="D38" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>51</v>
+      <c r="D39" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="C40" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>51</v>
+      <c r="D40" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="90">
       <c r="A41" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="C41" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>51</v>
+      <c r="D41" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="C42" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>51</v>
+      <c r="D42" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="C43" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>51</v>
+        <v>160</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>51</v>
+        <v>161</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>51</v>
+        <v>162</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="90">
       <c r="A46" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>51</v>
+        <v>163</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="E49" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
taking latest changes and appending ProfilePage.java changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="186">
   <si>
     <t>TCID</t>
   </si>
@@ -599,13 +599,52 @@
     <t>TestCase_B47</t>
   </si>
   <si>
+    <t>TestCase_B48</t>
+  </si>
+  <si>
+    <t>Verify that ALL option is selected in the left navigation pane by default when user searches using ALL option in the search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B49</t>
+  </si>
+  <si>
+    <t>Verify that search results related to all content types get displayed in the summary page when user searches using ALL option in search drop down</t>
+  </si>
+  <si>
+    <t>OPQA-301</t>
+  </si>
+  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>TestCase_B48</t>
-  </si>
-  <si>
-    <t>Verify that ALL option is selected in the left navigation pane by default when user searches using ALL option in the search drop down</t>
+    <t>TestCase_B50</t>
+  </si>
+  <si>
+    <t>OPQA-307</t>
+  </si>
+  <si>
+    <t>Verify that ARTICLES option is selected in the left navigation pane by default when user searches using ARTICLES option in the search drop down</t>
+  </si>
+  <si>
+    <t>Verify that PATENTS option is selected in the left navigation pane by default when user searches using PATENTS option in the search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B51</t>
+  </si>
+  <si>
+    <t>TestCase_B52</t>
+  </si>
+  <si>
+    <t>Verify that POSTS option is selected in the left navigation pane by default when user searches using POSTS option in the search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B53</t>
+  </si>
+  <si>
+    <t>Verify that PEOPLE option is selected in the left navigation pane by default when user searches using PEOPLE option in the search drop down</t>
+  </si>
+  <si>
+    <t>OPQA-375</t>
   </si>
 </sst>
 </file>
@@ -996,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="D54" sqref="D2:D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1037,8 +1076,8 @@
       <c r="C2" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>170</v>
+      <c r="D2" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>153</v>
@@ -1054,8 +1093,8 @@
       <c r="C3" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>170</v>
+      <c r="D3" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>153</v>
@@ -1071,8 +1110,8 @@
       <c r="C4" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>170</v>
+      <c r="D4" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>153</v>
@@ -1088,8 +1127,8 @@
       <c r="C5" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>170</v>
+      <c r="D5" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>153</v>
@@ -1105,8 +1144,8 @@
       <c r="C6" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>170</v>
+      <c r="D6" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>153</v>
@@ -1122,8 +1161,8 @@
       <c r="C7" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>170</v>
+      <c r="D7" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>153</v>
@@ -1139,8 +1178,8 @@
       <c r="C8" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>170</v>
+      <c r="D8" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>153</v>
@@ -1156,8 +1195,8 @@
       <c r="C9" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>170</v>
+      <c r="D9" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>153</v>
@@ -1173,8 +1212,8 @@
       <c r="C10" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>170</v>
+      <c r="D10" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>153</v>
@@ -1190,8 +1229,8 @@
       <c r="C11" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>170</v>
+      <c r="D11" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>153</v>
@@ -1207,8 +1246,8 @@
       <c r="C12" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>170</v>
+      <c r="D12" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>153</v>
@@ -1224,8 +1263,8 @@
       <c r="C13" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>170</v>
+      <c r="D13" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>153</v>
@@ -1241,8 +1280,8 @@
       <c r="C14" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>170</v>
+      <c r="D14" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>153</v>
@@ -1258,8 +1297,8 @@
       <c r="C15" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>170</v>
+      <c r="D15" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>153</v>
@@ -1275,8 +1314,8 @@
       <c r="C16" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>170</v>
+      <c r="D16" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>153</v>
@@ -1292,8 +1331,8 @@
       <c r="C17" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>170</v>
+      <c r="D17" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>153</v>
@@ -1309,8 +1348,8 @@
       <c r="C18" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>170</v>
+      <c r="D18" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>153</v>
@@ -1326,8 +1365,8 @@
       <c r="C19" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>170</v>
+      <c r="D19" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>153</v>
@@ -1343,8 +1382,8 @@
       <c r="C20" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>170</v>
+      <c r="D20" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>153</v>
@@ -1360,8 +1399,8 @@
       <c r="C21" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>170</v>
+      <c r="D21" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>153</v>
@@ -1377,8 +1416,8 @@
       <c r="C22" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>170</v>
+      <c r="D22" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>153</v>
@@ -1394,8 +1433,8 @@
       <c r="C23" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>170</v>
+      <c r="D23" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>153</v>
@@ -1411,8 +1450,8 @@
       <c r="C24" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>170</v>
+      <c r="D24" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>153</v>
@@ -1428,8 +1467,8 @@
       <c r="C25" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>170</v>
+      <c r="D25" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>153</v>
@@ -1445,8 +1484,8 @@
       <c r="C26" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="7" t="s">
-        <v>170</v>
+      <c r="D26" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>153</v>
@@ -1462,8 +1501,8 @@
       <c r="C27" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>170</v>
+      <c r="D27" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>153</v>
@@ -1479,8 +1518,8 @@
       <c r="C28" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>170</v>
+      <c r="D28" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>153</v>
@@ -1496,8 +1535,8 @@
       <c r="C29" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>170</v>
+      <c r="D29" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>153</v>
@@ -1513,8 +1552,8 @@
       <c r="C30" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D30" s="7" t="s">
-        <v>170</v>
+      <c r="D30" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>153</v>
@@ -1530,8 +1569,8 @@
       <c r="C31" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D31" s="7" t="s">
-        <v>170</v>
+      <c r="D31" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>153</v>
@@ -1547,8 +1586,8 @@
       <c r="C32" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="D32" s="7" t="s">
-        <v>170</v>
+      <c r="D32" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>153</v>
@@ -1564,8 +1603,8 @@
       <c r="C33" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="D33" s="7" t="s">
-        <v>170</v>
+      <c r="D33" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>153</v>
@@ -1581,8 +1620,8 @@
       <c r="C34" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="D34" s="7" t="s">
-        <v>170</v>
+      <c r="D34" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>153</v>
@@ -1598,8 +1637,8 @@
       <c r="C35" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="D35" s="7" t="s">
-        <v>170</v>
+      <c r="D35" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>153</v>
@@ -1615,8 +1654,8 @@
       <c r="C36" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D36" s="7" t="s">
-        <v>170</v>
+      <c r="D36" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>153</v>
@@ -1632,8 +1671,8 @@
       <c r="C37" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D37" s="7" t="s">
-        <v>170</v>
+      <c r="D37" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>153</v>
@@ -1649,8 +1688,8 @@
       <c r="C38" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D38" s="7" t="s">
-        <v>170</v>
+      <c r="D38" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>153</v>
@@ -1666,8 +1705,8 @@
       <c r="C39" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D39" s="7" t="s">
-        <v>170</v>
+      <c r="D39" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>153</v>
@@ -1683,8 +1722,8 @@
       <c r="C40" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D40" s="7" t="s">
-        <v>170</v>
+      <c r="D40" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>153</v>
@@ -1700,8 +1739,8 @@
       <c r="C41" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D41" s="7" t="s">
-        <v>170</v>
+      <c r="D41" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>153</v>
@@ -1717,8 +1756,8 @@
       <c r="C42" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="D42" s="7" t="s">
-        <v>170</v>
+      <c r="D42" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>153</v>
@@ -1734,8 +1773,8 @@
       <c r="C43" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="D43" s="7" t="s">
-        <v>170</v>
+      <c r="D43" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>153</v>
@@ -1751,8 +1790,8 @@
       <c r="C44" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D44" s="7" t="s">
-        <v>170</v>
+      <c r="D44" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>153</v>
@@ -1768,8 +1807,8 @@
       <c r="C45" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D45" s="7" t="s">
-        <v>170</v>
+      <c r="D45" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>153</v>
@@ -1785,8 +1824,8 @@
       <c r="C46" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D46" s="7" t="s">
-        <v>170</v>
+      <c r="D46" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>153</v>
@@ -1802,8 +1841,8 @@
       <c r="C47" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D47" s="7" t="s">
-        <v>170</v>
+      <c r="D47" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>153</v>
@@ -1819,8 +1858,8 @@
       <c r="C48" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="D48" s="7" t="s">
-        <v>170</v>
+      <c r="D48" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>153</v>
@@ -1828,18 +1867,103 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>76</v>
       </c>
       <c r="C49" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="D49" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="E49" s="3" t="s">
+      <c r="B50" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E54" s="3" t="s">
         <v>167</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding new test cases for watch list(TestCase_E30,TestCase_E31,TestCase_E32)
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="186">
   <si>
     <t>TCID</t>
   </si>
@@ -599,13 +599,52 @@
     <t>TestCase_B47</t>
   </si>
   <si>
+    <t>TestCase_B48</t>
+  </si>
+  <si>
+    <t>Verify that ALL option is selected in the left navigation pane by default when user searches using ALL option in the search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B49</t>
+  </si>
+  <si>
+    <t>Verify that search results related to all content types get displayed in the summary page when user searches using ALL option in search drop down</t>
+  </si>
+  <si>
+    <t>OPQA-301</t>
+  </si>
+  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>TestCase_B48</t>
-  </si>
-  <si>
-    <t>Verify that ALL option is selected in the left navigation pane by default when user searches using ALL option in the search drop down</t>
+    <t>TestCase_B50</t>
+  </si>
+  <si>
+    <t>OPQA-307</t>
+  </si>
+  <si>
+    <t>Verify that ARTICLES option is selected in the left navigation pane by default when user searches using ARTICLES option in the search drop down</t>
+  </si>
+  <si>
+    <t>Verify that PATENTS option is selected in the left navigation pane by default when user searches using PATENTS option in the search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B51</t>
+  </si>
+  <si>
+    <t>TestCase_B52</t>
+  </si>
+  <si>
+    <t>Verify that POSTS option is selected in the left navigation pane by default when user searches using POSTS option in the search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B53</t>
+  </si>
+  <si>
+    <t>Verify that PEOPLE option is selected in the left navigation pane by default when user searches using PEOPLE option in the search drop down</t>
+  </si>
+  <si>
+    <t>OPQA-375</t>
   </si>
 </sst>
 </file>
@@ -996,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="D54" sqref="D2:D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1037,8 +1076,8 @@
       <c r="C2" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>170</v>
+      <c r="D2" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>153</v>
@@ -1054,8 +1093,8 @@
       <c r="C3" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>170</v>
+      <c r="D3" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>153</v>
@@ -1071,8 +1110,8 @@
       <c r="C4" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>170</v>
+      <c r="D4" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>153</v>
@@ -1088,8 +1127,8 @@
       <c r="C5" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>170</v>
+      <c r="D5" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>153</v>
@@ -1105,8 +1144,8 @@
       <c r="C6" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>170</v>
+      <c r="D6" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>153</v>
@@ -1122,8 +1161,8 @@
       <c r="C7" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>170</v>
+      <c r="D7" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>153</v>
@@ -1139,8 +1178,8 @@
       <c r="C8" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>170</v>
+      <c r="D8" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>153</v>
@@ -1156,8 +1195,8 @@
       <c r="C9" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>170</v>
+      <c r="D9" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>153</v>
@@ -1173,8 +1212,8 @@
       <c r="C10" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>170</v>
+      <c r="D10" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>153</v>
@@ -1190,8 +1229,8 @@
       <c r="C11" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>170</v>
+      <c r="D11" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>153</v>
@@ -1207,8 +1246,8 @@
       <c r="C12" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>170</v>
+      <c r="D12" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>153</v>
@@ -1224,8 +1263,8 @@
       <c r="C13" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>170</v>
+      <c r="D13" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>153</v>
@@ -1241,8 +1280,8 @@
       <c r="C14" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>170</v>
+      <c r="D14" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>153</v>
@@ -1258,8 +1297,8 @@
       <c r="C15" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>170</v>
+      <c r="D15" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>153</v>
@@ -1275,8 +1314,8 @@
       <c r="C16" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>170</v>
+      <c r="D16" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>153</v>
@@ -1292,8 +1331,8 @@
       <c r="C17" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>170</v>
+      <c r="D17" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>153</v>
@@ -1309,8 +1348,8 @@
       <c r="C18" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>170</v>
+      <c r="D18" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>153</v>
@@ -1326,8 +1365,8 @@
       <c r="C19" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>170</v>
+      <c r="D19" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>153</v>
@@ -1343,8 +1382,8 @@
       <c r="C20" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>170</v>
+      <c r="D20" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>153</v>
@@ -1360,8 +1399,8 @@
       <c r="C21" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>170</v>
+      <c r="D21" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>153</v>
@@ -1377,8 +1416,8 @@
       <c r="C22" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>170</v>
+      <c r="D22" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>153</v>
@@ -1394,8 +1433,8 @@
       <c r="C23" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>170</v>
+      <c r="D23" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>153</v>
@@ -1411,8 +1450,8 @@
       <c r="C24" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>170</v>
+      <c r="D24" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>153</v>
@@ -1428,8 +1467,8 @@
       <c r="C25" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>170</v>
+      <c r="D25" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>153</v>
@@ -1445,8 +1484,8 @@
       <c r="C26" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="7" t="s">
-        <v>170</v>
+      <c r="D26" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>153</v>
@@ -1462,8 +1501,8 @@
       <c r="C27" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>170</v>
+      <c r="D27" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>153</v>
@@ -1479,8 +1518,8 @@
       <c r="C28" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>170</v>
+      <c r="D28" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>153</v>
@@ -1496,8 +1535,8 @@
       <c r="C29" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>170</v>
+      <c r="D29" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>153</v>
@@ -1513,8 +1552,8 @@
       <c r="C30" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D30" s="7" t="s">
-        <v>170</v>
+      <c r="D30" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>153</v>
@@ -1530,8 +1569,8 @@
       <c r="C31" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D31" s="7" t="s">
-        <v>170</v>
+      <c r="D31" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>153</v>
@@ -1547,8 +1586,8 @@
       <c r="C32" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="D32" s="7" t="s">
-        <v>170</v>
+      <c r="D32" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>153</v>
@@ -1564,8 +1603,8 @@
       <c r="C33" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="D33" s="7" t="s">
-        <v>170</v>
+      <c r="D33" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>153</v>
@@ -1581,8 +1620,8 @@
       <c r="C34" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="D34" s="7" t="s">
-        <v>170</v>
+      <c r="D34" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>153</v>
@@ -1598,8 +1637,8 @@
       <c r="C35" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="D35" s="7" t="s">
-        <v>170</v>
+      <c r="D35" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>153</v>
@@ -1615,8 +1654,8 @@
       <c r="C36" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D36" s="7" t="s">
-        <v>170</v>
+      <c r="D36" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>153</v>
@@ -1632,8 +1671,8 @@
       <c r="C37" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D37" s="7" t="s">
-        <v>170</v>
+      <c r="D37" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>153</v>
@@ -1649,8 +1688,8 @@
       <c r="C38" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D38" s="7" t="s">
-        <v>170</v>
+      <c r="D38" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>153</v>
@@ -1666,8 +1705,8 @@
       <c r="C39" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D39" s="7" t="s">
-        <v>170</v>
+      <c r="D39" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>153</v>
@@ -1683,8 +1722,8 @@
       <c r="C40" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D40" s="7" t="s">
-        <v>170</v>
+      <c r="D40" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>153</v>
@@ -1700,8 +1739,8 @@
       <c r="C41" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D41" s="7" t="s">
-        <v>170</v>
+      <c r="D41" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>153</v>
@@ -1717,8 +1756,8 @@
       <c r="C42" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="D42" s="7" t="s">
-        <v>170</v>
+      <c r="D42" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>153</v>
@@ -1734,8 +1773,8 @@
       <c r="C43" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="D43" s="7" t="s">
-        <v>170</v>
+      <c r="D43" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>153</v>
@@ -1751,8 +1790,8 @@
       <c r="C44" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D44" s="7" t="s">
-        <v>170</v>
+      <c r="D44" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>153</v>
@@ -1768,8 +1807,8 @@
       <c r="C45" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D45" s="7" t="s">
-        <v>170</v>
+      <c r="D45" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>153</v>
@@ -1785,8 +1824,8 @@
       <c r="C46" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D46" s="7" t="s">
-        <v>170</v>
+      <c r="D46" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>153</v>
@@ -1802,8 +1841,8 @@
       <c r="C47" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D47" s="7" t="s">
-        <v>170</v>
+      <c r="D47" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>153</v>
@@ -1819,8 +1858,8 @@
       <c r="C48" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="D48" s="7" t="s">
-        <v>170</v>
+      <c r="D48" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>153</v>
@@ -1828,18 +1867,103 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>76</v>
       </c>
       <c r="C49" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="D49" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="E49" s="3" t="s">
+      <c r="B50" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E54" s="3" t="s">
         <v>167</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding new test scripts for watch list(TestCase_E33,TestCase_E34)
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="196">
   <si>
     <t>TCID</t>
   </si>
@@ -645,6 +645,36 @@
   </si>
   <si>
     <t>OPQA-375</t>
+  </si>
+  <si>
+    <t>TestCase_B54</t>
+  </si>
+  <si>
+    <t>OPQA-316</t>
+  </si>
+  <si>
+    <t>Verify that only articles get displayed in the summary page when user searches using ARTICLES content type in search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B55</t>
+  </si>
+  <si>
+    <t>Verify that only patents get displayed in the summary page when user searches using PATENTS content type in search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B56</t>
+  </si>
+  <si>
+    <t>Verify that only posts get displayed in the summary page when user searches using POSTS content type in search drop down</t>
+  </si>
+  <si>
+    <t>Verify that only people get displayed in the summary page when user searches using people content type in search drop down</t>
+  </si>
+  <si>
+    <t>OPQA-380</t>
+  </si>
+  <si>
+    <t>TestCase_B57</t>
   </si>
 </sst>
 </file>
@@ -1035,10 +1065,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="D54" sqref="D2:D54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1076,7 +1106,7 @@
       <c r="C2" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -1093,7 +1123,7 @@
       <c r="C3" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -1110,7 +1140,7 @@
       <c r="C4" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -1127,7 +1157,7 @@
       <c r="C5" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -1144,7 +1174,7 @@
       <c r="C6" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -1161,7 +1191,7 @@
       <c r="C7" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -1178,7 +1208,7 @@
       <c r="C8" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -1195,7 +1225,7 @@
       <c r="C9" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -1212,7 +1242,7 @@
       <c r="C10" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -1229,7 +1259,7 @@
       <c r="C11" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -1246,7 +1276,7 @@
       <c r="C12" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -1263,7 +1293,7 @@
       <c r="C13" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -1280,7 +1310,7 @@
       <c r="C14" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -1297,7 +1327,7 @@
       <c r="C15" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -1314,7 +1344,7 @@
       <c r="C16" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -1331,7 +1361,7 @@
       <c r="C17" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E17" s="3" t="s">
@@ -1348,7 +1378,7 @@
       <c r="C18" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E18" s="3" t="s">
@@ -1365,7 +1395,7 @@
       <c r="C19" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E19" s="3" t="s">
@@ -1382,7 +1412,7 @@
       <c r="C20" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E20" s="3" t="s">
@@ -1399,7 +1429,7 @@
       <c r="C21" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E21" s="3" t="s">
@@ -1416,7 +1446,7 @@
       <c r="C22" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E22" s="3" t="s">
@@ -1433,7 +1463,7 @@
       <c r="C23" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E23" s="3" t="s">
@@ -1450,7 +1480,7 @@
       <c r="C24" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E24" s="3" t="s">
@@ -1467,7 +1497,7 @@
       <c r="C25" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E25" s="3" t="s">
@@ -1484,7 +1514,7 @@
       <c r="C26" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E26" s="3" t="s">
@@ -1501,7 +1531,7 @@
       <c r="C27" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E27" s="3" t="s">
@@ -1518,7 +1548,7 @@
       <c r="C28" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E28" s="3" t="s">
@@ -1535,7 +1565,7 @@
       <c r="C29" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E29" s="3" t="s">
@@ -1552,7 +1582,7 @@
       <c r="C30" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E30" s="3" t="s">
@@ -1569,7 +1599,7 @@
       <c r="C31" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E31" s="3" t="s">
@@ -1586,7 +1616,7 @@
       <c r="C32" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E32" s="3" t="s">
@@ -1603,7 +1633,7 @@
       <c r="C33" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E33" s="3" t="s">
@@ -1620,7 +1650,7 @@
       <c r="C34" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E34" s="3" t="s">
@@ -1637,7 +1667,7 @@
       <c r="C35" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E35" s="3" t="s">
@@ -1654,7 +1684,7 @@
       <c r="C36" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E36" s="3" t="s">
@@ -1671,7 +1701,7 @@
       <c r="C37" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E37" s="3" t="s">
@@ -1688,7 +1718,7 @@
       <c r="C38" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E38" s="3" t="s">
@@ -1705,7 +1735,7 @@
       <c r="C39" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E39" s="3" t="s">
@@ -1722,7 +1752,7 @@
       <c r="C40" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E40" s="3" t="s">
@@ -1739,7 +1769,7 @@
       <c r="C41" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E41" s="3" t="s">
@@ -1756,7 +1786,7 @@
       <c r="C42" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E42" s="3" t="s">
@@ -1773,7 +1803,7 @@
       <c r="C43" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E43" s="3" t="s">
@@ -1790,7 +1820,7 @@
       <c r="C44" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E44" s="3" t="s">
@@ -1807,7 +1837,7 @@
       <c r="C45" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E45" s="3" t="s">
@@ -1824,7 +1854,7 @@
       <c r="C46" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E46" s="3" t="s">
@@ -1841,7 +1871,7 @@
       <c r="C47" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E47" s="3" t="s">
@@ -1858,7 +1888,7 @@
       <c r="C48" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E48" s="3" t="s">
@@ -1875,7 +1905,7 @@
       <c r="C49" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E49" s="3" t="s">
@@ -1892,7 +1922,7 @@
       <c r="C50" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E50" s="3" t="s">
@@ -1909,7 +1939,7 @@
       <c r="C51" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D51" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E51" s="3" t="s">
@@ -1926,7 +1956,7 @@
       <c r="C52" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E52" s="3" t="s">
@@ -1943,7 +1973,7 @@
       <c r="C53" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D53" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E53" s="3" t="s">
@@ -1960,10 +1990,78 @@
       <c r="C54" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="D54" s="7" t="s">
         <v>175</v>
       </c>
       <c r="E54" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="E58" s="3" t="s">
         <v>167</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding 5 search test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="211">
   <si>
     <t>TCID</t>
   </si>
@@ -590,97 +590,149 @@
     <t>TestCase_B46</t>
   </si>
   <si>
+    <t>Verify that user is able to select any of the content types present in search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B47</t>
+  </si>
+  <si>
+    <t>TestCase_B48</t>
+  </si>
+  <si>
+    <t>Verify that ALL option is selected in the left navigation pane by default when user searches using ALL option in the search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B49</t>
+  </si>
+  <si>
+    <t>Verify that search results related to all content types get displayed in the summary page when user searches using ALL option in search drop down</t>
+  </si>
+  <si>
+    <t>OPQA-301</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>TestCase_B50</t>
+  </si>
+  <si>
+    <t>OPQA-307</t>
+  </si>
+  <si>
+    <t>Verify that ARTICLES option is selected in the left navigation pane by default when user searches using ARTICLES option in the search drop down</t>
+  </si>
+  <si>
+    <t>Verify that PATENTS option is selected in the left navigation pane by default when user searches using PATENTS option in the search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B51</t>
+  </si>
+  <si>
+    <t>TestCase_B52</t>
+  </si>
+  <si>
+    <t>Verify that POSTS option is selected in the left navigation pane by default when user searches using POSTS option in the search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B53</t>
+  </si>
+  <si>
+    <t>Verify that PEOPLE option is selected in the left navigation pane by default when user searches using PEOPLE option in the search drop down</t>
+  </si>
+  <si>
+    <t>OPQA-375</t>
+  </si>
+  <si>
+    <t>TestCase_B54</t>
+  </si>
+  <si>
+    <t>OPQA-316</t>
+  </si>
+  <si>
+    <t>Verify that only articles get displayed in the summary page when user searches using ARTICLES content type in search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B55</t>
+  </si>
+  <si>
+    <t>Verify that only patents get displayed in the summary page when user searches using PATENTS content type in search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B56</t>
+  </si>
+  <si>
+    <t>Verify that only posts get displayed in the summary page when user searches using POSTS content type in search drop down</t>
+  </si>
+  <si>
+    <t>Verify that only people get displayed in the summary page when user searches using people content type in search drop down</t>
+  </si>
+  <si>
+    <t>OPQA-380</t>
+  </si>
+  <si>
+    <t>TestCase_B57</t>
+  </si>
+  <si>
+    <t>TestCase_B58</t>
+  </si>
+  <si>
+    <t>OPQA-287</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Verify that the following sections get displayed in the search type ahead when user searches using ALL option in the search drop down and that the searched keyword is present in all the sections:
+a)Autocompleted keyword
+b)4 suggestions in CATEGORY section
+c)4 suggestions in ARTICLES section
+d)4 suggestions in PATENTS section
+e)4 suggestions in POSTS section
+f)4 suggestions in PEOPLE section</t>
+  </si>
+  <si>
+    <t>OPQA-311</t>
+  </si>
+  <si>
+    <t>Verify that 10 article suggestions get displayed in the search type ahead when user searches using ARTICLES option in the search drop down and that the searched keyword is present in all the suggestions</t>
+  </si>
+  <si>
+    <t>TestCase_B59</t>
+  </si>
+  <si>
+    <t>TestCase_B60</t>
+  </si>
+  <si>
+    <t>Verify that 10 patent suggestions get displayed in the search type ahead when user searches using PATENTS option in the search drop down and that the searched keyword is present in all the suggestions</t>
+  </si>
+  <si>
+    <t>TestCase_B61</t>
+  </si>
+  <si>
+    <t>Verify that 10 post suggestions get displayed in the search type ahead when user searches using POSTS option in the search drop down and that the searched keyword is present in all the suggestions</t>
+  </si>
+  <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>Verify that user is able to select any of the content types present in search drop down</t>
-  </si>
-  <si>
-    <t>TestCase_B47</t>
-  </si>
-  <si>
-    <t>TestCase_B48</t>
-  </si>
-  <si>
-    <t>Verify that ALL option is selected in the left navigation pane by default when user searches using ALL option in the search drop down</t>
-  </si>
-  <si>
-    <t>TestCase_B49</t>
-  </si>
-  <si>
-    <t>Verify that search results related to all content types get displayed in the summary page when user searches using ALL option in search drop down</t>
-  </si>
-  <si>
-    <t>OPQA-301</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>TestCase_B50</t>
-  </si>
-  <si>
-    <t>OPQA-307</t>
-  </si>
-  <si>
-    <t>Verify that ARTICLES option is selected in the left navigation pane by default when user searches using ARTICLES option in the search drop down</t>
-  </si>
-  <si>
-    <t>Verify that PATENTS option is selected in the left navigation pane by default when user searches using PATENTS option in the search drop down</t>
-  </si>
-  <si>
-    <t>TestCase_B51</t>
-  </si>
-  <si>
-    <t>TestCase_B52</t>
-  </si>
-  <si>
-    <t>Verify that POSTS option is selected in the left navigation pane by default when user searches using POSTS option in the search drop down</t>
-  </si>
-  <si>
-    <t>TestCase_B53</t>
-  </si>
-  <si>
-    <t>Verify that PEOPLE option is selected in the left navigation pane by default when user searches using PEOPLE option in the search drop down</t>
-  </si>
-  <si>
-    <t>OPQA-375</t>
-  </si>
-  <si>
-    <t>TestCase_B54</t>
-  </si>
-  <si>
-    <t>OPQA-316</t>
-  </si>
-  <si>
-    <t>Verify that only articles get displayed in the summary page when user searches using ARTICLES content type in search drop down</t>
-  </si>
-  <si>
-    <t>TestCase_B55</t>
-  </si>
-  <si>
-    <t>Verify that only patents get displayed in the summary page when user searches using PATENTS content type in search drop down</t>
-  </si>
-  <si>
-    <t>TestCase_B56</t>
-  </si>
-  <si>
-    <t>Verify that only posts get displayed in the summary page when user searches using POSTS content type in search drop down</t>
-  </si>
-  <si>
-    <t>Verify that only people get displayed in the summary page when user searches using people content type in search drop down</t>
-  </si>
-  <si>
-    <t>OPQA-380</t>
-  </si>
-  <si>
-    <t>TestCase_B57</t>
+    <t>TestCase_B62</t>
+  </si>
+  <si>
+    <t>Verify that 10 people suggestions get displayed in the search type ahead when user searches using PEOPLE option in the search drop down and that the searched keyword is present in all the suggestions</t>
+  </si>
+  <si>
+    <t>OPQA-378</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -1065,18 +1117,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="136.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="136.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1107,7 +1159,7 @@
         <v>97</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>153</v>
@@ -1124,7 +1176,7 @@
         <v>77</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>153</v>
@@ -1141,7 +1193,7 @@
         <v>78</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>153</v>
@@ -1158,7 +1210,7 @@
         <v>79</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>153</v>
@@ -1175,7 +1227,7 @@
         <v>80</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>153</v>
@@ -1192,7 +1244,7 @@
         <v>81</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>153</v>
@@ -1209,7 +1261,7 @@
         <v>74</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>153</v>
@@ -1226,7 +1278,7 @@
         <v>82</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>153</v>
@@ -1243,7 +1295,7 @@
         <v>83</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>153</v>
@@ -1260,7 +1312,7 @@
         <v>84</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>153</v>
@@ -1277,7 +1329,7 @@
         <v>85</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>153</v>
@@ -1294,7 +1346,7 @@
         <v>101</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>153</v>
@@ -1311,7 +1363,7 @@
         <v>86</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>153</v>
@@ -1328,7 +1380,7 @@
         <v>87</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>153</v>
@@ -1345,7 +1397,7 @@
         <v>88</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>153</v>
@@ -1362,7 +1414,7 @@
         <v>89</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>153</v>
@@ -1379,7 +1431,7 @@
         <v>140</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>153</v>
@@ -1396,7 +1448,7 @@
         <v>90</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>153</v>
@@ -1413,7 +1465,7 @@
         <v>91</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>153</v>
@@ -1430,7 +1482,7 @@
         <v>92</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>153</v>
@@ -1447,7 +1499,7 @@
         <v>93</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>153</v>
@@ -1464,7 +1516,7 @@
         <v>94</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>153</v>
@@ -1481,7 +1533,7 @@
         <v>95</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>153</v>
@@ -1498,7 +1550,7 @@
         <v>96</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>153</v>
@@ -1515,7 +1567,7 @@
         <v>104</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>153</v>
@@ -1532,7 +1584,7 @@
         <v>107</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>153</v>
@@ -1549,7 +1601,7 @@
         <v>110</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>153</v>
@@ -1566,7 +1618,7 @@
         <v>111</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>153</v>
@@ -1583,7 +1635,7 @@
         <v>116</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>153</v>
@@ -1600,7 +1652,7 @@
         <v>119</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>153</v>
@@ -1617,7 +1669,7 @@
         <v>122</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>153</v>
@@ -1634,7 +1686,7 @@
         <v>124</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>153</v>
@@ -1651,7 +1703,7 @@
         <v>126</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>153</v>
@@ -1668,7 +1720,7 @@
         <v>128</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>153</v>
@@ -1685,7 +1737,7 @@
         <v>134</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>153</v>
@@ -1702,7 +1754,7 @@
         <v>137</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>153</v>
@@ -1719,7 +1771,7 @@
         <v>140</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>153</v>
@@ -1736,7 +1788,7 @@
         <v>143</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>153</v>
@@ -1753,7 +1805,7 @@
         <v>146</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>153</v>
@@ -1770,7 +1822,7 @@
         <v>149</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>153</v>
@@ -1787,7 +1839,7 @@
         <v>152</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>153</v>
@@ -1804,7 +1856,7 @@
         <v>160</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>153</v>
@@ -1821,7 +1873,7 @@
         <v>161</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>153</v>
@@ -1838,7 +1890,7 @@
         <v>162</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>153</v>
@@ -1855,7 +1907,7 @@
         <v>163</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>153</v>
@@ -1872,7 +1924,7 @@
         <v>165</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>153</v>
@@ -1880,16 +1932,16 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>67</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>153</v>
@@ -1897,16 +1949,16 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>76</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>153</v>
@@ -1914,16 +1966,16 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C50" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B50" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>173</v>
-      </c>
       <c r="D50" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>153</v>
@@ -1931,16 +1983,16 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B51" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="C51" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="C51" s="4" t="s">
-        <v>178</v>
-      </c>
       <c r="D51" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>153</v>
@@ -1948,16 +2000,16 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>68</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>153</v>
@@ -1965,16 +2017,16 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>71</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>153</v>
@@ -1982,16 +2034,16 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C54" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="B54" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>184</v>
-      </c>
       <c r="D54" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>153</v>
@@ -1999,16 +2051,16 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="B55" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="C55" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="C55" s="4" t="s">
-        <v>188</v>
-      </c>
       <c r="D55" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>153</v>
@@ -2016,16 +2068,16 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>69</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>153</v>
@@ -2033,16 +2085,16 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>73</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>153</v>
@@ -2050,19 +2102,104 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="120">
+      <c r="A59" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="B58" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D58" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>167</v>
+      <c r="B59" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="30">
+      <c r="A60" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="30">
+      <c r="A61" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="30">
+      <c r="A62" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="30">
+      <c r="A63" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -2081,10 +2218,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="52.5703125" style="5" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.85546875" style="5" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="12.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="5" width="52.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="5" width="83.85546875" collapsed="true"/>
+    <col min="4" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="35.25" customHeight="1">

</xml_diff>

<commit_message>
B suite.xlsx and OR.properties files changed
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="209">
   <si>
     <t>TCID</t>
   </si>
@@ -680,9 +680,6 @@
     <t>OPQA-287</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>Verify that the following sections get displayed in the search type ahead when user searches using ALL option in the search drop down and that the searched keyword is present in all the sections:
 a)Autocompleted keyword
 b)4 suggestions in CATEGORY section
@@ -724,15 +721,11 @@
   <si>
     <t>OPQA-378</t>
   </si>
-  <si>
-    <t>FAIL</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -1119,16 +1112,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="136.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="2" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="136.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1159,7 +1152,7 @@
         <v>97</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>153</v>
@@ -1176,7 +1169,7 @@
         <v>77</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>153</v>
@@ -1193,7 +1186,7 @@
         <v>78</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>153</v>
@@ -1210,7 +1203,7 @@
         <v>79</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>153</v>
@@ -1227,7 +1220,7 @@
         <v>80</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>153</v>
@@ -1244,7 +1237,7 @@
         <v>81</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>153</v>
@@ -1261,7 +1254,7 @@
         <v>74</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>153</v>
@@ -1278,7 +1271,7 @@
         <v>82</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>153</v>
@@ -1295,7 +1288,7 @@
         <v>83</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>153</v>
@@ -1312,7 +1305,7 @@
         <v>84</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>153</v>
@@ -1329,7 +1322,7 @@
         <v>85</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>153</v>
@@ -1346,7 +1339,7 @@
         <v>101</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>153</v>
@@ -1363,7 +1356,7 @@
         <v>86</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>153</v>
@@ -1380,7 +1373,7 @@
         <v>87</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>153</v>
@@ -1397,7 +1390,7 @@
         <v>88</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>153</v>
@@ -1414,7 +1407,7 @@
         <v>89</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>153</v>
@@ -1431,7 +1424,7 @@
         <v>140</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>153</v>
@@ -1448,7 +1441,7 @@
         <v>90</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>153</v>
@@ -1465,7 +1458,7 @@
         <v>91</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>153</v>
@@ -1482,7 +1475,7 @@
         <v>92</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>153</v>
@@ -1499,7 +1492,7 @@
         <v>93</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>153</v>
@@ -1516,7 +1509,7 @@
         <v>94</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>153</v>
@@ -1533,7 +1526,7 @@
         <v>95</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>153</v>
@@ -1550,7 +1543,7 @@
         <v>96</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>153</v>
@@ -1567,7 +1560,7 @@
         <v>104</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>153</v>
@@ -1584,7 +1577,7 @@
         <v>107</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>153</v>
@@ -1601,7 +1594,7 @@
         <v>110</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>153</v>
@@ -1618,7 +1611,7 @@
         <v>111</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>153</v>
@@ -1635,7 +1628,7 @@
         <v>116</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>153</v>
@@ -1652,7 +1645,7 @@
         <v>119</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>153</v>
@@ -1669,7 +1662,7 @@
         <v>122</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>153</v>
@@ -1686,7 +1679,7 @@
         <v>124</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>153</v>
@@ -1703,7 +1696,7 @@
         <v>126</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>153</v>
@@ -1720,7 +1713,7 @@
         <v>128</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>153</v>
@@ -1737,7 +1730,7 @@
         <v>134</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>153</v>
@@ -1754,7 +1747,7 @@
         <v>137</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>153</v>
@@ -1771,7 +1764,7 @@
         <v>140</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>153</v>
@@ -1788,7 +1781,7 @@
         <v>143</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>153</v>
@@ -1805,7 +1798,7 @@
         <v>146</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>153</v>
@@ -1822,7 +1815,7 @@
         <v>149</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>153</v>
@@ -1839,7 +1832,7 @@
         <v>152</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>153</v>
@@ -1856,7 +1849,7 @@
         <v>160</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>153</v>
@@ -1873,7 +1866,7 @@
         <v>161</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>153</v>
@@ -1890,7 +1883,7 @@
         <v>162</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>153</v>
@@ -1907,7 +1900,7 @@
         <v>163</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>153</v>
@@ -1924,7 +1917,7 @@
         <v>165</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>153</v>
@@ -1941,7 +1934,7 @@
         <v>167</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>153</v>
@@ -1958,7 +1951,7 @@
         <v>170</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>153</v>
@@ -1975,7 +1968,7 @@
         <v>172</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>153</v>
@@ -1992,7 +1985,7 @@
         <v>177</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>153</v>
@@ -2009,7 +2002,7 @@
         <v>178</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>153</v>
@@ -2026,7 +2019,7 @@
         <v>181</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>153</v>
@@ -2043,7 +2036,7 @@
         <v>183</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>153</v>
@@ -2060,7 +2053,7 @@
         <v>187</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>153</v>
@@ -2077,7 +2070,7 @@
         <v>189</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>153</v>
@@ -2094,7 +2087,7 @@
         <v>191</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>153</v>
@@ -2111,7 +2104,7 @@
         <v>192</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>153</v>
@@ -2125,27 +2118,27 @@
         <v>196</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D59" s="7" t="s">
         <v>174</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="30">
       <c r="A60" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B60" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="C60" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="C60" s="4" t="s">
-        <v>200</v>
-      </c>
       <c r="D60" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>153</v>
@@ -2153,16 +2146,16 @@
     </row>
     <row r="61" spans="1:5" ht="30">
       <c r="A61" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>70</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>153</v>
@@ -2170,16 +2163,16 @@
     </row>
     <row r="62" spans="1:5" ht="30">
       <c r="A62" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B62" s="8" t="s">
         <v>72</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>153</v>
@@ -2187,16 +2180,16 @@
     </row>
     <row r="63" spans="1:5" ht="30">
       <c r="A63" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C63" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="B63" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>197</v>
+      <c r="D63" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>153</v>
@@ -2218,10 +2211,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="12.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="5" width="52.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="5" width="83.85546875" collapsed="true"/>
-    <col min="4" max="16384" style="5" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="52.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.85546875" style="5" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="35.25" customHeight="1">

</xml_diff>

<commit_message>
taking latest changes and appending new profile scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="209">
   <si>
     <t>TCID</t>
   </si>
@@ -590,61 +590,136 @@
     <t>TestCase_B46</t>
   </si>
   <si>
+    <t>Verify that user is able to select any of the content types present in search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B47</t>
+  </si>
+  <si>
+    <t>TestCase_B48</t>
+  </si>
+  <si>
+    <t>Verify that ALL option is selected in the left navigation pane by default when user searches using ALL option in the search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B49</t>
+  </si>
+  <si>
+    <t>Verify that search results related to all content types get displayed in the summary page when user searches using ALL option in search drop down</t>
+  </si>
+  <si>
+    <t>OPQA-301</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>TestCase_B50</t>
+  </si>
+  <si>
+    <t>OPQA-307</t>
+  </si>
+  <si>
+    <t>Verify that ARTICLES option is selected in the left navigation pane by default when user searches using ARTICLES option in the search drop down</t>
+  </si>
+  <si>
+    <t>Verify that PATENTS option is selected in the left navigation pane by default when user searches using PATENTS option in the search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B51</t>
+  </si>
+  <si>
+    <t>TestCase_B52</t>
+  </si>
+  <si>
+    <t>Verify that POSTS option is selected in the left navigation pane by default when user searches using POSTS option in the search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B53</t>
+  </si>
+  <si>
+    <t>Verify that PEOPLE option is selected in the left navigation pane by default when user searches using PEOPLE option in the search drop down</t>
+  </si>
+  <si>
+    <t>OPQA-375</t>
+  </si>
+  <si>
+    <t>TestCase_B54</t>
+  </si>
+  <si>
+    <t>OPQA-316</t>
+  </si>
+  <si>
+    <t>Verify that only articles get displayed in the summary page when user searches using ARTICLES content type in search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B55</t>
+  </si>
+  <si>
+    <t>Verify that only patents get displayed in the summary page when user searches using PATENTS content type in search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B56</t>
+  </si>
+  <si>
+    <t>Verify that only posts get displayed in the summary page when user searches using POSTS content type in search drop down</t>
+  </si>
+  <si>
+    <t>Verify that only people get displayed in the summary page when user searches using people content type in search drop down</t>
+  </si>
+  <si>
+    <t>OPQA-380</t>
+  </si>
+  <si>
+    <t>TestCase_B57</t>
+  </si>
+  <si>
+    <t>TestCase_B58</t>
+  </si>
+  <si>
+    <t>OPQA-287</t>
+  </si>
+  <si>
+    <t>Verify that the following sections get displayed in the search type ahead when user searches using ALL option in the search drop down and that the searched keyword is present in all the sections:
+a)Autocompleted keyword
+b)4 suggestions in CATEGORY section
+c)4 suggestions in ARTICLES section
+d)4 suggestions in PATENTS section
+e)4 suggestions in POSTS section
+f)4 suggestions in PEOPLE section</t>
+  </si>
+  <si>
+    <t>OPQA-311</t>
+  </si>
+  <si>
+    <t>Verify that 10 article suggestions get displayed in the search type ahead when user searches using ARTICLES option in the search drop down and that the searched keyword is present in all the suggestions</t>
+  </si>
+  <si>
+    <t>TestCase_B59</t>
+  </si>
+  <si>
+    <t>TestCase_B60</t>
+  </si>
+  <si>
+    <t>Verify that 10 patent suggestions get displayed in the search type ahead when user searches using PATENTS option in the search drop down and that the searched keyword is present in all the suggestions</t>
+  </si>
+  <si>
+    <t>TestCase_B61</t>
+  </si>
+  <si>
+    <t>Verify that 10 post suggestions get displayed in the search type ahead when user searches using POSTS option in the search drop down and that the searched keyword is present in all the suggestions</t>
+  </si>
+  <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>Verify that user is able to select any of the content types present in search drop down</t>
-  </si>
-  <si>
-    <t>TestCase_B47</t>
-  </si>
-  <si>
-    <t>TestCase_B48</t>
-  </si>
-  <si>
-    <t>Verify that ALL option is selected in the left navigation pane by default when user searches using ALL option in the search drop down</t>
-  </si>
-  <si>
-    <t>TestCase_B49</t>
-  </si>
-  <si>
-    <t>Verify that search results related to all content types get displayed in the summary page when user searches using ALL option in search drop down</t>
-  </si>
-  <si>
-    <t>OPQA-301</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>TestCase_B50</t>
-  </si>
-  <si>
-    <t>OPQA-307</t>
-  </si>
-  <si>
-    <t>Verify that ARTICLES option is selected in the left navigation pane by default when user searches using ARTICLES option in the search drop down</t>
-  </si>
-  <si>
-    <t>Verify that PATENTS option is selected in the left navigation pane by default when user searches using PATENTS option in the search drop down</t>
-  </si>
-  <si>
-    <t>TestCase_B51</t>
-  </si>
-  <si>
-    <t>TestCase_B52</t>
-  </si>
-  <si>
-    <t>Verify that POSTS option is selected in the left navigation pane by default when user searches using POSTS option in the search drop down</t>
-  </si>
-  <si>
-    <t>TestCase_B53</t>
-  </si>
-  <si>
-    <t>Verify that PEOPLE option is selected in the left navigation pane by default when user searches using PEOPLE option in the search drop down</t>
-  </si>
-  <si>
-    <t>OPQA-375</t>
+    <t>TestCase_B62</t>
+  </si>
+  <si>
+    <t>Verify that 10 people suggestions get displayed in the search type ahead when user searches using PEOPLE option in the search drop down and that the searched keyword is present in all the suggestions</t>
+  </si>
+  <si>
+    <t>OPQA-378</t>
   </si>
 </sst>
 </file>
@@ -1035,10 +1110,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="D54" sqref="D2:D54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1076,8 +1151,8 @@
       <c r="C2" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>175</v>
+      <c r="D2" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>153</v>
@@ -1093,8 +1168,8 @@
       <c r="C3" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>175</v>
+      <c r="D3" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>153</v>
@@ -1110,8 +1185,8 @@
       <c r="C4" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>175</v>
+      <c r="D4" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>153</v>
@@ -1127,8 +1202,8 @@
       <c r="C5" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>175</v>
+      <c r="D5" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>153</v>
@@ -1144,8 +1219,8 @@
       <c r="C6" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>175</v>
+      <c r="D6" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>153</v>
@@ -1161,8 +1236,8 @@
       <c r="C7" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>175</v>
+      <c r="D7" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>153</v>
@@ -1178,8 +1253,8 @@
       <c r="C8" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>175</v>
+      <c r="D8" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>153</v>
@@ -1195,8 +1270,8 @@
       <c r="C9" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>175</v>
+      <c r="D9" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>153</v>
@@ -1212,8 +1287,8 @@
       <c r="C10" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>175</v>
+      <c r="D10" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>153</v>
@@ -1229,8 +1304,8 @@
       <c r="C11" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>175</v>
+      <c r="D11" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>153</v>
@@ -1246,8 +1321,8 @@
       <c r="C12" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>175</v>
+      <c r="D12" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>153</v>
@@ -1263,8 +1338,8 @@
       <c r="C13" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>175</v>
+      <c r="D13" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>153</v>
@@ -1280,8 +1355,8 @@
       <c r="C14" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>175</v>
+      <c r="D14" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>153</v>
@@ -1297,8 +1372,8 @@
       <c r="C15" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>175</v>
+      <c r="D15" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>153</v>
@@ -1314,8 +1389,8 @@
       <c r="C16" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>175</v>
+      <c r="D16" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>153</v>
@@ -1331,8 +1406,8 @@
       <c r="C17" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>175</v>
+      <c r="D17" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>153</v>
@@ -1348,8 +1423,8 @@
       <c r="C18" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>175</v>
+      <c r="D18" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>153</v>
@@ -1365,8 +1440,8 @@
       <c r="C19" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>175</v>
+      <c r="D19" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>153</v>
@@ -1382,8 +1457,8 @@
       <c r="C20" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>175</v>
+      <c r="D20" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>153</v>
@@ -1399,8 +1474,8 @@
       <c r="C21" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>175</v>
+      <c r="D21" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>153</v>
@@ -1416,8 +1491,8 @@
       <c r="C22" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>175</v>
+      <c r="D22" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>153</v>
@@ -1433,8 +1508,8 @@
       <c r="C23" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>175</v>
+      <c r="D23" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>153</v>
@@ -1450,8 +1525,8 @@
       <c r="C24" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>175</v>
+      <c r="D24" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>153</v>
@@ -1467,8 +1542,8 @@
       <c r="C25" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>175</v>
+      <c r="D25" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>153</v>
@@ -1484,8 +1559,8 @@
       <c r="C26" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>175</v>
+      <c r="D26" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>153</v>
@@ -1501,8 +1576,8 @@
       <c r="C27" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>175</v>
+      <c r="D27" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>153</v>
@@ -1518,8 +1593,8 @@
       <c r="C28" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>175</v>
+      <c r="D28" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>153</v>
@@ -1535,8 +1610,8 @@
       <c r="C29" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>175</v>
+      <c r="D29" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>153</v>
@@ -1552,8 +1627,8 @@
       <c r="C30" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>175</v>
+      <c r="D30" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>153</v>
@@ -1569,8 +1644,8 @@
       <c r="C31" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>175</v>
+      <c r="D31" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>153</v>
@@ -1586,8 +1661,8 @@
       <c r="C32" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>175</v>
+      <c r="D32" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>153</v>
@@ -1603,8 +1678,8 @@
       <c r="C33" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>175</v>
+      <c r="D33" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>153</v>
@@ -1620,8 +1695,8 @@
       <c r="C34" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>175</v>
+      <c r="D34" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>153</v>
@@ -1637,8 +1712,8 @@
       <c r="C35" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>175</v>
+      <c r="D35" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>153</v>
@@ -1654,8 +1729,8 @@
       <c r="C36" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>175</v>
+      <c r="D36" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>153</v>
@@ -1671,8 +1746,8 @@
       <c r="C37" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>175</v>
+      <c r="D37" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>153</v>
@@ -1688,8 +1763,8 @@
       <c r="C38" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>175</v>
+      <c r="D38" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>153</v>
@@ -1705,8 +1780,8 @@
       <c r="C39" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>175</v>
+      <c r="D39" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>153</v>
@@ -1722,8 +1797,8 @@
       <c r="C40" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>175</v>
+      <c r="D40" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>153</v>
@@ -1739,8 +1814,8 @@
       <c r="C41" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>175</v>
+      <c r="D41" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>153</v>
@@ -1756,8 +1831,8 @@
       <c r="C42" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>175</v>
+      <c r="D42" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>153</v>
@@ -1773,8 +1848,8 @@
       <c r="C43" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>175</v>
+      <c r="D43" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>153</v>
@@ -1790,8 +1865,8 @@
       <c r="C44" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>175</v>
+      <c r="D44" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>153</v>
@@ -1807,8 +1882,8 @@
       <c r="C45" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>175</v>
+      <c r="D45" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>153</v>
@@ -1824,8 +1899,8 @@
       <c r="C46" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>175</v>
+      <c r="D46" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>153</v>
@@ -1841,8 +1916,8 @@
       <c r="C47" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>175</v>
+      <c r="D47" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>153</v>
@@ -1850,16 +1925,16 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>67</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>175</v>
+        <v>167</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>153</v>
@@ -1867,16 +1942,16 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>76</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>175</v>
+        <v>170</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>153</v>
@@ -1884,16 +1959,16 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C50" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B50" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>175</v>
+      <c r="D50" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>153</v>
@@ -1901,16 +1976,16 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B51" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="C51" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="C51" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>175</v>
+      <c r="D51" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>153</v>
@@ -1918,16 +1993,16 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>68</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>175</v>
+        <v>178</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>153</v>
@@ -1935,16 +2010,16 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>71</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>175</v>
+        <v>181</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>153</v>
@@ -1952,19 +2027,172 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C54" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="D54" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="C54" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>167</v>
+      <c r="B55" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="120">
+      <c r="A59" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="30">
+      <c r="A60" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="30">
+      <c r="A61" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="30">
+      <c r="A62" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="30">
+      <c r="A63" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding test cases for watch list
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="210">
   <si>
     <t>TCID</t>
   </si>
@@ -590,91 +590,139 @@
     <t>TestCase_B46</t>
   </si>
   <si>
+    <t>Verify that user is able to select any of the content types present in search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B47</t>
+  </si>
+  <si>
+    <t>TestCase_B48</t>
+  </si>
+  <si>
+    <t>Verify that ALL option is selected in the left navigation pane by default when user searches using ALL option in the search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B49</t>
+  </si>
+  <si>
+    <t>Verify that search results related to all content types get displayed in the summary page when user searches using ALL option in search drop down</t>
+  </si>
+  <si>
+    <t>OPQA-301</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>TestCase_B50</t>
+  </si>
+  <si>
+    <t>OPQA-307</t>
+  </si>
+  <si>
+    <t>Verify that ARTICLES option is selected in the left navigation pane by default when user searches using ARTICLES option in the search drop down</t>
+  </si>
+  <si>
+    <t>Verify that PATENTS option is selected in the left navigation pane by default when user searches using PATENTS option in the search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B51</t>
+  </si>
+  <si>
+    <t>TestCase_B52</t>
+  </si>
+  <si>
+    <t>Verify that POSTS option is selected in the left navigation pane by default when user searches using POSTS option in the search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B53</t>
+  </si>
+  <si>
+    <t>Verify that PEOPLE option is selected in the left navigation pane by default when user searches using PEOPLE option in the search drop down</t>
+  </si>
+  <si>
+    <t>OPQA-375</t>
+  </si>
+  <si>
+    <t>TestCase_B54</t>
+  </si>
+  <si>
+    <t>OPQA-316</t>
+  </si>
+  <si>
+    <t>Verify that only articles get displayed in the summary page when user searches using ARTICLES content type in search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B55</t>
+  </si>
+  <si>
+    <t>Verify that only patents get displayed in the summary page when user searches using PATENTS content type in search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B56</t>
+  </si>
+  <si>
+    <t>Verify that only posts get displayed in the summary page when user searches using POSTS content type in search drop down</t>
+  </si>
+  <si>
+    <t>Verify that only people get displayed in the summary page when user searches using people content type in search drop down</t>
+  </si>
+  <si>
+    <t>OPQA-380</t>
+  </si>
+  <si>
+    <t>TestCase_B57</t>
+  </si>
+  <si>
+    <t>TestCase_B58</t>
+  </si>
+  <si>
+    <t>OPQA-287</t>
+  </si>
+  <si>
+    <t>Verify that the following sections get displayed in the search type ahead when user searches using ALL option in the search drop down and that the searched keyword is present in all the sections:
+a)Autocompleted keyword
+b)4 suggestions in CATEGORY section
+c)4 suggestions in ARTICLES section
+d)4 suggestions in PATENTS section
+e)4 suggestions in POSTS section
+f)4 suggestions in PEOPLE section</t>
+  </si>
+  <si>
+    <t>OPQA-311</t>
+  </si>
+  <si>
+    <t>Verify that 10 article suggestions get displayed in the search type ahead when user searches using ARTICLES option in the search drop down and that the searched keyword is present in all the suggestions</t>
+  </si>
+  <si>
+    <t>TestCase_B59</t>
+  </si>
+  <si>
+    <t>TestCase_B60</t>
+  </si>
+  <si>
+    <t>Verify that 10 patent suggestions get displayed in the search type ahead when user searches using PATENTS option in the search drop down and that the searched keyword is present in all the suggestions</t>
+  </si>
+  <si>
+    <t>TestCase_B61</t>
+  </si>
+  <si>
+    <t>Verify that 10 post suggestions get displayed in the search type ahead when user searches using POSTS option in the search drop down and that the searched keyword is present in all the suggestions</t>
+  </si>
+  <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>Verify that user is able to select any of the content types present in search drop down</t>
-  </si>
-  <si>
-    <t>TestCase_B47</t>
-  </si>
-  <si>
-    <t>TestCase_B48</t>
-  </si>
-  <si>
-    <t>Verify that ALL option is selected in the left navigation pane by default when user searches using ALL option in the search drop down</t>
-  </si>
-  <si>
-    <t>TestCase_B49</t>
-  </si>
-  <si>
-    <t>Verify that search results related to all content types get displayed in the summary page when user searches using ALL option in search drop down</t>
-  </si>
-  <si>
-    <t>OPQA-301</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>TestCase_B50</t>
-  </si>
-  <si>
-    <t>OPQA-307</t>
-  </si>
-  <si>
-    <t>Verify that ARTICLES option is selected in the left navigation pane by default when user searches using ARTICLES option in the search drop down</t>
-  </si>
-  <si>
-    <t>Verify that PATENTS option is selected in the left navigation pane by default when user searches using PATENTS option in the search drop down</t>
-  </si>
-  <si>
-    <t>TestCase_B51</t>
-  </si>
-  <si>
-    <t>TestCase_B52</t>
-  </si>
-  <si>
-    <t>Verify that POSTS option is selected in the left navigation pane by default when user searches using POSTS option in the search drop down</t>
-  </si>
-  <si>
-    <t>TestCase_B53</t>
-  </si>
-  <si>
-    <t>Verify that PEOPLE option is selected in the left navigation pane by default when user searches using PEOPLE option in the search drop down</t>
-  </si>
-  <si>
-    <t>OPQA-375</t>
-  </si>
-  <si>
-    <t>TestCase_B54</t>
-  </si>
-  <si>
-    <t>OPQA-316</t>
-  </si>
-  <si>
-    <t>Verify that only articles get displayed in the summary page when user searches using ARTICLES content type in search drop down</t>
-  </si>
-  <si>
-    <t>TestCase_B55</t>
-  </si>
-  <si>
-    <t>Verify that only patents get displayed in the summary page when user searches using PATENTS content type in search drop down</t>
-  </si>
-  <si>
-    <t>TestCase_B56</t>
-  </si>
-  <si>
-    <t>Verify that only posts get displayed in the summary page when user searches using POSTS content type in search drop down</t>
-  </si>
-  <si>
-    <t>Verify that only people get displayed in the summary page when user searches using people content type in search drop down</t>
-  </si>
-  <si>
-    <t>OPQA-380</t>
-  </si>
-  <si>
-    <t>TestCase_B57</t>
+    <t>TestCase_B62</t>
+  </si>
+  <si>
+    <t>Verify that 10 people suggestions get displayed in the search type ahead when user searches using PEOPLE option in the search drop down and that the searched keyword is present in all the suggestions</t>
+  </si>
+  <si>
+    <t>OPQA-378</t>
+  </si>
+  <si>
+    <t>TestCase_B63</t>
   </si>
 </sst>
 </file>
@@ -1065,10 +1113,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1106,8 +1154,8 @@
       <c r="C2" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>175</v>
+      <c r="D2" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>153</v>
@@ -1123,8 +1171,8 @@
       <c r="C3" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>175</v>
+      <c r="D3" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>153</v>
@@ -1140,8 +1188,8 @@
       <c r="C4" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>175</v>
+      <c r="D4" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>153</v>
@@ -1157,8 +1205,8 @@
       <c r="C5" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>175</v>
+      <c r="D5" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>153</v>
@@ -1174,8 +1222,8 @@
       <c r="C6" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>175</v>
+      <c r="D6" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>153</v>
@@ -1191,8 +1239,8 @@
       <c r="C7" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>175</v>
+      <c r="D7" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>153</v>
@@ -1208,8 +1256,8 @@
       <c r="C8" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>175</v>
+      <c r="D8" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>153</v>
@@ -1225,8 +1273,8 @@
       <c r="C9" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>175</v>
+      <c r="D9" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>153</v>
@@ -1242,8 +1290,8 @@
       <c r="C10" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>175</v>
+      <c r="D10" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>153</v>
@@ -1259,8 +1307,8 @@
       <c r="C11" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>175</v>
+      <c r="D11" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>153</v>
@@ -1276,8 +1324,8 @@
       <c r="C12" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>175</v>
+      <c r="D12" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>153</v>
@@ -1293,8 +1341,8 @@
       <c r="C13" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>175</v>
+      <c r="D13" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>153</v>
@@ -1310,8 +1358,8 @@
       <c r="C14" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>175</v>
+      <c r="D14" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>153</v>
@@ -1327,8 +1375,8 @@
       <c r="C15" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>175</v>
+      <c r="D15" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>153</v>
@@ -1344,8 +1392,8 @@
       <c r="C16" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>175</v>
+      <c r="D16" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>153</v>
@@ -1361,8 +1409,8 @@
       <c r="C17" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>175</v>
+      <c r="D17" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>153</v>
@@ -1378,8 +1426,8 @@
       <c r="C18" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>175</v>
+      <c r="D18" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>153</v>
@@ -1395,8 +1443,8 @@
       <c r="C19" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>175</v>
+      <c r="D19" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>153</v>
@@ -1412,8 +1460,8 @@
       <c r="C20" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>175</v>
+      <c r="D20" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>153</v>
@@ -1429,8 +1477,8 @@
       <c r="C21" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>175</v>
+      <c r="D21" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>153</v>
@@ -1446,8 +1494,8 @@
       <c r="C22" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>175</v>
+      <c r="D22" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>153</v>
@@ -1463,8 +1511,8 @@
       <c r="C23" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>175</v>
+      <c r="D23" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>153</v>
@@ -1480,8 +1528,8 @@
       <c r="C24" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>175</v>
+      <c r="D24" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>153</v>
@@ -1497,8 +1545,8 @@
       <c r="C25" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>175</v>
+      <c r="D25" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>153</v>
@@ -1514,8 +1562,8 @@
       <c r="C26" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="7" t="s">
-        <v>175</v>
+      <c r="D26" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>153</v>
@@ -1531,8 +1579,8 @@
       <c r="C27" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>175</v>
+      <c r="D27" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>153</v>
@@ -1548,8 +1596,8 @@
       <c r="C28" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>175</v>
+      <c r="D28" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>153</v>
@@ -1565,8 +1613,8 @@
       <c r="C29" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>175</v>
+      <c r="D29" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>153</v>
@@ -1582,8 +1630,8 @@
       <c r="C30" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D30" s="7" t="s">
-        <v>175</v>
+      <c r="D30" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>153</v>
@@ -1599,8 +1647,8 @@
       <c r="C31" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D31" s="7" t="s">
-        <v>175</v>
+      <c r="D31" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>153</v>
@@ -1616,8 +1664,8 @@
       <c r="C32" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="D32" s="7" t="s">
-        <v>175</v>
+      <c r="D32" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>153</v>
@@ -1633,8 +1681,8 @@
       <c r="C33" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="D33" s="7" t="s">
-        <v>175</v>
+      <c r="D33" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>153</v>
@@ -1650,8 +1698,8 @@
       <c r="C34" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="D34" s="7" t="s">
-        <v>175</v>
+      <c r="D34" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>153</v>
@@ -1667,8 +1715,8 @@
       <c r="C35" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="D35" s="7" t="s">
-        <v>175</v>
+      <c r="D35" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>153</v>
@@ -1684,8 +1732,8 @@
       <c r="C36" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D36" s="7" t="s">
-        <v>175</v>
+      <c r="D36" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>153</v>
@@ -1701,8 +1749,8 @@
       <c r="C37" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D37" s="7" t="s">
-        <v>175</v>
+      <c r="D37" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>153</v>
@@ -1718,8 +1766,8 @@
       <c r="C38" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D38" s="7" t="s">
-        <v>175</v>
+      <c r="D38" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>153</v>
@@ -1735,8 +1783,8 @@
       <c r="C39" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D39" s="7" t="s">
-        <v>175</v>
+      <c r="D39" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>153</v>
@@ -1752,8 +1800,8 @@
       <c r="C40" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D40" s="7" t="s">
-        <v>175</v>
+      <c r="D40" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>153</v>
@@ -1769,8 +1817,8 @@
       <c r="C41" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D41" s="7" t="s">
-        <v>175</v>
+      <c r="D41" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>153</v>
@@ -1786,8 +1834,8 @@
       <c r="C42" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="D42" s="7" t="s">
-        <v>175</v>
+      <c r="D42" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>153</v>
@@ -1803,8 +1851,8 @@
       <c r="C43" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="D43" s="7" t="s">
-        <v>175</v>
+      <c r="D43" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>153</v>
@@ -1820,8 +1868,8 @@
       <c r="C44" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D44" s="7" t="s">
-        <v>175</v>
+      <c r="D44" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>153</v>
@@ -1837,8 +1885,8 @@
       <c r="C45" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D45" s="7" t="s">
-        <v>175</v>
+      <c r="D45" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>153</v>
@@ -1854,8 +1902,8 @@
       <c r="C46" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D46" s="7" t="s">
-        <v>175</v>
+      <c r="D46" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>153</v>
@@ -1871,8 +1919,8 @@
       <c r="C47" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D47" s="7" t="s">
-        <v>175</v>
+      <c r="D47" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>153</v>
@@ -1880,16 +1928,16 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>67</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>175</v>
+        <v>167</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>153</v>
@@ -1897,16 +1945,16 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>76</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>175</v>
+        <v>170</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>153</v>
@@ -1914,16 +1962,16 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C50" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B50" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>175</v>
+      <c r="D50" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>153</v>
@@ -1931,16 +1979,16 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B51" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="C51" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="C51" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>175</v>
+      <c r="D51" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>153</v>
@@ -1948,16 +1996,16 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>68</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>175</v>
+        <v>178</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>153</v>
@@ -1965,16 +2013,16 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>71</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>175</v>
+        <v>181</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>153</v>
@@ -1982,16 +2030,16 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C54" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="B54" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>175</v>
+      <c r="D54" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>153</v>
@@ -1999,16 +2047,16 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="B55" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="C55" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="C55" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>175</v>
+      <c r="D55" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>153</v>
@@ -2016,16 +2064,16 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>69</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="D56" s="7" t="s">
-        <v>175</v>
+        <v>189</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>153</v>
@@ -2033,16 +2081,16 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>73</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>175</v>
+        <v>191</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>153</v>
@@ -2050,19 +2098,121 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="120">
+      <c r="A59" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="B58" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D58" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>167</v>
+      <c r="B59" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="30">
+      <c r="A60" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="30">
+      <c r="A61" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="30">
+      <c r="A62" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="30">
+      <c r="A63" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding Trending Test Case
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="210">
   <si>
     <t>TCID</t>
   </si>
@@ -590,91 +590,139 @@
     <t>TestCase_B46</t>
   </si>
   <si>
+    <t>Verify that user is able to select any of the content types present in search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B47</t>
+  </si>
+  <si>
+    <t>TestCase_B48</t>
+  </si>
+  <si>
+    <t>Verify that ALL option is selected in the left navigation pane by default when user searches using ALL option in the search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B49</t>
+  </si>
+  <si>
+    <t>Verify that search results related to all content types get displayed in the summary page when user searches using ALL option in search drop down</t>
+  </si>
+  <si>
+    <t>OPQA-301</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>TestCase_B50</t>
+  </si>
+  <si>
+    <t>OPQA-307</t>
+  </si>
+  <si>
+    <t>Verify that ARTICLES option is selected in the left navigation pane by default when user searches using ARTICLES option in the search drop down</t>
+  </si>
+  <si>
+    <t>Verify that PATENTS option is selected in the left navigation pane by default when user searches using PATENTS option in the search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B51</t>
+  </si>
+  <si>
+    <t>TestCase_B52</t>
+  </si>
+  <si>
+    <t>Verify that POSTS option is selected in the left navigation pane by default when user searches using POSTS option in the search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B53</t>
+  </si>
+  <si>
+    <t>Verify that PEOPLE option is selected in the left navigation pane by default when user searches using PEOPLE option in the search drop down</t>
+  </si>
+  <si>
+    <t>OPQA-375</t>
+  </si>
+  <si>
+    <t>TestCase_B54</t>
+  </si>
+  <si>
+    <t>OPQA-316</t>
+  </si>
+  <si>
+    <t>Verify that only articles get displayed in the summary page when user searches using ARTICLES content type in search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B55</t>
+  </si>
+  <si>
+    <t>Verify that only patents get displayed in the summary page when user searches using PATENTS content type in search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B56</t>
+  </si>
+  <si>
+    <t>Verify that only posts get displayed in the summary page when user searches using POSTS content type in search drop down</t>
+  </si>
+  <si>
+    <t>Verify that only people get displayed in the summary page when user searches using people content type in search drop down</t>
+  </si>
+  <si>
+    <t>OPQA-380</t>
+  </si>
+  <si>
+    <t>TestCase_B57</t>
+  </si>
+  <si>
+    <t>TestCase_B58</t>
+  </si>
+  <si>
+    <t>OPQA-287</t>
+  </si>
+  <si>
+    <t>Verify that the following sections get displayed in the search type ahead when user searches using ALL option in the search drop down and that the searched keyword is present in all the sections:
+a)Autocompleted keyword
+b)4 suggestions in CATEGORY section
+c)4 suggestions in ARTICLES section
+d)4 suggestions in PATENTS section
+e)4 suggestions in POSTS section
+f)4 suggestions in PEOPLE section</t>
+  </si>
+  <si>
+    <t>OPQA-311</t>
+  </si>
+  <si>
+    <t>Verify that 10 article suggestions get displayed in the search type ahead when user searches using ARTICLES option in the search drop down and that the searched keyword is present in all the suggestions</t>
+  </si>
+  <si>
+    <t>TestCase_B59</t>
+  </si>
+  <si>
+    <t>TestCase_B60</t>
+  </si>
+  <si>
+    <t>Verify that 10 patent suggestions get displayed in the search type ahead when user searches using PATENTS option in the search drop down and that the searched keyword is present in all the suggestions</t>
+  </si>
+  <si>
+    <t>TestCase_B61</t>
+  </si>
+  <si>
+    <t>Verify that 10 post suggestions get displayed in the search type ahead when user searches using POSTS option in the search drop down and that the searched keyword is present in all the suggestions</t>
+  </si>
+  <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>Verify that user is able to select any of the content types present in search drop down</t>
-  </si>
-  <si>
-    <t>TestCase_B47</t>
-  </si>
-  <si>
-    <t>TestCase_B48</t>
-  </si>
-  <si>
-    <t>Verify that ALL option is selected in the left navigation pane by default when user searches using ALL option in the search drop down</t>
-  </si>
-  <si>
-    <t>TestCase_B49</t>
-  </si>
-  <si>
-    <t>Verify that search results related to all content types get displayed in the summary page when user searches using ALL option in search drop down</t>
-  </si>
-  <si>
-    <t>OPQA-301</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>TestCase_B50</t>
-  </si>
-  <si>
-    <t>OPQA-307</t>
-  </si>
-  <si>
-    <t>Verify that ARTICLES option is selected in the left navigation pane by default when user searches using ARTICLES option in the search drop down</t>
-  </si>
-  <si>
-    <t>Verify that PATENTS option is selected in the left navigation pane by default when user searches using PATENTS option in the search drop down</t>
-  </si>
-  <si>
-    <t>TestCase_B51</t>
-  </si>
-  <si>
-    <t>TestCase_B52</t>
-  </si>
-  <si>
-    <t>Verify that POSTS option is selected in the left navigation pane by default when user searches using POSTS option in the search drop down</t>
-  </si>
-  <si>
-    <t>TestCase_B53</t>
-  </si>
-  <si>
-    <t>Verify that PEOPLE option is selected in the left navigation pane by default when user searches using PEOPLE option in the search drop down</t>
-  </si>
-  <si>
-    <t>OPQA-375</t>
-  </si>
-  <si>
-    <t>TestCase_B54</t>
-  </si>
-  <si>
-    <t>OPQA-316</t>
-  </si>
-  <si>
-    <t>Verify that only articles get displayed in the summary page when user searches using ARTICLES content type in search drop down</t>
-  </si>
-  <si>
-    <t>TestCase_B55</t>
-  </si>
-  <si>
-    <t>Verify that only patents get displayed in the summary page when user searches using PATENTS content type in search drop down</t>
-  </si>
-  <si>
-    <t>TestCase_B56</t>
-  </si>
-  <si>
-    <t>Verify that only posts get displayed in the summary page when user searches using POSTS content type in search drop down</t>
-  </si>
-  <si>
-    <t>Verify that only people get displayed in the summary page when user searches using people content type in search drop down</t>
-  </si>
-  <si>
-    <t>OPQA-380</t>
-  </si>
-  <si>
-    <t>TestCase_B57</t>
+    <t>TestCase_B62</t>
+  </si>
+  <si>
+    <t>Verify that 10 people suggestions get displayed in the search type ahead when user searches using PEOPLE option in the search drop down and that the searched keyword is present in all the suggestions</t>
+  </si>
+  <si>
+    <t>OPQA-378</t>
+  </si>
+  <si>
+    <t>TestCase_B63</t>
   </si>
 </sst>
 </file>
@@ -1065,10 +1113,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1106,8 +1154,8 @@
       <c r="C2" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>175</v>
+      <c r="D2" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>153</v>
@@ -1123,8 +1171,8 @@
       <c r="C3" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>175</v>
+      <c r="D3" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>153</v>
@@ -1140,8 +1188,8 @@
       <c r="C4" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>175</v>
+      <c r="D4" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>153</v>
@@ -1157,8 +1205,8 @@
       <c r="C5" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>175</v>
+      <c r="D5" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>153</v>
@@ -1174,8 +1222,8 @@
       <c r="C6" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>175</v>
+      <c r="D6" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>153</v>
@@ -1191,8 +1239,8 @@
       <c r="C7" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>175</v>
+      <c r="D7" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>153</v>
@@ -1208,8 +1256,8 @@
       <c r="C8" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>175</v>
+      <c r="D8" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>153</v>
@@ -1225,8 +1273,8 @@
       <c r="C9" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>175</v>
+      <c r="D9" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>153</v>
@@ -1242,8 +1290,8 @@
       <c r="C10" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>175</v>
+      <c r="D10" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>153</v>
@@ -1259,8 +1307,8 @@
       <c r="C11" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>175</v>
+      <c r="D11" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>153</v>
@@ -1276,8 +1324,8 @@
       <c r="C12" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>175</v>
+      <c r="D12" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>153</v>
@@ -1293,8 +1341,8 @@
       <c r="C13" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>175</v>
+      <c r="D13" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>153</v>
@@ -1310,8 +1358,8 @@
       <c r="C14" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>175</v>
+      <c r="D14" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>153</v>
@@ -1327,8 +1375,8 @@
       <c r="C15" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>175</v>
+      <c r="D15" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>153</v>
@@ -1344,8 +1392,8 @@
       <c r="C16" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>175</v>
+      <c r="D16" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>153</v>
@@ -1361,8 +1409,8 @@
       <c r="C17" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>175</v>
+      <c r="D17" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>153</v>
@@ -1378,8 +1426,8 @@
       <c r="C18" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>175</v>
+      <c r="D18" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>153</v>
@@ -1395,8 +1443,8 @@
       <c r="C19" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>175</v>
+      <c r="D19" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>153</v>
@@ -1412,8 +1460,8 @@
       <c r="C20" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>175</v>
+      <c r="D20" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>153</v>
@@ -1429,8 +1477,8 @@
       <c r="C21" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>175</v>
+      <c r="D21" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>153</v>
@@ -1446,8 +1494,8 @@
       <c r="C22" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>175</v>
+      <c r="D22" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>153</v>
@@ -1463,8 +1511,8 @@
       <c r="C23" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>175</v>
+      <c r="D23" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>153</v>
@@ -1480,8 +1528,8 @@
       <c r="C24" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>175</v>
+      <c r="D24" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>153</v>
@@ -1497,8 +1545,8 @@
       <c r="C25" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>175</v>
+      <c r="D25" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>153</v>
@@ -1514,8 +1562,8 @@
       <c r="C26" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="7" t="s">
-        <v>175</v>
+      <c r="D26" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>153</v>
@@ -1531,8 +1579,8 @@
       <c r="C27" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>175</v>
+      <c r="D27" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>153</v>
@@ -1548,8 +1596,8 @@
       <c r="C28" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>175</v>
+      <c r="D28" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>153</v>
@@ -1565,8 +1613,8 @@
       <c r="C29" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>175</v>
+      <c r="D29" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>153</v>
@@ -1582,8 +1630,8 @@
       <c r="C30" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D30" s="7" t="s">
-        <v>175</v>
+      <c r="D30" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>153</v>
@@ -1599,8 +1647,8 @@
       <c r="C31" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D31" s="7" t="s">
-        <v>175</v>
+      <c r="D31" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>153</v>
@@ -1616,8 +1664,8 @@
       <c r="C32" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="D32" s="7" t="s">
-        <v>175</v>
+      <c r="D32" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>153</v>
@@ -1633,8 +1681,8 @@
       <c r="C33" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="D33" s="7" t="s">
-        <v>175</v>
+      <c r="D33" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>153</v>
@@ -1650,8 +1698,8 @@
       <c r="C34" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="D34" s="7" t="s">
-        <v>175</v>
+      <c r="D34" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>153</v>
@@ -1667,8 +1715,8 @@
       <c r="C35" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="D35" s="7" t="s">
-        <v>175</v>
+      <c r="D35" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>153</v>
@@ -1684,8 +1732,8 @@
       <c r="C36" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D36" s="7" t="s">
-        <v>175</v>
+      <c r="D36" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>153</v>
@@ -1701,8 +1749,8 @@
       <c r="C37" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D37" s="7" t="s">
-        <v>175</v>
+      <c r="D37" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>153</v>
@@ -1718,8 +1766,8 @@
       <c r="C38" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D38" s="7" t="s">
-        <v>175</v>
+      <c r="D38" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>153</v>
@@ -1735,8 +1783,8 @@
       <c r="C39" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D39" s="7" t="s">
-        <v>175</v>
+      <c r="D39" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>153</v>
@@ -1752,8 +1800,8 @@
       <c r="C40" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D40" s="7" t="s">
-        <v>175</v>
+      <c r="D40" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>153</v>
@@ -1769,8 +1817,8 @@
       <c r="C41" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D41" s="7" t="s">
-        <v>175</v>
+      <c r="D41" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>153</v>
@@ -1786,8 +1834,8 @@
       <c r="C42" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="D42" s="7" t="s">
-        <v>175</v>
+      <c r="D42" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>153</v>
@@ -1803,8 +1851,8 @@
       <c r="C43" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="D43" s="7" t="s">
-        <v>175</v>
+      <c r="D43" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>153</v>
@@ -1820,8 +1868,8 @@
       <c r="C44" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D44" s="7" t="s">
-        <v>175</v>
+      <c r="D44" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>153</v>
@@ -1837,8 +1885,8 @@
       <c r="C45" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D45" s="7" t="s">
-        <v>175</v>
+      <c r="D45" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>153</v>
@@ -1854,8 +1902,8 @@
       <c r="C46" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D46" s="7" t="s">
-        <v>175</v>
+      <c r="D46" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>153</v>
@@ -1871,8 +1919,8 @@
       <c r="C47" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D47" s="7" t="s">
-        <v>175</v>
+      <c r="D47" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>153</v>
@@ -1880,16 +1928,16 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>67</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>175</v>
+        <v>167</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>153</v>
@@ -1897,16 +1945,16 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>76</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>175</v>
+        <v>170</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>153</v>
@@ -1914,16 +1962,16 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C50" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B50" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>175</v>
+      <c r="D50" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>153</v>
@@ -1931,16 +1979,16 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B51" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="C51" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="C51" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>175</v>
+      <c r="D51" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>153</v>
@@ -1948,16 +1996,16 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>68</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>175</v>
+        <v>178</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>153</v>
@@ -1965,16 +2013,16 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>71</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>175</v>
+        <v>181</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>153</v>
@@ -1982,16 +2030,16 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C54" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="B54" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>175</v>
+      <c r="D54" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>153</v>
@@ -1999,16 +2047,16 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="B55" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="C55" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="C55" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>175</v>
+      <c r="D55" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>153</v>
@@ -2016,16 +2064,16 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>69</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="D56" s="7" t="s">
-        <v>175</v>
+        <v>189</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>153</v>
@@ -2033,16 +2081,16 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>73</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>175</v>
+        <v>191</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>153</v>
@@ -2050,19 +2098,121 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="120">
+      <c r="A59" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="B58" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D58" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>167</v>
+      <c r="B59" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="30">
+      <c r="A60" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="30">
+      <c r="A61" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="30">
+      <c r="A62" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="30">
+      <c r="A63" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding 4 search test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="224">
   <si>
     <t>TCID</t>
   </si>
@@ -724,11 +724,54 @@
   <si>
     <t>TestCase_B63</t>
   </si>
+  <si>
+    <t>TestCase_B64</t>
+  </si>
+  <si>
+    <t>OPQA-557</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>TestCase_B65</t>
+  </si>
+  <si>
+    <t>Verify that the searched keyword doesn't change in the search text box if any other content type is selected in the left navigation pane</t>
+  </si>
+  <si>
+    <t>OPQA-386</t>
+  </si>
+  <si>
+    <t>Verify that the searched keyword present in the search text box doesn't change if any other content type is selected in the search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B66</t>
+  </si>
+  <si>
+    <t>OPQA-387</t>
+  </si>
+  <si>
+    <t>Verify that counts of search results of all the content types should get displayed irrespective of the content type chosen for searching</t>
+  </si>
+  <si>
+    <t>TestCase_B67</t>
+  </si>
+  <si>
+    <t>Verify that ALL search results count is equal to the count of search results of other content types(ARTICLES+PATENTS+POSTS+PEOPLE)</t>
+  </si>
+  <si>
+    <t>OPQA-263</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -1113,18 +1156,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="136.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="136.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1155,7 +1198,7 @@
         <v>97</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>153</v>
@@ -1172,7 +1215,7 @@
         <v>77</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>153</v>
@@ -1189,7 +1232,7 @@
         <v>78</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>153</v>
@@ -1206,7 +1249,7 @@
         <v>79</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>153</v>
@@ -1223,7 +1266,7 @@
         <v>80</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>153</v>
@@ -1240,7 +1283,7 @@
         <v>81</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>153</v>
@@ -1257,7 +1300,7 @@
         <v>74</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>153</v>
@@ -1274,7 +1317,7 @@
         <v>82</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>153</v>
@@ -1291,7 +1334,7 @@
         <v>83</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>153</v>
@@ -1308,7 +1351,7 @@
         <v>84</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>153</v>
@@ -1325,7 +1368,7 @@
         <v>85</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>153</v>
@@ -1342,7 +1385,7 @@
         <v>101</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>153</v>
@@ -1359,7 +1402,7 @@
         <v>86</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>153</v>
@@ -1376,7 +1419,7 @@
         <v>87</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>153</v>
@@ -1393,7 +1436,7 @@
         <v>88</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>153</v>
@@ -1410,7 +1453,7 @@
         <v>89</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>153</v>
@@ -1427,7 +1470,7 @@
         <v>140</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>153</v>
@@ -1444,7 +1487,7 @@
         <v>90</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>153</v>
@@ -1461,7 +1504,7 @@
         <v>91</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>153</v>
@@ -1478,7 +1521,7 @@
         <v>92</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>153</v>
@@ -1495,7 +1538,7 @@
         <v>93</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>153</v>
@@ -1512,7 +1555,7 @@
         <v>94</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>153</v>
@@ -1529,7 +1572,7 @@
         <v>95</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>153</v>
@@ -1546,7 +1589,7 @@
         <v>96</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>153</v>
@@ -1563,7 +1606,7 @@
         <v>104</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>153</v>
@@ -1580,7 +1623,7 @@
         <v>107</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>153</v>
@@ -1597,7 +1640,7 @@
         <v>110</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>153</v>
@@ -1614,7 +1657,7 @@
         <v>111</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>153</v>
@@ -1631,7 +1674,7 @@
         <v>116</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>153</v>
@@ -1648,7 +1691,7 @@
         <v>119</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>153</v>
@@ -1665,7 +1708,7 @@
         <v>122</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>153</v>
@@ -1682,7 +1725,7 @@
         <v>124</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>153</v>
@@ -1699,7 +1742,7 @@
         <v>126</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>153</v>
@@ -1716,7 +1759,7 @@
         <v>128</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>153</v>
@@ -1733,7 +1776,7 @@
         <v>134</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>153</v>
@@ -1750,7 +1793,7 @@
         <v>137</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>153</v>
@@ -1767,7 +1810,7 @@
         <v>140</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>153</v>
@@ -1784,7 +1827,7 @@
         <v>143</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>153</v>
@@ -1801,7 +1844,7 @@
         <v>146</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>153</v>
@@ -1818,7 +1861,7 @@
         <v>149</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>153</v>
@@ -1835,7 +1878,7 @@
         <v>152</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>153</v>
@@ -1852,7 +1895,7 @@
         <v>160</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>153</v>
@@ -1869,7 +1912,7 @@
         <v>161</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>153</v>
@@ -1886,7 +1929,7 @@
         <v>162</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>153</v>
@@ -1903,7 +1946,7 @@
         <v>163</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>153</v>
@@ -1920,7 +1963,7 @@
         <v>165</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>153</v>
@@ -1937,7 +1980,7 @@
         <v>167</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>153</v>
@@ -1954,7 +1997,7 @@
         <v>170</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>153</v>
@@ -1971,7 +2014,7 @@
         <v>172</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>153</v>
@@ -1988,7 +2031,7 @@
         <v>177</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>153</v>
@@ -2005,7 +2048,7 @@
         <v>178</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>153</v>
@@ -2022,7 +2065,7 @@
         <v>181</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>153</v>
@@ -2039,7 +2082,7 @@
         <v>183</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>153</v>
@@ -2056,7 +2099,7 @@
         <v>187</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>153</v>
@@ -2073,7 +2116,7 @@
         <v>189</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>153</v>
@@ -2090,7 +2133,7 @@
         <v>191</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>153</v>
@@ -2107,7 +2150,7 @@
         <v>192</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>153</v>
@@ -2124,7 +2167,7 @@
         <v>197</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>153</v>
@@ -2141,7 +2184,7 @@
         <v>199</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>153</v>
@@ -2158,7 +2201,7 @@
         <v>202</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>153</v>
@@ -2175,7 +2218,7 @@
         <v>204</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>153</v>
@@ -2192,7 +2235,7 @@
         <v>207</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>153</v>
@@ -2209,9 +2252,77 @@
         <v>74</v>
       </c>
       <c r="D64" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="D68" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="E64" s="3" t="s">
+      <c r="E68" s="3" t="s">
         <v>205</v>
       </c>
     </row>
@@ -2231,10 +2342,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="52.5703125" style="5" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.85546875" style="5" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="12.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="5" width="52.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="5" width="83.85546875" collapsed="true"/>
+    <col min="4" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="35.25" customHeight="1">

</xml_diff>

<commit_message>
Taking latest changes and appending profile test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="222">
   <si>
     <t>TCID</t>
   </si>
@@ -720,6 +720,45 @@
   </si>
   <si>
     <t>OPQA-378</t>
+  </si>
+  <si>
+    <t>TestCase_B63</t>
+  </si>
+  <si>
+    <t>TestCase_B64</t>
+  </si>
+  <si>
+    <t>OPQA-557</t>
+  </si>
+  <si>
+    <t>TestCase_B65</t>
+  </si>
+  <si>
+    <t>Verify that the searched keyword doesn't change in the search text box if any other content type is selected in the left navigation pane</t>
+  </si>
+  <si>
+    <t>OPQA-386</t>
+  </si>
+  <si>
+    <t>Verify that the searched keyword present in the search text box doesn't change if any other content type is selected in the search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B66</t>
+  </si>
+  <si>
+    <t>OPQA-387</t>
+  </si>
+  <si>
+    <t>Verify that counts of search results of all the content types should get displayed irrespective of the content type chosen for searching</t>
+  </si>
+  <si>
+    <t>TestCase_B67</t>
+  </si>
+  <si>
+    <t>Verify that ALL search results count is equal to the count of search results of other content types(ARTICLES+PATENTS+POSTS+PEOPLE)</t>
+  </si>
+  <si>
+    <t>OPQA-263</t>
   </si>
 </sst>
 </file>
@@ -1110,10 +1149,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1151,7 +1190,7 @@
       <c r="C2" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -1168,7 +1207,7 @@
       <c r="C3" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -1185,7 +1224,7 @@
       <c r="C4" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -1202,7 +1241,7 @@
       <c r="C5" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -1219,7 +1258,7 @@
       <c r="C6" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -1236,7 +1275,7 @@
       <c r="C7" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -1253,7 +1292,7 @@
       <c r="C8" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -1270,7 +1309,7 @@
       <c r="C9" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -1287,7 +1326,7 @@
       <c r="C10" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -1304,7 +1343,7 @@
       <c r="C11" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -1321,7 +1360,7 @@
       <c r="C12" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -1338,7 +1377,7 @@
       <c r="C13" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -1355,7 +1394,7 @@
       <c r="C14" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -1372,7 +1411,7 @@
       <c r="C15" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -1389,7 +1428,7 @@
       <c r="C16" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -1406,7 +1445,7 @@
       <c r="C17" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E17" s="3" t="s">
@@ -1423,7 +1462,7 @@
       <c r="C18" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E18" s="3" t="s">
@@ -1440,7 +1479,7 @@
       <c r="C19" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E19" s="3" t="s">
@@ -1457,7 +1496,7 @@
       <c r="C20" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E20" s="3" t="s">
@@ -1474,7 +1513,7 @@
       <c r="C21" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E21" s="3" t="s">
@@ -1491,7 +1530,7 @@
       <c r="C22" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E22" s="3" t="s">
@@ -1508,7 +1547,7 @@
       <c r="C23" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E23" s="3" t="s">
@@ -1525,7 +1564,7 @@
       <c r="C24" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E24" s="3" t="s">
@@ -1542,7 +1581,7 @@
       <c r="C25" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E25" s="3" t="s">
@@ -1559,7 +1598,7 @@
       <c r="C26" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E26" s="3" t="s">
@@ -1576,7 +1615,7 @@
       <c r="C27" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E27" s="3" t="s">
@@ -1593,7 +1632,7 @@
       <c r="C28" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E28" s="3" t="s">
@@ -1610,7 +1649,7 @@
       <c r="C29" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E29" s="3" t="s">
@@ -1627,7 +1666,7 @@
       <c r="C30" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E30" s="3" t="s">
@@ -1644,7 +1683,7 @@
       <c r="C31" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E31" s="3" t="s">
@@ -1661,7 +1700,7 @@
       <c r="C32" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E32" s="3" t="s">
@@ -1678,7 +1717,7 @@
       <c r="C33" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E33" s="3" t="s">
@@ -1695,7 +1734,7 @@
       <c r="C34" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E34" s="3" t="s">
@@ -1712,7 +1751,7 @@
       <c r="C35" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E35" s="3" t="s">
@@ -1729,7 +1768,7 @@
       <c r="C36" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E36" s="3" t="s">
@@ -1746,7 +1785,7 @@
       <c r="C37" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E37" s="3" t="s">
@@ -1763,7 +1802,7 @@
       <c r="C38" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E38" s="3" t="s">
@@ -1780,7 +1819,7 @@
       <c r="C39" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E39" s="3" t="s">
@@ -1797,7 +1836,7 @@
       <c r="C40" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E40" s="3" t="s">
@@ -1814,7 +1853,7 @@
       <c r="C41" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E41" s="3" t="s">
@@ -1831,7 +1870,7 @@
       <c r="C42" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E42" s="3" t="s">
@@ -1848,7 +1887,7 @@
       <c r="C43" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E43" s="3" t="s">
@@ -1865,7 +1904,7 @@
       <c r="C44" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E44" s="3" t="s">
@@ -1882,7 +1921,7 @@
       <c r="C45" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D45" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E45" s="3" t="s">
@@ -1899,7 +1938,7 @@
       <c r="C46" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="D46" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E46" s="3" t="s">
@@ -1916,7 +1955,7 @@
       <c r="C47" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D47" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E47" s="3" t="s">
@@ -1933,7 +1972,7 @@
       <c r="C48" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E48" s="3" t="s">
@@ -1950,7 +1989,7 @@
       <c r="C49" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E49" s="3" t="s">
@@ -1967,7 +2006,7 @@
       <c r="C50" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D50" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E50" s="3" t="s">
@@ -1984,7 +2023,7 @@
       <c r="C51" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D51" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E51" s="3" t="s">
@@ -2001,7 +2040,7 @@
       <c r="C52" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="D52" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E52" s="3" t="s">
@@ -2018,7 +2057,7 @@
       <c r="C53" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D53" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E53" s="3" t="s">
@@ -2035,7 +2074,7 @@
       <c r="C54" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D54" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E54" s="3" t="s">
@@ -2052,7 +2091,7 @@
       <c r="C55" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="D55" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E55" s="3" t="s">
@@ -2069,7 +2108,7 @@
       <c r="C56" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="D56" s="7" t="s">
+      <c r="D56" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E56" s="3" t="s">
@@ -2086,7 +2125,7 @@
       <c r="C57" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="D57" s="7" t="s">
+      <c r="D57" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E57" s="3" t="s">
@@ -2103,7 +2142,7 @@
       <c r="C58" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="D58" s="7" t="s">
+      <c r="D58" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E58" s="3" t="s">
@@ -2120,11 +2159,11 @@
       <c r="C59" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="D59" s="7" t="s">
+      <c r="D59" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>205</v>
+        <v>153</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="30">
@@ -2137,7 +2176,7 @@
       <c r="C60" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="D60" s="7" t="s">
+      <c r="D60" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E60" s="3" t="s">
@@ -2154,7 +2193,7 @@
       <c r="C61" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="D61" s="7" t="s">
+      <c r="D61" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E61" s="3" t="s">
@@ -2171,7 +2210,7 @@
       <c r="C62" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="D62" s="7" t="s">
+      <c r="D62" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E62" s="3" t="s">
@@ -2188,11 +2227,96 @@
       <c r="C63" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="D63" s="7" t="s">
+      <c r="D63" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>153</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Taking changes to local
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="236">
   <si>
     <t>TCID</t>
   </si>
@@ -611,9 +611,6 @@
     <t>OPQA-301</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>TestCase_B50</t>
   </si>
   <si>
@@ -710,55 +707,102 @@
     <t>Verify that 10 post suggestions get displayed in the search type ahead when user searches using POSTS option in the search drop down and that the searched keyword is present in all the suggestions</t>
   </si>
   <si>
+    <t>TestCase_B62</t>
+  </si>
+  <si>
+    <t>Verify that 10 people suggestions get displayed in the search type ahead when user searches using PEOPLE option in the search drop down and that the searched keyword is present in all the suggestions</t>
+  </si>
+  <si>
+    <t>OPQA-378</t>
+  </si>
+  <si>
+    <t>TestCase_B63</t>
+  </si>
+  <si>
+    <t>TestCase_B64</t>
+  </si>
+  <si>
+    <t>OPQA-557</t>
+  </si>
+  <si>
+    <t>TestCase_B65</t>
+  </si>
+  <si>
+    <t>Verify that the searched keyword doesn't change in the search text box if any other content type is selected in the left navigation pane</t>
+  </si>
+  <si>
+    <t>OPQA-386</t>
+  </si>
+  <si>
+    <t>Verify that the searched keyword present in the search text box doesn't change if any other content type is selected in the search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B66</t>
+  </si>
+  <si>
+    <t>OPQA-387</t>
+  </si>
+  <si>
+    <t>Verify that counts of search results of all the content types should get displayed irrespective of the content type chosen for searching</t>
+  </si>
+  <si>
+    <t>TestCase_B67</t>
+  </si>
+  <si>
+    <t>Verify that ALL search results count is equal to the count of search results of other content types(ARTICLES+PATENTS+POSTS+PEOPLE)</t>
+  </si>
+  <si>
+    <t>OPQA-263</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>TestCase_B62</t>
-  </si>
-  <si>
-    <t>Verify that 10 people suggestions get displayed in the search type ahead when user searches using PEOPLE option in the search drop down and that the searched keyword is present in all the suggestions</t>
-  </si>
-  <si>
-    <t>OPQA-378</t>
-  </si>
-  <si>
-    <t>TestCase_B63</t>
-  </si>
-  <si>
-    <t>TestCase_B64</t>
-  </si>
-  <si>
-    <t>OPQA-557</t>
-  </si>
-  <si>
-    <t>TestCase_B65</t>
-  </si>
-  <si>
-    <t>Verify that the searched keyword doesn't change in the search text box if any other content type is selected in the left navigation pane</t>
-  </si>
-  <si>
-    <t>OPQA-386</t>
-  </si>
-  <si>
-    <t>Verify that the searched keyword present in the search text box doesn't change if any other content type is selected in the search drop down</t>
-  </si>
-  <si>
-    <t>TestCase_B66</t>
-  </si>
-  <si>
-    <t>OPQA-387</t>
-  </si>
-  <si>
-    <t>Verify that counts of search results of all the content types should get displayed irrespective of the content type chosen for searching</t>
-  </si>
-  <si>
-    <t>TestCase_B67</t>
-  </si>
-  <si>
-    <t>Verify that ALL search results count is equal to the count of search results of other content types(ARTICLES+PATENTS+POSTS+PEOPLE)</t>
-  </si>
-  <si>
-    <t>OPQA-263</t>
+    <t>TestCase_B68</t>
+  </si>
+  <si>
+    <t>Verify that count of the selected content type(in the left navigation pane) gets displayed at the top</t>
+  </si>
+  <si>
+    <t>TestCase_B69</t>
+  </si>
+  <si>
+    <t>OPQA-384</t>
+  </si>
+  <si>
+    <t>Verify that the following changes take place when user switches over to any other content type in the left navigation pane:
+a)Search results related to the switched content type get displayed in the summary page
+b)Search drop down option gets changed automatically to the switched content type</t>
+  </si>
+  <si>
+    <t>TestCase_B70</t>
+  </si>
+  <si>
+    <t>Verify that record view of an article gets displayed when user clicks on any article option in the search type ahead while ALL option is selected in the search drop down</t>
+  </si>
+  <si>
+    <t>OPQA-396</t>
+  </si>
+  <si>
+    <t>TestCase_B71</t>
+  </si>
+  <si>
+    <t>OPQA-398</t>
+  </si>
+  <si>
+    <t>Verify that record view of a patent gets displayed when user clicks on any patent option in the search type ahead while ALL option is selected in the search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B72</t>
+  </si>
+  <si>
+    <t>Verify that record view of a post gets displayed when user clicks on any post option in the search type ahead while ALL option is selected in the search drop down</t>
+  </si>
+  <si>
+    <t>OPQA-401</t>
   </si>
 </sst>
 </file>
@@ -1149,10 +1193,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1191,7 +1235,7 @@
         <v>97</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>153</v>
@@ -1208,7 +1252,7 @@
         <v>77</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>153</v>
@@ -1225,7 +1269,7 @@
         <v>78</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>153</v>
@@ -1242,7 +1286,7 @@
         <v>79</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>153</v>
@@ -1259,7 +1303,7 @@
         <v>80</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>153</v>
@@ -1276,7 +1320,7 @@
         <v>81</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>153</v>
@@ -1293,7 +1337,7 @@
         <v>74</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>153</v>
@@ -1310,7 +1354,7 @@
         <v>82</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>153</v>
@@ -1327,7 +1371,7 @@
         <v>83</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>153</v>
@@ -1344,7 +1388,7 @@
         <v>84</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>153</v>
@@ -1361,7 +1405,7 @@
         <v>85</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>153</v>
@@ -1378,7 +1422,7 @@
         <v>101</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>153</v>
@@ -1395,7 +1439,7 @@
         <v>86</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>153</v>
@@ -1412,7 +1456,7 @@
         <v>87</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>153</v>
@@ -1429,7 +1473,7 @@
         <v>88</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>153</v>
@@ -1446,7 +1490,7 @@
         <v>89</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>153</v>
@@ -1463,7 +1507,7 @@
         <v>140</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>153</v>
@@ -1480,7 +1524,7 @@
         <v>90</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>153</v>
@@ -1497,7 +1541,7 @@
         <v>91</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>153</v>
@@ -1514,7 +1558,7 @@
         <v>92</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>153</v>
@@ -1531,7 +1575,7 @@
         <v>93</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>153</v>
@@ -1548,7 +1592,7 @@
         <v>94</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>153</v>
@@ -1565,7 +1609,7 @@
         <v>95</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>153</v>
@@ -1582,7 +1626,7 @@
         <v>96</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>153</v>
@@ -1599,7 +1643,7 @@
         <v>104</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>153</v>
@@ -1616,7 +1660,7 @@
         <v>107</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>153</v>
@@ -1633,7 +1677,7 @@
         <v>110</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>153</v>
@@ -1650,7 +1694,7 @@
         <v>111</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>153</v>
@@ -1667,7 +1711,7 @@
         <v>116</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>153</v>
@@ -1684,7 +1728,7 @@
         <v>119</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>153</v>
@@ -1701,7 +1745,7 @@
         <v>122</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>153</v>
@@ -1718,7 +1762,7 @@
         <v>124</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>153</v>
@@ -1735,7 +1779,7 @@
         <v>126</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>153</v>
@@ -1752,7 +1796,7 @@
         <v>128</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>153</v>
@@ -1769,7 +1813,7 @@
         <v>134</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>153</v>
@@ -1786,7 +1830,7 @@
         <v>137</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>153</v>
@@ -1803,7 +1847,7 @@
         <v>140</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>153</v>
@@ -1820,7 +1864,7 @@
         <v>143</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>153</v>
@@ -1837,7 +1881,7 @@
         <v>146</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>153</v>
@@ -1854,7 +1898,7 @@
         <v>149</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>153</v>
@@ -1871,7 +1915,7 @@
         <v>152</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>153</v>
@@ -1888,7 +1932,7 @@
         <v>160</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>153</v>
@@ -1905,7 +1949,7 @@
         <v>161</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>153</v>
@@ -1922,7 +1966,7 @@
         <v>162</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>153</v>
@@ -1939,7 +1983,7 @@
         <v>163</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>153</v>
@@ -1956,7 +2000,7 @@
         <v>165</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>153</v>
@@ -1973,7 +2017,7 @@
         <v>167</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>153</v>
@@ -1990,7 +2034,7 @@
         <v>170</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>153</v>
@@ -2007,7 +2051,7 @@
         <v>172</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>153</v>
@@ -2015,16 +2059,16 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="B51" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="C51" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="C51" s="4" t="s">
-        <v>177</v>
-      </c>
       <c r="D51" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>153</v>
@@ -2032,16 +2076,16 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>68</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>153</v>
@@ -2049,16 +2093,16 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>71</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>153</v>
@@ -2066,16 +2110,16 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C54" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="B54" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>183</v>
-      </c>
       <c r="D54" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>153</v>
@@ -2083,16 +2127,16 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="B55" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="C55" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C55" s="4" t="s">
-        <v>187</v>
-      </c>
       <c r="D55" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>153</v>
@@ -2100,16 +2144,16 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>69</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>153</v>
@@ -2117,16 +2161,16 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>73</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>153</v>
@@ -2134,16 +2178,16 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>153</v>
@@ -2151,16 +2195,16 @@
     </row>
     <row r="59" spans="1:5" ht="120">
       <c r="A59" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B59" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="C59" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C59" s="4" t="s">
-        <v>197</v>
-      </c>
       <c r="D59" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>153</v>
@@ -2168,16 +2212,16 @@
     </row>
     <row r="60" spans="1:5" ht="30">
       <c r="A60" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B60" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C60" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C60" s="4" t="s">
-        <v>199</v>
-      </c>
       <c r="D60" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>153</v>
@@ -2185,16 +2229,16 @@
     </row>
     <row r="61" spans="1:5" ht="30">
       <c r="A61" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>70</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>153</v>
@@ -2202,16 +2246,16 @@
     </row>
     <row r="62" spans="1:5" ht="30">
       <c r="A62" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B62" s="8" t="s">
         <v>72</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>153</v>
@@ -2219,16 +2263,16 @@
     </row>
     <row r="63" spans="1:5" ht="30">
       <c r="A63" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="B63" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="B63" s="8" t="s">
-        <v>208</v>
-      </c>
       <c r="C63" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>153</v>
@@ -2236,7 +2280,7 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B64" s="8" t="s">
         <v>75</v>
@@ -2245,7 +2289,7 @@
         <v>74</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>153</v>
@@ -2253,16 +2297,16 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>153</v>
@@ -2270,16 +2314,16 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="B66" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="B66" s="8" t="s">
-        <v>214</v>
-      </c>
       <c r="C66" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>153</v>
@@ -2287,16 +2331,16 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C67" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="B67" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>218</v>
-      </c>
       <c r="D67" s="3" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>153</v>
@@ -2304,19 +2348,104 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="B68" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="B68" s="8" t="s">
+      <c r="C68" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E69" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="C68" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>205</v>
+    </row>
+    <row r="70" spans="1:5" ht="45">
+      <c r="A70" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="30">
+      <c r="A71" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="30">
+      <c r="A72" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="30">
+      <c r="A73" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes for watch list test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="251">
   <si>
     <t>TCID</t>
   </si>
@@ -803,6 +803,51 @@
   </si>
   <si>
     <t>OPQA-401</t>
+  </si>
+  <si>
+    <t>TestCase_B73</t>
+  </si>
+  <si>
+    <t>OPQA-402</t>
+  </si>
+  <si>
+    <t>Verify that profile page of a person gets displayed when user clicks on any PEOPLE option in the search type ahead while ALL option is selected in the search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B74</t>
+  </si>
+  <si>
+    <t>OPQA-403</t>
+  </si>
+  <si>
+    <t>Verify that record view of an article gets displayed when user clicks on any article option in the search type ahead while ARTICLES option is selected in the search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B75</t>
+  </si>
+  <si>
+    <t>OPQA-404</t>
+  </si>
+  <si>
+    <t>Verify that record view of a patent gets displayed when user clicks on any patent option in the search type ahead while PATENTS option is selected in the search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B76</t>
+  </si>
+  <si>
+    <t>Verify that record view of a post gets displayed when user clicks on any post option in the search type ahead while POSTS option is selected in the search drop down</t>
+  </si>
+  <si>
+    <t>OPQA-407</t>
+  </si>
+  <si>
+    <t>TestCase_B77</t>
+  </si>
+  <si>
+    <t>Verify that profile page of a person gets displayed when user clicks on any PEOPLE option in the search type ahead while PEOPLE option is selected in the search drop down</t>
+  </si>
+  <si>
+    <t>OPQA-409</t>
   </si>
 </sst>
 </file>
@@ -1193,10 +1238,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="D75" sqref="D2:D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1234,7 +1279,7 @@
       <c r="C2" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -1251,7 +1296,7 @@
       <c r="C3" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -1268,7 +1313,7 @@
       <c r="C4" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -1285,7 +1330,7 @@
       <c r="C5" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -1302,7 +1347,7 @@
       <c r="C6" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -1319,7 +1364,7 @@
       <c r="C7" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -1336,7 +1381,7 @@
       <c r="C8" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -1353,7 +1398,7 @@
       <c r="C9" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -1370,7 +1415,7 @@
       <c r="C10" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -1387,7 +1432,7 @@
       <c r="C11" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -1404,7 +1449,7 @@
       <c r="C12" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -1421,7 +1466,7 @@
       <c r="C13" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -1438,7 +1483,7 @@
       <c r="C14" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -1455,7 +1500,7 @@
       <c r="C15" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -1472,7 +1517,7 @@
       <c r="C16" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -1489,7 +1534,7 @@
       <c r="C17" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E17" s="3" t="s">
@@ -1506,7 +1551,7 @@
       <c r="C18" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E18" s="3" t="s">
@@ -1523,7 +1568,7 @@
       <c r="C19" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E19" s="3" t="s">
@@ -1540,7 +1585,7 @@
       <c r="C20" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E20" s="3" t="s">
@@ -1557,7 +1602,7 @@
       <c r="C21" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E21" s="3" t="s">
@@ -1574,7 +1619,7 @@
       <c r="C22" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E22" s="3" t="s">
@@ -1591,7 +1636,7 @@
       <c r="C23" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E23" s="3" t="s">
@@ -1608,7 +1653,7 @@
       <c r="C24" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E24" s="3" t="s">
@@ -1625,7 +1670,7 @@
       <c r="C25" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E25" s="3" t="s">
@@ -1642,7 +1687,7 @@
       <c r="C26" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E26" s="3" t="s">
@@ -1659,7 +1704,7 @@
       <c r="C27" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E27" s="3" t="s">
@@ -1676,7 +1721,7 @@
       <c r="C28" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E28" s="3" t="s">
@@ -1693,7 +1738,7 @@
       <c r="C29" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E29" s="3" t="s">
@@ -1710,7 +1755,7 @@
       <c r="C30" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E30" s="3" t="s">
@@ -1727,7 +1772,7 @@
       <c r="C31" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E31" s="3" t="s">
@@ -1744,7 +1789,7 @@
       <c r="C32" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E32" s="3" t="s">
@@ -1761,7 +1806,7 @@
       <c r="C33" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E33" s="3" t="s">
@@ -1778,7 +1823,7 @@
       <c r="C34" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E34" s="3" t="s">
@@ -1795,7 +1840,7 @@
       <c r="C35" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E35" s="3" t="s">
@@ -1812,7 +1857,7 @@
       <c r="C36" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E36" s="3" t="s">
@@ -1829,7 +1874,7 @@
       <c r="C37" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E37" s="3" t="s">
@@ -1846,7 +1891,7 @@
       <c r="C38" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E38" s="3" t="s">
@@ -1863,7 +1908,7 @@
       <c r="C39" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E39" s="3" t="s">
@@ -1880,7 +1925,7 @@
       <c r="C40" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E40" s="3" t="s">
@@ -1897,7 +1942,7 @@
       <c r="C41" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E41" s="3" t="s">
@@ -1914,7 +1959,7 @@
       <c r="C42" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E42" s="3" t="s">
@@ -1931,7 +1976,7 @@
       <c r="C43" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E43" s="3" t="s">
@@ -1948,7 +1993,7 @@
       <c r="C44" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E44" s="3" t="s">
@@ -1965,7 +2010,7 @@
       <c r="C45" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E45" s="3" t="s">
@@ -1982,7 +2027,7 @@
       <c r="C46" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E46" s="3" t="s">
@@ -1999,7 +2044,7 @@
       <c r="C47" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E47" s="3" t="s">
@@ -2016,7 +2061,7 @@
       <c r="C48" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E48" s="3" t="s">
@@ -2033,7 +2078,7 @@
       <c r="C49" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E49" s="3" t="s">
@@ -2050,7 +2095,7 @@
       <c r="C50" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E50" s="3" t="s">
@@ -2067,7 +2112,7 @@
       <c r="C51" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D51" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E51" s="3" t="s">
@@ -2084,7 +2129,7 @@
       <c r="C52" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E52" s="3" t="s">
@@ -2101,7 +2146,7 @@
       <c r="C53" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D53" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E53" s="3" t="s">
@@ -2118,7 +2163,7 @@
       <c r="C54" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="D54" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E54" s="3" t="s">
@@ -2135,7 +2180,7 @@
       <c r="C55" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D55" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E55" s="3" t="s">
@@ -2152,7 +2197,7 @@
       <c r="C56" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D56" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E56" s="3" t="s">
@@ -2169,7 +2214,7 @@
       <c r="C57" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="D57" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E57" s="3" t="s">
@@ -2186,7 +2231,7 @@
       <c r="C58" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="D58" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E58" s="3" t="s">
@@ -2203,7 +2248,7 @@
       <c r="C59" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="D59" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E59" s="3" t="s">
@@ -2220,7 +2265,7 @@
       <c r="C60" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="D60" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E60" s="3" t="s">
@@ -2237,7 +2282,7 @@
       <c r="C61" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="D61" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E61" s="3" t="s">
@@ -2254,7 +2299,7 @@
       <c r="C62" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="D62" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E62" s="3" t="s">
@@ -2271,7 +2316,7 @@
       <c r="C63" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="D63" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E63" s="3" t="s">
@@ -2288,7 +2333,7 @@
       <c r="C64" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="D64" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E64" s="3" t="s">
@@ -2305,7 +2350,7 @@
       <c r="C65" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="D65" s="3" t="s">
+      <c r="D65" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E65" s="3" t="s">
@@ -2322,7 +2367,7 @@
       <c r="C66" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="D66" s="3" t="s">
+      <c r="D66" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E66" s="3" t="s">
@@ -2339,7 +2384,7 @@
       <c r="C67" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="D67" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E67" s="3" t="s">
@@ -2356,7 +2401,7 @@
       <c r="C68" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="D68" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E68" s="3" t="s">
@@ -2373,11 +2418,11 @@
       <c r="C69" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="D69" s="3" t="s">
+      <c r="D69" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>221</v>
+        <v>153</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="45">
@@ -2390,11 +2435,11 @@
       <c r="C70" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="D70" s="3" t="s">
+      <c r="D70" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>221</v>
+        <v>153</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="30">
@@ -2407,11 +2452,11 @@
       <c r="C71" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="D71" s="3" t="s">
+      <c r="D71" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>221</v>
+        <v>153</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="30">
@@ -2424,11 +2469,11 @@
       <c r="C72" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="D72" s="3" t="s">
+      <c r="D72" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>221</v>
+        <v>153</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="30">
@@ -2441,10 +2486,95 @@
       <c r="C73" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="D73" s="3" t="s">
+      <c r="D73" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E73" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="30">
+      <c r="A74" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="30">
+      <c r="A75" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="30">
+      <c r="A76" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="30">
+      <c r="A77" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="30">
+      <c r="A78" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E78" s="3" t="s">
         <v>221</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding test case to authoring
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="251">
   <si>
     <t>TCID</t>
   </si>
@@ -803,6 +803,51 @@
   </si>
   <si>
     <t>OPQA-401</t>
+  </si>
+  <si>
+    <t>TestCase_B73</t>
+  </si>
+  <si>
+    <t>OPQA-402</t>
+  </si>
+  <si>
+    <t>Verify that profile page of a person gets displayed when user clicks on any PEOPLE option in the search type ahead while ALL option is selected in the search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B74</t>
+  </si>
+  <si>
+    <t>OPQA-403</t>
+  </si>
+  <si>
+    <t>Verify that record view of an article gets displayed when user clicks on any article option in the search type ahead while ARTICLES option is selected in the search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B75</t>
+  </si>
+  <si>
+    <t>OPQA-404</t>
+  </si>
+  <si>
+    <t>Verify that record view of a patent gets displayed when user clicks on any patent option in the search type ahead while PATENTS option is selected in the search drop down</t>
+  </si>
+  <si>
+    <t>TestCase_B76</t>
+  </si>
+  <si>
+    <t>Verify that record view of a post gets displayed when user clicks on any post option in the search type ahead while POSTS option is selected in the search drop down</t>
+  </si>
+  <si>
+    <t>OPQA-407</t>
+  </si>
+  <si>
+    <t>TestCase_B77</t>
+  </si>
+  <si>
+    <t>Verify that profile page of a person gets displayed when user clicks on any PEOPLE option in the search type ahead while PEOPLE option is selected in the search drop down</t>
+  </si>
+  <si>
+    <t>OPQA-409</t>
   </si>
 </sst>
 </file>
@@ -1193,10 +1238,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="D75" sqref="D2:D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1234,7 +1279,7 @@
       <c r="C2" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -1251,7 +1296,7 @@
       <c r="C3" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -1268,7 +1313,7 @@
       <c r="C4" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -1285,7 +1330,7 @@
       <c r="C5" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -1302,7 +1347,7 @@
       <c r="C6" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -1319,7 +1364,7 @@
       <c r="C7" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -1336,7 +1381,7 @@
       <c r="C8" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -1353,7 +1398,7 @@
       <c r="C9" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -1370,7 +1415,7 @@
       <c r="C10" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -1387,7 +1432,7 @@
       <c r="C11" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -1404,7 +1449,7 @@
       <c r="C12" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -1421,7 +1466,7 @@
       <c r="C13" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -1438,7 +1483,7 @@
       <c r="C14" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -1455,7 +1500,7 @@
       <c r="C15" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -1472,7 +1517,7 @@
       <c r="C16" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -1489,7 +1534,7 @@
       <c r="C17" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E17" s="3" t="s">
@@ -1506,7 +1551,7 @@
       <c r="C18" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E18" s="3" t="s">
@@ -1523,7 +1568,7 @@
       <c r="C19" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E19" s="3" t="s">
@@ -1540,7 +1585,7 @@
       <c r="C20" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E20" s="3" t="s">
@@ -1557,7 +1602,7 @@
       <c r="C21" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E21" s="3" t="s">
@@ -1574,7 +1619,7 @@
       <c r="C22" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E22" s="3" t="s">
@@ -1591,7 +1636,7 @@
       <c r="C23" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E23" s="3" t="s">
@@ -1608,7 +1653,7 @@
       <c r="C24" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E24" s="3" t="s">
@@ -1625,7 +1670,7 @@
       <c r="C25" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E25" s="3" t="s">
@@ -1642,7 +1687,7 @@
       <c r="C26" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E26" s="3" t="s">
@@ -1659,7 +1704,7 @@
       <c r="C27" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E27" s="3" t="s">
@@ -1676,7 +1721,7 @@
       <c r="C28" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E28" s="3" t="s">
@@ -1693,7 +1738,7 @@
       <c r="C29" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E29" s="3" t="s">
@@ -1710,7 +1755,7 @@
       <c r="C30" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E30" s="3" t="s">
@@ -1727,7 +1772,7 @@
       <c r="C31" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E31" s="3" t="s">
@@ -1744,7 +1789,7 @@
       <c r="C32" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E32" s="3" t="s">
@@ -1761,7 +1806,7 @@
       <c r="C33" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E33" s="3" t="s">
@@ -1778,7 +1823,7 @@
       <c r="C34" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E34" s="3" t="s">
@@ -1795,7 +1840,7 @@
       <c r="C35" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E35" s="3" t="s">
@@ -1812,7 +1857,7 @@
       <c r="C36" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E36" s="3" t="s">
@@ -1829,7 +1874,7 @@
       <c r="C37" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E37" s="3" t="s">
@@ -1846,7 +1891,7 @@
       <c r="C38" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E38" s="3" t="s">
@@ -1863,7 +1908,7 @@
       <c r="C39" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E39" s="3" t="s">
@@ -1880,7 +1925,7 @@
       <c r="C40" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E40" s="3" t="s">
@@ -1897,7 +1942,7 @@
       <c r="C41" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E41" s="3" t="s">
@@ -1914,7 +1959,7 @@
       <c r="C42" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E42" s="3" t="s">
@@ -1931,7 +1976,7 @@
       <c r="C43" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E43" s="3" t="s">
@@ -1948,7 +1993,7 @@
       <c r="C44" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E44" s="3" t="s">
@@ -1965,7 +2010,7 @@
       <c r="C45" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E45" s="3" t="s">
@@ -1982,7 +2027,7 @@
       <c r="C46" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E46" s="3" t="s">
@@ -1999,7 +2044,7 @@
       <c r="C47" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E47" s="3" t="s">
@@ -2016,7 +2061,7 @@
       <c r="C48" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E48" s="3" t="s">
@@ -2033,7 +2078,7 @@
       <c r="C49" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E49" s="3" t="s">
@@ -2050,7 +2095,7 @@
       <c r="C50" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E50" s="3" t="s">
@@ -2067,7 +2112,7 @@
       <c r="C51" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D51" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E51" s="3" t="s">
@@ -2084,7 +2129,7 @@
       <c r="C52" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E52" s="3" t="s">
@@ -2101,7 +2146,7 @@
       <c r="C53" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D53" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E53" s="3" t="s">
@@ -2118,7 +2163,7 @@
       <c r="C54" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="D54" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E54" s="3" t="s">
@@ -2135,7 +2180,7 @@
       <c r="C55" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D55" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E55" s="3" t="s">
@@ -2152,7 +2197,7 @@
       <c r="C56" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D56" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E56" s="3" t="s">
@@ -2169,7 +2214,7 @@
       <c r="C57" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="D57" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E57" s="3" t="s">
@@ -2186,7 +2231,7 @@
       <c r="C58" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="D58" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E58" s="3" t="s">
@@ -2203,7 +2248,7 @@
       <c r="C59" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="D59" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E59" s="3" t="s">
@@ -2220,7 +2265,7 @@
       <c r="C60" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="D60" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E60" s="3" t="s">
@@ -2237,7 +2282,7 @@
       <c r="C61" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="D61" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E61" s="3" t="s">
@@ -2254,7 +2299,7 @@
       <c r="C62" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="D62" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E62" s="3" t="s">
@@ -2271,7 +2316,7 @@
       <c r="C63" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="D63" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E63" s="3" t="s">
@@ -2288,7 +2333,7 @@
       <c r="C64" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="D64" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E64" s="3" t="s">
@@ -2305,7 +2350,7 @@
       <c r="C65" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="D65" s="3" t="s">
+      <c r="D65" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E65" s="3" t="s">
@@ -2322,7 +2367,7 @@
       <c r="C66" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="D66" s="3" t="s">
+      <c r="D66" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E66" s="3" t="s">
@@ -2339,7 +2384,7 @@
       <c r="C67" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="D67" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E67" s="3" t="s">
@@ -2356,7 +2401,7 @@
       <c r="C68" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="D68" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E68" s="3" t="s">
@@ -2373,11 +2418,11 @@
       <c r="C69" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="D69" s="3" t="s">
+      <c r="D69" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>221</v>
+        <v>153</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="45">
@@ -2390,11 +2435,11 @@
       <c r="C70" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="D70" s="3" t="s">
+      <c r="D70" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>221</v>
+        <v>153</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="30">
@@ -2407,11 +2452,11 @@
       <c r="C71" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="D71" s="3" t="s">
+      <c r="D71" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>221</v>
+        <v>153</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="30">
@@ -2424,11 +2469,11 @@
       <c r="C72" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="D72" s="3" t="s">
+      <c r="D72" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>221</v>
+        <v>153</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="30">
@@ -2441,10 +2486,95 @@
       <c r="C73" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="D73" s="3" t="s">
+      <c r="D73" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E73" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="30">
+      <c r="A74" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="30">
+      <c r="A75" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="30">
+      <c r="A76" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="30">
+      <c r="A77" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="30">
+      <c r="A78" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E78" s="3" t="s">
         <v>221</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changing waits in suite B
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="284">
   <si>
     <t>TCID</t>
   </si>
@@ -758,9 +758,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
     <t>TestCase_B68</t>
   </si>
   <si>
@@ -909,9 +906,6 @@
   </si>
   <si>
     <t>OPQA-563</t>
-  </si>
-  <si>
-    <t>FAIL</t>
   </si>
   <si>
     <t>TestCase_B84</t>
@@ -983,6 +977,9 @@
   </si>
   <si>
     <t>TestCase_B88</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -1375,8 +1372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1418,7 +1415,7 @@
         <v>220</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>269</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1571,7 +1568,7 @@
         <v>220</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>153</v>
+        <v>283</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16.5" customHeight="1">
@@ -2545,13 +2542,13 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>64</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D69" s="7" t="s">
         <v>220</v>
@@ -2562,13 +2559,13 @@
     </row>
     <row r="70" spans="1:5" ht="45">
       <c r="A70" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="B70" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="B70" s="8" t="s">
+      <c r="C70" s="4" t="s">
         <v>225</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>226</v>
       </c>
       <c r="D70" s="7" t="s">
         <v>220</v>
@@ -2579,13 +2576,13 @@
     </row>
     <row r="71" spans="1:5" ht="30">
       <c r="A71" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="C71" s="4" t="s">
         <v>227</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>228</v>
       </c>
       <c r="D71" s="7" t="s">
         <v>220</v>
@@ -2596,13 +2593,13 @@
     </row>
     <row r="72" spans="1:5" ht="30">
       <c r="A72" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="B72" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="B72" s="6" t="s">
+      <c r="C72" s="4" t="s">
         <v>231</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>232</v>
       </c>
       <c r="D72" s="7" t="s">
         <v>220</v>
@@ -2613,13 +2610,13 @@
     </row>
     <row r="73" spans="1:5" ht="30">
       <c r="A73" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="C73" s="4" t="s">
         <v>233</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>234</v>
       </c>
       <c r="D73" s="7" t="s">
         <v>220</v>
@@ -2630,13 +2627,13 @@
     </row>
     <row r="74" spans="1:5" ht="30">
       <c r="A74" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="B74" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="B74" s="6" t="s">
+      <c r="C74" s="4" t="s">
         <v>237</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>238</v>
       </c>
       <c r="D74" s="7" t="s">
         <v>220</v>
@@ -2647,13 +2644,13 @@
     </row>
     <row r="75" spans="1:5" ht="30">
       <c r="A75" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="B75" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="B75" s="6" t="s">
+      <c r="C75" s="4" t="s">
         <v>240</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>241</v>
       </c>
       <c r="D75" s="7" t="s">
         <v>220</v>
@@ -2664,13 +2661,13 @@
     </row>
     <row r="76" spans="1:5" ht="30">
       <c r="A76" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="B76" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="B76" s="6" t="s">
+      <c r="C76" s="4" t="s">
         <v>243</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>244</v>
       </c>
       <c r="D76" s="7" t="s">
         <v>220</v>
@@ -2681,13 +2678,13 @@
     </row>
     <row r="77" spans="1:5" ht="30">
       <c r="A77" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="C77" s="4" t="s">
         <v>245</v>
-      </c>
-      <c r="B77" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>246</v>
       </c>
       <c r="D77" s="7" t="s">
         <v>220</v>
@@ -2698,13 +2695,13 @@
     </row>
     <row r="78" spans="1:5" ht="30">
       <c r="A78" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="C78" s="4" t="s">
         <v>248</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>249</v>
       </c>
       <c r="D78" s="7" t="s">
         <v>220</v>
@@ -2715,13 +2712,13 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="B79" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="B79" s="6" t="s">
+      <c r="C79" s="4" t="s">
         <v>252</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>253</v>
       </c>
       <c r="D79" s="7" t="s">
         <v>220</v>
@@ -2732,13 +2729,13 @@
     </row>
     <row r="80" spans="1:5" ht="90">
       <c r="A80" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B80" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="B80" s="6" t="s">
+      <c r="C80" s="4" t="s">
         <v>255</v>
-      </c>
-      <c r="C80" s="4" t="s">
-        <v>256</v>
       </c>
       <c r="D80" s="7" t="s">
         <v>220</v>
@@ -2749,13 +2746,13 @@
     </row>
     <row r="81" spans="1:5" ht="60">
       <c r="A81" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="C81" s="4" t="s">
         <v>257</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>258</v>
       </c>
       <c r="D81" s="7" t="s">
         <v>220</v>
@@ -2766,13 +2763,13 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="B82" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="B82" s="6" t="s">
+      <c r="C82" s="4" t="s">
         <v>261</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>262</v>
       </c>
       <c r="D82" s="7" t="s">
         <v>220</v>
@@ -2783,13 +2780,13 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="B83" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="B83" s="6" t="s">
+      <c r="C83" s="4" t="s">
         <v>264</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>265</v>
       </c>
       <c r="D83" s="7" t="s">
         <v>220</v>
@@ -2800,95 +2797,105 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="B84" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="B84" s="6" t="s">
-        <v>268</v>
-      </c>
       <c r="C84" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D84" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>221</v>
+        <v>153</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="120">
       <c r="A85" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D85" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="E85" s="3"/>
+      <c r="E85" s="3" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="86" spans="1:5" ht="120">
       <c r="A86" s="7" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D86" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="E86" s="3"/>
+      <c r="E86" s="3" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="87" spans="1:5" ht="195">
       <c r="A87" s="7" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D87" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="E87" s="3"/>
+      <c r="E87" s="3" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="7" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D88" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="E88" s="3"/>
+      <c r="E88" s="3" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="7" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D89" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="E89" s="3"/>
+      <c r="E89" s="3" t="s">
+        <v>153</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
removing thread sleeps for search testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="284">
   <si>
     <t>TCID</t>
   </si>
@@ -758,9 +758,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
     <t>TestCase_B68</t>
   </si>
   <si>
@@ -909,9 +906,6 @@
   </si>
   <si>
     <t>OPQA-563</t>
-  </si>
-  <si>
-    <t>FAIL</t>
   </si>
   <si>
     <t>TestCase_B84</t>
@@ -983,6 +977,9 @@
   </si>
   <si>
     <t>TestCase_B88</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -1375,8 +1372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1418,7 +1415,7 @@
         <v>220</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>269</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1571,7 +1568,7 @@
         <v>220</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>153</v>
+        <v>283</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16.5" customHeight="1">
@@ -2545,13 +2542,13 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>64</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D69" s="7" t="s">
         <v>220</v>
@@ -2562,13 +2559,13 @@
     </row>
     <row r="70" spans="1:5" ht="45">
       <c r="A70" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="B70" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="B70" s="8" t="s">
+      <c r="C70" s="4" t="s">
         <v>225</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>226</v>
       </c>
       <c r="D70" s="7" t="s">
         <v>220</v>
@@ -2579,13 +2576,13 @@
     </row>
     <row r="71" spans="1:5" ht="30">
       <c r="A71" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="C71" s="4" t="s">
         <v>227</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>228</v>
       </c>
       <c r="D71" s="7" t="s">
         <v>220</v>
@@ -2596,13 +2593,13 @@
     </row>
     <row r="72" spans="1:5" ht="30">
       <c r="A72" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="B72" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="B72" s="6" t="s">
+      <c r="C72" s="4" t="s">
         <v>231</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>232</v>
       </c>
       <c r="D72" s="7" t="s">
         <v>220</v>
@@ -2613,13 +2610,13 @@
     </row>
     <row r="73" spans="1:5" ht="30">
       <c r="A73" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="C73" s="4" t="s">
         <v>233</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>234</v>
       </c>
       <c r="D73" s="7" t="s">
         <v>220</v>
@@ -2630,13 +2627,13 @@
     </row>
     <row r="74" spans="1:5" ht="30">
       <c r="A74" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="B74" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="B74" s="6" t="s">
+      <c r="C74" s="4" t="s">
         <v>237</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>238</v>
       </c>
       <c r="D74" s="7" t="s">
         <v>220</v>
@@ -2647,13 +2644,13 @@
     </row>
     <row r="75" spans="1:5" ht="30">
       <c r="A75" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="B75" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="B75" s="6" t="s">
+      <c r="C75" s="4" t="s">
         <v>240</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>241</v>
       </c>
       <c r="D75" s="7" t="s">
         <v>220</v>
@@ -2664,13 +2661,13 @@
     </row>
     <row r="76" spans="1:5" ht="30">
       <c r="A76" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="B76" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="B76" s="6" t="s">
+      <c r="C76" s="4" t="s">
         <v>243</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>244</v>
       </c>
       <c r="D76" s="7" t="s">
         <v>220</v>
@@ -2681,13 +2678,13 @@
     </row>
     <row r="77" spans="1:5" ht="30">
       <c r="A77" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="C77" s="4" t="s">
         <v>245</v>
-      </c>
-      <c r="B77" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>246</v>
       </c>
       <c r="D77" s="7" t="s">
         <v>220</v>
@@ -2698,13 +2695,13 @@
     </row>
     <row r="78" spans="1:5" ht="30">
       <c r="A78" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="C78" s="4" t="s">
         <v>248</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>249</v>
       </c>
       <c r="D78" s="7" t="s">
         <v>220</v>
@@ -2715,13 +2712,13 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="B79" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="B79" s="6" t="s">
+      <c r="C79" s="4" t="s">
         <v>252</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>253</v>
       </c>
       <c r="D79" s="7" t="s">
         <v>220</v>
@@ -2732,13 +2729,13 @@
     </row>
     <row r="80" spans="1:5" ht="90">
       <c r="A80" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B80" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="B80" s="6" t="s">
+      <c r="C80" s="4" t="s">
         <v>255</v>
-      </c>
-      <c r="C80" s="4" t="s">
-        <v>256</v>
       </c>
       <c r="D80" s="7" t="s">
         <v>220</v>
@@ -2749,13 +2746,13 @@
     </row>
     <row r="81" spans="1:5" ht="60">
       <c r="A81" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="C81" s="4" t="s">
         <v>257</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>258</v>
       </c>
       <c r="D81" s="7" t="s">
         <v>220</v>
@@ -2766,13 +2763,13 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="B82" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="B82" s="6" t="s">
+      <c r="C82" s="4" t="s">
         <v>261</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>262</v>
       </c>
       <c r="D82" s="7" t="s">
         <v>220</v>
@@ -2783,13 +2780,13 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="B83" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="B83" s="6" t="s">
+      <c r="C83" s="4" t="s">
         <v>264</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>265</v>
       </c>
       <c r="D83" s="7" t="s">
         <v>220</v>
@@ -2800,95 +2797,105 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="B84" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="B84" s="6" t="s">
-        <v>268</v>
-      </c>
       <c r="C84" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D84" s="7" t="s">
         <v>220</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>221</v>
+        <v>153</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="120">
       <c r="A85" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D85" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="E85" s="3"/>
+      <c r="E85" s="3" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="86" spans="1:5" ht="120">
       <c r="A86" s="7" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D86" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="E86" s="3"/>
+      <c r="E86" s="3" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="87" spans="1:5" ht="195">
       <c r="A87" s="7" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D87" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="E87" s="3"/>
+      <c r="E87" s="3" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="7" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D88" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="E88" s="3"/>
+      <c r="E88" s="3" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="7" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D89" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="E89" s="3"/>
+      <c r="E89" s="3" t="s">
+        <v>153</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changing wait statements in search test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -979,7 +979,7 @@
     <t>TestCase_B88</t>
   </si>
   <si>
-    <t>FAIL</t>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
@@ -1568,7 +1568,7 @@
         <v>220</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>283</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16.5" customHeight="1">
@@ -1738,7 +1738,7 @@
         <v>220</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>153</v>
+        <v>283</v>
       </c>
     </row>
     <row r="22" spans="1:5">

</xml_diff>

<commit_message>
Adding 3 search test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="294">
   <si>
     <t>TCID</t>
   </si>
@@ -977,6 +977,36 @@
   </si>
   <si>
     <t>TestCase_B88</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>TestCase_B89</t>
+  </si>
+  <si>
+    <t>OPQA-575</t>
+  </si>
+  <si>
+    <t>Verify that DETAILS link is working correctly in record view page of a patent</t>
+  </si>
+  <si>
+    <t>TestCase_B90</t>
+  </si>
+  <si>
+    <t>TestCase_B91</t>
+  </si>
+  <si>
+    <t>Verify that following options get displayed in SORT BY drop down in ARTICLES search results page: a)Relevance b)Times Cited c)Publication Date(Newest) d)Publication Date(Oldest)</t>
+  </si>
+  <si>
+    <t>OPQA-577</t>
+  </si>
+  <si>
+    <t>OPQA-579</t>
+  </si>
+  <si>
+    <t>Verify that search results are sorted by RELEVANCE by default in PATENTS search results page</t>
   </si>
   <si>
     <t>PASS</t>
@@ -1370,10 +1400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E89"/>
+  <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D89"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="D92" sqref="D2:D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1411,7 +1441,7 @@
       <c r="C2" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -1428,7 +1458,7 @@
       <c r="C3" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -1445,7 +1475,7 @@
       <c r="C4" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -1462,7 +1492,7 @@
       <c r="C5" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -1479,7 +1509,7 @@
       <c r="C6" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -1496,7 +1526,7 @@
       <c r="C7" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -1513,7 +1543,7 @@
       <c r="C8" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -1530,7 +1560,7 @@
       <c r="C9" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -1547,7 +1577,7 @@
       <c r="C10" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -1564,7 +1594,7 @@
       <c r="C11" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -1581,7 +1611,7 @@
       <c r="C12" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -1598,7 +1628,7 @@
       <c r="C13" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -1615,7 +1645,7 @@
       <c r="C14" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -1632,7 +1662,7 @@
       <c r="C15" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -1649,7 +1679,7 @@
       <c r="C16" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -1666,7 +1696,7 @@
       <c r="C17" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E17" s="3" t="s">
@@ -1683,7 +1713,7 @@
       <c r="C18" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E18" s="3" t="s">
@@ -1700,7 +1730,7 @@
       <c r="C19" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E19" s="3" t="s">
@@ -1717,7 +1747,7 @@
       <c r="C20" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E20" s="3" t="s">
@@ -1734,11 +1764,11 @@
       <c r="C21" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>283</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1751,7 +1781,7 @@
       <c r="C22" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E22" s="3" t="s">
@@ -1768,7 +1798,7 @@
       <c r="C23" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E23" s="3" t="s">
@@ -1785,7 +1815,7 @@
       <c r="C24" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E24" s="3" t="s">
@@ -1802,7 +1832,7 @@
       <c r="C25" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E25" s="3" t="s">
@@ -1819,7 +1849,7 @@
       <c r="C26" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E26" s="3" t="s">
@@ -1836,7 +1866,7 @@
       <c r="C27" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E27" s="3" t="s">
@@ -1853,7 +1883,7 @@
       <c r="C28" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E28" s="3" t="s">
@@ -1870,7 +1900,7 @@
       <c r="C29" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E29" s="3" t="s">
@@ -1887,7 +1917,7 @@
       <c r="C30" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E30" s="3" t="s">
@@ -1904,7 +1934,7 @@
       <c r="C31" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E31" s="3" t="s">
@@ -1921,7 +1951,7 @@
       <c r="C32" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E32" s="3" t="s">
@@ -1938,7 +1968,7 @@
       <c r="C33" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E33" s="3" t="s">
@@ -1955,7 +1985,7 @@
       <c r="C34" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E34" s="3" t="s">
@@ -1972,7 +2002,7 @@
       <c r="C35" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E35" s="3" t="s">
@@ -1989,7 +2019,7 @@
       <c r="C36" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E36" s="3" t="s">
@@ -2006,7 +2036,7 @@
       <c r="C37" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E37" s="3" t="s">
@@ -2023,7 +2053,7 @@
       <c r="C38" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E38" s="3" t="s">
@@ -2040,7 +2070,7 @@
       <c r="C39" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E39" s="3" t="s">
@@ -2057,7 +2087,7 @@
       <c r="C40" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E40" s="3" t="s">
@@ -2074,7 +2104,7 @@
       <c r="C41" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E41" s="3" t="s">
@@ -2091,7 +2121,7 @@
       <c r="C42" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E42" s="3" t="s">
@@ -2108,7 +2138,7 @@
       <c r="C43" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E43" s="3" t="s">
@@ -2125,7 +2155,7 @@
       <c r="C44" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E44" s="3" t="s">
@@ -2142,7 +2172,7 @@
       <c r="C45" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D45" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E45" s="3" t="s">
@@ -2159,7 +2189,7 @@
       <c r="C46" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="D46" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E46" s="3" t="s">
@@ -2176,7 +2206,7 @@
       <c r="C47" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D47" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E47" s="3" t="s">
@@ -2193,7 +2223,7 @@
       <c r="C48" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E48" s="3" t="s">
@@ -2210,7 +2240,7 @@
       <c r="C49" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E49" s="3" t="s">
@@ -2227,7 +2257,7 @@
       <c r="C50" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D50" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E50" s="3" t="s">
@@ -2244,7 +2274,7 @@
       <c r="C51" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D51" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E51" s="3" t="s">
@@ -2261,7 +2291,7 @@
       <c r="C52" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="D52" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E52" s="3" t="s">
@@ -2278,7 +2308,7 @@
       <c r="C53" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D53" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E53" s="3" t="s">
@@ -2295,7 +2325,7 @@
       <c r="C54" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D54" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E54" s="3" t="s">
@@ -2312,7 +2342,7 @@
       <c r="C55" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="D55" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E55" s="3" t="s">
@@ -2329,7 +2359,7 @@
       <c r="C56" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="D56" s="7" t="s">
+      <c r="D56" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E56" s="3" t="s">
@@ -2346,7 +2376,7 @@
       <c r="C57" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="D57" s="7" t="s">
+      <c r="D57" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E57" s="3" t="s">
@@ -2363,7 +2393,7 @@
       <c r="C58" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="D58" s="7" t="s">
+      <c r="D58" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E58" s="3" t="s">
@@ -2380,7 +2410,7 @@
       <c r="C59" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="D59" s="7" t="s">
+      <c r="D59" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E59" s="3" t="s">
@@ -2397,7 +2427,7 @@
       <c r="C60" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="D60" s="7" t="s">
+      <c r="D60" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E60" s="3" t="s">
@@ -2414,7 +2444,7 @@
       <c r="C61" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="D61" s="7" t="s">
+      <c r="D61" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E61" s="3" t="s">
@@ -2431,7 +2461,7 @@
       <c r="C62" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="D62" s="7" t="s">
+      <c r="D62" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E62" s="3" t="s">
@@ -2448,7 +2478,7 @@
       <c r="C63" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="D63" s="7" t="s">
+      <c r="D63" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E63" s="3" t="s">
@@ -2465,7 +2495,7 @@
       <c r="C64" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D64" s="7" t="s">
+      <c r="D64" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E64" s="3" t="s">
@@ -2482,7 +2512,7 @@
       <c r="C65" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="D65" s="7" t="s">
+      <c r="D65" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E65" s="3" t="s">
@@ -2499,7 +2529,7 @@
       <c r="C66" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="D66" s="7" t="s">
+      <c r="D66" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E66" s="3" t="s">
@@ -2516,7 +2546,7 @@
       <c r="C67" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="D67" s="7" t="s">
+      <c r="D67" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E67" s="3" t="s">
@@ -2533,7 +2563,7 @@
       <c r="C68" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="D68" s="7" t="s">
+      <c r="D68" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E68" s="3" t="s">
@@ -2550,7 +2580,7 @@
       <c r="C69" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="D69" s="7" t="s">
+      <c r="D69" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E69" s="3" t="s">
@@ -2567,7 +2597,7 @@
       <c r="C70" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="D70" s="7" t="s">
+      <c r="D70" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E70" s="3" t="s">
@@ -2584,7 +2614,7 @@
       <c r="C71" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="D71" s="7" t="s">
+      <c r="D71" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E71" s="3" t="s">
@@ -2601,7 +2631,7 @@
       <c r="C72" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="D72" s="7" t="s">
+      <c r="D72" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E72" s="3" t="s">
@@ -2618,7 +2648,7 @@
       <c r="C73" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="D73" s="7" t="s">
+      <c r="D73" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E73" s="3" t="s">
@@ -2635,7 +2665,7 @@
       <c r="C74" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="D74" s="7" t="s">
+      <c r="D74" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E74" s="3" t="s">
@@ -2652,7 +2682,7 @@
       <c r="C75" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="D75" s="7" t="s">
+      <c r="D75" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E75" s="3" t="s">
@@ -2669,7 +2699,7 @@
       <c r="C76" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="D76" s="7" t="s">
+      <c r="D76" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E76" s="3" t="s">
@@ -2686,7 +2716,7 @@
       <c r="C77" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="D77" s="7" t="s">
+      <c r="D77" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E77" s="3" t="s">
@@ -2703,7 +2733,7 @@
       <c r="C78" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="D78" s="7" t="s">
+      <c r="D78" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E78" s="3" t="s">
@@ -2720,7 +2750,7 @@
       <c r="C79" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="D79" s="7" t="s">
+      <c r="D79" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E79" s="3" t="s">
@@ -2737,7 +2767,7 @@
       <c r="C80" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="D80" s="7" t="s">
+      <c r="D80" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E80" s="3" t="s">
@@ -2754,7 +2784,7 @@
       <c r="C81" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="D81" s="7" t="s">
+      <c r="D81" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E81" s="3" t="s">
@@ -2771,7 +2801,7 @@
       <c r="C82" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="D82" s="7" t="s">
+      <c r="D82" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E82" s="3" t="s">
@@ -2788,7 +2818,7 @@
       <c r="C83" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="D83" s="7" t="s">
+      <c r="D83" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E83" s="3" t="s">
@@ -2805,7 +2835,7 @@
       <c r="C84" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="D84" s="7" t="s">
+      <c r="D84" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E84" s="3" t="s">
@@ -2822,7 +2852,7 @@
       <c r="C85" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="D85" s="7" t="s">
+      <c r="D85" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E85" s="3" t="s">
@@ -2839,7 +2869,7 @@
       <c r="C86" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="D86" s="7" t="s">
+      <c r="D86" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E86" s="3" t="s">
@@ -2856,7 +2886,7 @@
       <c r="C87" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="D87" s="7" t="s">
+      <c r="D87" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E87" s="3" t="s">
@@ -2873,7 +2903,7 @@
       <c r="C88" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="D88" s="7" t="s">
+      <c r="D88" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E88" s="3" t="s">
@@ -2890,11 +2920,62 @@
       <c r="C89" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="D89" s="7" t="s">
+      <c r="D89" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>153</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="30">
+      <c r="A91" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes for TestCaseE1 to TestCaseE3
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="294">
   <si>
     <t>TCID</t>
   </si>
@@ -977,6 +977,36 @@
   </si>
   <si>
     <t>TestCase_B88</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>TestCase_B89</t>
+  </si>
+  <si>
+    <t>OPQA-575</t>
+  </si>
+  <si>
+    <t>Verify that DETAILS link is working correctly in record view page of a patent</t>
+  </si>
+  <si>
+    <t>TestCase_B90</t>
+  </si>
+  <si>
+    <t>TestCase_B91</t>
+  </si>
+  <si>
+    <t>Verify that following options get displayed in SORT BY drop down in ARTICLES search results page: a)Relevance b)Times Cited c)Publication Date(Newest) d)Publication Date(Oldest)</t>
+  </si>
+  <si>
+    <t>OPQA-577</t>
+  </si>
+  <si>
+    <t>OPQA-579</t>
+  </si>
+  <si>
+    <t>Verify that search results are sorted by RELEVANCE by default in PATENTS search results page</t>
   </si>
   <si>
     <t>PASS</t>
@@ -1370,10 +1400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E89"/>
+  <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D89"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="D92" sqref="D2:D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1411,7 +1441,7 @@
       <c r="C2" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -1428,7 +1458,7 @@
       <c r="C3" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -1445,7 +1475,7 @@
       <c r="C4" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -1462,7 +1492,7 @@
       <c r="C5" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -1479,7 +1509,7 @@
       <c r="C6" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -1496,7 +1526,7 @@
       <c r="C7" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -1513,7 +1543,7 @@
       <c r="C8" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -1530,7 +1560,7 @@
       <c r="C9" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -1547,7 +1577,7 @@
       <c r="C10" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -1564,7 +1594,7 @@
       <c r="C11" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -1581,7 +1611,7 @@
       <c r="C12" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -1598,7 +1628,7 @@
       <c r="C13" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -1615,7 +1645,7 @@
       <c r="C14" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -1632,7 +1662,7 @@
       <c r="C15" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -1649,7 +1679,7 @@
       <c r="C16" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -1666,7 +1696,7 @@
       <c r="C17" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E17" s="3" t="s">
@@ -1683,7 +1713,7 @@
       <c r="C18" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E18" s="3" t="s">
@@ -1700,7 +1730,7 @@
       <c r="C19" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E19" s="3" t="s">
@@ -1717,7 +1747,7 @@
       <c r="C20" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E20" s="3" t="s">
@@ -1734,11 +1764,11 @@
       <c r="C21" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>283</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1751,7 +1781,7 @@
       <c r="C22" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E22" s="3" t="s">
@@ -1768,7 +1798,7 @@
       <c r="C23" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E23" s="3" t="s">
@@ -1785,7 +1815,7 @@
       <c r="C24" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E24" s="3" t="s">
@@ -1802,7 +1832,7 @@
       <c r="C25" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E25" s="3" t="s">
@@ -1819,7 +1849,7 @@
       <c r="C26" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E26" s="3" t="s">
@@ -1836,7 +1866,7 @@
       <c r="C27" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E27" s="3" t="s">
@@ -1853,7 +1883,7 @@
       <c r="C28" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E28" s="3" t="s">
@@ -1870,7 +1900,7 @@
       <c r="C29" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E29" s="3" t="s">
@@ -1887,7 +1917,7 @@
       <c r="C30" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E30" s="3" t="s">
@@ -1904,7 +1934,7 @@
       <c r="C31" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E31" s="3" t="s">
@@ -1921,7 +1951,7 @@
       <c r="C32" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E32" s="3" t="s">
@@ -1938,7 +1968,7 @@
       <c r="C33" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E33" s="3" t="s">
@@ -1955,7 +1985,7 @@
       <c r="C34" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E34" s="3" t="s">
@@ -1972,7 +2002,7 @@
       <c r="C35" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E35" s="3" t="s">
@@ -1989,7 +2019,7 @@
       <c r="C36" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E36" s="3" t="s">
@@ -2006,7 +2036,7 @@
       <c r="C37" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E37" s="3" t="s">
@@ -2023,7 +2053,7 @@
       <c r="C38" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E38" s="3" t="s">
@@ -2040,7 +2070,7 @@
       <c r="C39" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E39" s="3" t="s">
@@ -2057,7 +2087,7 @@
       <c r="C40" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E40" s="3" t="s">
@@ -2074,7 +2104,7 @@
       <c r="C41" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E41" s="3" t="s">
@@ -2091,7 +2121,7 @@
       <c r="C42" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E42" s="3" t="s">
@@ -2108,7 +2138,7 @@
       <c r="C43" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E43" s="3" t="s">
@@ -2125,7 +2155,7 @@
       <c r="C44" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E44" s="3" t="s">
@@ -2142,7 +2172,7 @@
       <c r="C45" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D45" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E45" s="3" t="s">
@@ -2159,7 +2189,7 @@
       <c r="C46" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="D46" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E46" s="3" t="s">
@@ -2176,7 +2206,7 @@
       <c r="C47" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D47" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E47" s="3" t="s">
@@ -2193,7 +2223,7 @@
       <c r="C48" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E48" s="3" t="s">
@@ -2210,7 +2240,7 @@
       <c r="C49" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E49" s="3" t="s">
@@ -2227,7 +2257,7 @@
       <c r="C50" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D50" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E50" s="3" t="s">
@@ -2244,7 +2274,7 @@
       <c r="C51" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D51" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E51" s="3" t="s">
@@ -2261,7 +2291,7 @@
       <c r="C52" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="D52" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E52" s="3" t="s">
@@ -2278,7 +2308,7 @@
       <c r="C53" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D53" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E53" s="3" t="s">
@@ -2295,7 +2325,7 @@
       <c r="C54" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D54" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E54" s="3" t="s">
@@ -2312,7 +2342,7 @@
       <c r="C55" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="D55" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E55" s="3" t="s">
@@ -2329,7 +2359,7 @@
       <c r="C56" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="D56" s="7" t="s">
+      <c r="D56" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E56" s="3" t="s">
@@ -2346,7 +2376,7 @@
       <c r="C57" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="D57" s="7" t="s">
+      <c r="D57" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E57" s="3" t="s">
@@ -2363,7 +2393,7 @@
       <c r="C58" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="D58" s="7" t="s">
+      <c r="D58" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E58" s="3" t="s">
@@ -2380,7 +2410,7 @@
       <c r="C59" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="D59" s="7" t="s">
+      <c r="D59" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E59" s="3" t="s">
@@ -2397,7 +2427,7 @@
       <c r="C60" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="D60" s="7" t="s">
+      <c r="D60" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E60" s="3" t="s">
@@ -2414,7 +2444,7 @@
       <c r="C61" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="D61" s="7" t="s">
+      <c r="D61" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E61" s="3" t="s">
@@ -2431,7 +2461,7 @@
       <c r="C62" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="D62" s="7" t="s">
+      <c r="D62" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E62" s="3" t="s">
@@ -2448,7 +2478,7 @@
       <c r="C63" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="D63" s="7" t="s">
+      <c r="D63" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E63" s="3" t="s">
@@ -2465,7 +2495,7 @@
       <c r="C64" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D64" s="7" t="s">
+      <c r="D64" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E64" s="3" t="s">
@@ -2482,7 +2512,7 @@
       <c r="C65" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="D65" s="7" t="s">
+      <c r="D65" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E65" s="3" t="s">
@@ -2499,7 +2529,7 @@
       <c r="C66" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="D66" s="7" t="s">
+      <c r="D66" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E66" s="3" t="s">
@@ -2516,7 +2546,7 @@
       <c r="C67" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="D67" s="7" t="s">
+      <c r="D67" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E67" s="3" t="s">
@@ -2533,7 +2563,7 @@
       <c r="C68" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="D68" s="7" t="s">
+      <c r="D68" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E68" s="3" t="s">
@@ -2550,7 +2580,7 @@
       <c r="C69" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="D69" s="7" t="s">
+      <c r="D69" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E69" s="3" t="s">
@@ -2567,7 +2597,7 @@
       <c r="C70" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="D70" s="7" t="s">
+      <c r="D70" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E70" s="3" t="s">
@@ -2584,7 +2614,7 @@
       <c r="C71" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="D71" s="7" t="s">
+      <c r="D71" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E71" s="3" t="s">
@@ -2601,7 +2631,7 @@
       <c r="C72" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="D72" s="7" t="s">
+      <c r="D72" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E72" s="3" t="s">
@@ -2618,7 +2648,7 @@
       <c r="C73" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="D73" s="7" t="s">
+      <c r="D73" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E73" s="3" t="s">
@@ -2635,7 +2665,7 @@
       <c r="C74" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="D74" s="7" t="s">
+      <c r="D74" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E74" s="3" t="s">
@@ -2652,7 +2682,7 @@
       <c r="C75" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="D75" s="7" t="s">
+      <c r="D75" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E75" s="3" t="s">
@@ -2669,7 +2699,7 @@
       <c r="C76" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="D76" s="7" t="s">
+      <c r="D76" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E76" s="3" t="s">
@@ -2686,7 +2716,7 @@
       <c r="C77" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="D77" s="7" t="s">
+      <c r="D77" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E77" s="3" t="s">
@@ -2703,7 +2733,7 @@
       <c r="C78" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="D78" s="7" t="s">
+      <c r="D78" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E78" s="3" t="s">
@@ -2720,7 +2750,7 @@
       <c r="C79" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="D79" s="7" t="s">
+      <c r="D79" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E79" s="3" t="s">
@@ -2737,7 +2767,7 @@
       <c r="C80" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="D80" s="7" t="s">
+      <c r="D80" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E80" s="3" t="s">
@@ -2754,7 +2784,7 @@
       <c r="C81" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="D81" s="7" t="s">
+      <c r="D81" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E81" s="3" t="s">
@@ -2771,7 +2801,7 @@
       <c r="C82" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="D82" s="7" t="s">
+      <c r="D82" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E82" s="3" t="s">
@@ -2788,7 +2818,7 @@
       <c r="C83" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="D83" s="7" t="s">
+      <c r="D83" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E83" s="3" t="s">
@@ -2805,7 +2835,7 @@
       <c r="C84" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="D84" s="7" t="s">
+      <c r="D84" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E84" s="3" t="s">
@@ -2822,7 +2852,7 @@
       <c r="C85" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="D85" s="7" t="s">
+      <c r="D85" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E85" s="3" t="s">
@@ -2839,7 +2869,7 @@
       <c r="C86" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="D86" s="7" t="s">
+      <c r="D86" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E86" s="3" t="s">
@@ -2856,7 +2886,7 @@
       <c r="C87" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="D87" s="7" t="s">
+      <c r="D87" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E87" s="3" t="s">
@@ -2873,7 +2903,7 @@
       <c r="C88" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="D88" s="7" t="s">
+      <c r="D88" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E88" s="3" t="s">
@@ -2890,11 +2920,62 @@
       <c r="C89" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="D89" s="7" t="s">
+      <c r="D89" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>153</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="30">
+      <c r="A91" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding Test case for search module OpQA-1237
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="296">
   <si>
     <t>TCID</t>
   </si>
@@ -979,9 +979,6 @@
     <t>TestCase_B88</t>
   </si>
   <si>
-    <t>FAIL</t>
-  </si>
-  <si>
     <t>TestCase_B89</t>
   </si>
   <si>
@@ -1010,6 +1007,15 @@
   </si>
   <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>Verify that following fields get displayed correctly for a person in ALL search results page: a)Person name b)Person details</t>
+  </si>
+  <si>
+    <t>OPQA-1237</t>
+  </si>
+  <si>
+    <t>TestCase_B92</t>
   </si>
 </sst>
 </file>
@@ -1400,10 +1406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E92"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="D92" sqref="D2:D92"/>
+    <sheetView tabSelected="1" topLeftCell="C85" workbookViewId="0">
+      <selection activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2929,53 +2935,70 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="B90" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="B90" s="6" t="s">
+      <c r="C90" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="C90" s="4" t="s">
-        <v>286</v>
-      </c>
       <c r="D90" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>283</v>
+        <v>153</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="30">
       <c r="A91" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>293</v>
+        <v>153</v>
       </c>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B92" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="C92" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="C92" s="4" t="s">
+      <c r="D92" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E93" s="7" t="s">
         <v>292</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="E92" s="3" t="s">
-        <v>293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding test case for Search Module OPQA-1238
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="299">
   <si>
     <t>TCID</t>
   </si>
@@ -1016,6 +1016,15 @@
   </si>
   <si>
     <t>TestCase_B92</t>
+  </si>
+  <si>
+    <t>TestCase_B93</t>
+  </si>
+  <si>
+    <t>OPQA-1238</t>
+  </si>
+  <si>
+    <t>Verify that profile page of a person gets displayed when clicks on any PEOPLE search result in ALL search results page</t>
   </si>
 </sst>
 </file>
@@ -1406,10 +1415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E93"/>
+  <dimension ref="A1:E94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C85" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView tabSelected="1" topLeftCell="C86" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2998,6 +3007,23 @@
         <v>220</v>
       </c>
       <c r="E93" s="7" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D94" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E94" s="7" t="s">
         <v>292</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding test case to Search Module OPQA-1239
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="303">
   <si>
     <t>TCID</t>
   </si>
@@ -1025,6 +1025,18 @@
   </si>
   <si>
     <t>Verify that profile page of a person gets displayed when clicks on any PEOPLE search result in ALL search results page</t>
+  </si>
+  <si>
+    <t>Verify that record view page of a person gets displayed when user clicks on any PEOPLE in PEOPLE search results page.</t>
+  </si>
+  <si>
+    <t>TestCase_B94</t>
+  </si>
+  <si>
+    <t>OPQA-1239</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -1415,10 +1427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E94"/>
+  <dimension ref="A1:E95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C86" workbookViewId="0">
-      <selection activeCell="D91" sqref="D91"/>
+    <sheetView tabSelected="1" topLeftCell="C78" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3003,7 +3015,7 @@
       <c r="C93" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="D93" s="7" t="s">
+      <c r="D93" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E93" s="7" t="s">
@@ -3020,11 +3032,28 @@
       <c r="C94" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="D94" s="7" t="s">
+      <c r="D94" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E94" s="7" t="s">
         <v>292</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="D95" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E95" s="7" t="s">
+        <v>302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Taking updated code to local
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="315">
   <si>
     <t>TCID</t>
   </si>
@@ -1016,6 +1016,75 @@
   </si>
   <si>
     <t>TestCase_B92</t>
+  </si>
+  <si>
+    <t>TestCase_B93</t>
+  </si>
+  <si>
+    <t>OPQA-1238</t>
+  </si>
+  <si>
+    <t>Verify that profile page of a person gets displayed when clicks on any PEOPLE search result in ALL search results page</t>
+  </si>
+  <si>
+    <t>Verify that record view page of a person gets displayed when user clicks on any PEOPLE in PEOPLE search results page.</t>
+  </si>
+  <si>
+    <t>TestCase_B94</t>
+  </si>
+  <si>
+    <t>OPQA-1239</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>TestCase_B95</t>
+  </si>
+  <si>
+    <t>TestCase_B96</t>
+  </si>
+  <si>
+    <t>OPQA-599</t>
+  </si>
+  <si>
+    <t>OPQA-553</t>
+  </si>
+  <si>
+    <t>Verify that following fields get displayed correctly for a post in ALL search results page: 
+a)Title 
+b)Creation date and time 
+c)Author 
+d)Author details 
+e)Likes count 
+f)Comments count</t>
+  </si>
+  <si>
+    <t>Verify that following fields get displayed correctly for a post in POSTS search results page: 
+a)Title 
+b)Creation date and time 
+c)Author 
+d)Author details 
+e)Likes count 
+f)Comments count</t>
+  </si>
+  <si>
+    <t>TestCase_B97</t>
+  </si>
+  <si>
+    <t>OPQA-565</t>
+  </si>
+  <si>
+    <t>Verify that no filtering options are present in ALL search results page</t>
+  </si>
+  <si>
+    <t>TestCase_B98</t>
+  </si>
+  <si>
+    <t>OPQA-571</t>
+  </si>
+  <si>
+    <t>Verify that search drop down content type is retained when user navigates back to ALL search results page from record view page</t>
   </si>
 </sst>
 </file>
@@ -1406,10 +1475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E93"/>
+  <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C85" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2994,10 +3063,108 @@
       <c r="C93" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="D93" s="7" t="s">
+      <c r="D93" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E93" s="7" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E94" s="7" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="D95" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E95" s="7" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="105">
+      <c r="A96" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="B96" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="D96" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E96" s="3"/>
+    </row>
+    <row r="97" spans="1:5" ht="105">
+      <c r="A97" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="B97" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="D97" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E97" s="3"/>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="D98" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E98" s="7" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="B99" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E99" s="3" t="s">
         <v>292</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding test cases to Search Module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="317">
   <si>
     <t>TCID</t>
   </si>
@@ -1036,9 +1036,6 @@
     <t>OPQA-1239</t>
   </si>
   <si>
-    <t>FAIL</t>
-  </si>
-  <si>
     <t>TestCase_B95</t>
   </si>
   <si>
@@ -1085,6 +1082,16 @@
   </si>
   <si>
     <t>Verify that search drop down content type is retained when user navigates back to ALL search results page from record view page</t>
+  </si>
+  <si>
+    <t>TestCase_B99</t>
+  </si>
+  <si>
+    <t>Verify that following options get displayed in SORT BY drop down in PEOPLE search results page: a)Relevance b)Registration Date and search results are
+sorted by Relevance by default.</t>
+  </si>
+  <si>
+    <t>OPQA-1240 |OPQA-1241</t>
   </si>
 </sst>
 </file>
@@ -1475,10 +1482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E99"/>
+  <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="C96" sqref="C96"/>
+    <sheetView tabSelected="1" topLeftCell="C88" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3067,7 +3074,7 @@
         <v>220</v>
       </c>
       <c r="E93" s="7" t="s">
-        <v>292</v>
+        <v>153</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -3084,7 +3091,7 @@
         <v>220</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>292</v>
+        <v>153</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -3097,74 +3104,95 @@
       <c r="C95" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="D95" s="7" t="s">
+      <c r="D95" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>302</v>
+        <v>153</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="105">
       <c r="A96" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="D96" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="E96" s="3"/>
+        <v>306</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="97" spans="1:5" ht="105">
       <c r="A97" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="D97" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="E97" s="3"/>
+        <v>307</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="B98" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="B98" s="6" t="s">
+      <c r="C98" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="C98" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="D98" s="7" t="s">
+      <c r="D98" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E98" s="7" t="s">
-        <v>292</v>
+        <v>153</v>
       </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="B99" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="B99" s="6" t="s">
+      <c r="C99" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="C99" s="4" t="s">
+      <c r="D99" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="45">
+      <c r="A100" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="D99" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="E99" s="3" t="s">
+      <c r="B100" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="D100" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E100" s="7" t="s">
         <v>292</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added 4 tests to Search suite.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="329">
   <si>
     <t>TCID</t>
   </si>
@@ -1092,6 +1092,42 @@
   </si>
   <si>
     <t>OPQA-1240 |OPQA-1241</t>
+  </si>
+  <si>
+    <t>TestCase_B100</t>
+  </si>
+  <si>
+    <t>OPQA-582</t>
+  </si>
+  <si>
+    <t>Verify that more search results get displayed when user scrolls down in PATENTS search results page</t>
+  </si>
+  <si>
+    <t>TestCase_B101</t>
+  </si>
+  <si>
+    <t>OPQA-584</t>
+  </si>
+  <si>
+    <t>Verify that sorting is retained when user navigates back to PATENTS search results page from record view page</t>
+  </si>
+  <si>
+    <t>TestCase_B102</t>
+  </si>
+  <si>
+    <t>OPQA-586</t>
+  </si>
+  <si>
+    <t>Verify that search drop down content type is retained when user navigates back to PATENTS search results page from record view page</t>
+  </si>
+  <si>
+    <t>TestCase_B103</t>
+  </si>
+  <si>
+    <t>OPQA-591</t>
+  </si>
+  <si>
+    <t>Verify that filtering is retained when user navigates back to PATENTS search results page from record view page</t>
   </si>
 </sst>
 </file>
@@ -1482,10 +1518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E100"/>
+  <dimension ref="A1:E104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C88" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D99"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3195,6 +3231,66 @@
       <c r="E100" s="7" t="s">
         <v>292</v>
       </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E101" s="3"/>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E102" s="3"/>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E103" s="3"/>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E104" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adding new search testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="323">
   <si>
     <t>TCID</t>
   </si>
@@ -1093,12 +1093,30 @@
   <si>
     <t>OPQA-1240 |OPQA-1241</t>
   </si>
+  <si>
+    <t>TestCase_B100</t>
+  </si>
+  <si>
+    <t>TestCase_B101</t>
+  </si>
+  <si>
+    <t>Verify that record view page of a post gets displayed when user clicks on article title in POSTs search results page</t>
+  </si>
+  <si>
+    <t>Verify that record view page of a post gets displayed when user clicks on article title in ALL search results page</t>
+  </si>
+  <si>
+    <t>OPQA-554</t>
+  </si>
+  <si>
+    <t>OPQA-555</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1110,6 +1128,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1162,7 +1187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1183,6 +1208,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1482,10 +1508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E100"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C88" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D99"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3195,6 +3221,36 @@
       <c r="E100" s="7" t="s">
         <v>292</v>
       </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="B101" s="10" t="s">
+        <v>321</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="D101" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E101" s="3"/>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="B102" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="D102" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E102" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adding two search testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="335">
   <si>
     <t>TCID</t>
   </si>
@@ -1128,6 +1128,24 @@
   </si>
   <si>
     <t>Verify that filtering is retained when user navigates back to PATENTS search results page from record view page</t>
+  </si>
+  <si>
+    <t>TestCase_B104</t>
+  </si>
+  <si>
+    <t>TestCase_B105</t>
+  </si>
+  <si>
+    <t>OPQA-554</t>
+  </si>
+  <si>
+    <t>OPQA-555</t>
+  </si>
+  <si>
+    <t>Verify that record view page of a post gets displayed when user clicks on article title in POSTs search results page</t>
+  </si>
+  <si>
+    <t>Verify that record view page of a post gets displayed when user clicks on article title in ALL  search results page</t>
   </si>
 </sst>
 </file>
@@ -1518,10 +1536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E104"/>
+  <dimension ref="A1:E106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="C103" sqref="C103"/>
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3291,6 +3309,36 @@
         <v>220</v>
       </c>
       <c r="E104" s="3"/>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="D105" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E105" s="3"/>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D106" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E106" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixes to reduce wait time for watch list script
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="329">
   <si>
     <t>TCID</t>
   </si>
@@ -1036,9 +1036,6 @@
     <t>OPQA-1239</t>
   </si>
   <si>
-    <t>FAIL</t>
-  </si>
-  <si>
     <t>TestCase_B95</t>
   </si>
   <si>
@@ -1085,6 +1082,52 @@
   </si>
   <si>
     <t>Verify that search drop down content type is retained when user navigates back to ALL search results page from record view page</t>
+  </si>
+  <si>
+    <t>TestCase_B99</t>
+  </si>
+  <si>
+    <t>Verify that following options get displayed in SORT BY drop down in PEOPLE search results page: a)Relevance b)Registration Date and search results are
+sorted by Relevance by default.</t>
+  </si>
+  <si>
+    <t>OPQA-1240 |OPQA-1241</t>
+  </si>
+  <si>
+    <t>TestCase_B100</t>
+  </si>
+  <si>
+    <t>OPQA-582</t>
+  </si>
+  <si>
+    <t>Verify that more search results get displayed when user scrolls down in PATENTS search results page</t>
+  </si>
+  <si>
+    <t>TestCase_B101</t>
+  </si>
+  <si>
+    <t>OPQA-584</t>
+  </si>
+  <si>
+    <t>Verify that sorting is retained when user navigates back to PATENTS search results page from record view page</t>
+  </si>
+  <si>
+    <t>TestCase_B102</t>
+  </si>
+  <si>
+    <t>OPQA-586</t>
+  </si>
+  <si>
+    <t>Verify that search drop down content type is retained when user navigates back to PATENTS search results page from record view page</t>
+  </si>
+  <si>
+    <t>TestCase_B103</t>
+  </si>
+  <si>
+    <t>OPQA-591</t>
+  </si>
+  <si>
+    <t>Verify that filtering is retained when user navigates back to PATENTS search results page from record view page</t>
   </si>
 </sst>
 </file>
@@ -1475,10 +1518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E99"/>
+  <dimension ref="A1:E104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="C96" sqref="C96"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3067,7 +3110,7 @@
         <v>220</v>
       </c>
       <c r="E93" s="7" t="s">
-        <v>292</v>
+        <v>153</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -3084,7 +3127,7 @@
         <v>220</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>292</v>
+        <v>153</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -3097,76 +3140,157 @@
       <c r="C95" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="D95" s="7" t="s">
+      <c r="D95" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>302</v>
+        <v>153</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="105">
       <c r="A96" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="D96" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="E96" s="3"/>
+        <v>306</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="97" spans="1:5" ht="105">
       <c r="A97" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="D97" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="E97" s="3"/>
+        <v>307</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="B98" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="B98" s="6" t="s">
+      <c r="C98" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="C98" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="D98" s="7" t="s">
+      <c r="D98" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E98" s="7" t="s">
-        <v>292</v>
+        <v>153</v>
       </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="B99" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="B99" s="6" t="s">
+      <c r="C99" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="C99" s="4" t="s">
+      <c r="D99" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="45">
+      <c r="A100" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="D99" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="E99" s="3" t="s">
+      <c r="B100" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="D100" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E100" s="7" t="s">
         <v>292</v>
       </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E101" s="3"/>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E102" s="3"/>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E103" s="3"/>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E104" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adding one new search testcase
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="336">
   <si>
     <t>TCID</t>
   </si>
@@ -1139,13 +1139,26 @@
     <t>OPQA-554</t>
   </si>
   <si>
-    <t>OPQA-555</t>
-  </si>
-  <si>
-    <t>Verify that record view page of a post gets displayed when user clicks on article title in POSTs search results page</t>
-  </si>
-  <si>
     <t>Verify that record view page of a post gets displayed when user clicks on article title in ALL  search results page</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Verify that record view page of a post gets displayed when user clicks on article title in POSTs search results page
+Verify that following fields get displayed correctly for a post in record view page:
+a)Title
+ b)Creation date and time 
+c)Last edited date and time 
+d)Author 
+e)Author details 
+f)Post content 
+g)Likes count 
+h)Comments count 
+i)Views count</t>
+  </si>
+  <si>
+    <t>OPQA-555|OPQA-556</t>
   </si>
 </sst>
 </file>
@@ -1538,13 +1551,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="C97" sqref="C97"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="136.7109375" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1578,7 +1592,7 @@
         <v>97</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>153</v>
@@ -1595,7 +1609,7 @@
         <v>77</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>153</v>
@@ -1612,7 +1626,7 @@
         <v>78</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>153</v>
@@ -1629,7 +1643,7 @@
         <v>79</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>153</v>
@@ -1646,7 +1660,7 @@
         <v>80</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>153</v>
@@ -1663,7 +1677,7 @@
         <v>81</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>153</v>
@@ -1680,7 +1694,7 @@
         <v>74</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>153</v>
@@ -1697,7 +1711,7 @@
         <v>82</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>153</v>
@@ -1714,7 +1728,7 @@
         <v>83</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>153</v>
@@ -1731,7 +1745,7 @@
         <v>84</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>153</v>
@@ -1748,7 +1762,7 @@
         <v>85</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>153</v>
@@ -1765,7 +1779,7 @@
         <v>101</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>153</v>
@@ -1782,7 +1796,7 @@
         <v>86</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>153</v>
@@ -1799,7 +1813,7 @@
         <v>87</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>153</v>
@@ -1816,7 +1830,7 @@
         <v>88</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>153</v>
@@ -1833,7 +1847,7 @@
         <v>89</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>153</v>
@@ -1850,7 +1864,7 @@
         <v>140</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>153</v>
@@ -1867,7 +1881,7 @@
         <v>90</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>153</v>
@@ -1884,7 +1898,7 @@
         <v>91</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>153</v>
@@ -1901,7 +1915,7 @@
         <v>92</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>153</v>
@@ -1918,7 +1932,7 @@
         <v>93</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>153</v>
@@ -1935,7 +1949,7 @@
         <v>94</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>153</v>
@@ -1952,7 +1966,7 @@
         <v>95</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>153</v>
@@ -1969,7 +1983,7 @@
         <v>96</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>153</v>
@@ -1986,7 +2000,7 @@
         <v>104</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>153</v>
@@ -2003,7 +2017,7 @@
         <v>107</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>153</v>
@@ -2020,7 +2034,7 @@
         <v>110</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>153</v>
@@ -2037,7 +2051,7 @@
         <v>111</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>153</v>
@@ -2054,7 +2068,7 @@
         <v>116</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>153</v>
@@ -2071,7 +2085,7 @@
         <v>119</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>153</v>
@@ -2088,7 +2102,7 @@
         <v>122</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>153</v>
@@ -2105,7 +2119,7 @@
         <v>124</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>153</v>
@@ -2122,7 +2136,7 @@
         <v>126</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>153</v>
@@ -2139,7 +2153,7 @@
         <v>128</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>153</v>
@@ -2156,7 +2170,7 @@
         <v>134</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>153</v>
@@ -2173,7 +2187,7 @@
         <v>137</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>153</v>
@@ -2190,7 +2204,7 @@
         <v>140</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>153</v>
@@ -2207,7 +2221,7 @@
         <v>143</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>153</v>
@@ -2224,7 +2238,7 @@
         <v>146</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>153</v>
@@ -2241,7 +2255,7 @@
         <v>149</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>153</v>
@@ -2258,7 +2272,7 @@
         <v>152</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>153</v>
@@ -2275,7 +2289,7 @@
         <v>160</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>153</v>
@@ -2292,7 +2306,7 @@
         <v>161</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>153</v>
@@ -2309,7 +2323,7 @@
         <v>162</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>153</v>
@@ -2326,7 +2340,7 @@
         <v>163</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>153</v>
@@ -2343,7 +2357,7 @@
         <v>165</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>153</v>
@@ -2360,7 +2374,7 @@
         <v>167</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>153</v>
@@ -2377,7 +2391,7 @@
         <v>170</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>153</v>
@@ -2394,7 +2408,7 @@
         <v>172</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>153</v>
@@ -2411,7 +2425,7 @@
         <v>176</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>153</v>
@@ -2428,7 +2442,7 @@
         <v>177</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>153</v>
@@ -2445,7 +2459,7 @@
         <v>180</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>153</v>
@@ -2462,7 +2476,7 @@
         <v>182</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>153</v>
@@ -2479,7 +2493,7 @@
         <v>186</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>153</v>
@@ -2496,7 +2510,7 @@
         <v>188</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>153</v>
@@ -2513,7 +2527,7 @@
         <v>190</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>153</v>
@@ -2530,7 +2544,7 @@
         <v>191</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>153</v>
@@ -2547,7 +2561,7 @@
         <v>196</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>153</v>
@@ -2564,7 +2578,7 @@
         <v>198</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>153</v>
@@ -2581,7 +2595,7 @@
         <v>201</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>153</v>
@@ -2598,7 +2612,7 @@
         <v>203</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>153</v>
@@ -2615,7 +2629,7 @@
         <v>205</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>153</v>
@@ -2632,7 +2646,7 @@
         <v>74</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>153</v>
@@ -2649,7 +2663,7 @@
         <v>213</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>153</v>
@@ -2666,7 +2680,7 @@
         <v>211</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>153</v>
@@ -2683,7 +2697,7 @@
         <v>216</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>153</v>
@@ -2700,7 +2714,7 @@
         <v>218</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>153</v>
@@ -2717,7 +2731,7 @@
         <v>222</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>153</v>
@@ -2734,7 +2748,7 @@
         <v>225</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>153</v>
@@ -2751,7 +2765,7 @@
         <v>227</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>153</v>
@@ -2768,7 +2782,7 @@
         <v>231</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>153</v>
@@ -2785,7 +2799,7 @@
         <v>233</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>153</v>
@@ -2802,7 +2816,7 @@
         <v>237</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>153</v>
@@ -2819,7 +2833,7 @@
         <v>240</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>153</v>
@@ -2836,7 +2850,7 @@
         <v>243</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>153</v>
@@ -2853,7 +2867,7 @@
         <v>245</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>153</v>
@@ -2870,7 +2884,7 @@
         <v>248</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>153</v>
@@ -2887,7 +2901,7 @@
         <v>252</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>153</v>
@@ -2904,7 +2918,7 @@
         <v>255</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>153</v>
@@ -2921,7 +2935,7 @@
         <v>257</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>153</v>
@@ -2938,7 +2952,7 @@
         <v>261</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>153</v>
@@ -2955,7 +2969,7 @@
         <v>264</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>153</v>
@@ -2972,7 +2986,7 @@
         <v>265</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>153</v>
@@ -2989,7 +3003,7 @@
         <v>271</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>153</v>
@@ -3006,7 +3020,7 @@
         <v>272</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>153</v>
@@ -3023,7 +3037,7 @@
         <v>275</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>153</v>
@@ -3040,7 +3054,7 @@
         <v>277</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>153</v>
@@ -3057,7 +3071,7 @@
         <v>278</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>153</v>
@@ -3074,7 +3088,7 @@
         <v>285</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>153</v>
@@ -3091,7 +3105,7 @@
         <v>288</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>153</v>
@@ -3108,7 +3122,7 @@
         <v>291</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>153</v>
@@ -3125,7 +3139,7 @@
         <v>293</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E93" s="7" t="s">
         <v>153</v>
@@ -3142,7 +3156,7 @@
         <v>298</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E94" s="7" t="s">
         <v>153</v>
@@ -3159,7 +3173,7 @@
         <v>299</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E95" s="7" t="s">
         <v>153</v>
@@ -3176,7 +3190,7 @@
         <v>306</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>153</v>
@@ -3193,7 +3207,7 @@
         <v>307</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>153</v>
@@ -3210,7 +3224,7 @@
         <v>310</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E98" s="7" t="s">
         <v>153</v>
@@ -3227,7 +3241,7 @@
         <v>313</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>153</v>
@@ -3243,11 +3257,11 @@
       <c r="C100" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="D100" s="7" t="s">
-        <v>220</v>
+      <c r="D100" s="3" t="s">
+        <v>333</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>292</v>
+        <v>153</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -3261,9 +3275,11 @@
         <v>319</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="E101" s="3"/>
+        <v>333</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="3" t="s">
@@ -3276,9 +3292,11 @@
         <v>322</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="E102" s="3"/>
+        <v>333</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="3" t="s">
@@ -3291,9 +3309,11 @@
         <v>325</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="E103" s="3"/>
+        <v>333</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="3" t="s">
@@ -3306,9 +3326,11 @@
         <v>328</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="E104" s="3"/>
+        <v>333</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="3" t="s">
@@ -3318,27 +3340,31 @@
         <v>331</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="D105" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="E105" s="3"/>
-    </row>
-    <row r="106" spans="1:5">
+        <v>332</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="165">
       <c r="A106" s="3" t="s">
         <v>330</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>333</v>
+        <v>335</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>334</v>
       </c>
       <c r="D106" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="E106" s="3"/>
+      <c r="E106" s="3" t="s">
+        <v>292</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Taking Latest to local from Search Module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="344">
   <si>
     <t>TCID</t>
   </si>
@@ -1093,12 +1093,106 @@
   <si>
     <t>OPQA-1240 |OPQA-1241</t>
   </si>
+  <si>
+    <t>TestCase_B100</t>
+  </si>
+  <si>
+    <t>OPQA-582</t>
+  </si>
+  <si>
+    <t>Verify that more search results get displayed when user scrolls down in PATENTS search results page</t>
+  </si>
+  <si>
+    <t>TestCase_B101</t>
+  </si>
+  <si>
+    <t>OPQA-584</t>
+  </si>
+  <si>
+    <t>Verify that sorting is retained when user navigates back to PATENTS search results page from record view page</t>
+  </si>
+  <si>
+    <t>TestCase_B102</t>
+  </si>
+  <si>
+    <t>OPQA-586</t>
+  </si>
+  <si>
+    <t>Verify that search drop down content type is retained when user navigates back to PATENTS search results page from record view page</t>
+  </si>
+  <si>
+    <t>TestCase_B103</t>
+  </si>
+  <si>
+    <t>OPQA-591</t>
+  </si>
+  <si>
+    <t>Verify that filtering is retained when user navigates back to PATENTS search results page from record view page</t>
+  </si>
+  <si>
+    <t>TestCase_B104</t>
+  </si>
+  <si>
+    <t>TestCase_B105</t>
+  </si>
+  <si>
+    <t>OPQA-554</t>
+  </si>
+  <si>
+    <t>Verify that record view page of a post gets displayed when user clicks on article title in ALL  search results page</t>
+  </si>
+  <si>
+    <t>Verify that record view page of a post gets displayed when user clicks on article title in POSTs search results page
+Verify that following fields get displayed correctly for a post in record view page:
+a)Title
+ b)Creation date and time 
+c)Last edited date and time 
+d)Author 
+e)Author details 
+f)Post content 
+g)Likes count 
+h)Comments count 
+i)Views count</t>
+  </si>
+  <si>
+    <t>OPQA-555|OPQA-556</t>
+  </si>
+  <si>
+    <t>TestCase_B106</t>
+  </si>
+  <si>
+    <t>Verify that following options get displayed in SORT BY drop down in POSTS search results page: 
+a)Relevance 
+b)Create Date(Newest) 
+c)Create Date(Oldest)</t>
+  </si>
+  <si>
+    <t>OPQA-1226</t>
+  </si>
+  <si>
+    <t>TestCase_B107</t>
+  </si>
+  <si>
+    <t>OPQA-574</t>
+  </si>
+  <si>
+    <t>Verify that left navigation pane content type is retained when user navigates back to ALL search results page from record view page</t>
+  </si>
+  <si>
+    <t>TestCase_B108</t>
+  </si>
+  <si>
+    <t>OPQA-569</t>
+  </si>
+  <si>
+    <t>Verify that sorting is retained when user navigates back to ALL search results page from record view page</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1110,6 +1204,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1162,7 +1263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1183,6 +1284,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1482,15 +1584,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E100"/>
+  <dimension ref="A1:E109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C88" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D99"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="C122" sqref="C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="136.7109375" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -3189,10 +3292,163 @@
       <c r="C100" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="D100" s="7" t="s">
+      <c r="D100" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E100" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="165">
+      <c r="A106" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="60">
+      <c r="A107" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B107" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="B108" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E108" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="B109" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E109" s="3" t="s">
         <v>292</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding Test Case to search-OPQA-1242
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="353">
   <si>
     <t>TCID</t>
   </si>
@@ -1186,6 +1186,33 @@
   </si>
   <si>
     <t>Verify that sorting is retained when user navigates back to ALL search results page from record view page</t>
+  </si>
+  <si>
+    <t>OPQA-581</t>
+  </si>
+  <si>
+    <t>Verify that search results are sorted correctly by TIMES CITED field in SORT BY drop down in PATENTS search results page</t>
+  </si>
+  <si>
+    <t>OPQA-592</t>
+  </si>
+  <si>
+    <t>Verify that following filters are present in PATENTS search results page: a)Inventor b)IPC Codes c)Assignee</t>
+  </si>
+  <si>
+    <t>TestCase_B109</t>
+  </si>
+  <si>
+    <t>TestCase_B110</t>
+  </si>
+  <si>
+    <t>TestCase_B111</t>
+  </si>
+  <si>
+    <t>OPQA-1242</t>
+  </si>
+  <si>
+    <t>Verify that more search results get displayed when user scrolls down in PEOPLE search results page.</t>
   </si>
 </sst>
 </file>
@@ -1584,10 +1611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E109"/>
+  <dimension ref="A1:E112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="C122" sqref="C122"/>
+    <sheetView tabSelected="1" topLeftCell="C98" workbookViewId="0">
+      <selection activeCell="D107" sqref="D107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3415,7 +3442,7 @@
         <v>220</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>292</v>
+        <v>153</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -3449,6 +3476,57 @@
         <v>220</v>
       </c>
       <c r="E109" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="D112" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E112" s="7" t="s">
         <v>292</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding Test Case to Search Module OPQA-1243
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="356">
   <si>
     <t>TCID</t>
   </si>
@@ -1213,6 +1213,15 @@
   </si>
   <si>
     <t>Verify that more search results get displayed when user scrolls down in PEOPLE search results page.</t>
+  </si>
+  <si>
+    <t>Verify that sorting is retained when user navigates back to PEOPLE search results page from record view page</t>
+  </si>
+  <si>
+    <t>OPQA-1243</t>
+  </si>
+  <si>
+    <t>TestCase_B112</t>
   </si>
 </sst>
 </file>
@@ -1611,10 +1620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E112"/>
+  <dimension ref="A1:E113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C106" workbookViewId="0">
-      <selection activeCell="C111" sqref="C111"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3523,6 +3532,23 @@
         <v>220</v>
       </c>
       <c r="E112" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D113" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E113" s="7" t="s">
         <v>153</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixing automation script for suite E
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="362">
   <si>
     <t>TCID</t>
   </si>
@@ -1139,20 +1139,114 @@
     <t>OPQA-554</t>
   </si>
   <si>
-    <t>OPQA-555</t>
-  </si>
-  <si>
-    <t>Verify that record view page of a post gets displayed when user clicks on article title in POSTs search results page</t>
-  </si>
-  <si>
     <t>Verify that record view page of a post gets displayed when user clicks on article title in ALL  search results page</t>
+  </si>
+  <si>
+    <t>Verify that record view page of a post gets displayed when user clicks on article title in POSTs search results page
+Verify that following fields get displayed correctly for a post in record view page:
+a)Title
+ b)Creation date and time 
+c)Last edited date and time 
+d)Author 
+e)Author details 
+f)Post content 
+g)Likes count 
+h)Comments count 
+i)Views count</t>
+  </si>
+  <si>
+    <t>OPQA-555|OPQA-556</t>
+  </si>
+  <si>
+    <t>TestCase_B106</t>
+  </si>
+  <si>
+    <t>Verify that following options get displayed in SORT BY drop down in POSTS search results page: 
+a)Relevance 
+b)Create Date(Newest) 
+c)Create Date(Oldest)</t>
+  </si>
+  <si>
+    <t>OPQA-1226</t>
+  </si>
+  <si>
+    <t>TestCase_B107</t>
+  </si>
+  <si>
+    <t>OPQA-574</t>
+  </si>
+  <si>
+    <t>Verify that left navigation pane content type is retained when user navigates back to ALL search results page from record view page</t>
+  </si>
+  <si>
+    <t>TestCase_B108</t>
+  </si>
+  <si>
+    <t>OPQA-569</t>
+  </si>
+  <si>
+    <t>Verify that sorting is retained when user navigates back to ALL search results page from record view page</t>
+  </si>
+  <si>
+    <t>OPQA-581</t>
+  </si>
+  <si>
+    <t>Verify that search results are sorted correctly by TIMES CITED field in SORT BY drop down in PATENTS search results page</t>
+  </si>
+  <si>
+    <t>OPQA-592</t>
+  </si>
+  <si>
+    <t>Verify that following filters are present in PATENTS search results page: a)Inventor b)IPC Codes c)Assignee</t>
+  </si>
+  <si>
+    <t>TestCase_B109</t>
+  </si>
+  <si>
+    <t>TestCase_B110</t>
+  </si>
+  <si>
+    <t>TestCase_B111</t>
+  </si>
+  <si>
+    <t>OPQA-1242</t>
+  </si>
+  <si>
+    <t>Verify that more search results get displayed when user scrolls down in PEOPLE search results page.</t>
+  </si>
+  <si>
+    <t>Verify that sorting is retained when user navigates back to PEOPLE search results page from record view page</t>
+  </si>
+  <si>
+    <t>OPQA-1243</t>
+  </si>
+  <si>
+    <t>TestCase_B112</t>
+  </si>
+  <si>
+    <t>OPQA-593</t>
+  </si>
+  <si>
+    <t>Verify that MORE and LESS links are working correctly in INVENTOR filter in PATENTS search results page</t>
+  </si>
+  <si>
+    <t>OPQA-588</t>
+  </si>
+  <si>
+    <t>Verify that left navigation pane content type is retained when user navigates back to PATENTS search results page from record view page</t>
+  </si>
+  <si>
+    <t>TestCase_B113</t>
+  </si>
+  <si>
+    <t>TestCase_B114</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1164,6 +1258,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1216,7 +1317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1237,6 +1338,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1536,15 +1638,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E106"/>
+  <dimension ref="A1:E115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="C97" sqref="C97"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="A115" sqref="A115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="136.7109375" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -3243,11 +3346,11 @@
       <c r="C100" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="D100" s="7" t="s">
+      <c r="D100" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>292</v>
+        <v>153</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -3263,7 +3366,9 @@
       <c r="D101" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="E101" s="3"/>
+      <c r="E101" s="3" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="3" t="s">
@@ -3278,7 +3383,9 @@
       <c r="D102" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="E102" s="3"/>
+      <c r="E102" s="3" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="3" t="s">
@@ -3293,7 +3400,9 @@
       <c r="D103" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="E103" s="3"/>
+      <c r="E103" s="3" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="3" t="s">
@@ -3308,7 +3417,9 @@
       <c r="D104" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="E104" s="3"/>
+      <c r="E104" s="3" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="3" t="s">
@@ -3318,27 +3429,180 @@
         <v>331</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="D105" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="E105" s="3"/>
-    </row>
-    <row r="106" spans="1:5">
+        <v>332</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="165">
       <c r="A106" s="3" t="s">
         <v>330</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="C106" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="C106" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="D106" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="E106" s="3"/>
+      <c r="D106" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="60">
+      <c r="A107" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B107" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="B108" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E108" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="B109" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E110" s="3"/>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E111" s="3"/>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="D112" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E112" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D113" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E113" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="A114" t="s">
+        <v>360</v>
+      </c>
+      <c r="B114" t="s">
+        <v>356</v>
+      </c>
+      <c r="C114" t="s">
+        <v>357</v>
+      </c>
+      <c r="D114" t="s">
+        <v>220</v>
+      </c>
+      <c r="E114" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" t="s">
+        <v>361</v>
+      </c>
+      <c r="B115" t="s">
+        <v>358</v>
+      </c>
+      <c r="C115" t="s">
+        <v>359</v>
+      </c>
+      <c r="D115" t="s">
+        <v>220</v>
+      </c>
+      <c r="E115" t="s">
+        <v>292</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding test Case to Search Module OPQA_1243
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="362">
   <si>
     <t>TCID</t>
   </si>
@@ -1222,6 +1222,24 @@
   </si>
   <si>
     <t>TestCase_B112</t>
+  </si>
+  <si>
+    <t>OPQA-593</t>
+  </si>
+  <si>
+    <t>Verify that MORE and LESS links are working correctly in INVENTOR filter in PATENTS search results page</t>
+  </si>
+  <si>
+    <t>OPQA-588</t>
+  </si>
+  <si>
+    <t>Verify that left navigation pane content type is retained when user navigates back to PATENTS search results page from record view page</t>
+  </si>
+  <si>
+    <t>TestCase_B113</t>
+  </si>
+  <si>
+    <t>TestCase_B114</t>
   </si>
 </sst>
 </file>
@@ -1620,10 +1638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E113"/>
+  <dimension ref="A1:E115"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="B113" sqref="B113"/>
+      <selection activeCell="A115" sqref="A1:E115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3550,6 +3568,40 @@
       </c>
       <c r="E113" s="7" t="s">
         <v>153</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="A114" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E114" s="3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E115" s="3" t="s">
+        <v>292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding test case to search OPQA-1244
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="365">
   <si>
     <t>TCID</t>
   </si>
@@ -1240,6 +1240,15 @@
   </si>
   <si>
     <t>TestCase_B114</t>
+  </si>
+  <si>
+    <t>Verify that search drop down content type is retained when user navigates back to PEOPLE search results page from profile page</t>
+  </si>
+  <si>
+    <t>OPQA-1244</t>
+  </si>
+  <si>
+    <t>TestCase_B115</t>
   </si>
 </sst>
 </file>
@@ -1638,10 +1647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E115"/>
+  <dimension ref="A1:E116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="A115" sqref="A115"/>
+    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="A116" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3469,7 +3478,7 @@
         <v>220</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>292</v>
+        <v>153</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -3503,7 +3512,7 @@
         <v>220</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>292</v>
+        <v>153</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -3519,7 +3528,9 @@
       <c r="D110" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="E110" s="3"/>
+      <c r="E110" s="3" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="3" t="s">
@@ -3534,7 +3545,9 @@
       <c r="D111" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="E111" s="3"/>
+      <c r="E111" s="3" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="7" t="s">
@@ -3546,7 +3559,7 @@
       <c r="C112" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="D112" s="7" t="s">
+      <c r="D112" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E112" s="7" t="s">
@@ -3563,45 +3576,62 @@
       <c r="C113" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="D113" s="7" t="s">
+      <c r="D113" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E113" s="7" t="s">
-        <v>153</v>
+        <v>292</v>
       </c>
     </row>
     <row r="114" spans="1:5">
-      <c r="A114" t="s">
+      <c r="A114" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B114" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C114" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="D114" t="s">
-        <v>220</v>
-      </c>
-      <c r="E114" t="s">
-        <v>292</v>
+      <c r="D114" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E114" s="3" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="115" spans="1:5">
-      <c r="A115" t="s">
+      <c r="A115" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B115" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C115" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="D115" t="s">
-        <v>220</v>
-      </c>
-      <c r="E115" t="s">
-        <v>292</v>
+      <c r="D115" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E115" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="A116" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="B116" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="D116" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E116" s="7" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new search testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="371">
   <si>
     <t>TCID</t>
   </si>
@@ -1161,94 +1161,114 @@
     <t>TestCase_B106</t>
   </si>
   <si>
+    <t>TestCase_B107</t>
+  </si>
+  <si>
+    <t>OPQA-574</t>
+  </si>
+  <si>
+    <t>Verify that left navigation pane content type is retained when user navigates back to ALL search results page from record view page</t>
+  </si>
+  <si>
+    <t>TestCase_B108</t>
+  </si>
+  <si>
+    <t>OPQA-569</t>
+  </si>
+  <si>
+    <t>Verify that sorting is retained when user navigates back to ALL search results page from record view page</t>
+  </si>
+  <si>
+    <t>OPQA-581</t>
+  </si>
+  <si>
+    <t>Verify that search results are sorted correctly by TIMES CITED field in SORT BY drop down in PATENTS search results page</t>
+  </si>
+  <si>
+    <t>OPQA-592</t>
+  </si>
+  <si>
+    <t>Verify that following filters are present in PATENTS search results page: a)Inventor b)IPC Codes c)Assignee</t>
+  </si>
+  <si>
+    <t>TestCase_B109</t>
+  </si>
+  <si>
+    <t>TestCase_B110</t>
+  </si>
+  <si>
+    <t>TestCase_B111</t>
+  </si>
+  <si>
+    <t>OPQA-1242</t>
+  </si>
+  <si>
+    <t>Verify that more search results get displayed when user scrolls down in PEOPLE search results page.</t>
+  </si>
+  <si>
+    <t>Verify that sorting is retained when user navigates back to PEOPLE search results page from record view page</t>
+  </si>
+  <si>
+    <t>OPQA-1243</t>
+  </si>
+  <si>
+    <t>TestCase_B112</t>
+  </si>
+  <si>
+    <t>OPQA-593</t>
+  </si>
+  <si>
+    <t>Verify that MORE and LESS links are working correctly in INVENTOR filter in PATENTS search results page</t>
+  </si>
+  <si>
+    <t>OPQA-588</t>
+  </si>
+  <si>
+    <t>Verify that left navigation pane content type is retained when user navigates back to PATENTS search results page from record view page</t>
+  </si>
+  <si>
+    <t>TestCase_B113</t>
+  </si>
+  <si>
+    <t>TestCase_B114</t>
+  </si>
+  <si>
+    <t>Verify that search drop down content type is retained when user navigates back to PEOPLE search results page from profile page</t>
+  </si>
+  <si>
+    <t>OPQA-1244</t>
+  </si>
+  <si>
+    <t>TestCase_B115</t>
+  </si>
+  <si>
     <t>Verify that following options get displayed in SORT BY drop down in POSTS search results page: 
 a)Relevance 
 b)Create Date(Newest) 
-c)Create Date(Oldest)</t>
-  </si>
-  <si>
-    <t>OPQA-1226</t>
-  </si>
-  <si>
-    <t>TestCase_B107</t>
-  </si>
-  <si>
-    <t>OPQA-574</t>
-  </si>
-  <si>
-    <t>Verify that left navigation pane content type is retained when user navigates back to ALL search results page from record view page</t>
-  </si>
-  <si>
-    <t>TestCase_B108</t>
-  </si>
-  <si>
-    <t>OPQA-569</t>
-  </si>
-  <si>
-    <t>Verify that sorting is retained when user navigates back to ALL search results page from record view page</t>
-  </si>
-  <si>
-    <t>OPQA-581</t>
-  </si>
-  <si>
-    <t>Verify that search results are sorted correctly by TIMES CITED field in SORT BY drop down in PATENTS search results page</t>
-  </si>
-  <si>
-    <t>OPQA-592</t>
-  </si>
-  <si>
-    <t>Verify that following filters are present in PATENTS search results page: a)Inventor b)IPC Codes c)Assignee</t>
-  </si>
-  <si>
-    <t>TestCase_B109</t>
-  </si>
-  <si>
-    <t>TestCase_B110</t>
-  </si>
-  <si>
-    <t>TestCase_B111</t>
-  </si>
-  <si>
-    <t>OPQA-1242</t>
-  </si>
-  <si>
-    <t>Verify that more search results get displayed when user scrolls down in PEOPLE search results page.</t>
-  </si>
-  <si>
-    <t>Verify that sorting is retained when user navigates back to PEOPLE search results page from record view page</t>
-  </si>
-  <si>
-    <t>OPQA-1243</t>
-  </si>
-  <si>
-    <t>TestCase_B112</t>
-  </si>
-  <si>
-    <t>OPQA-593</t>
-  </si>
-  <si>
-    <t>Verify that MORE and LESS links are working correctly in INVENTOR filter in PATENTS search results page</t>
-  </si>
-  <si>
-    <t>OPQA-588</t>
-  </si>
-  <si>
-    <t>Verify that left navigation pane content type is retained when user navigates back to PATENTS search results page from record view page</t>
-  </si>
-  <si>
-    <t>TestCase_B113</t>
-  </si>
-  <si>
-    <t>TestCase_B114</t>
-  </si>
-  <si>
-    <t>Verify that search drop down content type is retained when user navigates back to PEOPLE search results page from profile page</t>
-  </si>
-  <si>
-    <t>OPQA-1244</t>
-  </si>
-  <si>
-    <t>TestCase_B115</t>
+c)Create Date(Oldest)
+Verify that search results are sorted by CREATE DATE(NEWEST) by default in POSTS search results page</t>
+  </si>
+  <si>
+    <t>OOPQA-1226|PQA-1227</t>
+  </si>
+  <si>
+    <t>TestCase_B116</t>
+  </si>
+  <si>
+    <t>TestCase_B117</t>
+  </si>
+  <si>
+    <t>Verify that more search results get displayed when user scrolls down in POSTS search results page</t>
+  </si>
+  <si>
+    <t>OPQA-1228</t>
+  </si>
+  <si>
+    <t>Verify that sorting is retained when user navigates back to POSTS search results page from record view page
+Verify that search drop down content type is retained when user navigates back to POSTS search results page from record view page</t>
+  </si>
+  <si>
+    <t>OPQA-1229|OPQA-1230</t>
   </si>
 </sst>
 </file>
@@ -1326,7 +1346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1348,6 +1368,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1647,16 +1670,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E116"/>
+  <dimension ref="A1:E118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="A116" sqref="A116"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="D125" sqref="D125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="136.7109375" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -3464,15 +3487,15 @@
         <v>153</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="60">
+    <row r="107" spans="1:5" ht="75">
       <c r="A107" s="3" t="s">
         <v>335</v>
       </c>
       <c r="B107" s="10" t="s">
-        <v>337</v>
+        <v>364</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>336</v>
+        <v>363</v>
       </c>
       <c r="D107" s="3" t="s">
         <v>220</v>
@@ -3483,13 +3506,13 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="B108" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="C108" s="4" t="s">
         <v>338</v>
-      </c>
-      <c r="B108" s="6" t="s">
-        <v>339</v>
-      </c>
-      <c r="C108" s="4" t="s">
-        <v>340</v>
       </c>
       <c r="D108" s="3" t="s">
         <v>220</v>
@@ -3500,13 +3523,13 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="B109" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="C109" s="4" t="s">
         <v>341</v>
-      </c>
-      <c r="B109" s="6" t="s">
-        <v>342</v>
-      </c>
-      <c r="C109" s="4" t="s">
-        <v>343</v>
       </c>
       <c r="D109" s="3" t="s">
         <v>220</v>
@@ -3517,13 +3540,13 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="3" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D110" s="3" t="s">
         <v>220</v>
@@ -3534,13 +3557,13 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D111" s="3" t="s">
         <v>220</v>
@@ -3551,13 +3574,13 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="C112" s="3" t="s">
         <v>350</v>
-      </c>
-      <c r="B112" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="C112" s="3" t="s">
-        <v>352</v>
       </c>
       <c r="D112" s="3" t="s">
         <v>220</v>
@@ -3568,13 +3591,13 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>220</v>
@@ -3585,13 +3608,13 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D114" s="3" t="s">
         <v>220</v>
@@ -3602,13 +3625,13 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="3" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D115" s="3" t="s">
         <v>220</v>
@@ -3619,13 +3642,13 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="7" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D116" s="7" t="s">
         <v>220</v>
@@ -3633,6 +3656,36 @@
       <c r="E116" s="7" t="s">
         <v>153</v>
       </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="B117" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="C117" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="D117" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E117" s="3"/>
+    </row>
+    <row r="118" spans="1:5" ht="30">
+      <c r="A118" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="B118" s="10" t="s">
+        <v>370</v>
+      </c>
+      <c r="C118" s="11" t="s">
+        <v>369</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E118" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added new tests to Search module.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="374">
   <si>
     <t>TCID</t>
   </si>
@@ -1269,6 +1269,19 @@
   </si>
   <si>
     <t>OPQA-1229|OPQA-1230</t>
+  </si>
+  <si>
+    <t>OPQA-590</t>
+  </si>
+  <si>
+    <t>Verify that following things are retained when user navigates back to PATENTS search results page from record view page:
+a)Sorting
+b)Left navigation pane content type
+c)Search drop down content type
+d)Filtering</t>
+  </si>
+  <si>
+    <t>TestCase_B118</t>
   </si>
 </sst>
 </file>
@@ -1670,10 +1683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E118"/>
+  <dimension ref="A1:E119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="D125" sqref="D125"/>
+      <selection activeCell="A119" sqref="A119:E119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3686,6 +3699,23 @@
         <v>220</v>
       </c>
       <c r="E118" s="3"/>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="C119" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E119" s="3" t="s">
+        <v>292</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Committing new excel files as the previous ones got corrupted
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="398">
   <si>
     <t>TCID</t>
   </si>
@@ -1004,6 +1004,9 @@
   </si>
   <si>
     <t>Verify that search results are sorted by RELEVANCE by default in PATENTS search results page</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
   <si>
     <t>Verify that following fields get displayed correctly for a person in ALL search results page: a)Person name b)Person details</t>
@@ -1777,8 +1780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="C127" sqref="C127"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="C126" sqref="C126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3356,13 +3359,13 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="B93" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="B93" s="7" t="s">
+      <c r="C93" s="8" t="s">
         <v>293</v>
-      </c>
-      <c r="C93" s="8" t="s">
-        <v>292</v>
       </c>
       <c r="D93" s="8" t="s">
         <v>220</v>
@@ -3373,13 +3376,13 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="8" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D94" s="8" t="s">
         <v>220</v>
@@ -3390,13 +3393,13 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="C95" s="8" t="s">
         <v>299</v>
-      </c>
-      <c r="B95" s="7" t="s">
-        <v>300</v>
-      </c>
-      <c r="C95" s="8" t="s">
-        <v>298</v>
       </c>
       <c r="D95" s="8" t="s">
         <v>220</v>
@@ -3407,13 +3410,13 @@
     </row>
     <row r="96" spans="1:5" ht="105">
       <c r="A96" s="8" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D96" s="8" t="s">
         <v>220</v>
@@ -3424,13 +3427,13 @@
     </row>
     <row r="97" spans="1:5" ht="105">
       <c r="A97" s="8" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D97" s="8" t="s">
         <v>220</v>
@@ -3441,13 +3444,13 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="8" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D98" s="8" t="s">
         <v>220</v>
@@ -3458,13 +3461,13 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="8" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D99" s="8" t="s">
         <v>220</v>
@@ -3475,13 +3478,13 @@
     </row>
     <row r="100" spans="1:5" ht="45">
       <c r="A100" s="8" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B100" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="C100" s="7" t="s">
         <v>315</v>
-      </c>
-      <c r="C100" s="7" t="s">
-        <v>314</v>
       </c>
       <c r="D100" s="8" t="s">
         <v>220</v>
@@ -3492,13 +3495,13 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="8" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D101" s="8" t="s">
         <v>220</v>
@@ -3509,13 +3512,13 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="8" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D102" s="8" t="s">
         <v>220</v>
@@ -3526,13 +3529,13 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="8" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D103" s="8" t="s">
         <v>220</v>
@@ -3543,13 +3546,13 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="8" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D104" s="8" t="s">
         <v>220</v>
@@ -3560,13 +3563,13 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="8" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D105" s="8" t="s">
         <v>220</v>
@@ -3577,13 +3580,13 @@
     </row>
     <row r="106" spans="1:5" ht="165">
       <c r="A106" s="8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B106" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="C106" s="7" t="s">
         <v>333</v>
-      </c>
-      <c r="C106" s="7" t="s">
-        <v>332</v>
       </c>
       <c r="D106" s="8" t="s">
         <v>220</v>
@@ -3594,13 +3597,13 @@
     </row>
     <row r="107" spans="1:5" ht="75">
       <c r="A107" s="8" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B107" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="C107" s="7" t="s">
         <v>363</v>
-      </c>
-      <c r="C107" s="7" t="s">
-        <v>362</v>
       </c>
       <c r="D107" s="8" t="s">
         <v>220</v>
@@ -3611,13 +3614,13 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="8" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D108" s="8" t="s">
         <v>220</v>
@@ -3628,13 +3631,13 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="8" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D109" s="8" t="s">
         <v>220</v>
@@ -3645,13 +3648,13 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="B110" s="8" t="s">
+        <v>344</v>
+      </c>
+      <c r="C110" s="8" t="s">
         <v>345</v>
-      </c>
-      <c r="B110" s="8" t="s">
-        <v>343</v>
-      </c>
-      <c r="C110" s="8" t="s">
-        <v>344</v>
       </c>
       <c r="D110" s="8" t="s">
         <v>220</v>
@@ -3662,13 +3665,13 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="8" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D111" s="8" t="s">
         <v>220</v>
@@ -3679,13 +3682,13 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="8" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D112" s="8" t="s">
         <v>220</v>
@@ -3696,13 +3699,13 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="B113" s="8" t="s">
         <v>352</v>
       </c>
-      <c r="B113" s="8" t="s">
+      <c r="C113" s="8" t="s">
         <v>351</v>
-      </c>
-      <c r="C113" s="8" t="s">
-        <v>350</v>
       </c>
       <c r="D113" s="8" t="s">
         <v>220</v>
@@ -3713,13 +3716,13 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="8" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D114" s="8" t="s">
         <v>220</v>
@@ -3730,13 +3733,13 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="8" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D115" s="8" t="s">
         <v>220</v>
@@ -3747,13 +3750,13 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="B116" s="8" t="s">
         <v>361</v>
       </c>
-      <c r="B116" s="8" t="s">
+      <c r="C116" s="8" t="s">
         <v>360</v>
-      </c>
-      <c r="C116" s="8" t="s">
-        <v>359</v>
       </c>
       <c r="D116" s="8" t="s">
         <v>220</v>
@@ -3764,13 +3767,13 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="8" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B117" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="C117" s="9" t="s">
         <v>367</v>
-      </c>
-      <c r="C117" s="9" t="s">
-        <v>366</v>
       </c>
       <c r="D117" s="8" t="s">
         <v>220</v>
@@ -3781,13 +3784,13 @@
     </row>
     <row r="118" spans="1:5" ht="30">
       <c r="A118" s="8" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B118" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="C118" s="10" t="s">
         <v>369</v>
-      </c>
-      <c r="C118" s="10" t="s">
-        <v>368</v>
       </c>
       <c r="D118" s="8" t="s">
         <v>220</v>
@@ -3798,13 +3801,13 @@
     </row>
     <row r="119" spans="1:5" ht="75">
       <c r="A119" s="8" t="s">
+        <v>373</v>
+      </c>
+      <c r="B119" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="C119" s="7" t="s">
         <v>372</v>
-      </c>
-      <c r="B119" s="8" t="s">
-        <v>370</v>
-      </c>
-      <c r="C119" s="7" t="s">
-        <v>371</v>
       </c>
       <c r="D119" s="8" t="s">
         <v>220</v>
@@ -3815,13 +3818,13 @@
     </row>
     <row r="120" spans="1:5" ht="60">
       <c r="A120" s="8" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D120" s="8" t="s">
         <v>220</v>
@@ -3832,13 +3835,13 @@
     </row>
     <row r="121" spans="1:5" ht="105">
       <c r="A121" s="8" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C121" s="7" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D121" s="8" t="s">
         <v>220</v>
@@ -3849,13 +3852,13 @@
     </row>
     <row r="122" spans="1:5" ht="105">
       <c r="A122" s="8" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D122" s="8" t="s">
         <v>220</v>
@@ -3866,13 +3869,13 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="8" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D123" s="8" t="s">
         <v>220</v>
@@ -3883,71 +3886,65 @@
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="8" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D124" s="8" t="s">
         <v>220</v>
       </c>
       <c r="E124" s="8" t="s">
-        <v>153</v>
+        <v>292</v>
       </c>
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="D125" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="E125" s="3" t="s">
-        <v>153</v>
-      </c>
+        <v>390</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E125" s="3"/>
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="3" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="D126" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="E126" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" ht="150">
+        <v>392</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E126" s="3"/>
+    </row>
+    <row r="127" spans="1:5">
       <c r="A127" s="3" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>393</v>
-      </c>
-      <c r="D127" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="E127" s="3" t="s">
-        <v>153</v>
-      </c>
+        <v>394</v>
+      </c>
+      <c r="D127" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E127" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Running only search suite
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -755,9 +755,6 @@
     <t>OPQA-263</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>TestCase_B68</t>
   </si>
   <si>
@@ -1378,6 +1375,9 @@
   </si>
   <si>
     <t>TestCase_B126</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -1780,8 +1780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="C126" sqref="C126"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1821,7 +1821,7 @@
         <v>97</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>153</v>
@@ -1838,7 +1838,7 @@
         <v>77</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>153</v>
@@ -1855,7 +1855,7 @@
         <v>78</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>153</v>
@@ -1872,7 +1872,7 @@
         <v>79</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>153</v>
@@ -1889,7 +1889,7 @@
         <v>80</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>153</v>
@@ -1906,7 +1906,7 @@
         <v>81</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>153</v>
@@ -1923,7 +1923,7 @@
         <v>74</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>153</v>
@@ -1940,7 +1940,7 @@
         <v>82</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>153</v>
@@ -1957,7 +1957,7 @@
         <v>83</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>153</v>
@@ -1974,7 +1974,7 @@
         <v>84</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>153</v>
@@ -1991,7 +1991,7 @@
         <v>85</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>153</v>
@@ -2008,7 +2008,7 @@
         <v>101</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>153</v>
@@ -2025,7 +2025,7 @@
         <v>86</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>153</v>
@@ -2042,7 +2042,7 @@
         <v>87</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>153</v>
@@ -2059,7 +2059,7 @@
         <v>88</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>153</v>
@@ -2076,7 +2076,7 @@
         <v>89</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>153</v>
@@ -2093,7 +2093,7 @@
         <v>140</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>153</v>
@@ -2110,7 +2110,7 @@
         <v>90</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>153</v>
@@ -2127,7 +2127,7 @@
         <v>91</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>153</v>
@@ -2144,7 +2144,7 @@
         <v>92</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>153</v>
@@ -2161,7 +2161,7 @@
         <v>93</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>153</v>
@@ -2178,7 +2178,7 @@
         <v>94</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>153</v>
@@ -2195,7 +2195,7 @@
         <v>95</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>153</v>
@@ -2212,7 +2212,7 @@
         <v>96</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>153</v>
@@ -2229,7 +2229,7 @@
         <v>104</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>153</v>
@@ -2246,7 +2246,7 @@
         <v>107</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>153</v>
@@ -2263,7 +2263,7 @@
         <v>110</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>153</v>
@@ -2280,7 +2280,7 @@
         <v>111</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>153</v>
@@ -2297,7 +2297,7 @@
         <v>116</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>153</v>
@@ -2314,7 +2314,7 @@
         <v>119</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>153</v>
@@ -2331,7 +2331,7 @@
         <v>122</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>153</v>
@@ -2348,7 +2348,7 @@
         <v>124</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>153</v>
@@ -2365,7 +2365,7 @@
         <v>126</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>153</v>
@@ -2382,7 +2382,7 @@
         <v>128</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>153</v>
@@ -2399,7 +2399,7 @@
         <v>134</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>153</v>
@@ -2416,7 +2416,7 @@
         <v>137</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E37" s="8" t="s">
         <v>153</v>
@@ -2433,7 +2433,7 @@
         <v>140</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>153</v>
@@ -2450,7 +2450,7 @@
         <v>143</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>153</v>
@@ -2467,7 +2467,7 @@
         <v>146</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>153</v>
@@ -2484,7 +2484,7 @@
         <v>149</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E41" s="8" t="s">
         <v>153</v>
@@ -2501,7 +2501,7 @@
         <v>152</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E42" s="8" t="s">
         <v>153</v>
@@ -2518,7 +2518,7 @@
         <v>160</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E43" s="8" t="s">
         <v>153</v>
@@ -2535,7 +2535,7 @@
         <v>161</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>153</v>
@@ -2552,7 +2552,7 @@
         <v>162</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E45" s="8" t="s">
         <v>153</v>
@@ -2569,7 +2569,7 @@
         <v>163</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>153</v>
@@ -2586,7 +2586,7 @@
         <v>165</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E47" s="8" t="s">
         <v>153</v>
@@ -2603,7 +2603,7 @@
         <v>167</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E48" s="8" t="s">
         <v>153</v>
@@ -2620,7 +2620,7 @@
         <v>170</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E49" s="8" t="s">
         <v>153</v>
@@ -2637,7 +2637,7 @@
         <v>172</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>153</v>
@@ -2654,7 +2654,7 @@
         <v>176</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E51" s="8" t="s">
         <v>153</v>
@@ -2671,7 +2671,7 @@
         <v>177</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E52" s="8" t="s">
         <v>153</v>
@@ -2688,7 +2688,7 @@
         <v>180</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E53" s="8" t="s">
         <v>153</v>
@@ -2705,7 +2705,7 @@
         <v>182</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E54" s="8" t="s">
         <v>153</v>
@@ -2722,7 +2722,7 @@
         <v>186</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E55" s="8" t="s">
         <v>153</v>
@@ -2739,7 +2739,7 @@
         <v>188</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E56" s="8" t="s">
         <v>153</v>
@@ -2756,7 +2756,7 @@
         <v>190</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E57" s="8" t="s">
         <v>153</v>
@@ -2773,7 +2773,7 @@
         <v>191</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E58" s="8" t="s">
         <v>153</v>
@@ -2790,7 +2790,7 @@
         <v>196</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E59" s="8" t="s">
         <v>153</v>
@@ -2807,7 +2807,7 @@
         <v>198</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E60" s="8" t="s">
         <v>153</v>
@@ -2824,7 +2824,7 @@
         <v>201</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E61" s="8" t="s">
         <v>153</v>
@@ -2841,7 +2841,7 @@
         <v>203</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E62" s="8" t="s">
         <v>153</v>
@@ -2858,7 +2858,7 @@
         <v>205</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E63" s="8" t="s">
         <v>153</v>
@@ -2875,7 +2875,7 @@
         <v>74</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>153</v>
@@ -2892,7 +2892,7 @@
         <v>213</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E65" s="8" t="s">
         <v>153</v>
@@ -2909,7 +2909,7 @@
         <v>211</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E66" s="8" t="s">
         <v>153</v>
@@ -2926,7 +2926,7 @@
         <v>216</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E67" s="8" t="s">
         <v>153</v>
@@ -2943,7 +2943,7 @@
         <v>218</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E68" s="8" t="s">
         <v>153</v>
@@ -2951,16 +2951,16 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B69" s="7" t="s">
         <v>64</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E69" s="8" t="s">
         <v>153</v>
@@ -2968,16 +2968,16 @@
     </row>
     <row r="70" spans="1:5" ht="45">
       <c r="A70" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="B70" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="B70" s="7" t="s">
+      <c r="C70" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="C70" s="7" t="s">
-        <v>225</v>
-      </c>
       <c r="D70" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E70" s="8" t="s">
         <v>153</v>
@@ -2985,16 +2985,16 @@
     </row>
     <row r="71" spans="1:5" ht="30">
       <c r="A71" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C71" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="B71" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>227</v>
-      </c>
       <c r="D71" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E71" s="8" t="s">
         <v>153</v>
@@ -3002,16 +3002,16 @@
     </row>
     <row r="72" spans="1:5" ht="30">
       <c r="A72" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B72" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="B72" s="7" t="s">
+      <c r="C72" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="C72" s="7" t="s">
-        <v>231</v>
-      </c>
       <c r="D72" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E72" s="8" t="s">
         <v>153</v>
@@ -3019,16 +3019,16 @@
     </row>
     <row r="73" spans="1:5" ht="30">
       <c r="A73" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="C73" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="B73" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>233</v>
-      </c>
       <c r="D73" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E73" s="8" t="s">
         <v>153</v>
@@ -3036,16 +3036,16 @@
     </row>
     <row r="74" spans="1:5" ht="30">
       <c r="A74" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="B74" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="B74" s="7" t="s">
+      <c r="C74" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="C74" s="7" t="s">
-        <v>237</v>
-      </c>
       <c r="D74" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E74" s="8" t="s">
         <v>153</v>
@@ -3053,16 +3053,16 @@
     </row>
     <row r="75" spans="1:5" ht="30">
       <c r="A75" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="B75" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="B75" s="7" t="s">
+      <c r="C75" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="C75" s="7" t="s">
-        <v>240</v>
-      </c>
       <c r="D75" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E75" s="8" t="s">
         <v>153</v>
@@ -3070,16 +3070,16 @@
     </row>
     <row r="76" spans="1:5" ht="30">
       <c r="A76" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="B76" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="B76" s="7" t="s">
+      <c r="C76" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="C76" s="7" t="s">
-        <v>243</v>
-      </c>
       <c r="D76" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E76" s="8" t="s">
         <v>153</v>
@@ -3087,16 +3087,16 @@
     </row>
     <row r="77" spans="1:5" ht="30">
       <c r="A77" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="C77" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B77" s="7" t="s">
-        <v>246</v>
-      </c>
-      <c r="C77" s="7" t="s">
-        <v>245</v>
-      </c>
       <c r="D77" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E77" s="8" t="s">
         <v>153</v>
@@ -3104,16 +3104,16 @@
     </row>
     <row r="78" spans="1:5" ht="30">
       <c r="A78" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="C78" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="B78" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="C78" s="7" t="s">
-        <v>248</v>
-      </c>
       <c r="D78" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E78" s="8" t="s">
         <v>153</v>
@@ -3121,16 +3121,16 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B79" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="B79" s="7" t="s">
+      <c r="C79" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="C79" s="7" t="s">
-        <v>252</v>
-      </c>
       <c r="D79" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E79" s="8" t="s">
         <v>153</v>
@@ -3138,16 +3138,16 @@
     </row>
     <row r="80" spans="1:5" ht="90">
       <c r="A80" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B80" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="B80" s="7" t="s">
+      <c r="C80" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="C80" s="7" t="s">
-        <v>255</v>
-      </c>
       <c r="D80" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E80" s="8" t="s">
         <v>153</v>
@@ -3155,16 +3155,16 @@
     </row>
     <row r="81" spans="1:5" ht="60">
       <c r="A81" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="C81" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="B81" s="7" t="s">
-        <v>258</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>257</v>
-      </c>
       <c r="D81" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E81" s="8" t="s">
         <v>153</v>
@@ -3172,16 +3172,16 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="B82" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="B82" s="7" t="s">
+      <c r="C82" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="C82" s="7" t="s">
-        <v>261</v>
-      </c>
       <c r="D82" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E82" s="8" t="s">
         <v>153</v>
@@ -3189,16 +3189,16 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="B83" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="B83" s="7" t="s">
+      <c r="C83" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="C83" s="7" t="s">
-        <v>264</v>
-      </c>
       <c r="D83" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E83" s="8" t="s">
         <v>153</v>
@@ -3206,16 +3206,16 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="B84" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="B84" s="7" t="s">
-        <v>267</v>
-      </c>
       <c r="C84" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E84" s="8" t="s">
         <v>153</v>
@@ -3223,16 +3223,16 @@
     </row>
     <row r="85" spans="1:5" ht="120">
       <c r="A85" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E85" s="8" t="s">
         <v>153</v>
@@ -3240,16 +3240,16 @@
     </row>
     <row r="86" spans="1:5" ht="120">
       <c r="A86" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E86" s="8" t="s">
         <v>153</v>
@@ -3257,16 +3257,16 @@
     </row>
     <row r="87" spans="1:5" ht="195">
       <c r="A87" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E87" s="8" t="s">
         <v>153</v>
@@ -3274,16 +3274,16 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E88" s="8" t="s">
         <v>153</v>
@@ -3291,16 +3291,16 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E89" s="8" t="s">
         <v>153</v>
@@ -3308,16 +3308,16 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="B90" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="B90" s="7" t="s">
+      <c r="C90" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="C90" s="7" t="s">
-        <v>285</v>
-      </c>
       <c r="D90" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E90" s="8" t="s">
         <v>153</v>
@@ -3325,16 +3325,16 @@
     </row>
     <row r="91" spans="1:5" ht="30">
       <c r="A91" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E91" s="8" t="s">
         <v>153</v>
@@ -3342,16 +3342,16 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B92" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="C92" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="C92" s="7" t="s">
-        <v>291</v>
-      </c>
       <c r="D92" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E92" s="8" t="s">
         <v>153</v>
@@ -3359,16 +3359,16 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E93" s="8" t="s">
         <v>153</v>
@@ -3376,16 +3376,16 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="B94" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="B94" s="7" t="s">
+      <c r="C94" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="C94" s="8" t="s">
-        <v>298</v>
-      </c>
       <c r="D94" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E94" s="8" t="s">
         <v>153</v>
@@ -3393,16 +3393,16 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="B95" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="B95" s="7" t="s">
-        <v>301</v>
-      </c>
       <c r="C95" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E95" s="8" t="s">
         <v>153</v>
@@ -3410,16 +3410,16 @@
     </row>
     <row r="96" spans="1:5" ht="105">
       <c r="A96" s="8" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E96" s="8" t="s">
         <v>153</v>
@@ -3427,16 +3427,16 @@
     </row>
     <row r="97" spans="1:5" ht="105">
       <c r="A97" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E97" s="8" t="s">
         <v>153</v>
@@ -3444,16 +3444,16 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="B98" s="7" t="s">
         <v>308</v>
       </c>
-      <c r="B98" s="7" t="s">
+      <c r="C98" s="7" t="s">
         <v>309</v>
       </c>
-      <c r="C98" s="7" t="s">
-        <v>310</v>
-      </c>
       <c r="D98" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E98" s="8" t="s">
         <v>153</v>
@@ -3461,16 +3461,16 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="B99" s="7" t="s">
         <v>311</v>
       </c>
-      <c r="B99" s="7" t="s">
+      <c r="C99" s="7" t="s">
         <v>312</v>
       </c>
-      <c r="C99" s="7" t="s">
-        <v>313</v>
-      </c>
       <c r="D99" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E99" s="8" t="s">
         <v>153</v>
@@ -3478,16 +3478,16 @@
     </row>
     <row r="100" spans="1:5" ht="45">
       <c r="A100" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="C100" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="B100" s="7" t="s">
-        <v>316</v>
-      </c>
-      <c r="C100" s="7" t="s">
-        <v>315</v>
-      </c>
       <c r="D100" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E100" s="8" t="s">
         <v>153</v>
@@ -3495,16 +3495,16 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="B101" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="B101" s="8" t="s">
+      <c r="C101" s="8" t="s">
         <v>318</v>
       </c>
-      <c r="C101" s="8" t="s">
-        <v>319</v>
-      </c>
       <c r="D101" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E101" s="8" t="s">
         <v>153</v>
@@ -3512,16 +3512,16 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="B102" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="B102" s="8" t="s">
+      <c r="C102" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="C102" s="8" t="s">
-        <v>322</v>
-      </c>
       <c r="D102" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E102" s="8" t="s">
         <v>153</v>
@@ -3529,16 +3529,16 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="B103" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="B103" s="8" t="s">
+      <c r="C103" s="8" t="s">
         <v>324</v>
       </c>
-      <c r="C103" s="8" t="s">
-        <v>325</v>
-      </c>
       <c r="D103" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E103" s="8" t="s">
         <v>153</v>
@@ -3546,16 +3546,16 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="B104" s="8" t="s">
         <v>326</v>
       </c>
-      <c r="B104" s="8" t="s">
+      <c r="C104" s="8" t="s">
         <v>327</v>
       </c>
-      <c r="C104" s="8" t="s">
-        <v>328</v>
-      </c>
       <c r="D104" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E104" s="8" t="s">
         <v>153</v>
@@ -3563,16 +3563,16 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="8" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B105" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="C105" s="8" t="s">
         <v>331</v>
       </c>
-      <c r="C105" s="8" t="s">
-        <v>332</v>
-      </c>
       <c r="D105" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E105" s="8" t="s">
         <v>153</v>
@@ -3580,16 +3580,16 @@
     </row>
     <row r="106" spans="1:5" ht="165">
       <c r="A106" s="8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E106" s="8" t="s">
         <v>153</v>
@@ -3597,16 +3597,16 @@
     </row>
     <row r="107" spans="1:5" ht="75">
       <c r="A107" s="8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E107" s="8" t="s">
         <v>153</v>
@@ -3614,16 +3614,16 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="B108" s="7" t="s">
         <v>336</v>
       </c>
-      <c r="B108" s="7" t="s">
+      <c r="C108" s="7" t="s">
         <v>337</v>
       </c>
-      <c r="C108" s="7" t="s">
-        <v>338</v>
-      </c>
       <c r="D108" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E108" s="8" t="s">
         <v>153</v>
@@ -3631,16 +3631,16 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="B109" s="7" t="s">
         <v>339</v>
       </c>
-      <c r="B109" s="7" t="s">
+      <c r="C109" s="7" t="s">
         <v>340</v>
       </c>
-      <c r="C109" s="7" t="s">
-        <v>341</v>
-      </c>
       <c r="D109" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E109" s="8" t="s">
         <v>153</v>
@@ -3648,16 +3648,16 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="8" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B110" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="C110" s="8" t="s">
         <v>344</v>
       </c>
-      <c r="C110" s="8" t="s">
-        <v>345</v>
-      </c>
       <c r="D110" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E110" s="8" t="s">
         <v>153</v>
@@ -3665,16 +3665,16 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="8" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B111" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="C111" s="8" t="s">
         <v>342</v>
       </c>
-      <c r="C111" s="8" t="s">
-        <v>343</v>
-      </c>
       <c r="D111" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E111" s="8" t="s">
         <v>153</v>
@@ -3682,16 +3682,16 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="B112" s="8" t="s">
         <v>348</v>
       </c>
-      <c r="B112" s="8" t="s">
+      <c r="C112" s="8" t="s">
         <v>349</v>
       </c>
-      <c r="C112" s="8" t="s">
-        <v>350</v>
-      </c>
       <c r="D112" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E112" s="8" t="s">
         <v>153</v>
@@ -3699,16 +3699,16 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E113" s="8" t="s">
         <v>153</v>
@@ -3716,16 +3716,16 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B114" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="C114" s="8" t="s">
         <v>354</v>
       </c>
-      <c r="C114" s="8" t="s">
-        <v>355</v>
-      </c>
       <c r="D114" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E114" s="8" t="s">
         <v>153</v>
@@ -3733,16 +3733,16 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="8" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B115" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="C115" s="8" t="s">
         <v>356</v>
       </c>
-      <c r="C115" s="8" t="s">
-        <v>357</v>
-      </c>
       <c r="D115" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E115" s="8" t="s">
         <v>153</v>
@@ -3750,16 +3750,16 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="8" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E116" s="8" t="s">
         <v>153</v>
@@ -3767,16 +3767,16 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E117" s="8" t="s">
         <v>153</v>
@@ -3784,16 +3784,16 @@
     </row>
     <row r="118" spans="1:5" ht="30">
       <c r="A118" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C118" s="10" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E118" s="8" t="s">
         <v>153</v>
@@ -3801,16 +3801,16 @@
     </row>
     <row r="119" spans="1:5" ht="75">
       <c r="A119" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B119" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="C119" s="7" t="s">
         <v>371</v>
       </c>
-      <c r="C119" s="7" t="s">
-        <v>372</v>
-      </c>
       <c r="D119" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E119" s="8" t="s">
         <v>153</v>
@@ -3818,16 +3818,16 @@
     </row>
     <row r="120" spans="1:5" ht="60">
       <c r="A120" s="8" t="s">
+        <v>373</v>
+      </c>
+      <c r="B120" s="7" t="s">
         <v>374</v>
       </c>
-      <c r="B120" s="7" t="s">
+      <c r="C120" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="C120" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="D120" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E120" s="8" t="s">
         <v>153</v>
@@ -3835,16 +3835,16 @@
     </row>
     <row r="121" spans="1:5" ht="105">
       <c r="A121" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="B121" s="7" t="s">
         <v>377</v>
       </c>
-      <c r="B121" s="7" t="s">
+      <c r="C121" s="7" t="s">
         <v>378</v>
       </c>
-      <c r="C121" s="7" t="s">
-        <v>379</v>
-      </c>
       <c r="D121" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E121" s="8" t="s">
         <v>153</v>
@@ -3852,16 +3852,16 @@
     </row>
     <row r="122" spans="1:5" ht="105">
       <c r="A122" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="B122" s="7" t="s">
         <v>380</v>
       </c>
-      <c r="B122" s="7" t="s">
+      <c r="C122" s="7" t="s">
         <v>381</v>
       </c>
-      <c r="C122" s="7" t="s">
-        <v>382</v>
-      </c>
       <c r="D122" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E122" s="8" t="s">
         <v>153</v>
@@ -3869,16 +3869,16 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="B123" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="B123" s="7" t="s">
+      <c r="C123" s="8" t="s">
         <v>384</v>
       </c>
-      <c r="C123" s="8" t="s">
-        <v>385</v>
-      </c>
       <c r="D123" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E123" s="8" t="s">
         <v>153</v>
@@ -3886,63 +3886,63 @@
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="B124" s="7" t="s">
         <v>386</v>
       </c>
-      <c r="B124" s="7" t="s">
+      <c r="C124" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="C124" s="3" t="s">
-        <v>388</v>
-      </c>
       <c r="D124" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E124" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B125" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C125" s="3" t="s">
         <v>389</v>
       </c>
-      <c r="C125" s="3" t="s">
-        <v>390</v>
-      </c>
-      <c r="D125" s="3" t="s">
-        <v>220</v>
+      <c r="D125" s="8" t="s">
+        <v>397</v>
       </c>
       <c r="E125" s="3"/>
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="D126" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="E126" s="3"/>
+    </row>
+    <row r="127" spans="1:5" ht="150">
+      <c r="A127" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="B126" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="C126" s="3" t="s">
+      <c r="B127" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="D126" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="E126" s="3"/>
-    </row>
-    <row r="127" spans="1:5">
-      <c r="A127" s="3" t="s">
-        <v>397</v>
-      </c>
-      <c r="B127" s="3" t="s">
+      <c r="C127" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="C127" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="D127" s="3" t="s">
-        <v>220</v>
+      <c r="D127" s="8" t="s">
+        <v>397</v>
       </c>
       <c r="E127" s="3"/>
     </row>

</xml_diff>

<commit_message>
Committing changes to search test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -755,9 +755,6 @@
     <t>OPQA-263</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>TestCase_B68</t>
   </si>
   <si>
@@ -1378,6 +1375,9 @@
   </si>
   <si>
     <t>TestCase_B126</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -1780,8 +1780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="C126" sqref="C126"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1821,7 +1821,7 @@
         <v>97</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>153</v>
@@ -1838,7 +1838,7 @@
         <v>77</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>153</v>
@@ -1855,7 +1855,7 @@
         <v>78</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>153</v>
@@ -1872,7 +1872,7 @@
         <v>79</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>153</v>
@@ -1889,7 +1889,7 @@
         <v>80</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>153</v>
@@ -1906,7 +1906,7 @@
         <v>81</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>153</v>
@@ -1923,7 +1923,7 @@
         <v>74</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>153</v>
@@ -1940,7 +1940,7 @@
         <v>82</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>153</v>
@@ -1957,7 +1957,7 @@
         <v>83</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>153</v>
@@ -1974,7 +1974,7 @@
         <v>84</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>153</v>
@@ -1991,7 +1991,7 @@
         <v>85</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>153</v>
@@ -2008,7 +2008,7 @@
         <v>101</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>153</v>
@@ -2025,7 +2025,7 @@
         <v>86</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>153</v>
@@ -2042,7 +2042,7 @@
         <v>87</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>153</v>
@@ -2059,7 +2059,7 @@
         <v>88</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>153</v>
@@ -2076,7 +2076,7 @@
         <v>89</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>153</v>
@@ -2093,7 +2093,7 @@
         <v>140</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>153</v>
@@ -2110,7 +2110,7 @@
         <v>90</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>153</v>
@@ -2127,7 +2127,7 @@
         <v>91</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>153</v>
@@ -2144,7 +2144,7 @@
         <v>92</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>153</v>
@@ -2161,7 +2161,7 @@
         <v>93</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>153</v>
@@ -2178,7 +2178,7 @@
         <v>94</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>153</v>
@@ -2195,7 +2195,7 @@
         <v>95</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>153</v>
@@ -2212,7 +2212,7 @@
         <v>96</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>153</v>
@@ -2229,7 +2229,7 @@
         <v>104</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>153</v>
@@ -2246,7 +2246,7 @@
         <v>107</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>153</v>
@@ -2263,7 +2263,7 @@
         <v>110</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>153</v>
@@ -2280,7 +2280,7 @@
         <v>111</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>153</v>
@@ -2297,7 +2297,7 @@
         <v>116</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>153</v>
@@ -2314,7 +2314,7 @@
         <v>119</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>153</v>
@@ -2331,7 +2331,7 @@
         <v>122</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>153</v>
@@ -2348,7 +2348,7 @@
         <v>124</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>153</v>
@@ -2365,7 +2365,7 @@
         <v>126</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>153</v>
@@ -2382,7 +2382,7 @@
         <v>128</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>153</v>
@@ -2399,7 +2399,7 @@
         <v>134</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>153</v>
@@ -2416,7 +2416,7 @@
         <v>137</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E37" s="8" t="s">
         <v>153</v>
@@ -2433,7 +2433,7 @@
         <v>140</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>153</v>
@@ -2450,7 +2450,7 @@
         <v>143</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>153</v>
@@ -2467,7 +2467,7 @@
         <v>146</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>153</v>
@@ -2484,7 +2484,7 @@
         <v>149</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E41" s="8" t="s">
         <v>153</v>
@@ -2501,7 +2501,7 @@
         <v>152</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E42" s="8" t="s">
         <v>153</v>
@@ -2518,7 +2518,7 @@
         <v>160</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E43" s="8" t="s">
         <v>153</v>
@@ -2535,7 +2535,7 @@
         <v>161</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>153</v>
@@ -2552,7 +2552,7 @@
         <v>162</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E45" s="8" t="s">
         <v>153</v>
@@ -2569,7 +2569,7 @@
         <v>163</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>153</v>
@@ -2586,7 +2586,7 @@
         <v>165</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E47" s="8" t="s">
         <v>153</v>
@@ -2603,7 +2603,7 @@
         <v>167</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E48" s="8" t="s">
         <v>153</v>
@@ -2620,7 +2620,7 @@
         <v>170</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E49" s="8" t="s">
         <v>153</v>
@@ -2637,7 +2637,7 @@
         <v>172</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>153</v>
@@ -2654,7 +2654,7 @@
         <v>176</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E51" s="8" t="s">
         <v>153</v>
@@ -2671,7 +2671,7 @@
         <v>177</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E52" s="8" t="s">
         <v>153</v>
@@ -2688,7 +2688,7 @@
         <v>180</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E53" s="8" t="s">
         <v>153</v>
@@ -2705,7 +2705,7 @@
         <v>182</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E54" s="8" t="s">
         <v>153</v>
@@ -2722,7 +2722,7 @@
         <v>186</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E55" s="8" t="s">
         <v>153</v>
@@ -2739,7 +2739,7 @@
         <v>188</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E56" s="8" t="s">
         <v>153</v>
@@ -2756,7 +2756,7 @@
         <v>190</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E57" s="8" t="s">
         <v>153</v>
@@ -2773,7 +2773,7 @@
         <v>191</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E58" s="8" t="s">
         <v>153</v>
@@ -2790,7 +2790,7 @@
         <v>196</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E59" s="8" t="s">
         <v>153</v>
@@ -2807,7 +2807,7 @@
         <v>198</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E60" s="8" t="s">
         <v>153</v>
@@ -2824,7 +2824,7 @@
         <v>201</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E61" s="8" t="s">
         <v>153</v>
@@ -2841,7 +2841,7 @@
         <v>203</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E62" s="8" t="s">
         <v>153</v>
@@ -2858,7 +2858,7 @@
         <v>205</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E63" s="8" t="s">
         <v>153</v>
@@ -2875,7 +2875,7 @@
         <v>74</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>153</v>
@@ -2892,7 +2892,7 @@
         <v>213</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E65" s="8" t="s">
         <v>153</v>
@@ -2909,7 +2909,7 @@
         <v>211</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E66" s="8" t="s">
         <v>153</v>
@@ -2926,7 +2926,7 @@
         <v>216</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E67" s="8" t="s">
         <v>153</v>
@@ -2943,7 +2943,7 @@
         <v>218</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E68" s="8" t="s">
         <v>153</v>
@@ -2951,16 +2951,16 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B69" s="7" t="s">
         <v>64</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E69" s="8" t="s">
         <v>153</v>
@@ -2968,16 +2968,16 @@
     </row>
     <row r="70" spans="1:5" ht="45">
       <c r="A70" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="B70" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="B70" s="7" t="s">
+      <c r="C70" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="C70" s="7" t="s">
-        <v>225</v>
-      </c>
       <c r="D70" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E70" s="8" t="s">
         <v>153</v>
@@ -2985,16 +2985,16 @@
     </row>
     <row r="71" spans="1:5" ht="30">
       <c r="A71" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C71" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="B71" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>227</v>
-      </c>
       <c r="D71" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E71" s="8" t="s">
         <v>153</v>
@@ -3002,16 +3002,16 @@
     </row>
     <row r="72" spans="1:5" ht="30">
       <c r="A72" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B72" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="B72" s="7" t="s">
+      <c r="C72" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="C72" s="7" t="s">
-        <v>231</v>
-      </c>
       <c r="D72" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E72" s="8" t="s">
         <v>153</v>
@@ -3019,16 +3019,16 @@
     </row>
     <row r="73" spans="1:5" ht="30">
       <c r="A73" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="C73" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="B73" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>233</v>
-      </c>
       <c r="D73" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E73" s="8" t="s">
         <v>153</v>
@@ -3036,16 +3036,16 @@
     </row>
     <row r="74" spans="1:5" ht="30">
       <c r="A74" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="B74" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="B74" s="7" t="s">
+      <c r="C74" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="C74" s="7" t="s">
-        <v>237</v>
-      </c>
       <c r="D74" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E74" s="8" t="s">
         <v>153</v>
@@ -3053,16 +3053,16 @@
     </row>
     <row r="75" spans="1:5" ht="30">
       <c r="A75" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="B75" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="B75" s="7" t="s">
+      <c r="C75" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="C75" s="7" t="s">
-        <v>240</v>
-      </c>
       <c r="D75" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E75" s="8" t="s">
         <v>153</v>
@@ -3070,16 +3070,16 @@
     </row>
     <row r="76" spans="1:5" ht="30">
       <c r="A76" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="B76" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="B76" s="7" t="s">
+      <c r="C76" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="C76" s="7" t="s">
-        <v>243</v>
-      </c>
       <c r="D76" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E76" s="8" t="s">
         <v>153</v>
@@ -3087,16 +3087,16 @@
     </row>
     <row r="77" spans="1:5" ht="30">
       <c r="A77" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="C77" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B77" s="7" t="s">
-        <v>246</v>
-      </c>
-      <c r="C77" s="7" t="s">
-        <v>245</v>
-      </c>
       <c r="D77" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E77" s="8" t="s">
         <v>153</v>
@@ -3104,16 +3104,16 @@
     </row>
     <row r="78" spans="1:5" ht="30">
       <c r="A78" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="C78" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="B78" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="C78" s="7" t="s">
-        <v>248</v>
-      </c>
       <c r="D78" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E78" s="8" t="s">
         <v>153</v>
@@ -3121,16 +3121,16 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B79" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="B79" s="7" t="s">
+      <c r="C79" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="C79" s="7" t="s">
-        <v>252</v>
-      </c>
       <c r="D79" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E79" s="8" t="s">
         <v>153</v>
@@ -3138,16 +3138,16 @@
     </row>
     <row r="80" spans="1:5" ht="90">
       <c r="A80" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B80" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="B80" s="7" t="s">
+      <c r="C80" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="C80" s="7" t="s">
-        <v>255</v>
-      </c>
       <c r="D80" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E80" s="8" t="s">
         <v>153</v>
@@ -3155,16 +3155,16 @@
     </row>
     <row r="81" spans="1:5" ht="60">
       <c r="A81" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="C81" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="B81" s="7" t="s">
-        <v>258</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>257</v>
-      </c>
       <c r="D81" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E81" s="8" t="s">
         <v>153</v>
@@ -3172,16 +3172,16 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="B82" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="B82" s="7" t="s">
+      <c r="C82" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="C82" s="7" t="s">
-        <v>261</v>
-      </c>
       <c r="D82" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E82" s="8" t="s">
         <v>153</v>
@@ -3189,16 +3189,16 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="B83" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="B83" s="7" t="s">
+      <c r="C83" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="C83" s="7" t="s">
-        <v>264</v>
-      </c>
       <c r="D83" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E83" s="8" t="s">
         <v>153</v>
@@ -3206,16 +3206,16 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="B84" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="B84" s="7" t="s">
-        <v>267</v>
-      </c>
       <c r="C84" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E84" s="8" t="s">
         <v>153</v>
@@ -3223,16 +3223,16 @@
     </row>
     <row r="85" spans="1:5" ht="120">
       <c r="A85" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E85" s="8" t="s">
         <v>153</v>
@@ -3240,16 +3240,16 @@
     </row>
     <row r="86" spans="1:5" ht="120">
       <c r="A86" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E86" s="8" t="s">
         <v>153</v>
@@ -3257,16 +3257,16 @@
     </row>
     <row r="87" spans="1:5" ht="195">
       <c r="A87" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E87" s="8" t="s">
         <v>153</v>
@@ -3274,16 +3274,16 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E88" s="8" t="s">
         <v>153</v>
@@ -3291,16 +3291,16 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E89" s="8" t="s">
         <v>153</v>
@@ -3308,16 +3308,16 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="B90" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="B90" s="7" t="s">
+      <c r="C90" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="C90" s="7" t="s">
-        <v>285</v>
-      </c>
       <c r="D90" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E90" s="8" t="s">
         <v>153</v>
@@ -3325,16 +3325,16 @@
     </row>
     <row r="91" spans="1:5" ht="30">
       <c r="A91" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E91" s="8" t="s">
         <v>153</v>
@@ -3342,16 +3342,16 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B92" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="C92" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="C92" s="7" t="s">
-        <v>291</v>
-      </c>
       <c r="D92" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E92" s="8" t="s">
         <v>153</v>
@@ -3359,16 +3359,16 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E93" s="8" t="s">
         <v>153</v>
@@ -3376,16 +3376,16 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="B94" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="B94" s="7" t="s">
+      <c r="C94" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="C94" s="8" t="s">
-        <v>298</v>
-      </c>
       <c r="D94" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E94" s="8" t="s">
         <v>153</v>
@@ -3393,16 +3393,16 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="B95" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="B95" s="7" t="s">
-        <v>301</v>
-      </c>
       <c r="C95" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E95" s="8" t="s">
         <v>153</v>
@@ -3410,16 +3410,16 @@
     </row>
     <row r="96" spans="1:5" ht="105">
       <c r="A96" s="8" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E96" s="8" t="s">
         <v>153</v>
@@ -3427,16 +3427,16 @@
     </row>
     <row r="97" spans="1:5" ht="105">
       <c r="A97" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E97" s="8" t="s">
         <v>153</v>
@@ -3444,16 +3444,16 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="B98" s="7" t="s">
         <v>308</v>
       </c>
-      <c r="B98" s="7" t="s">
+      <c r="C98" s="7" t="s">
         <v>309</v>
       </c>
-      <c r="C98" s="7" t="s">
-        <v>310</v>
-      </c>
       <c r="D98" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E98" s="8" t="s">
         <v>153</v>
@@ -3461,16 +3461,16 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="B99" s="7" t="s">
         <v>311</v>
       </c>
-      <c r="B99" s="7" t="s">
+      <c r="C99" s="7" t="s">
         <v>312</v>
       </c>
-      <c r="C99" s="7" t="s">
-        <v>313</v>
-      </c>
       <c r="D99" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E99" s="8" t="s">
         <v>153</v>
@@ -3478,16 +3478,16 @@
     </row>
     <row r="100" spans="1:5" ht="45">
       <c r="A100" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="C100" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="B100" s="7" t="s">
-        <v>316</v>
-      </c>
-      <c r="C100" s="7" t="s">
-        <v>315</v>
-      </c>
       <c r="D100" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E100" s="8" t="s">
         <v>153</v>
@@ -3495,16 +3495,16 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="B101" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="B101" s="8" t="s">
+      <c r="C101" s="8" t="s">
         <v>318</v>
       </c>
-      <c r="C101" s="8" t="s">
-        <v>319</v>
-      </c>
       <c r="D101" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E101" s="8" t="s">
         <v>153</v>
@@ -3512,16 +3512,16 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="B102" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="B102" s="8" t="s">
+      <c r="C102" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="C102" s="8" t="s">
-        <v>322</v>
-      </c>
       <c r="D102" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E102" s="8" t="s">
         <v>153</v>
@@ -3529,16 +3529,16 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="B103" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="B103" s="8" t="s">
+      <c r="C103" s="8" t="s">
         <v>324</v>
       </c>
-      <c r="C103" s="8" t="s">
-        <v>325</v>
-      </c>
       <c r="D103" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E103" s="8" t="s">
         <v>153</v>
@@ -3546,16 +3546,16 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="B104" s="8" t="s">
         <v>326</v>
       </c>
-      <c r="B104" s="8" t="s">
+      <c r="C104" s="8" t="s">
         <v>327</v>
       </c>
-      <c r="C104" s="8" t="s">
-        <v>328</v>
-      </c>
       <c r="D104" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E104" s="8" t="s">
         <v>153</v>
@@ -3563,16 +3563,16 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="8" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B105" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="C105" s="8" t="s">
         <v>331</v>
       </c>
-      <c r="C105" s="8" t="s">
-        <v>332</v>
-      </c>
       <c r="D105" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E105" s="8" t="s">
         <v>153</v>
@@ -3580,16 +3580,16 @@
     </row>
     <row r="106" spans="1:5" ht="165">
       <c r="A106" s="8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E106" s="8" t="s">
         <v>153</v>
@@ -3597,16 +3597,16 @@
     </row>
     <row r="107" spans="1:5" ht="75">
       <c r="A107" s="8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E107" s="8" t="s">
         <v>153</v>
@@ -3614,16 +3614,16 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="B108" s="7" t="s">
         <v>336</v>
       </c>
-      <c r="B108" s="7" t="s">
+      <c r="C108" s="7" t="s">
         <v>337</v>
       </c>
-      <c r="C108" s="7" t="s">
-        <v>338</v>
-      </c>
       <c r="D108" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E108" s="8" t="s">
         <v>153</v>
@@ -3631,16 +3631,16 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="B109" s="7" t="s">
         <v>339</v>
       </c>
-      <c r="B109" s="7" t="s">
+      <c r="C109" s="7" t="s">
         <v>340</v>
       </c>
-      <c r="C109" s="7" t="s">
-        <v>341</v>
-      </c>
       <c r="D109" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E109" s="8" t="s">
         <v>153</v>
@@ -3648,16 +3648,16 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="8" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B110" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="C110" s="8" t="s">
         <v>344</v>
       </c>
-      <c r="C110" s="8" t="s">
-        <v>345</v>
-      </c>
       <c r="D110" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E110" s="8" t="s">
         <v>153</v>
@@ -3665,16 +3665,16 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="8" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B111" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="C111" s="8" t="s">
         <v>342</v>
       </c>
-      <c r="C111" s="8" t="s">
-        <v>343</v>
-      </c>
       <c r="D111" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E111" s="8" t="s">
         <v>153</v>
@@ -3682,16 +3682,16 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="B112" s="8" t="s">
         <v>348</v>
       </c>
-      <c r="B112" s="8" t="s">
+      <c r="C112" s="8" t="s">
         <v>349</v>
       </c>
-      <c r="C112" s="8" t="s">
-        <v>350</v>
-      </c>
       <c r="D112" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E112" s="8" t="s">
         <v>153</v>
@@ -3699,16 +3699,16 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E113" s="8" t="s">
         <v>153</v>
@@ -3716,16 +3716,16 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B114" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="C114" s="8" t="s">
         <v>354</v>
       </c>
-      <c r="C114" s="8" t="s">
-        <v>355</v>
-      </c>
       <c r="D114" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E114" s="8" t="s">
         <v>153</v>
@@ -3733,16 +3733,16 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="8" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B115" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="C115" s="8" t="s">
         <v>356</v>
       </c>
-      <c r="C115" s="8" t="s">
-        <v>357</v>
-      </c>
       <c r="D115" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E115" s="8" t="s">
         <v>153</v>
@@ -3750,16 +3750,16 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="8" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E116" s="8" t="s">
         <v>153</v>
@@ -3767,16 +3767,16 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E117" s="8" t="s">
         <v>153</v>
@@ -3784,16 +3784,16 @@
     </row>
     <row r="118" spans="1:5" ht="30">
       <c r="A118" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C118" s="10" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E118" s="8" t="s">
         <v>153</v>
@@ -3801,16 +3801,16 @@
     </row>
     <row r="119" spans="1:5" ht="75">
       <c r="A119" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B119" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="C119" s="7" t="s">
         <v>371</v>
       </c>
-      <c r="C119" s="7" t="s">
-        <v>372</v>
-      </c>
       <c r="D119" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E119" s="8" t="s">
         <v>153</v>
@@ -3818,16 +3818,16 @@
     </row>
     <row r="120" spans="1:5" ht="60">
       <c r="A120" s="8" t="s">
+        <v>373</v>
+      </c>
+      <c r="B120" s="7" t="s">
         <v>374</v>
       </c>
-      <c r="B120" s="7" t="s">
+      <c r="C120" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="C120" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="D120" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E120" s="8" t="s">
         <v>153</v>
@@ -3835,16 +3835,16 @@
     </row>
     <row r="121" spans="1:5" ht="105">
       <c r="A121" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="B121" s="7" t="s">
         <v>377</v>
       </c>
-      <c r="B121" s="7" t="s">
+      <c r="C121" s="7" t="s">
         <v>378</v>
       </c>
-      <c r="C121" s="7" t="s">
-        <v>379</v>
-      </c>
       <c r="D121" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E121" s="8" t="s">
         <v>153</v>
@@ -3852,16 +3852,16 @@
     </row>
     <row r="122" spans="1:5" ht="105">
       <c r="A122" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="B122" s="7" t="s">
         <v>380</v>
       </c>
-      <c r="B122" s="7" t="s">
+      <c r="C122" s="7" t="s">
         <v>381</v>
       </c>
-      <c r="C122" s="7" t="s">
-        <v>382</v>
-      </c>
       <c r="D122" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E122" s="8" t="s">
         <v>153</v>
@@ -3869,16 +3869,16 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="B123" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="B123" s="7" t="s">
+      <c r="C123" s="8" t="s">
         <v>384</v>
       </c>
-      <c r="C123" s="8" t="s">
-        <v>385</v>
-      </c>
       <c r="D123" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E123" s="8" t="s">
         <v>153</v>
@@ -3886,63 +3886,63 @@
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="B124" s="7" t="s">
         <v>386</v>
       </c>
-      <c r="B124" s="7" t="s">
+      <c r="C124" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="C124" s="3" t="s">
-        <v>388</v>
-      </c>
       <c r="D124" s="8" t="s">
-        <v>220</v>
+        <v>397</v>
       </c>
       <c r="E124" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B125" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C125" s="3" t="s">
         <v>389</v>
       </c>
-      <c r="C125" s="3" t="s">
-        <v>390</v>
-      </c>
-      <c r="D125" s="3" t="s">
-        <v>220</v>
+      <c r="D125" s="8" t="s">
+        <v>397</v>
       </c>
       <c r="E125" s="3"/>
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="D126" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="E126" s="3"/>
+    </row>
+    <row r="127" spans="1:5" ht="150">
+      <c r="A127" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="B126" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="C126" s="3" t="s">
+      <c r="B127" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="D126" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="E126" s="3"/>
-    </row>
-    <row r="127" spans="1:5">
-      <c r="A127" s="3" t="s">
-        <v>397</v>
-      </c>
-      <c r="B127" s="3" t="s">
+      <c r="C127" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="C127" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="D127" s="3" t="s">
-        <v>220</v>
+      <c r="D127" s="8" t="s">
+        <v>397</v>
       </c>
       <c r="E127" s="3"/>
     </row>

</xml_diff>

<commit_message>
Check in Suite B xls
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -371,16 +371,10 @@
     <t>TestCase_B25</t>
   </si>
   <si>
-    <t>TBD-1</t>
-  </si>
-  <si>
     <t>Verify that autocomplete feature is working correctly</t>
   </si>
   <si>
     <t>TestCase_B26</t>
-  </si>
-  <si>
-    <t>TBD-2</t>
   </si>
   <si>
     <t>Verify that following sections get displayed in type ahead:
@@ -393,43 +387,28 @@
     <t>TestCase_B27</t>
   </si>
   <si>
-    <t>TBD-3</t>
-  </si>
-  <si>
     <t>Verify that 4 suggested categories get displayed in type ahead and the typed keyword is present in all the 4 categories</t>
   </si>
   <si>
     <t>Verify that 4 suggested articles get displayed in type ahead and the typed keyword is present in all the 4 articles</t>
   </si>
   <si>
-    <t>TBD-4</t>
-  </si>
-  <si>
     <t>TestCase_B28</t>
   </si>
   <si>
     <t>TestCase_B29</t>
   </si>
   <si>
-    <t>TBD-5</t>
-  </si>
-  <si>
     <t>Verify that 4 suggested patents get displayed in type ahead and the typed keyword is present in all the 4 patents</t>
   </si>
   <si>
     <t>TestCase_B30</t>
   </si>
   <si>
-    <t>TBD-6</t>
-  </si>
-  <si>
     <t>Verify that 4 suggested people get displayed in type ahead and the typed keyword is present in all the 4 people</t>
   </si>
   <si>
     <t>TestCase_B31</t>
-  </si>
-  <si>
-    <t>OPQA-610</t>
   </si>
   <si>
     <t>Verify that the following content type tabs get displayed in the left navigation pane:
@@ -461,28 +440,13 @@
     <t>Verify that user is able to sort the items by TIMES CITED field in ALL content type</t>
   </si>
   <si>
-    <t>TBD-7</t>
-  </si>
-  <si>
-    <t>TDB-8</t>
-  </si>
-  <si>
-    <t>TBD-9</t>
-  </si>
-  <si>
     <t>TestCase_B35</t>
   </si>
   <si>
-    <t>TBD-10</t>
-  </si>
-  <si>
     <t>Verify that no filtering options are present in ALL content type</t>
   </si>
   <si>
     <t>TestCase_B36</t>
-  </si>
-  <si>
-    <t>TBD-11</t>
   </si>
   <si>
     <t xml:space="preserve">Verify that the following fields get displayed in the SORT BY drop down when ARTICLES is selected as content type in the left navigation pane:
@@ -496,34 +460,22 @@
     <t>TestCase_B37</t>
   </si>
   <si>
-    <t>TBD-12</t>
-  </si>
-  <si>
     <t>Verify that user is able to sort the articles by TIMES CITED field in ARTICLES content type</t>
   </si>
   <si>
     <t>TestCase_B38</t>
   </si>
   <si>
-    <t>TBD-13</t>
-  </si>
-  <si>
     <t>Verify that only articles get displayed when user chooses ARTICLES as content type</t>
   </si>
   <si>
     <t>TestCase_B39</t>
   </si>
   <si>
-    <t>TBD-14</t>
-  </si>
-  <si>
     <t>Verify that all articles are sorted by RELEVANCE by default in ARTICLES content type</t>
   </si>
   <si>
     <t>TestCase_B40</t>
-  </si>
-  <si>
-    <t>TBD-15</t>
   </si>
   <si>
     <t xml:space="preserve">Verify that following filters are present for ARTICLES content type:
@@ -537,9 +489,6 @@
     <t>TestCase_B41</t>
   </si>
   <si>
-    <t>TBD-16</t>
-  </si>
-  <si>
     <t>Verify that user is able to expand and collapse the Document Type filter in ARTICLES content type</t>
   </si>
   <si>
@@ -549,19 +498,10 @@
     <t>TestCase_B42</t>
   </si>
   <si>
-    <t>TBD-17</t>
-  </si>
-  <si>
     <t>TestCase_B43</t>
   </si>
   <si>
     <t>TestCase_B44</t>
-  </si>
-  <si>
-    <t>TBD-18</t>
-  </si>
-  <si>
-    <t>TBD-19</t>
   </si>
   <si>
     <t>Verify that user is able to expand and collapse the Authors filter in ARTICLES content type</t>
@@ -1378,6 +1318,66 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>OPQA-1434</t>
+  </si>
+  <si>
+    <t>OPQA-1435</t>
+  </si>
+  <si>
+    <t>OPQA-1436</t>
+  </si>
+  <si>
+    <t>OPQA-1437</t>
+  </si>
+  <si>
+    <t>OPQA-1438</t>
+  </si>
+  <si>
+    <t>OPQA-1439</t>
+  </si>
+  <si>
+    <t>OPQA-1440</t>
+  </si>
+  <si>
+    <t>OPQA-1441</t>
+  </si>
+  <si>
+    <t>OPQA-1442</t>
+  </si>
+  <si>
+    <t>OPQA-1443</t>
+  </si>
+  <si>
+    <t>OPQA-1444</t>
+  </si>
+  <si>
+    <t>OPQA-1445</t>
+  </si>
+  <si>
+    <t>OPQA-1447</t>
+  </si>
+  <si>
+    <t>OPQA-1449</t>
+  </si>
+  <si>
+    <t>OPQA-1450</t>
+  </si>
+  <si>
+    <t>OPQA-1452</t>
+  </si>
+  <si>
+    <t>OPQA-1453</t>
+  </si>
+  <si>
+    <t>OPQA-1455</t>
+  </si>
+  <si>
+    <t>OPQA-1456</t>
+  </si>
+  <si>
+    <t>OPQA-1501</t>
   </si>
 </sst>
 </file>
@@ -1821,10 +1821,10 @@
         <v>97</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1838,10 +1838,10 @@
         <v>77</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1855,10 +1855,10 @@
         <v>78</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1872,10 +1872,10 @@
         <v>79</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1889,10 +1889,10 @@
         <v>80</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1906,10 +1906,10 @@
         <v>81</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
@@ -1923,10 +1923,10 @@
         <v>74</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1940,10 +1940,10 @@
         <v>82</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1957,10 +1957,10 @@
         <v>83</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1974,10 +1974,10 @@
         <v>84</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16.5" customHeight="1">
@@ -1991,10 +1991,10 @@
         <v>85</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2008,10 +2008,10 @@
         <v>101</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -2025,10 +2025,10 @@
         <v>86</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -2042,10 +2042,10 @@
         <v>87</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -2059,10 +2059,10 @@
         <v>88</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -2076,10 +2076,10 @@
         <v>89</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -2090,13 +2090,13 @@
         <v>76</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -2110,10 +2110,10 @@
         <v>90</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -2127,10 +2127,10 @@
         <v>91</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -2144,10 +2144,10 @@
         <v>92</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -2161,10 +2161,10 @@
         <v>93</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -2178,10 +2178,10 @@
         <v>94</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -2195,10 +2195,10 @@
         <v>95</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -2212,10 +2212,10 @@
         <v>96</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -2223,650 +2223,650 @@
         <v>102</v>
       </c>
       <c r="B26" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="C26" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="D26" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="75">
       <c r="A27" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>107</v>
-      </c>
       <c r="D27" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>109</v>
+        <v>380</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>112</v>
+        <v>381</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>115</v>
+        <v>382</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="8" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>118</v>
+        <v>383</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="90">
       <c r="A32" s="8" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>121</v>
+        <v>384</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="60">
       <c r="A33" s="8" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>129</v>
+        <v>385</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="8" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>130</v>
+        <v>386</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="8" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>131</v>
+        <v>387</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="8" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>133</v>
+        <v>388</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="90">
       <c r="A37" s="8" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>136</v>
+        <v>389</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="8" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>139</v>
+        <v>390</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="8" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>142</v>
+        <v>391</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="8" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>145</v>
+        <v>392</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="90">
       <c r="A41" s="8" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>148</v>
+        <v>393</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="8" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>151</v>
+        <v>394</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="8" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>155</v>
+        <v>395</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="8" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>158</v>
+        <v>396</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="8" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>159</v>
+        <v>397</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="90">
       <c r="A46" s="8" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>65</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="8" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>66</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="8" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>67</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="8" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>76</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="8" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="8" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="8" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>68</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="8" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="8" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="8" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="8" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>69</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="8" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="B57" s="7" t="s">
         <v>73</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="8" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="120">
       <c r="A59" s="8" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="30">
       <c r="A60" s="8" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="30">
       <c r="A61" s="8" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>70</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="30">
       <c r="A62" s="8" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>72</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="30">
       <c r="A63" s="8" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="8" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="B64" s="7" t="s">
         <v>75</v>
@@ -2875,1074 +2875,1074 @@
         <v>74</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="8" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="8" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="8" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="8" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>219</v>
+        <v>199</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="8" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="B69" s="7" t="s">
         <v>64</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E69" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="45">
       <c r="A70" s="8" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="30">
       <c r="A71" s="8" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="30">
       <c r="A72" s="8" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="30">
       <c r="A73" s="8" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="30">
       <c r="A74" s="8" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="30">
       <c r="A75" s="8" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="30">
       <c r="A76" s="8" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="30">
       <c r="A77" s="8" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="30">
       <c r="A78" s="8" t="s">
-        <v>246</v>
+        <v>226</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>248</v>
+        <v>228</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>247</v>
+        <v>227</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="8" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>251</v>
+        <v>231</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="90">
       <c r="A80" s="8" t="s">
-        <v>252</v>
+        <v>232</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>253</v>
+        <v>233</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>254</v>
+        <v>234</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E80" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="60">
       <c r="A81" s="8" t="s">
-        <v>255</v>
+        <v>235</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>256</v>
+        <v>236</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="8" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>259</v>
+        <v>239</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="8" t="s">
-        <v>261</v>
+        <v>241</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>262</v>
+        <v>242</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="8" t="s">
-        <v>265</v>
+        <v>245</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>266</v>
+        <v>246</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>264</v>
+        <v>244</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="120">
       <c r="A85" s="8" t="s">
-        <v>267</v>
+        <v>247</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>272</v>
+        <v>252</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="120">
       <c r="A86" s="8" t="s">
-        <v>268</v>
+        <v>248</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>273</v>
+        <v>253</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>271</v>
+        <v>251</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="195">
       <c r="A87" s="8" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>275</v>
+        <v>255</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>274</v>
+        <v>254</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E87" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="8" t="s">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>278</v>
+        <v>258</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>276</v>
+        <v>256</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E88" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="8" t="s">
-        <v>281</v>
+        <v>261</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>279</v>
+        <v>259</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>277</v>
+        <v>257</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="8" t="s">
-        <v>282</v>
+        <v>262</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>283</v>
+        <v>263</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>284</v>
+        <v>264</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="30">
       <c r="A91" s="8" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>288</v>
+        <v>268</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>287</v>
+        <v>267</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E91" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="8" t="s">
-        <v>286</v>
+        <v>266</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>289</v>
+        <v>269</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>290</v>
+        <v>270</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E92" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="8" t="s">
-        <v>294</v>
+        <v>274</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="8" t="s">
-        <v>295</v>
+        <v>275</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>296</v>
+        <v>276</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>297</v>
+        <v>277</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="8" t="s">
-        <v>299</v>
+        <v>279</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>300</v>
+        <v>280</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>298</v>
+        <v>278</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="105">
       <c r="A96" s="8" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>303</v>
+        <v>283</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>305</v>
+        <v>285</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E96" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="105">
       <c r="A97" s="8" t="s">
-        <v>302</v>
+        <v>282</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>304</v>
+        <v>284</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="8" t="s">
-        <v>307</v>
+        <v>287</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>308</v>
+        <v>288</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>309</v>
+        <v>289</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="8" t="s">
-        <v>310</v>
+        <v>290</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>311</v>
+        <v>291</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>312</v>
+        <v>292</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="45">
       <c r="A100" s="8" t="s">
-        <v>313</v>
+        <v>293</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>315</v>
+        <v>295</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>314</v>
+        <v>294</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="8" t="s">
-        <v>316</v>
+        <v>296</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>317</v>
+        <v>297</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E101" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="8" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>321</v>
+        <v>301</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E102" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="8" t="s">
-        <v>322</v>
+        <v>302</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>323</v>
+        <v>303</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>324</v>
+        <v>304</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E103" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="8" t="s">
-        <v>325</v>
+        <v>305</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>327</v>
+        <v>307</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E104" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="8" t="s">
-        <v>328</v>
+        <v>308</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>330</v>
+        <v>310</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>331</v>
+        <v>311</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E105" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="165">
       <c r="A106" s="8" t="s">
-        <v>329</v>
+        <v>309</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>333</v>
+        <v>313</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>332</v>
+        <v>312</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E106" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="75">
       <c r="A107" s="8" t="s">
-        <v>334</v>
+        <v>314</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>363</v>
+        <v>343</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>362</v>
+        <v>342</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E107" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="8" t="s">
-        <v>335</v>
+        <v>315</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>336</v>
+        <v>316</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>337</v>
+        <v>317</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E108" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="8" t="s">
-        <v>338</v>
+        <v>318</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>339</v>
+        <v>319</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>340</v>
+        <v>320</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E109" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="8" t="s">
-        <v>345</v>
+        <v>325</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>343</v>
+        <v>323</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>344</v>
+        <v>324</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E110" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="8" t="s">
-        <v>346</v>
+        <v>326</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>341</v>
+        <v>321</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>342</v>
+        <v>322</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E111" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="8" t="s">
-        <v>347</v>
+        <v>327</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>348</v>
+        <v>328</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>349</v>
+        <v>329</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E112" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="8" t="s">
-        <v>352</v>
+        <v>332</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>351</v>
+        <v>331</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>350</v>
+        <v>330</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E113" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="8" t="s">
-        <v>357</v>
+        <v>337</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>353</v>
+        <v>333</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>354</v>
+        <v>334</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E114" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="8" t="s">
-        <v>358</v>
+        <v>338</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>355</v>
+        <v>335</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>356</v>
+        <v>336</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E115" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="8" t="s">
-        <v>361</v>
+        <v>341</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>360</v>
+        <v>340</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>359</v>
+        <v>339</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E116" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="8" t="s">
-        <v>364</v>
+        <v>344</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>367</v>
+        <v>347</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>366</v>
+        <v>346</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E117" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="30">
       <c r="A118" s="8" t="s">
-        <v>365</v>
+        <v>345</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>369</v>
+        <v>349</v>
       </c>
       <c r="C118" s="10" t="s">
-        <v>368</v>
+        <v>348</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E118" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="75">
       <c r="A119" s="8" t="s">
-        <v>372</v>
+        <v>352</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>370</v>
+        <v>350</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>371</v>
+        <v>351</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E119" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="60">
       <c r="A120" s="8" t="s">
-        <v>373</v>
+        <v>353</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>374</v>
+        <v>354</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>375</v>
+        <v>355</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E120" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="105">
       <c r="A121" s="8" t="s">
-        <v>376</v>
+        <v>356</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>377</v>
+        <v>357</v>
       </c>
       <c r="C121" s="7" t="s">
-        <v>378</v>
+        <v>358</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E121" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="105">
       <c r="A122" s="8" t="s">
-        <v>379</v>
+        <v>359</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>380</v>
+        <v>360</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>381</v>
+        <v>361</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E122" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="8" t="s">
-        <v>382</v>
+        <v>362</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>383</v>
+        <v>363</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>384</v>
+        <v>364</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E123" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="8" t="s">
-        <v>385</v>
+        <v>365</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>386</v>
+        <v>366</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>387</v>
+        <v>367</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E124" s="8" t="s">
-        <v>291</v>
+        <v>271</v>
       </c>
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="3" t="s">
-        <v>394</v>
+        <v>374</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>388</v>
+        <v>368</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>389</v>
+        <v>369</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E125" s="3"/>
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="3" t="s">
-        <v>395</v>
+        <v>375</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>390</v>
+        <v>370</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>391</v>
+        <v>371</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E126" s="3"/>
     </row>
     <row r="127" spans="1:5" ht="150">
       <c r="A127" s="3" t="s">
-        <v>396</v>
+        <v>376</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>392</v>
+        <v>372</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>393</v>
+        <v>373</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E127" s="3"/>
     </row>

</xml_diff>

<commit_message>
class name and xml changes for profile scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -371,16 +371,10 @@
     <t>TestCase_B25</t>
   </si>
   <si>
-    <t>TBD-1</t>
-  </si>
-  <si>
     <t>Verify that autocomplete feature is working correctly</t>
   </si>
   <si>
     <t>TestCase_B26</t>
-  </si>
-  <si>
-    <t>TBD-2</t>
   </si>
   <si>
     <t>Verify that following sections get displayed in type ahead:
@@ -393,43 +387,28 @@
     <t>TestCase_B27</t>
   </si>
   <si>
-    <t>TBD-3</t>
-  </si>
-  <si>
     <t>Verify that 4 suggested categories get displayed in type ahead and the typed keyword is present in all the 4 categories</t>
   </si>
   <si>
     <t>Verify that 4 suggested articles get displayed in type ahead and the typed keyword is present in all the 4 articles</t>
   </si>
   <si>
-    <t>TBD-4</t>
-  </si>
-  <si>
     <t>TestCase_B28</t>
   </si>
   <si>
     <t>TestCase_B29</t>
   </si>
   <si>
-    <t>TBD-5</t>
-  </si>
-  <si>
     <t>Verify that 4 suggested patents get displayed in type ahead and the typed keyword is present in all the 4 patents</t>
   </si>
   <si>
     <t>TestCase_B30</t>
   </si>
   <si>
-    <t>TBD-6</t>
-  </si>
-  <si>
     <t>Verify that 4 suggested people get displayed in type ahead and the typed keyword is present in all the 4 people</t>
   </si>
   <si>
     <t>TestCase_B31</t>
-  </si>
-  <si>
-    <t>OPQA-610</t>
   </si>
   <si>
     <t>Verify that the following content type tabs get displayed in the left navigation pane:
@@ -461,28 +440,13 @@
     <t>Verify that user is able to sort the items by TIMES CITED field in ALL content type</t>
   </si>
   <si>
-    <t>TBD-7</t>
-  </si>
-  <si>
-    <t>TDB-8</t>
-  </si>
-  <si>
-    <t>TBD-9</t>
-  </si>
-  <si>
     <t>TestCase_B35</t>
   </si>
   <si>
-    <t>TBD-10</t>
-  </si>
-  <si>
     <t>Verify that no filtering options are present in ALL content type</t>
   </si>
   <si>
     <t>TestCase_B36</t>
-  </si>
-  <si>
-    <t>TBD-11</t>
   </si>
   <si>
     <t xml:space="preserve">Verify that the following fields get displayed in the SORT BY drop down when ARTICLES is selected as content type in the left navigation pane:
@@ -496,34 +460,22 @@
     <t>TestCase_B37</t>
   </si>
   <si>
-    <t>TBD-12</t>
-  </si>
-  <si>
     <t>Verify that user is able to sort the articles by TIMES CITED field in ARTICLES content type</t>
   </si>
   <si>
     <t>TestCase_B38</t>
   </si>
   <si>
-    <t>TBD-13</t>
-  </si>
-  <si>
     <t>Verify that only articles get displayed when user chooses ARTICLES as content type</t>
   </si>
   <si>
     <t>TestCase_B39</t>
   </si>
   <si>
-    <t>TBD-14</t>
-  </si>
-  <si>
     <t>Verify that all articles are sorted by RELEVANCE by default in ARTICLES content type</t>
   </si>
   <si>
     <t>TestCase_B40</t>
-  </si>
-  <si>
-    <t>TBD-15</t>
   </si>
   <si>
     <t xml:space="preserve">Verify that following filters are present for ARTICLES content type:
@@ -537,9 +489,6 @@
     <t>TestCase_B41</t>
   </si>
   <si>
-    <t>TBD-16</t>
-  </si>
-  <si>
     <t>Verify that user is able to expand and collapse the Document Type filter in ARTICLES content type</t>
   </si>
   <si>
@@ -549,19 +498,10 @@
     <t>TestCase_B42</t>
   </si>
   <si>
-    <t>TBD-17</t>
-  </si>
-  <si>
     <t>TestCase_B43</t>
   </si>
   <si>
     <t>TestCase_B44</t>
-  </si>
-  <si>
-    <t>TBD-18</t>
-  </si>
-  <si>
-    <t>TBD-19</t>
   </si>
   <si>
     <t>Verify that user is able to expand and collapse the Authors filter in ARTICLES content type</t>
@@ -1378,6 +1318,66 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>OPQA-1434</t>
+  </si>
+  <si>
+    <t>OPQA-1435</t>
+  </si>
+  <si>
+    <t>OPQA-1436</t>
+  </si>
+  <si>
+    <t>OPQA-1437</t>
+  </si>
+  <si>
+    <t>OPQA-1438</t>
+  </si>
+  <si>
+    <t>OPQA-1439</t>
+  </si>
+  <si>
+    <t>OPQA-1440</t>
+  </si>
+  <si>
+    <t>OPQA-1441</t>
+  </si>
+  <si>
+    <t>OPQA-1442</t>
+  </si>
+  <si>
+    <t>OPQA-1443</t>
+  </si>
+  <si>
+    <t>OPQA-1444</t>
+  </si>
+  <si>
+    <t>OPQA-1445</t>
+  </si>
+  <si>
+    <t>OPQA-1447</t>
+  </si>
+  <si>
+    <t>OPQA-1449</t>
+  </si>
+  <si>
+    <t>OPQA-1450</t>
+  </si>
+  <si>
+    <t>OPQA-1452</t>
+  </si>
+  <si>
+    <t>OPQA-1453</t>
+  </si>
+  <si>
+    <t>OPQA-1455</t>
+  </si>
+  <si>
+    <t>OPQA-1456</t>
+  </si>
+  <si>
+    <t>OPQA-1501</t>
   </si>
 </sst>
 </file>
@@ -1821,10 +1821,10 @@
         <v>97</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1838,10 +1838,10 @@
         <v>77</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1855,10 +1855,10 @@
         <v>78</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1872,10 +1872,10 @@
         <v>79</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1889,10 +1889,10 @@
         <v>80</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1906,10 +1906,10 @@
         <v>81</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
@@ -1923,10 +1923,10 @@
         <v>74</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1940,10 +1940,10 @@
         <v>82</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1957,10 +1957,10 @@
         <v>83</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1974,10 +1974,10 @@
         <v>84</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16.5" customHeight="1">
@@ -1991,10 +1991,10 @@
         <v>85</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2008,10 +2008,10 @@
         <v>101</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -2025,10 +2025,10 @@
         <v>86</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -2042,10 +2042,10 @@
         <v>87</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -2059,10 +2059,10 @@
         <v>88</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -2076,10 +2076,10 @@
         <v>89</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -2090,13 +2090,13 @@
         <v>76</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -2110,10 +2110,10 @@
         <v>90</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -2127,10 +2127,10 @@
         <v>91</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -2144,10 +2144,10 @@
         <v>92</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -2161,10 +2161,10 @@
         <v>93</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -2178,10 +2178,10 @@
         <v>94</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -2195,10 +2195,10 @@
         <v>95</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -2212,10 +2212,10 @@
         <v>96</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -2223,650 +2223,650 @@
         <v>102</v>
       </c>
       <c r="B26" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="C26" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="D26" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="75">
       <c r="A27" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>107</v>
-      </c>
       <c r="D27" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>109</v>
+        <v>380</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>112</v>
+        <v>381</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>115</v>
+        <v>382</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="8" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>118</v>
+        <v>383</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="90">
       <c r="A32" s="8" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>121</v>
+        <v>384</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="60">
       <c r="A33" s="8" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>129</v>
+        <v>385</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="8" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>130</v>
+        <v>386</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="8" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>131</v>
+        <v>387</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="8" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>133</v>
+        <v>388</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="90">
       <c r="A37" s="8" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>136</v>
+        <v>389</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="8" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>139</v>
+        <v>390</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="8" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>142</v>
+        <v>391</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="8" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>145</v>
+        <v>392</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="90">
       <c r="A41" s="8" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>148</v>
+        <v>393</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="8" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>151</v>
+        <v>394</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="8" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>155</v>
+        <v>395</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="8" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>158</v>
+        <v>396</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="8" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>159</v>
+        <v>397</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="90">
       <c r="A46" s="8" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>65</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="8" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>66</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="8" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>67</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="8" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>76</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="8" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="8" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="8" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>68</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="8" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="8" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="8" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="8" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>69</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="8" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="B57" s="7" t="s">
         <v>73</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="8" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="120">
       <c r="A59" s="8" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="30">
       <c r="A60" s="8" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="30">
       <c r="A61" s="8" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>70</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="30">
       <c r="A62" s="8" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>72</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="30">
       <c r="A63" s="8" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="8" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="B64" s="7" t="s">
         <v>75</v>
@@ -2875,1074 +2875,1074 @@
         <v>74</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="8" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="8" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="8" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="8" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>219</v>
+        <v>199</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="8" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="B69" s="7" t="s">
         <v>64</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E69" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="45">
       <c r="A70" s="8" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="30">
       <c r="A71" s="8" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="30">
       <c r="A72" s="8" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="30">
       <c r="A73" s="8" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="30">
       <c r="A74" s="8" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="30">
       <c r="A75" s="8" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="30">
       <c r="A76" s="8" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="30">
       <c r="A77" s="8" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="30">
       <c r="A78" s="8" t="s">
-        <v>246</v>
+        <v>226</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>248</v>
+        <v>228</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>247</v>
+        <v>227</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="8" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>251</v>
+        <v>231</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="90">
       <c r="A80" s="8" t="s">
-        <v>252</v>
+        <v>232</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>253</v>
+        <v>233</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>254</v>
+        <v>234</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E80" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="60">
       <c r="A81" s="8" t="s">
-        <v>255</v>
+        <v>235</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>256</v>
+        <v>236</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="8" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>259</v>
+        <v>239</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="8" t="s">
-        <v>261</v>
+        <v>241</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>262</v>
+        <v>242</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="8" t="s">
-        <v>265</v>
+        <v>245</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>266</v>
+        <v>246</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>264</v>
+        <v>244</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="120">
       <c r="A85" s="8" t="s">
-        <v>267</v>
+        <v>247</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>272</v>
+        <v>252</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="120">
       <c r="A86" s="8" t="s">
-        <v>268</v>
+        <v>248</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>273</v>
+        <v>253</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>271</v>
+        <v>251</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="195">
       <c r="A87" s="8" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>275</v>
+        <v>255</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>274</v>
+        <v>254</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E87" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="8" t="s">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>278</v>
+        <v>258</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>276</v>
+        <v>256</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E88" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="8" t="s">
-        <v>281</v>
+        <v>261</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>279</v>
+        <v>259</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>277</v>
+        <v>257</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="8" t="s">
-        <v>282</v>
+        <v>262</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>283</v>
+        <v>263</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>284</v>
+        <v>264</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="30">
       <c r="A91" s="8" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>288</v>
+        <v>268</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>287</v>
+        <v>267</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E91" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="8" t="s">
-        <v>286</v>
+        <v>266</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>289</v>
+        <v>269</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>290</v>
+        <v>270</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E92" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="8" t="s">
-        <v>294</v>
+        <v>274</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="8" t="s">
-        <v>295</v>
+        <v>275</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>296</v>
+        <v>276</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>297</v>
+        <v>277</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="8" t="s">
-        <v>299</v>
+        <v>279</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>300</v>
+        <v>280</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>298</v>
+        <v>278</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="105">
       <c r="A96" s="8" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>303</v>
+        <v>283</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>305</v>
+        <v>285</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E96" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="105">
       <c r="A97" s="8" t="s">
-        <v>302</v>
+        <v>282</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>304</v>
+        <v>284</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="8" t="s">
-        <v>307</v>
+        <v>287</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>308</v>
+        <v>288</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>309</v>
+        <v>289</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="8" t="s">
-        <v>310</v>
+        <v>290</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>311</v>
+        <v>291</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>312</v>
+        <v>292</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="45">
       <c r="A100" s="8" t="s">
-        <v>313</v>
+        <v>293</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>315</v>
+        <v>295</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>314</v>
+        <v>294</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="8" t="s">
-        <v>316</v>
+        <v>296</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>317</v>
+        <v>297</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E101" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="8" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>321</v>
+        <v>301</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E102" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="8" t="s">
-        <v>322</v>
+        <v>302</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>323</v>
+        <v>303</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>324</v>
+        <v>304</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E103" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="8" t="s">
-        <v>325</v>
+        <v>305</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>327</v>
+        <v>307</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E104" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="8" t="s">
-        <v>328</v>
+        <v>308</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>330</v>
+        <v>310</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>331</v>
+        <v>311</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E105" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="165">
       <c r="A106" s="8" t="s">
-        <v>329</v>
+        <v>309</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>333</v>
+        <v>313</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>332</v>
+        <v>312</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E106" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="75">
       <c r="A107" s="8" t="s">
-        <v>334</v>
+        <v>314</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>363</v>
+        <v>343</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>362</v>
+        <v>342</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E107" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="8" t="s">
-        <v>335</v>
+        <v>315</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>336</v>
+        <v>316</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>337</v>
+        <v>317</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E108" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="8" t="s">
-        <v>338</v>
+        <v>318</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>339</v>
+        <v>319</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>340</v>
+        <v>320</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E109" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="8" t="s">
-        <v>345</v>
+        <v>325</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>343</v>
+        <v>323</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>344</v>
+        <v>324</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E110" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="8" t="s">
-        <v>346</v>
+        <v>326</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>341</v>
+        <v>321</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>342</v>
+        <v>322</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E111" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="8" t="s">
-        <v>347</v>
+        <v>327</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>348</v>
+        <v>328</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>349</v>
+        <v>329</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E112" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="8" t="s">
-        <v>352</v>
+        <v>332</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>351</v>
+        <v>331</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>350</v>
+        <v>330</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E113" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="8" t="s">
-        <v>357</v>
+        <v>337</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>353</v>
+        <v>333</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>354</v>
+        <v>334</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E114" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="8" t="s">
-        <v>358</v>
+        <v>338</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>355</v>
+        <v>335</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>356</v>
+        <v>336</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E115" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="8" t="s">
-        <v>361</v>
+        <v>341</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>360</v>
+        <v>340</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>359</v>
+        <v>339</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E116" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="8" t="s">
-        <v>364</v>
+        <v>344</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>367</v>
+        <v>347</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>366</v>
+        <v>346</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E117" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="30">
       <c r="A118" s="8" t="s">
-        <v>365</v>
+        <v>345</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>369</v>
+        <v>349</v>
       </c>
       <c r="C118" s="10" t="s">
-        <v>368</v>
+        <v>348</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E118" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="75">
       <c r="A119" s="8" t="s">
-        <v>372</v>
+        <v>352</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>370</v>
+        <v>350</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>371</v>
+        <v>351</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E119" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="60">
       <c r="A120" s="8" t="s">
-        <v>373</v>
+        <v>353</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>374</v>
+        <v>354</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>375</v>
+        <v>355</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E120" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="105">
       <c r="A121" s="8" t="s">
-        <v>376</v>
+        <v>356</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>377</v>
+        <v>357</v>
       </c>
       <c r="C121" s="7" t="s">
-        <v>378</v>
+        <v>358</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E121" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="105">
       <c r="A122" s="8" t="s">
-        <v>379</v>
+        <v>359</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>380</v>
+        <v>360</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>381</v>
+        <v>361</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E122" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="8" t="s">
-        <v>382</v>
+        <v>362</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>383</v>
+        <v>363</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>384</v>
+        <v>364</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E123" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="8" t="s">
-        <v>385</v>
+        <v>365</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>386</v>
+        <v>366</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>387</v>
+        <v>367</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E124" s="8" t="s">
-        <v>291</v>
+        <v>271</v>
       </c>
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="3" t="s">
-        <v>394</v>
+        <v>374</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>388</v>
+        <v>368</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>389</v>
+        <v>369</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E125" s="3"/>
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="3" t="s">
-        <v>395</v>
+        <v>375</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>390</v>
+        <v>370</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>391</v>
+        <v>371</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E126" s="3"/>
     </row>
     <row r="127" spans="1:5" ht="150">
       <c r="A127" s="3" t="s">
-        <v>396</v>
+        <v>376</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>392</v>
+        <v>372</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>393</v>
+        <v>373</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E127" s="3"/>
     </row>

</xml_diff>

<commit_message>
Changing test case name for watch list scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -371,16 +371,10 @@
     <t>TestCase_B25</t>
   </si>
   <si>
-    <t>TBD-1</t>
-  </si>
-  <si>
     <t>Verify that autocomplete feature is working correctly</t>
   </si>
   <si>
     <t>TestCase_B26</t>
-  </si>
-  <si>
-    <t>TBD-2</t>
   </si>
   <si>
     <t>Verify that following sections get displayed in type ahead:
@@ -393,43 +387,28 @@
     <t>TestCase_B27</t>
   </si>
   <si>
-    <t>TBD-3</t>
-  </si>
-  <si>
     <t>Verify that 4 suggested categories get displayed in type ahead and the typed keyword is present in all the 4 categories</t>
   </si>
   <si>
     <t>Verify that 4 suggested articles get displayed in type ahead and the typed keyword is present in all the 4 articles</t>
   </si>
   <si>
-    <t>TBD-4</t>
-  </si>
-  <si>
     <t>TestCase_B28</t>
   </si>
   <si>
     <t>TestCase_B29</t>
   </si>
   <si>
-    <t>TBD-5</t>
-  </si>
-  <si>
     <t>Verify that 4 suggested patents get displayed in type ahead and the typed keyword is present in all the 4 patents</t>
   </si>
   <si>
     <t>TestCase_B30</t>
   </si>
   <si>
-    <t>TBD-6</t>
-  </si>
-  <si>
     <t>Verify that 4 suggested people get displayed in type ahead and the typed keyword is present in all the 4 people</t>
   </si>
   <si>
     <t>TestCase_B31</t>
-  </si>
-  <si>
-    <t>OPQA-610</t>
   </si>
   <si>
     <t>Verify that the following content type tabs get displayed in the left navigation pane:
@@ -461,28 +440,13 @@
     <t>Verify that user is able to sort the items by TIMES CITED field in ALL content type</t>
   </si>
   <si>
-    <t>TBD-7</t>
-  </si>
-  <si>
-    <t>TDB-8</t>
-  </si>
-  <si>
-    <t>TBD-9</t>
-  </si>
-  <si>
     <t>TestCase_B35</t>
   </si>
   <si>
-    <t>TBD-10</t>
-  </si>
-  <si>
     <t>Verify that no filtering options are present in ALL content type</t>
   </si>
   <si>
     <t>TestCase_B36</t>
-  </si>
-  <si>
-    <t>TBD-11</t>
   </si>
   <si>
     <t xml:space="preserve">Verify that the following fields get displayed in the SORT BY drop down when ARTICLES is selected as content type in the left navigation pane:
@@ -496,34 +460,22 @@
     <t>TestCase_B37</t>
   </si>
   <si>
-    <t>TBD-12</t>
-  </si>
-  <si>
     <t>Verify that user is able to sort the articles by TIMES CITED field in ARTICLES content type</t>
   </si>
   <si>
     <t>TestCase_B38</t>
   </si>
   <si>
-    <t>TBD-13</t>
-  </si>
-  <si>
     <t>Verify that only articles get displayed when user chooses ARTICLES as content type</t>
   </si>
   <si>
     <t>TestCase_B39</t>
   </si>
   <si>
-    <t>TBD-14</t>
-  </si>
-  <si>
     <t>Verify that all articles are sorted by RELEVANCE by default in ARTICLES content type</t>
   </si>
   <si>
     <t>TestCase_B40</t>
-  </si>
-  <si>
-    <t>TBD-15</t>
   </si>
   <si>
     <t xml:space="preserve">Verify that following filters are present for ARTICLES content type:
@@ -537,9 +489,6 @@
     <t>TestCase_B41</t>
   </si>
   <si>
-    <t>TBD-16</t>
-  </si>
-  <si>
     <t>Verify that user is able to expand and collapse the Document Type filter in ARTICLES content type</t>
   </si>
   <si>
@@ -549,19 +498,10 @@
     <t>TestCase_B42</t>
   </si>
   <si>
-    <t>TBD-17</t>
-  </si>
-  <si>
     <t>TestCase_B43</t>
   </si>
   <si>
     <t>TestCase_B44</t>
-  </si>
-  <si>
-    <t>TBD-18</t>
-  </si>
-  <si>
-    <t>TBD-19</t>
   </si>
   <si>
     <t>Verify that user is able to expand and collapse the Authors filter in ARTICLES content type</t>
@@ -1378,6 +1318,66 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>OPQA-1434</t>
+  </si>
+  <si>
+    <t>OPQA-1435</t>
+  </si>
+  <si>
+    <t>OPQA-1436</t>
+  </si>
+  <si>
+    <t>OPQA-1437</t>
+  </si>
+  <si>
+    <t>OPQA-1438</t>
+  </si>
+  <si>
+    <t>OPQA-1439</t>
+  </si>
+  <si>
+    <t>OPQA-1440</t>
+  </si>
+  <si>
+    <t>OPQA-1441</t>
+  </si>
+  <si>
+    <t>OPQA-1442</t>
+  </si>
+  <si>
+    <t>OPQA-1443</t>
+  </si>
+  <si>
+    <t>OPQA-1444</t>
+  </si>
+  <si>
+    <t>OPQA-1445</t>
+  </si>
+  <si>
+    <t>OPQA-1447</t>
+  </si>
+  <si>
+    <t>OPQA-1449</t>
+  </si>
+  <si>
+    <t>OPQA-1450</t>
+  </si>
+  <si>
+    <t>OPQA-1452</t>
+  </si>
+  <si>
+    <t>OPQA-1453</t>
+  </si>
+  <si>
+    <t>OPQA-1455</t>
+  </si>
+  <si>
+    <t>OPQA-1456</t>
+  </si>
+  <si>
+    <t>OPQA-1501</t>
   </si>
 </sst>
 </file>
@@ -1821,10 +1821,10 @@
         <v>97</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1838,10 +1838,10 @@
         <v>77</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1855,10 +1855,10 @@
         <v>78</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1872,10 +1872,10 @@
         <v>79</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1889,10 +1889,10 @@
         <v>80</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1906,10 +1906,10 @@
         <v>81</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
@@ -1923,10 +1923,10 @@
         <v>74</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1940,10 +1940,10 @@
         <v>82</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1957,10 +1957,10 @@
         <v>83</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1974,10 +1974,10 @@
         <v>84</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16.5" customHeight="1">
@@ -1991,10 +1991,10 @@
         <v>85</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2008,10 +2008,10 @@
         <v>101</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -2025,10 +2025,10 @@
         <v>86</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -2042,10 +2042,10 @@
         <v>87</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -2059,10 +2059,10 @@
         <v>88</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -2076,10 +2076,10 @@
         <v>89</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -2090,13 +2090,13 @@
         <v>76</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -2110,10 +2110,10 @@
         <v>90</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -2127,10 +2127,10 @@
         <v>91</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -2144,10 +2144,10 @@
         <v>92</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -2161,10 +2161,10 @@
         <v>93</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -2178,10 +2178,10 @@
         <v>94</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -2195,10 +2195,10 @@
         <v>95</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -2212,10 +2212,10 @@
         <v>96</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -2223,650 +2223,650 @@
         <v>102</v>
       </c>
       <c r="B26" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="C26" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="D26" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="75">
       <c r="A27" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>107</v>
-      </c>
       <c r="D27" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>109</v>
+        <v>380</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>112</v>
+        <v>381</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>115</v>
+        <v>382</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="8" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>118</v>
+        <v>383</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="90">
       <c r="A32" s="8" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>121</v>
+        <v>384</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="60">
       <c r="A33" s="8" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>129</v>
+        <v>385</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="8" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>130</v>
+        <v>386</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="8" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>131</v>
+        <v>387</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="8" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>133</v>
+        <v>388</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="90">
       <c r="A37" s="8" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>136</v>
+        <v>389</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="8" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>139</v>
+        <v>390</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="8" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>142</v>
+        <v>391</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="8" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>145</v>
+        <v>392</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="90">
       <c r="A41" s="8" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>148</v>
+        <v>393</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="8" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>151</v>
+        <v>394</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="8" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>155</v>
+        <v>395</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="8" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>158</v>
+        <v>396</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="8" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>159</v>
+        <v>397</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="90">
       <c r="A46" s="8" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>65</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="8" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>66</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="8" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>67</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="8" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>76</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="8" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="8" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="8" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>68</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="8" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="8" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="8" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="8" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>69</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="8" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="B57" s="7" t="s">
         <v>73</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="8" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="120">
       <c r="A59" s="8" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="30">
       <c r="A60" s="8" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="30">
       <c r="A61" s="8" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>70</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="30">
       <c r="A62" s="8" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>72</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="30">
       <c r="A63" s="8" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="8" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="B64" s="7" t="s">
         <v>75</v>
@@ -2875,1074 +2875,1074 @@
         <v>74</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="8" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="8" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="8" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="8" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>219</v>
+        <v>199</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="8" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="B69" s="7" t="s">
         <v>64</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E69" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="45">
       <c r="A70" s="8" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="30">
       <c r="A71" s="8" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="30">
       <c r="A72" s="8" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="30">
       <c r="A73" s="8" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="30">
       <c r="A74" s="8" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="30">
       <c r="A75" s="8" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="30">
       <c r="A76" s="8" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="30">
       <c r="A77" s="8" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="30">
       <c r="A78" s="8" t="s">
-        <v>246</v>
+        <v>226</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>248</v>
+        <v>228</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>247</v>
+        <v>227</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="8" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>251</v>
+        <v>231</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="90">
       <c r="A80" s="8" t="s">
-        <v>252</v>
+        <v>232</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>253</v>
+        <v>233</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>254</v>
+        <v>234</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E80" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="60">
       <c r="A81" s="8" t="s">
-        <v>255</v>
+        <v>235</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>256</v>
+        <v>236</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="8" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>259</v>
+        <v>239</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="8" t="s">
-        <v>261</v>
+        <v>241</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>262</v>
+        <v>242</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="8" t="s">
-        <v>265</v>
+        <v>245</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>266</v>
+        <v>246</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>264</v>
+        <v>244</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="120">
       <c r="A85" s="8" t="s">
-        <v>267</v>
+        <v>247</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>272</v>
+        <v>252</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="120">
       <c r="A86" s="8" t="s">
-        <v>268</v>
+        <v>248</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>273</v>
+        <v>253</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>271</v>
+        <v>251</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="195">
       <c r="A87" s="8" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>275</v>
+        <v>255</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>274</v>
+        <v>254</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E87" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="8" t="s">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>278</v>
+        <v>258</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>276</v>
+        <v>256</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E88" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="8" t="s">
-        <v>281</v>
+        <v>261</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>279</v>
+        <v>259</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>277</v>
+        <v>257</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="8" t="s">
-        <v>282</v>
+        <v>262</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>283</v>
+        <v>263</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>284</v>
+        <v>264</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="30">
       <c r="A91" s="8" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>288</v>
+        <v>268</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>287</v>
+        <v>267</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E91" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="8" t="s">
-        <v>286</v>
+        <v>266</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>289</v>
+        <v>269</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>290</v>
+        <v>270</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E92" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="8" t="s">
-        <v>294</v>
+        <v>274</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="8" t="s">
-        <v>295</v>
+        <v>275</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>296</v>
+        <v>276</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>297</v>
+        <v>277</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="8" t="s">
-        <v>299</v>
+        <v>279</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>300</v>
+        <v>280</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>298</v>
+        <v>278</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="105">
       <c r="A96" s="8" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>303</v>
+        <v>283</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>305</v>
+        <v>285</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E96" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="105">
       <c r="A97" s="8" t="s">
-        <v>302</v>
+        <v>282</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>304</v>
+        <v>284</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="8" t="s">
-        <v>307</v>
+        <v>287</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>308</v>
+        <v>288</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>309</v>
+        <v>289</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="8" t="s">
-        <v>310</v>
+        <v>290</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>311</v>
+        <v>291</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>312</v>
+        <v>292</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="45">
       <c r="A100" s="8" t="s">
-        <v>313</v>
+        <v>293</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>315</v>
+        <v>295</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>314</v>
+        <v>294</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="8" t="s">
-        <v>316</v>
+        <v>296</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>317</v>
+        <v>297</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E101" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="8" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>321</v>
+        <v>301</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E102" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="8" t="s">
-        <v>322</v>
+        <v>302</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>323</v>
+        <v>303</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>324</v>
+        <v>304</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E103" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="8" t="s">
-        <v>325</v>
+        <v>305</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>327</v>
+        <v>307</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E104" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="8" t="s">
-        <v>328</v>
+        <v>308</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>330</v>
+        <v>310</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>331</v>
+        <v>311</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E105" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="165">
       <c r="A106" s="8" t="s">
-        <v>329</v>
+        <v>309</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>333</v>
+        <v>313</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>332</v>
+        <v>312</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E106" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="75">
       <c r="A107" s="8" t="s">
-        <v>334</v>
+        <v>314</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>363</v>
+        <v>343</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>362</v>
+        <v>342</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E107" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="8" t="s">
-        <v>335</v>
+        <v>315</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>336</v>
+        <v>316</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>337</v>
+        <v>317</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E108" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="8" t="s">
-        <v>338</v>
+        <v>318</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>339</v>
+        <v>319</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>340</v>
+        <v>320</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E109" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="8" t="s">
-        <v>345</v>
+        <v>325</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>343</v>
+        <v>323</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>344</v>
+        <v>324</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E110" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="8" t="s">
-        <v>346</v>
+        <v>326</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>341</v>
+        <v>321</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>342</v>
+        <v>322</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E111" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="8" t="s">
-        <v>347</v>
+        <v>327</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>348</v>
+        <v>328</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>349</v>
+        <v>329</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E112" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="8" t="s">
-        <v>352</v>
+        <v>332</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>351</v>
+        <v>331</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>350</v>
+        <v>330</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E113" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="8" t="s">
-        <v>357</v>
+        <v>337</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>353</v>
+        <v>333</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>354</v>
+        <v>334</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E114" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="8" t="s">
-        <v>358</v>
+        <v>338</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>355</v>
+        <v>335</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>356</v>
+        <v>336</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E115" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="8" t="s">
-        <v>361</v>
+        <v>341</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>360</v>
+        <v>340</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>359</v>
+        <v>339</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E116" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="8" t="s">
-        <v>364</v>
+        <v>344</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>367</v>
+        <v>347</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>366</v>
+        <v>346</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E117" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="30">
       <c r="A118" s="8" t="s">
-        <v>365</v>
+        <v>345</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>369</v>
+        <v>349</v>
       </c>
       <c r="C118" s="10" t="s">
-        <v>368</v>
+        <v>348</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E118" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="75">
       <c r="A119" s="8" t="s">
-        <v>372</v>
+        <v>352</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>370</v>
+        <v>350</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>371</v>
+        <v>351</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E119" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="60">
       <c r="A120" s="8" t="s">
-        <v>373</v>
+        <v>353</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>374</v>
+        <v>354</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>375</v>
+        <v>355</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E120" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="105">
       <c r="A121" s="8" t="s">
-        <v>376</v>
+        <v>356</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>377</v>
+        <v>357</v>
       </c>
       <c r="C121" s="7" t="s">
-        <v>378</v>
+        <v>358</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E121" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="105">
       <c r="A122" s="8" t="s">
-        <v>379</v>
+        <v>359</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>380</v>
+        <v>360</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>381</v>
+        <v>361</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E122" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="8" t="s">
-        <v>382</v>
+        <v>362</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>383</v>
+        <v>363</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>384</v>
+        <v>364</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E123" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="8" t="s">
-        <v>385</v>
+        <v>365</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>386</v>
+        <v>366</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>387</v>
+        <v>367</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E124" s="8" t="s">
-        <v>291</v>
+        <v>271</v>
       </c>
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="3" t="s">
-        <v>394</v>
+        <v>374</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>388</v>
+        <v>368</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>389</v>
+        <v>369</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E125" s="3"/>
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="3" t="s">
-        <v>395</v>
+        <v>375</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>390</v>
+        <v>370</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>391</v>
+        <v>371</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E126" s="3"/>
     </row>
     <row r="127" spans="1:5" ht="150">
       <c r="A127" s="3" t="s">
-        <v>396</v>
+        <v>376</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>392</v>
+        <v>372</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>393</v>
+        <v>373</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E127" s="3"/>
     </row>

</xml_diff>

<commit_message>
Committing fixed search test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -371,16 +371,10 @@
     <t>TestCase_B25</t>
   </si>
   <si>
-    <t>TBD-1</t>
-  </si>
-  <si>
     <t>Verify that autocomplete feature is working correctly</t>
   </si>
   <si>
     <t>TestCase_B26</t>
-  </si>
-  <si>
-    <t>TBD-2</t>
   </si>
   <si>
     <t>Verify that following sections get displayed in type ahead:
@@ -393,43 +387,28 @@
     <t>TestCase_B27</t>
   </si>
   <si>
-    <t>TBD-3</t>
-  </si>
-  <si>
     <t>Verify that 4 suggested categories get displayed in type ahead and the typed keyword is present in all the 4 categories</t>
   </si>
   <si>
     <t>Verify that 4 suggested articles get displayed in type ahead and the typed keyword is present in all the 4 articles</t>
   </si>
   <si>
-    <t>TBD-4</t>
-  </si>
-  <si>
     <t>TestCase_B28</t>
   </si>
   <si>
     <t>TestCase_B29</t>
   </si>
   <si>
-    <t>TBD-5</t>
-  </si>
-  <si>
     <t>Verify that 4 suggested patents get displayed in type ahead and the typed keyword is present in all the 4 patents</t>
   </si>
   <si>
     <t>TestCase_B30</t>
   </si>
   <si>
-    <t>TBD-6</t>
-  </si>
-  <si>
     <t>Verify that 4 suggested people get displayed in type ahead and the typed keyword is present in all the 4 people</t>
   </si>
   <si>
     <t>TestCase_B31</t>
-  </si>
-  <si>
-    <t>OPQA-610</t>
   </si>
   <si>
     <t>Verify that the following content type tabs get displayed in the left navigation pane:
@@ -461,28 +440,13 @@
     <t>Verify that user is able to sort the items by TIMES CITED field in ALL content type</t>
   </si>
   <si>
-    <t>TBD-7</t>
-  </si>
-  <si>
-    <t>TDB-8</t>
-  </si>
-  <si>
-    <t>TBD-9</t>
-  </si>
-  <si>
     <t>TestCase_B35</t>
   </si>
   <si>
-    <t>TBD-10</t>
-  </si>
-  <si>
     <t>Verify that no filtering options are present in ALL content type</t>
   </si>
   <si>
     <t>TestCase_B36</t>
-  </si>
-  <si>
-    <t>TBD-11</t>
   </si>
   <si>
     <t xml:space="preserve">Verify that the following fields get displayed in the SORT BY drop down when ARTICLES is selected as content type in the left navigation pane:
@@ -496,34 +460,22 @@
     <t>TestCase_B37</t>
   </si>
   <si>
-    <t>TBD-12</t>
-  </si>
-  <si>
     <t>Verify that user is able to sort the articles by TIMES CITED field in ARTICLES content type</t>
   </si>
   <si>
     <t>TestCase_B38</t>
   </si>
   <si>
-    <t>TBD-13</t>
-  </si>
-  <si>
     <t>Verify that only articles get displayed when user chooses ARTICLES as content type</t>
   </si>
   <si>
     <t>TestCase_B39</t>
   </si>
   <si>
-    <t>TBD-14</t>
-  </si>
-  <si>
     <t>Verify that all articles are sorted by RELEVANCE by default in ARTICLES content type</t>
   </si>
   <si>
     <t>TestCase_B40</t>
-  </si>
-  <si>
-    <t>TBD-15</t>
   </si>
   <si>
     <t xml:space="preserve">Verify that following filters are present for ARTICLES content type:
@@ -537,9 +489,6 @@
     <t>TestCase_B41</t>
   </si>
   <si>
-    <t>TBD-16</t>
-  </si>
-  <si>
     <t>Verify that user is able to expand and collapse the Document Type filter in ARTICLES content type</t>
   </si>
   <si>
@@ -549,19 +498,10 @@
     <t>TestCase_B42</t>
   </si>
   <si>
-    <t>TBD-17</t>
-  </si>
-  <si>
     <t>TestCase_B43</t>
   </si>
   <si>
     <t>TestCase_B44</t>
-  </si>
-  <si>
-    <t>TBD-18</t>
-  </si>
-  <si>
-    <t>TBD-19</t>
   </si>
   <si>
     <t>Verify that user is able to expand and collapse the Authors filter in ARTICLES content type</t>
@@ -1378,6 +1318,66 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>OPQA-1434</t>
+  </si>
+  <si>
+    <t>OPQA-1435</t>
+  </si>
+  <si>
+    <t>OPQA-1436</t>
+  </si>
+  <si>
+    <t>OPQA-1437</t>
+  </si>
+  <si>
+    <t>OPQA-1438</t>
+  </si>
+  <si>
+    <t>OPQA-1439</t>
+  </si>
+  <si>
+    <t>OPQA-1440</t>
+  </si>
+  <si>
+    <t>OPQA-1441</t>
+  </si>
+  <si>
+    <t>OPQA-1442</t>
+  </si>
+  <si>
+    <t>OPQA-1443</t>
+  </si>
+  <si>
+    <t>OPQA-1444</t>
+  </si>
+  <si>
+    <t>OPQA-1445</t>
+  </si>
+  <si>
+    <t>OPQA-1447</t>
+  </si>
+  <si>
+    <t>OPQA-1449</t>
+  </si>
+  <si>
+    <t>OPQA-1450</t>
+  </si>
+  <si>
+    <t>OPQA-1452</t>
+  </si>
+  <si>
+    <t>OPQA-1453</t>
+  </si>
+  <si>
+    <t>OPQA-1455</t>
+  </si>
+  <si>
+    <t>OPQA-1456</t>
+  </si>
+  <si>
+    <t>OPQA-1501</t>
   </si>
 </sst>
 </file>
@@ -1821,10 +1821,10 @@
         <v>97</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1838,10 +1838,10 @@
         <v>77</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1855,10 +1855,10 @@
         <v>78</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1872,10 +1872,10 @@
         <v>79</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1889,10 +1889,10 @@
         <v>80</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1906,10 +1906,10 @@
         <v>81</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
@@ -1923,10 +1923,10 @@
         <v>74</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1940,10 +1940,10 @@
         <v>82</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1957,10 +1957,10 @@
         <v>83</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1974,10 +1974,10 @@
         <v>84</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16.5" customHeight="1">
@@ -1991,10 +1991,10 @@
         <v>85</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2008,10 +2008,10 @@
         <v>101</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -2025,10 +2025,10 @@
         <v>86</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -2042,10 +2042,10 @@
         <v>87</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -2059,10 +2059,10 @@
         <v>88</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -2076,10 +2076,10 @@
         <v>89</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -2090,13 +2090,13 @@
         <v>76</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -2110,10 +2110,10 @@
         <v>90</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -2127,10 +2127,10 @@
         <v>91</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -2144,10 +2144,10 @@
         <v>92</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -2161,10 +2161,10 @@
         <v>93</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -2178,10 +2178,10 @@
         <v>94</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -2195,10 +2195,10 @@
         <v>95</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -2212,10 +2212,10 @@
         <v>96</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -2223,650 +2223,650 @@
         <v>102</v>
       </c>
       <c r="B26" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="C26" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="D26" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="75">
       <c r="A27" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>107</v>
-      </c>
       <c r="D27" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>109</v>
+        <v>380</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>112</v>
+        <v>381</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>115</v>
+        <v>382</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="8" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>118</v>
+        <v>383</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="90">
       <c r="A32" s="8" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>121</v>
+        <v>384</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="60">
       <c r="A33" s="8" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>129</v>
+        <v>385</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="8" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>130</v>
+        <v>386</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="8" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>131</v>
+        <v>387</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="8" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>133</v>
+        <v>388</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="90">
       <c r="A37" s="8" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>136</v>
+        <v>389</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="8" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>139</v>
+        <v>390</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="8" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>142</v>
+        <v>391</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="8" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>145</v>
+        <v>392</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="90">
       <c r="A41" s="8" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>148</v>
+        <v>393</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="8" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>151</v>
+        <v>394</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="8" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>155</v>
+        <v>395</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="8" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>158</v>
+        <v>396</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="8" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>159</v>
+        <v>397</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="90">
       <c r="A46" s="8" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>65</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="8" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>66</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="8" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>67</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="8" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>76</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="8" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="8" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="8" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>68</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="8" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="8" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="8" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="8" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>69</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="8" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="B57" s="7" t="s">
         <v>73</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="8" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="120">
       <c r="A59" s="8" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="30">
       <c r="A60" s="8" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="30">
       <c r="A61" s="8" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>70</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="30">
       <c r="A62" s="8" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>72</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="30">
       <c r="A63" s="8" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="8" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="B64" s="7" t="s">
         <v>75</v>
@@ -2875,1074 +2875,1074 @@
         <v>74</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="8" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="8" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="8" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="8" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>219</v>
+        <v>199</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="8" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="B69" s="7" t="s">
         <v>64</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E69" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="45">
       <c r="A70" s="8" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="30">
       <c r="A71" s="8" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="30">
       <c r="A72" s="8" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="30">
       <c r="A73" s="8" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="30">
       <c r="A74" s="8" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="30">
       <c r="A75" s="8" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="30">
       <c r="A76" s="8" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="30">
       <c r="A77" s="8" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="30">
       <c r="A78" s="8" t="s">
-        <v>246</v>
+        <v>226</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>248</v>
+        <v>228</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>247</v>
+        <v>227</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="8" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>251</v>
+        <v>231</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="90">
       <c r="A80" s="8" t="s">
-        <v>252</v>
+        <v>232</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>253</v>
+        <v>233</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>254</v>
+        <v>234</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E80" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="60">
       <c r="A81" s="8" t="s">
-        <v>255</v>
+        <v>235</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>256</v>
+        <v>236</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="8" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>259</v>
+        <v>239</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="8" t="s">
-        <v>261</v>
+        <v>241</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>262</v>
+        <v>242</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="8" t="s">
-        <v>265</v>
+        <v>245</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>266</v>
+        <v>246</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>264</v>
+        <v>244</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="120">
       <c r="A85" s="8" t="s">
-        <v>267</v>
+        <v>247</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>272</v>
+        <v>252</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="120">
       <c r="A86" s="8" t="s">
-        <v>268</v>
+        <v>248</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>273</v>
+        <v>253</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>271</v>
+        <v>251</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="195">
       <c r="A87" s="8" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>275</v>
+        <v>255</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>274</v>
+        <v>254</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E87" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="8" t="s">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>278</v>
+        <v>258</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>276</v>
+        <v>256</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E88" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="8" t="s">
-        <v>281</v>
+        <v>261</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>279</v>
+        <v>259</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>277</v>
+        <v>257</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="8" t="s">
-        <v>282</v>
+        <v>262</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>283</v>
+        <v>263</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>284</v>
+        <v>264</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="30">
       <c r="A91" s="8" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>288</v>
+        <v>268</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>287</v>
+        <v>267</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E91" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="8" t="s">
-        <v>286</v>
+        <v>266</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>289</v>
+        <v>269</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>290</v>
+        <v>270</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E92" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="8" t="s">
-        <v>294</v>
+        <v>274</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="8" t="s">
-        <v>295</v>
+        <v>275</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>296</v>
+        <v>276</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>297</v>
+        <v>277</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="8" t="s">
-        <v>299</v>
+        <v>279</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>300</v>
+        <v>280</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>298</v>
+        <v>278</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="105">
       <c r="A96" s="8" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>303</v>
+        <v>283</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>305</v>
+        <v>285</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E96" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="105">
       <c r="A97" s="8" t="s">
-        <v>302</v>
+        <v>282</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>304</v>
+        <v>284</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="8" t="s">
-        <v>307</v>
+        <v>287</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>308</v>
+        <v>288</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>309</v>
+        <v>289</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="8" t="s">
-        <v>310</v>
+        <v>290</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>311</v>
+        <v>291</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>312</v>
+        <v>292</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="45">
       <c r="A100" s="8" t="s">
-        <v>313</v>
+        <v>293</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>315</v>
+        <v>295</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>314</v>
+        <v>294</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="8" t="s">
-        <v>316</v>
+        <v>296</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>317</v>
+        <v>297</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E101" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="8" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>321</v>
+        <v>301</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E102" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="8" t="s">
-        <v>322</v>
+        <v>302</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>323</v>
+        <v>303</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>324</v>
+        <v>304</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E103" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="8" t="s">
-        <v>325</v>
+        <v>305</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>327</v>
+        <v>307</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E104" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="8" t="s">
-        <v>328</v>
+        <v>308</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>330</v>
+        <v>310</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>331</v>
+        <v>311</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E105" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="165">
       <c r="A106" s="8" t="s">
-        <v>329</v>
+        <v>309</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>333</v>
+        <v>313</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>332</v>
+        <v>312</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E106" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="75">
       <c r="A107" s="8" t="s">
-        <v>334</v>
+        <v>314</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>363</v>
+        <v>343</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>362</v>
+        <v>342</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E107" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="8" t="s">
-        <v>335</v>
+        <v>315</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>336</v>
+        <v>316</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>337</v>
+        <v>317</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E108" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="8" t="s">
-        <v>338</v>
+        <v>318</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>339</v>
+        <v>319</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>340</v>
+        <v>320</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E109" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="8" t="s">
-        <v>345</v>
+        <v>325</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>343</v>
+        <v>323</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>344</v>
+        <v>324</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E110" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="8" t="s">
-        <v>346</v>
+        <v>326</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>341</v>
+        <v>321</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>342</v>
+        <v>322</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E111" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="8" t="s">
-        <v>347</v>
+        <v>327</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>348</v>
+        <v>328</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>349</v>
+        <v>329</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E112" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="8" t="s">
-        <v>352</v>
+        <v>332</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>351</v>
+        <v>331</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>350</v>
+        <v>330</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E113" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="8" t="s">
-        <v>357</v>
+        <v>337</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>353</v>
+        <v>333</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>354</v>
+        <v>334</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E114" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="8" t="s">
-        <v>358</v>
+        <v>338</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>355</v>
+        <v>335</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>356</v>
+        <v>336</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E115" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="8" t="s">
-        <v>361</v>
+        <v>341</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>360</v>
+        <v>340</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>359</v>
+        <v>339</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E116" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="8" t="s">
-        <v>364</v>
+        <v>344</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>367</v>
+        <v>347</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>366</v>
+        <v>346</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E117" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="30">
       <c r="A118" s="8" t="s">
-        <v>365</v>
+        <v>345</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>369</v>
+        <v>349</v>
       </c>
       <c r="C118" s="10" t="s">
-        <v>368</v>
+        <v>348</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E118" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="75">
       <c r="A119" s="8" t="s">
-        <v>372</v>
+        <v>352</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>370</v>
+        <v>350</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>371</v>
+        <v>351</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E119" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="60">
       <c r="A120" s="8" t="s">
-        <v>373</v>
+        <v>353</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>374</v>
+        <v>354</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>375</v>
+        <v>355</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E120" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="105">
       <c r="A121" s="8" t="s">
-        <v>376</v>
+        <v>356</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>377</v>
+        <v>357</v>
       </c>
       <c r="C121" s="7" t="s">
-        <v>378</v>
+        <v>358</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E121" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="105">
       <c r="A122" s="8" t="s">
-        <v>379</v>
+        <v>359</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>380</v>
+        <v>360</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>381</v>
+        <v>361</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E122" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="8" t="s">
-        <v>382</v>
+        <v>362</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>383</v>
+        <v>363</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>384</v>
+        <v>364</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E123" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="8" t="s">
-        <v>385</v>
+        <v>365</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>386</v>
+        <v>366</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>387</v>
+        <v>367</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E124" s="8" t="s">
-        <v>291</v>
+        <v>271</v>
       </c>
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="3" t="s">
-        <v>394</v>
+        <v>374</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>388</v>
+        <v>368</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>389</v>
+        <v>369</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E125" s="3"/>
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="3" t="s">
-        <v>395</v>
+        <v>375</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>390</v>
+        <v>370</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>391</v>
+        <v>371</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E126" s="3"/>
     </row>
     <row r="127" spans="1:5" ht="150">
       <c r="A127" s="3" t="s">
-        <v>396</v>
+        <v>376</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>392</v>
+        <v>372</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>393</v>
+        <v>373</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E127" s="3"/>
     </row>

</xml_diff>

<commit_message>
Changes made in Notification test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/B suite.xlsx
+++ b/src/test/resources/xls/B suite.xlsx
@@ -152,69 +152,6 @@
 2)Click on NOTES tab and verify that NOTES tab gets displayed with all the notes(if present).</t>
   </si>
   <si>
-    <t>TestCase_B1</t>
-  </si>
-  <si>
-    <t>TestCase_B2</t>
-  </si>
-  <si>
-    <t>TestCase_B3</t>
-  </si>
-  <si>
-    <t>TestCase_B4</t>
-  </si>
-  <si>
-    <t>TestCase_B5</t>
-  </si>
-  <si>
-    <t>TestCase_B6</t>
-  </si>
-  <si>
-    <t>TestCase_B7</t>
-  </si>
-  <si>
-    <t>TestCase_B8</t>
-  </si>
-  <si>
-    <t>TestCase_B9</t>
-  </si>
-  <si>
-    <t>TestCase_B10</t>
-  </si>
-  <si>
-    <t>TestCase_B11</t>
-  </si>
-  <si>
-    <t>TestCase_B12</t>
-  </si>
-  <si>
-    <t>TestCase_B18</t>
-  </si>
-  <si>
-    <t>TestCase_B19</t>
-  </si>
-  <si>
-    <t>TestCase_B20</t>
-  </si>
-  <si>
-    <t>TestCase_B21</t>
-  </si>
-  <si>
-    <t>TestCase_B22</t>
-  </si>
-  <si>
-    <t>TestCase_B23</t>
-  </si>
-  <si>
-    <t>TestCase_B13</t>
-  </si>
-  <si>
-    <t>TestCase_B14</t>
-  </si>
-  <si>
-    <t>TestCase_B24</t>
-  </si>
-  <si>
     <t>Jira id</t>
   </si>
   <si>
@@ -356,25 +293,10 @@
     <t>Verify that MINIMUM SHOULD MATCH rule is working correctly</t>
   </si>
   <si>
-    <t>TestCase_B15</t>
-  </si>
-  <si>
-    <t>TestCase_B16</t>
-  </si>
-  <si>
-    <t>TestCase_B17</t>
-  </si>
-  <si>
     <t>Verify that ALL content type count is equal to the sum of the counts of other content types</t>
   </si>
   <si>
-    <t>TestCase_B25</t>
-  </si>
-  <si>
     <t>Verify that autocomplete feature is working correctly</t>
-  </si>
-  <si>
-    <t>TestCase_B26</t>
   </si>
   <si>
     <t>Verify that following sections get displayed in type ahead:
@@ -384,31 +306,16 @@
 d)People</t>
   </si>
   <si>
-    <t>TestCase_B27</t>
-  </si>
-  <si>
     <t>Verify that 4 suggested categories get displayed in type ahead and the typed keyword is present in all the 4 categories</t>
   </si>
   <si>
     <t>Verify that 4 suggested articles get displayed in type ahead and the typed keyword is present in all the 4 articles</t>
   </si>
   <si>
-    <t>TestCase_B28</t>
-  </si>
-  <si>
-    <t>TestCase_B29</t>
-  </si>
-  <si>
     <t>Verify that 4 suggested patents get displayed in type ahead and the typed keyword is present in all the 4 patents</t>
   </si>
   <si>
-    <t>TestCase_B30</t>
-  </si>
-  <si>
     <t>Verify that 4 suggested people get displayed in type ahead and the typed keyword is present in all the 4 people</t>
-  </si>
-  <si>
-    <t>TestCase_B31</t>
   </si>
   <si>
     <t>Verify that the following content type tabs get displayed in the left navigation pane:
@@ -419,34 +326,19 @@
 e)POSTS</t>
   </si>
   <si>
-    <t>TestCase_B32</t>
-  </si>
-  <si>
     <t>Verify that the following fields get displayed in the SORT BY drop down when ALL is selected as content type in the left navigation pane:
 a)Relevance
 b)Times cited
 c)Date</t>
   </si>
   <si>
-    <t>TestCase_B33</t>
-  </si>
-  <si>
     <t>Verify that the items are sorted by RELEVANCE by default in ALL content type</t>
   </si>
   <si>
-    <t>TestCase_B34</t>
-  </si>
-  <si>
     <t>Verify that user is able to sort the items by TIMES CITED field in ALL content type</t>
   </si>
   <si>
-    <t>TestCase_B35</t>
-  </si>
-  <si>
     <t>Verify that no filtering options are present in ALL content type</t>
-  </si>
-  <si>
-    <t>TestCase_B36</t>
   </si>
   <si>
     <t xml:space="preserve">Verify that the following fields get displayed in the SORT BY drop down when ARTICLES is selected as content type in the left navigation pane:
@@ -457,25 +349,13 @@
 </t>
   </si>
   <si>
-    <t>TestCase_B37</t>
-  </si>
-  <si>
     <t>Verify that user is able to sort the articles by TIMES CITED field in ARTICLES content type</t>
   </si>
   <si>
-    <t>TestCase_B38</t>
-  </si>
-  <si>
     <t>Verify that only articles get displayed when user chooses ARTICLES as content type</t>
   </si>
   <si>
-    <t>TestCase_B39</t>
-  </si>
-  <si>
     <t>Verify that all articles are sorted by RELEVANCE by default in ARTICLES content type</t>
-  </si>
-  <si>
-    <t>TestCase_B40</t>
   </si>
   <si>
     <t xml:space="preserve">Verify that following filters are present for ARTICLES content type:
@@ -486,22 +366,10 @@
 </t>
   </si>
   <si>
-    <t>TestCase_B41</t>
-  </si>
-  <si>
     <t>Verify that user is able to expand and collapse the Document Type filter in ARTICLES content type</t>
   </si>
   <si>
     <t>SKIP</t>
-  </si>
-  <si>
-    <t>TestCase_B42</t>
-  </si>
-  <si>
-    <t>TestCase_B43</t>
-  </si>
-  <si>
-    <t>TestCase_B44</t>
   </si>
   <si>
     <t>Verify that user is able to expand and collapse the Authors filter in ARTICLES content type</t>
@@ -521,39 +389,21 @@
 e)Posts</t>
   </si>
   <si>
-    <t>TestCase_B45</t>
-  </si>
-  <si>
     <t>Verify that ALL content type is selected in the search drop down by default</t>
   </si>
   <si>
-    <t>TestCase_B46</t>
-  </si>
-  <si>
     <t>Verify that user is able to select any of the content types present in search drop down</t>
   </si>
   <si>
-    <t>TestCase_B47</t>
-  </si>
-  <si>
-    <t>TestCase_B48</t>
-  </si>
-  <si>
     <t>Verify that ALL option is selected in the left navigation pane by default when user searches using ALL option in the search drop down</t>
   </si>
   <si>
-    <t>TestCase_B49</t>
-  </si>
-  <si>
     <t>Verify that search results related to all content types get displayed in the summary page when user searches using ALL option in search drop down</t>
   </si>
   <si>
     <t>OPQA-301</t>
   </si>
   <si>
-    <t>TestCase_B50</t>
-  </si>
-  <si>
     <t>OPQA-307</t>
   </si>
   <si>
@@ -563,42 +413,24 @@
     <t>Verify that PATENTS option is selected in the left navigation pane by default when user searches using PATENTS option in the search drop down</t>
   </si>
   <si>
-    <t>TestCase_B51</t>
-  </si>
-  <si>
-    <t>TestCase_B52</t>
-  </si>
-  <si>
     <t>Verify that POSTS option is selected in the left navigation pane by default when user searches using POSTS option in the search drop down</t>
   </si>
   <si>
-    <t>TestCase_B53</t>
-  </si>
-  <si>
     <t>Verify that PEOPLE option is selected in the left navigation pane by default when user searches using PEOPLE option in the search drop down</t>
   </si>
   <si>
     <t>OPQA-375</t>
   </si>
   <si>
-    <t>TestCase_B54</t>
-  </si>
-  <si>
     <t>OPQA-316</t>
   </si>
   <si>
     <t>Verify that only articles get displayed in the summary page when user searches using ARTICLES content type in search drop down</t>
   </si>
   <si>
-    <t>TestCase_B55</t>
-  </si>
-  <si>
     <t>Verify that only patents get displayed in the summary page when user searches using PATENTS content type in search drop down</t>
   </si>
   <si>
-    <t>TestCase_B56</t>
-  </si>
-  <si>
     <t>Verify that only posts get displayed in the summary page when user searches using POSTS content type in search drop down</t>
   </si>
   <si>
@@ -606,12 +438,6 @@
   </si>
   <si>
     <t>OPQA-380</t>
-  </si>
-  <si>
-    <t>TestCase_B57</t>
-  </si>
-  <si>
-    <t>TestCase_B58</t>
   </si>
   <si>
     <t>OPQA-287</t>
@@ -632,42 +458,21 @@
     <t>Verify that 10 article suggestions get displayed in the search type ahead when user searches using ARTICLES option in the search drop down and that the searched keyword is present in all the suggestions</t>
   </si>
   <si>
-    <t>TestCase_B59</t>
-  </si>
-  <si>
-    <t>TestCase_B60</t>
-  </si>
-  <si>
     <t>Verify that 10 patent suggestions get displayed in the search type ahead when user searches using PATENTS option in the search drop down and that the searched keyword is present in all the suggestions</t>
   </si>
   <si>
-    <t>TestCase_B61</t>
-  </si>
-  <si>
     <t>Verify that 10 post suggestions get displayed in the search type ahead when user searches using POSTS option in the search drop down and that the searched keyword is present in all the suggestions</t>
   </si>
   <si>
-    <t>TestCase_B62</t>
-  </si>
-  <si>
     <t>Verify that 10 people suggestions get displayed in the search type ahead when user searches using PEOPLE option in the search drop down and that the searched keyword is present in all the suggestions</t>
   </si>
   <si>
     <t>OPQA-378</t>
   </si>
   <si>
-    <t>TestCase_B63</t>
-  </si>
-  <si>
-    <t>TestCase_B64</t>
-  </si>
-  <si>
     <t>OPQA-557</t>
   </si>
   <si>
-    <t>TestCase_B65</t>
-  </si>
-  <si>
     <t>Verify that the searched keyword doesn't change in the search text box if any other content type is selected in the left navigation pane</t>
   </si>
   <si>
@@ -677,31 +482,19 @@
     <t>Verify that the searched keyword present in the search text box doesn't change if any other content type is selected in the search drop down</t>
   </si>
   <si>
-    <t>TestCase_B66</t>
-  </si>
-  <si>
     <t>OPQA-387</t>
   </si>
   <si>
     <t>Verify that counts of search results of all the content types should get displayed irrespective of the content type chosen for searching</t>
   </si>
   <si>
-    <t>TestCase_B67</t>
-  </si>
-  <si>
     <t>Verify that ALL search results count is equal to the count of search results of other content types(ARTICLES+PATENTS+POSTS+PEOPLE)</t>
   </si>
   <si>
     <t>OPQA-263</t>
   </si>
   <si>
-    <t>TestCase_B68</t>
-  </si>
-  <si>
     <t>Verify that count of the selected content type(in the left navigation pane) gets displayed at the top</t>
-  </si>
-  <si>
-    <t>TestCase_B69</t>
   </si>
   <si>
     <t>OPQA-384</t>
@@ -712,88 +505,58 @@
 b)Search drop down option gets changed automatically to the switched content type</t>
   </si>
   <si>
-    <t>TestCase_B70</t>
-  </si>
-  <si>
     <t>Verify that record view of an article gets displayed when user clicks on any article option in the search type ahead while ALL option is selected in the search drop down</t>
   </si>
   <si>
     <t>OPQA-396</t>
   </si>
   <si>
-    <t>TestCase_B71</t>
-  </si>
-  <si>
     <t>OPQA-398</t>
   </si>
   <si>
     <t>Verify that record view of a patent gets displayed when user clicks on any patent option in the search type ahead while ALL option is selected in the search drop down</t>
   </si>
   <si>
-    <t>TestCase_B72</t>
-  </si>
-  <si>
     <t>Verify that record view of a post gets displayed when user clicks on any post option in the search type ahead while ALL option is selected in the search drop down</t>
   </si>
   <si>
     <t>OPQA-401</t>
   </si>
   <si>
-    <t>TestCase_B73</t>
-  </si>
-  <si>
     <t>OPQA-402</t>
   </si>
   <si>
     <t>Verify that profile page of a person gets displayed when user clicks on any PEOPLE option in the search type ahead while ALL option is selected in the search drop down</t>
   </si>
   <si>
-    <t>TestCase_B74</t>
-  </si>
-  <si>
     <t>OPQA-403</t>
   </si>
   <si>
     <t>Verify that record view of an article gets displayed when user clicks on any article option in the search type ahead while ARTICLES option is selected in the search drop down</t>
   </si>
   <si>
-    <t>TestCase_B75</t>
-  </si>
-  <si>
     <t>OPQA-404</t>
   </si>
   <si>
     <t>Verify that record view of a patent gets displayed when user clicks on any patent option in the search type ahead while PATENTS option is selected in the search drop down</t>
   </si>
   <si>
-    <t>TestCase_B76</t>
-  </si>
-  <si>
     <t>Verify that record view of a post gets displayed when user clicks on any post option in the search type ahead while POSTS option is selected in the search drop down</t>
   </si>
   <si>
     <t>OPQA-407</t>
   </si>
   <si>
-    <t>TestCase_B77</t>
-  </si>
-  <si>
     <t>Verify that profile page of a person gets displayed when user clicks on any PEOPLE option in the search type ahead while PEOPLE option is selected in the search drop down</t>
   </si>
   <si>
     <t>OPQA-409</t>
   </si>
   <si>
-    <t>TestCase_B78</t>
-  </si>
-  <si>
     <t>OPQA-412</t>
   </si>
   <si>
     <t>Verify that nothing gets displayed in the search type ahead if search query is not interpreted by the system</t>
-  </si>
-  <si>
-    <t>TestCase_B79</t>
   </si>
   <si>
     <t>OPQA-392</t>
@@ -806,9 +569,6 @@
 d)Correct category gets selected in CATEGORIES filter in the left navigation pane with filter in expanded state</t>
   </si>
   <si>
-    <t>TestCase_B80</t>
-  </si>
-  <si>
     <t>Verify that following options get displayed in SORT BY drop down in ALL search results page:
 a)Relevance
 b)Times Cited
@@ -818,18 +578,12 @@
     <t>OPQA-413</t>
   </si>
   <si>
-    <t>TestCase_B81</t>
-  </si>
-  <si>
     <t>OPQA-414</t>
   </si>
   <si>
     <t>Verify that search results are sorted by RELEVANCE by default in ALL search results page</t>
   </si>
   <si>
-    <t>TestCase_B82</t>
-  </si>
-  <si>
     <t>OPQA-560</t>
   </si>
   <si>
@@ -839,19 +593,7 @@
     <t>Verify that more search results get displayed when user scrolls down in ALL search results page</t>
   </si>
   <si>
-    <t>TestCase_B83</t>
-  </si>
-  <si>
     <t>OPQA-563</t>
-  </si>
-  <si>
-    <t>TestCase_B84</t>
-  </si>
-  <si>
-    <t>TestCase_B85</t>
-  </si>
-  <si>
-    <t>TestCase_B86</t>
   </si>
   <si>
     <t>Verify that following fields get displayed correctly for a patent in ALL search results page:
@@ -910,27 +652,12 @@
     <t>OPQA-573</t>
   </si>
   <si>
-    <t>TestCase_B87</t>
-  </si>
-  <si>
-    <t>TestCase_B88</t>
-  </si>
-  <si>
-    <t>TestCase_B89</t>
-  </si>
-  <si>
     <t>OPQA-575</t>
   </si>
   <si>
     <t>Verify that DETAILS link is working correctly in record view page of a patent</t>
   </si>
   <si>
-    <t>TestCase_B90</t>
-  </si>
-  <si>
-    <t>TestCase_B91</t>
-  </si>
-  <si>
     <t>Verify that following options get displayed in SORT BY drop down in ARTICLES search results page: a)Relevance b)Times Cited c)Publication Date(Newest) d)Publication Date(Oldest)</t>
   </si>
   <si>
@@ -952,12 +679,6 @@
     <t>OPQA-1237</t>
   </si>
   <si>
-    <t>TestCase_B92</t>
-  </si>
-  <si>
-    <t>TestCase_B93</t>
-  </si>
-  <si>
     <t>OPQA-1238</t>
   </si>
   <si>
@@ -967,16 +688,7 @@
     <t>Verify that record view page of a person gets displayed when user clicks on any PEOPLE in PEOPLE search results page.</t>
   </si>
   <si>
-    <t>TestCase_B94</t>
-  </si>
-  <si>
     <t>OPQA-1239</t>
-  </si>
-  <si>
-    <t>TestCase_B95</t>
-  </si>
-  <si>
-    <t>TestCase_B96</t>
   </si>
   <si>
     <t>OPQA-599</t>
@@ -1003,25 +715,16 @@
 f)Comments count</t>
   </si>
   <si>
-    <t>TestCase_B97</t>
-  </si>
-  <si>
     <t>OPQA-565</t>
   </si>
   <si>
     <t>Verify that no filtering options are present in ALL search results page</t>
   </si>
   <si>
-    <t>TestCase_B98</t>
-  </si>
-  <si>
     <t>OPQA-571</t>
   </si>
   <si>
     <t>Verify that search drop down content type is retained when user navigates back to ALL search results page from record view page</t>
-  </si>
-  <si>
-    <t>TestCase_B99</t>
   </si>
   <si>
     <t>Verify that following options get displayed in SORT BY drop down in PEOPLE search results page: a)Relevance b)Registration Date and search results are
@@ -1031,46 +734,28 @@
     <t>OPQA-1240 |OPQA-1241</t>
   </si>
   <si>
-    <t>TestCase_B100</t>
-  </si>
-  <si>
     <t>OPQA-582</t>
   </si>
   <si>
     <t>Verify that more search results get displayed when user scrolls down in PATENTS search results page</t>
   </si>
   <si>
-    <t>TestCase_B101</t>
-  </si>
-  <si>
     <t>OPQA-584</t>
   </si>
   <si>
     <t>Verify that sorting is retained when user navigates back to PATENTS search results page from record view page</t>
   </si>
   <si>
-    <t>TestCase_B102</t>
-  </si>
-  <si>
     <t>OPQA-586</t>
   </si>
   <si>
     <t>Verify that search drop down content type is retained when user navigates back to PATENTS search results page from record view page</t>
   </si>
   <si>
-    <t>TestCase_B103</t>
-  </si>
-  <si>
     <t>OPQA-591</t>
   </si>
   <si>
     <t>Verify that filtering is retained when user navigates back to PATENTS search results page from record view page</t>
-  </si>
-  <si>
-    <t>TestCase_B104</t>
-  </si>
-  <si>
-    <t>TestCase_B105</t>
   </si>
   <si>
     <t>OPQA-554</t>
@@ -1095,21 +780,12 @@
     <t>OPQA-555|OPQA-556</t>
   </si>
   <si>
-    <t>TestCase_B106</t>
-  </si>
-  <si>
-    <t>TestCase_B107</t>
-  </si>
-  <si>
     <t>OPQA-574</t>
   </si>
   <si>
     <t>Verify that left navigation pane content type is retained when user navigates back to ALL search results page from record view page</t>
   </si>
   <si>
-    <t>TestCase_B108</t>
-  </si>
-  <si>
     <t>OPQA-569</t>
   </si>
   <si>
@@ -1128,15 +804,6 @@
     <t>Verify that following filters are present in PATENTS search results page: a)Inventor b)IPC Codes c)Assignee</t>
   </si>
   <si>
-    <t>TestCase_B109</t>
-  </si>
-  <si>
-    <t>TestCase_B110</t>
-  </si>
-  <si>
-    <t>TestCase_B111</t>
-  </si>
-  <si>
     <t>OPQA-1242</t>
   </si>
   <si>
@@ -1149,9 +816,6 @@
     <t>OPQA-1243</t>
   </si>
   <si>
-    <t>TestCase_B112</t>
-  </si>
-  <si>
     <t>OPQA-593</t>
   </si>
   <si>
@@ -1164,19 +828,10 @@
     <t>Verify that left navigation pane content type is retained when user navigates back to PATENTS search results page from record view page</t>
   </si>
   <si>
-    <t>TestCase_B113</t>
-  </si>
-  <si>
-    <t>TestCase_B114</t>
-  </si>
-  <si>
     <t>Verify that search drop down content type is retained when user navigates back to PEOPLE search results page from profile page</t>
   </si>
   <si>
     <t>OPQA-1244</t>
-  </si>
-  <si>
-    <t>TestCase_B115</t>
   </si>
   <si>
     <t>Verify that following options get displayed in SORT BY drop down in POSTS search results page: 
@@ -1189,12 +844,6 @@
     <t>OOPQA-1226|PQA-1227</t>
   </si>
   <si>
-    <t>TestCase_B116</t>
-  </si>
-  <si>
-    <t>TestCase_B117</t>
-  </si>
-  <si>
     <t>Verify that more search results get displayed when user scrolls down in POSTS search results page</t>
   </si>
   <si>
@@ -1218,12 +867,6 @@
 d)Filtering</t>
   </si>
   <si>
-    <t>TestCase_B118</t>
-  </si>
-  <si>
-    <t>TestCase_B119</t>
-  </si>
-  <si>
     <t>OPQA-576</t>
   </si>
   <si>
@@ -1231,9 +874,6 @@
 a)Sorting
 b)Left navigation pane content type
 c)Search drop down content type</t>
-  </si>
-  <si>
-    <t>TestCase_B120</t>
   </si>
   <si>
     <t>OPQA-578</t>
@@ -1248,9 +888,6 @@
 f)Comments count</t>
   </si>
   <si>
-    <t>TestCase_B121</t>
-  </si>
-  <si>
     <t>OPQA-580</t>
   </si>
   <si>
@@ -1263,16 +900,10 @@
 f)Comments count</t>
   </si>
   <si>
-    <t>TestCase_B122</t>
-  </si>
-  <si>
     <t>OPQA-1245</t>
   </si>
   <si>
     <t>Verify that left navigation pane content type is retained when user navigates back to PEOPLE search results page from record view page</t>
-  </si>
-  <si>
-    <t>TestCase_B123</t>
   </si>
   <si>
     <t>OPQA-1246</t>
@@ -1308,15 +939,6 @@
 g)DETAILS link</t>
   </si>
   <si>
-    <t>TestCase_B124</t>
-  </si>
-  <si>
-    <t>TestCase_B125</t>
-  </si>
-  <si>
-    <t>TestCase_B126</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -1378,6 +1000,384 @@
   </si>
   <si>
     <t>OPQA-1501</t>
+  </si>
+  <si>
+    <t>Search1</t>
+  </si>
+  <si>
+    <t>Search2</t>
+  </si>
+  <si>
+    <t>Search3</t>
+  </si>
+  <si>
+    <t>Search4</t>
+  </si>
+  <si>
+    <t>Search5</t>
+  </si>
+  <si>
+    <t>Search6</t>
+  </si>
+  <si>
+    <t>Search7</t>
+  </si>
+  <si>
+    <t>Search8</t>
+  </si>
+  <si>
+    <t>Search9</t>
+  </si>
+  <si>
+    <t>Search10</t>
+  </si>
+  <si>
+    <t>Search11</t>
+  </si>
+  <si>
+    <t>Search12</t>
+  </si>
+  <si>
+    <t>Search13</t>
+  </si>
+  <si>
+    <t>Search14</t>
+  </si>
+  <si>
+    <t>Search15</t>
+  </si>
+  <si>
+    <t>Search16</t>
+  </si>
+  <si>
+    <t>Search17</t>
+  </si>
+  <si>
+    <t>Search18</t>
+  </si>
+  <si>
+    <t>Search19</t>
+  </si>
+  <si>
+    <t>Search20</t>
+  </si>
+  <si>
+    <t>Search21</t>
+  </si>
+  <si>
+    <t>Search22</t>
+  </si>
+  <si>
+    <t>Search23</t>
+  </si>
+  <si>
+    <t>Search24</t>
+  </si>
+  <si>
+    <t>Search25</t>
+  </si>
+  <si>
+    <t>Search26</t>
+  </si>
+  <si>
+    <t>Search27</t>
+  </si>
+  <si>
+    <t>Search28</t>
+  </si>
+  <si>
+    <t>Search29</t>
+  </si>
+  <si>
+    <t>Search30</t>
+  </si>
+  <si>
+    <t>Search31</t>
+  </si>
+  <si>
+    <t>Search32</t>
+  </si>
+  <si>
+    <t>Search33</t>
+  </si>
+  <si>
+    <t>Search34</t>
+  </si>
+  <si>
+    <t>Search35</t>
+  </si>
+  <si>
+    <t>Search36</t>
+  </si>
+  <si>
+    <t>Search37</t>
+  </si>
+  <si>
+    <t>Search38</t>
+  </si>
+  <si>
+    <t>Search39</t>
+  </si>
+  <si>
+    <t>Search40</t>
+  </si>
+  <si>
+    <t>Search41</t>
+  </si>
+  <si>
+    <t>Search42</t>
+  </si>
+  <si>
+    <t>Search43</t>
+  </si>
+  <si>
+    <t>Search44</t>
+  </si>
+  <si>
+    <t>Search45</t>
+  </si>
+  <si>
+    <t>Search46</t>
+  </si>
+  <si>
+    <t>Search47</t>
+  </si>
+  <si>
+    <t>Search48</t>
+  </si>
+  <si>
+    <t>Search49</t>
+  </si>
+  <si>
+    <t>Search50</t>
+  </si>
+  <si>
+    <t>Search51</t>
+  </si>
+  <si>
+    <t>Search52</t>
+  </si>
+  <si>
+    <t>Search53</t>
+  </si>
+  <si>
+    <t>Search54</t>
+  </si>
+  <si>
+    <t>Search55</t>
+  </si>
+  <si>
+    <t>Search56</t>
+  </si>
+  <si>
+    <t>Search57</t>
+  </si>
+  <si>
+    <t>Search58</t>
+  </si>
+  <si>
+    <t>Search59</t>
+  </si>
+  <si>
+    <t>Search60</t>
+  </si>
+  <si>
+    <t>Search61</t>
+  </si>
+  <si>
+    <t>Search62</t>
+  </si>
+  <si>
+    <t>Search63</t>
+  </si>
+  <si>
+    <t>Search64</t>
+  </si>
+  <si>
+    <t>Search65</t>
+  </si>
+  <si>
+    <t>Search66</t>
+  </si>
+  <si>
+    <t>Search67</t>
+  </si>
+  <si>
+    <t>Search68</t>
+  </si>
+  <si>
+    <t>Search69</t>
+  </si>
+  <si>
+    <t>Search70</t>
+  </si>
+  <si>
+    <t>Search71</t>
+  </si>
+  <si>
+    <t>Search72</t>
+  </si>
+  <si>
+    <t>Search73</t>
+  </si>
+  <si>
+    <t>Search74</t>
+  </si>
+  <si>
+    <t>Search75</t>
+  </si>
+  <si>
+    <t>Search76</t>
+  </si>
+  <si>
+    <t>Search77</t>
+  </si>
+  <si>
+    <t>Search78</t>
+  </si>
+  <si>
+    <t>Search79</t>
+  </si>
+  <si>
+    <t>Search80</t>
+  </si>
+  <si>
+    <t>Search81</t>
+  </si>
+  <si>
+    <t>Search82</t>
+  </si>
+  <si>
+    <t>Search83</t>
+  </si>
+  <si>
+    <t>Search84</t>
+  </si>
+  <si>
+    <t>Search85</t>
+  </si>
+  <si>
+    <t>Search86</t>
+  </si>
+  <si>
+    <t>Search87</t>
+  </si>
+  <si>
+    <t>Search88</t>
+  </si>
+  <si>
+    <t>Search89</t>
+  </si>
+  <si>
+    <t>Search90</t>
+  </si>
+  <si>
+    <t>Search91</t>
+  </si>
+  <si>
+    <t>Search92</t>
+  </si>
+  <si>
+    <t>Search93</t>
+  </si>
+  <si>
+    <t>Search94</t>
+  </si>
+  <si>
+    <t>Search95</t>
+  </si>
+  <si>
+    <t>Search96</t>
+  </si>
+  <si>
+    <t>Search97</t>
+  </si>
+  <si>
+    <t>Search98</t>
+  </si>
+  <si>
+    <t>Search99</t>
+  </si>
+  <si>
+    <t>Search100</t>
+  </si>
+  <si>
+    <t>Search101</t>
+  </si>
+  <si>
+    <t>Search102</t>
+  </si>
+  <si>
+    <t>Search103</t>
+  </si>
+  <si>
+    <t>Search104</t>
+  </si>
+  <si>
+    <t>Search105</t>
+  </si>
+  <si>
+    <t>Search106</t>
+  </si>
+  <si>
+    <t>Search107</t>
+  </si>
+  <si>
+    <t>Search108</t>
+  </si>
+  <si>
+    <t>Search109</t>
+  </si>
+  <si>
+    <t>Search110</t>
+  </si>
+  <si>
+    <t>Search111</t>
+  </si>
+  <si>
+    <t>Search112</t>
+  </si>
+  <si>
+    <t>Search113</t>
+  </si>
+  <si>
+    <t>Search114</t>
+  </si>
+  <si>
+    <t>Search115</t>
+  </si>
+  <si>
+    <t>Search116</t>
+  </si>
+  <si>
+    <t>Search117</t>
+  </si>
+  <si>
+    <t>Search118</t>
+  </si>
+  <si>
+    <t>Search119</t>
+  </si>
+  <si>
+    <t>Search120</t>
+  </si>
+  <si>
+    <t>Search121</t>
+  </si>
+  <si>
+    <t>Search122</t>
+  </si>
+  <si>
+    <t>Search123</t>
+  </si>
+  <si>
+    <t>Search124</t>
+  </si>
+  <si>
+    <t>Search125</t>
+  </si>
+  <si>
+    <t>Search126</t>
   </si>
 </sst>
 </file>
@@ -1781,7 +1781,7 @@
   <dimension ref="A1:E127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D127"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1798,7 +1798,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1812,2137 +1812,2137 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="8" t="s">
-        <v>30</v>
+        <v>272</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="8" t="s">
-        <v>31</v>
+        <v>273</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="8" t="s">
-        <v>32</v>
+        <v>274</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="8" t="s">
-        <v>33</v>
+        <v>275</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="8" t="s">
-        <v>34</v>
+        <v>276</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="8" t="s">
-        <v>35</v>
+        <v>277</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
       <c r="A8" s="8" t="s">
-        <v>36</v>
+        <v>278</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="8" t="s">
-        <v>37</v>
+        <v>279</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="8" t="s">
-        <v>38</v>
+        <v>280</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="8" t="s">
-        <v>39</v>
+        <v>281</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16.5" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>40</v>
+        <v>282</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="8" t="s">
-        <v>41</v>
+        <v>283</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="8" t="s">
-        <v>48</v>
+        <v>284</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="8" t="s">
-        <v>49</v>
+        <v>285</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="8" t="s">
-        <v>98</v>
+        <v>286</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="8" t="s">
-        <v>99</v>
+        <v>287</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="8" t="s">
-        <v>100</v>
+        <v>288</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>127</v>
+        <v>90</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="8" t="s">
-        <v>42</v>
+        <v>289</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="8" t="s">
-        <v>43</v>
+        <v>290</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="8" t="s">
-        <v>44</v>
+        <v>291</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="8" t="s">
-        <v>45</v>
+        <v>292</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="8" t="s">
-        <v>46</v>
+        <v>293</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="8" t="s">
-        <v>47</v>
+        <v>294</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="8" t="s">
-        <v>50</v>
+        <v>295</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="8" t="s">
-        <v>102</v>
+        <v>296</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>378</v>
+        <v>252</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="75">
       <c r="A27" s="8" t="s">
-        <v>104</v>
+        <v>297</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>379</v>
+        <v>253</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="8" t="s">
-        <v>106</v>
+        <v>298</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>380</v>
+        <v>254</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="8" t="s">
-        <v>109</v>
+        <v>299</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>381</v>
+        <v>255</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="8" t="s">
-        <v>110</v>
+        <v>300</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>382</v>
+        <v>256</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>111</v>
+        <v>82</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="8" t="s">
-        <v>112</v>
+        <v>301</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>383</v>
+        <v>257</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>113</v>
+        <v>83</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="90">
       <c r="A32" s="8" t="s">
-        <v>114</v>
+        <v>302</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>384</v>
+        <v>258</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="60">
       <c r="A33" s="8" t="s">
-        <v>116</v>
+        <v>303</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>385</v>
+        <v>259</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>117</v>
+        <v>85</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="8" t="s">
-        <v>118</v>
+        <v>304</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>386</v>
+        <v>260</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="8" t="s">
-        <v>120</v>
+        <v>305</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>387</v>
+        <v>261</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>121</v>
+        <v>87</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="8" t="s">
-        <v>122</v>
+        <v>306</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>388</v>
+        <v>262</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>123</v>
+        <v>88</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="90">
       <c r="A37" s="8" t="s">
-        <v>124</v>
+        <v>307</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>389</v>
+        <v>263</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>125</v>
+        <v>89</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="8" t="s">
-        <v>126</v>
+        <v>308</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>390</v>
+        <v>264</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>127</v>
+        <v>90</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="8" t="s">
-        <v>128</v>
+        <v>309</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>391</v>
+        <v>265</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>129</v>
+        <v>91</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="8" t="s">
-        <v>130</v>
+        <v>310</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>392</v>
+        <v>266</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>131</v>
+        <v>92</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="90">
       <c r="A41" s="8" t="s">
-        <v>132</v>
+        <v>311</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>393</v>
+        <v>267</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>133</v>
+        <v>93</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="8" t="s">
-        <v>134</v>
+        <v>312</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>394</v>
+        <v>268</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>135</v>
+        <v>94</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="8" t="s">
-        <v>137</v>
+        <v>313</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>395</v>
+        <v>269</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>140</v>
+        <v>96</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="8" t="s">
-        <v>138</v>
+        <v>314</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>396</v>
+        <v>270</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>141</v>
+        <v>97</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="8" t="s">
-        <v>139</v>
+        <v>315</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>397</v>
+        <v>271</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>142</v>
+        <v>98</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="90">
       <c r="A46" s="8" t="s">
-        <v>144</v>
+        <v>316</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>143</v>
+        <v>99</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="8" t="s">
-        <v>146</v>
+        <v>317</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>145</v>
+        <v>100</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="8" t="s">
-        <v>148</v>
+        <v>318</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>147</v>
+        <v>101</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="8" t="s">
-        <v>149</v>
+        <v>319</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>150</v>
+        <v>102</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="8" t="s">
-        <v>151</v>
+        <v>320</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>153</v>
+        <v>104</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>152</v>
+        <v>103</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="8" t="s">
-        <v>154</v>
+        <v>321</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>156</v>
+        <v>106</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="8" t="s">
-        <v>158</v>
+        <v>322</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>157</v>
+        <v>107</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="8" t="s">
-        <v>159</v>
+        <v>323</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>160</v>
+        <v>108</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="8" t="s">
-        <v>161</v>
+        <v>324</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>163</v>
+        <v>110</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>162</v>
+        <v>109</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="8" t="s">
-        <v>164</v>
+        <v>325</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>165</v>
+        <v>111</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>166</v>
+        <v>112</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="8" t="s">
-        <v>167</v>
+        <v>326</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>168</v>
+        <v>113</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="8" t="s">
-        <v>169</v>
+        <v>327</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>170</v>
+        <v>114</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="8" t="s">
-        <v>173</v>
+        <v>328</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>172</v>
+        <v>116</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>171</v>
+        <v>115</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="120">
       <c r="A59" s="8" t="s">
-        <v>174</v>
+        <v>329</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>175</v>
+        <v>117</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>176</v>
+        <v>118</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="30">
       <c r="A60" s="8" t="s">
-        <v>179</v>
+        <v>330</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>177</v>
+        <v>119</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>178</v>
+        <v>120</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="30">
       <c r="A61" s="8" t="s">
-        <v>180</v>
+        <v>331</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>181</v>
+        <v>121</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="30">
       <c r="A62" s="8" t="s">
-        <v>182</v>
+        <v>332</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>183</v>
+        <v>122</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="30">
       <c r="A63" s="8" t="s">
-        <v>184</v>
+        <v>333</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>186</v>
+        <v>124</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>185</v>
+        <v>123</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="8" t="s">
-        <v>187</v>
+        <v>334</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="8" t="s">
-        <v>188</v>
+        <v>335</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>189</v>
+        <v>125</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>193</v>
+        <v>128</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="8" t="s">
-        <v>190</v>
+        <v>336</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>192</v>
+        <v>127</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>191</v>
+        <v>126</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="8" t="s">
-        <v>194</v>
+        <v>337</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>195</v>
+        <v>129</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>196</v>
+        <v>130</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="8" t="s">
-        <v>197</v>
+        <v>338</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>199</v>
+        <v>132</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>198</v>
+        <v>131</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="8" t="s">
-        <v>200</v>
+        <v>339</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>201</v>
+        <v>133</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E69" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="45">
       <c r="A70" s="8" t="s">
-        <v>202</v>
+        <v>340</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>203</v>
+        <v>134</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>204</v>
+        <v>135</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="30">
       <c r="A71" s="8" t="s">
-        <v>205</v>
+        <v>341</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>207</v>
+        <v>137</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>206</v>
+        <v>136</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="30">
       <c r="A72" s="8" t="s">
-        <v>208</v>
+        <v>342</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>209</v>
+        <v>138</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>210</v>
+        <v>139</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="30">
       <c r="A73" s="8" t="s">
-        <v>211</v>
+        <v>343</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>213</v>
+        <v>141</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>212</v>
+        <v>140</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="30">
       <c r="A74" s="8" t="s">
-        <v>214</v>
+        <v>344</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>215</v>
+        <v>142</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>216</v>
+        <v>143</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="30">
       <c r="A75" s="8" t="s">
-        <v>217</v>
+        <v>345</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>218</v>
+        <v>144</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>219</v>
+        <v>145</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="30">
       <c r="A76" s="8" t="s">
-        <v>220</v>
+        <v>346</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>221</v>
+        <v>146</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>222</v>
+        <v>147</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="30">
       <c r="A77" s="8" t="s">
-        <v>223</v>
+        <v>347</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>225</v>
+        <v>149</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>224</v>
+        <v>148</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="30">
       <c r="A78" s="8" t="s">
-        <v>226</v>
+        <v>348</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>228</v>
+        <v>151</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>227</v>
+        <v>150</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="8" t="s">
-        <v>229</v>
+        <v>349</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>230</v>
+        <v>152</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>231</v>
+        <v>153</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="90">
       <c r="A80" s="8" t="s">
-        <v>232</v>
+        <v>350</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>233</v>
+        <v>154</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>234</v>
+        <v>155</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E80" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="60">
       <c r="A81" s="8" t="s">
-        <v>235</v>
+        <v>351</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>237</v>
+        <v>157</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>236</v>
+        <v>156</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="8" t="s">
-        <v>238</v>
+        <v>352</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>239</v>
+        <v>158</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>240</v>
+        <v>159</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="8" t="s">
-        <v>241</v>
+        <v>353</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>242</v>
+        <v>160</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>243</v>
+        <v>161</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="8" t="s">
-        <v>245</v>
+        <v>354</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>246</v>
+        <v>163</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>244</v>
+        <v>162</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="120">
       <c r="A85" s="8" t="s">
-        <v>247</v>
+        <v>355</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>252</v>
+        <v>166</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>250</v>
+        <v>164</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="120">
       <c r="A86" s="8" t="s">
-        <v>248</v>
+        <v>356</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>253</v>
+        <v>167</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>251</v>
+        <v>165</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="195">
       <c r="A87" s="8" t="s">
-        <v>249</v>
+        <v>357</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>255</v>
+        <v>169</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>254</v>
+        <v>168</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E87" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="8" t="s">
-        <v>260</v>
+        <v>358</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>258</v>
+        <v>172</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>256</v>
+        <v>170</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E88" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="8" t="s">
-        <v>261</v>
+        <v>359</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>259</v>
+        <v>173</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>257</v>
+        <v>171</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="8" t="s">
-        <v>262</v>
+        <v>360</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>263</v>
+        <v>174</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>264</v>
+        <v>175</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="30">
       <c r="A91" s="8" t="s">
-        <v>265</v>
+        <v>361</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>268</v>
+        <v>177</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>267</v>
+        <v>176</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E91" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="8" t="s">
-        <v>266</v>
+        <v>362</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>269</v>
+        <v>178</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>270</v>
+        <v>179</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E92" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="8" t="s">
-        <v>274</v>
+        <v>363</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>273</v>
+        <v>182</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>272</v>
+        <v>181</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="8" t="s">
-        <v>275</v>
+        <v>364</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>276</v>
+        <v>183</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>277</v>
+        <v>184</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="8" t="s">
-        <v>279</v>
+        <v>365</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>280</v>
+        <v>186</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>278</v>
+        <v>185</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="105">
       <c r="A96" s="8" t="s">
-        <v>281</v>
+        <v>366</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>283</v>
+        <v>187</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>285</v>
+        <v>189</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E96" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="105">
       <c r="A97" s="8" t="s">
-        <v>282</v>
+        <v>367</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>284</v>
+        <v>188</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>286</v>
+        <v>190</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="8" t="s">
-        <v>287</v>
+        <v>368</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>288</v>
+        <v>191</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>289</v>
+        <v>192</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="8" t="s">
-        <v>290</v>
+        <v>369</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>291</v>
+        <v>193</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>292</v>
+        <v>194</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="45">
       <c r="A100" s="8" t="s">
-        <v>293</v>
+        <v>370</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>295</v>
+        <v>196</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>294</v>
+        <v>195</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="8" t="s">
-        <v>296</v>
+        <v>371</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>297</v>
+        <v>197</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>298</v>
+        <v>198</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E101" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="8" t="s">
-        <v>299</v>
+        <v>372</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>300</v>
+        <v>199</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>301</v>
+        <v>200</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E102" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="8" t="s">
-        <v>302</v>
+        <v>373</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>303</v>
+        <v>201</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>304</v>
+        <v>202</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E103" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="8" t="s">
-        <v>305</v>
+        <v>374</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>306</v>
+        <v>203</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>307</v>
+        <v>204</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E104" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="8" t="s">
-        <v>308</v>
+        <v>375</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>310</v>
+        <v>205</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>311</v>
+        <v>206</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E105" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="165">
       <c r="A106" s="8" t="s">
-        <v>309</v>
+        <v>376</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>313</v>
+        <v>208</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>312</v>
+        <v>207</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E106" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="75">
       <c r="A107" s="8" t="s">
-        <v>314</v>
+        <v>377</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>343</v>
+        <v>228</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>342</v>
+        <v>227</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E107" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="8" t="s">
-        <v>315</v>
+        <v>378</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>316</v>
+        <v>209</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>317</v>
+        <v>210</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E108" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="8" t="s">
-        <v>318</v>
+        <v>379</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>319</v>
+        <v>211</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>320</v>
+        <v>212</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E109" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="8" t="s">
-        <v>325</v>
+        <v>380</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>323</v>
+        <v>215</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>324</v>
+        <v>216</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E110" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="8" t="s">
-        <v>326</v>
+        <v>381</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>321</v>
+        <v>213</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>322</v>
+        <v>214</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E111" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="8" t="s">
-        <v>327</v>
+        <v>382</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>328</v>
+        <v>217</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>329</v>
+        <v>218</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E112" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="8" t="s">
-        <v>332</v>
+        <v>383</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>331</v>
+        <v>220</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>330</v>
+        <v>219</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E113" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="8" t="s">
-        <v>337</v>
+        <v>384</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>333</v>
+        <v>221</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>334</v>
+        <v>222</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E114" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="8" t="s">
-        <v>338</v>
+        <v>385</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>335</v>
+        <v>223</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>336</v>
+        <v>224</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E115" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="8" t="s">
-        <v>341</v>
+        <v>386</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>340</v>
+        <v>226</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>339</v>
+        <v>225</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E116" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="8" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>347</v>
+        <v>230</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>346</v>
+        <v>229</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E117" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="30">
       <c r="A118" s="8" t="s">
-        <v>345</v>
+        <v>388</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>349</v>
+        <v>232</v>
       </c>
       <c r="C118" s="10" t="s">
-        <v>348</v>
+        <v>231</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E118" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="75">
       <c r="A119" s="8" t="s">
-        <v>352</v>
+        <v>389</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>350</v>
+        <v>233</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>351</v>
+        <v>234</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E119" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="60">
       <c r="A120" s="8" t="s">
-        <v>353</v>
+        <v>390</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>354</v>
+        <v>235</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>355</v>
+        <v>236</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E120" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="105">
       <c r="A121" s="8" t="s">
-        <v>356</v>
+        <v>391</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>357</v>
+        <v>237</v>
       </c>
       <c r="C121" s="7" t="s">
-        <v>358</v>
+        <v>238</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E121" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="105">
       <c r="A122" s="8" t="s">
-        <v>359</v>
+        <v>392</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>360</v>
+        <v>239</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>361</v>
+        <v>240</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E122" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="8" t="s">
-        <v>362</v>
+        <v>393</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>363</v>
+        <v>241</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>364</v>
+        <v>242</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E123" s="8" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="8" t="s">
-        <v>365</v>
+        <v>394</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>366</v>
+        <v>243</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>367</v>
+        <v>244</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E124" s="8" t="s">
-        <v>271</v>
+        <v>180</v>
       </c>
     </row>
     <row r="125" spans="1:5">
-      <c r="A125" s="3" t="s">
-        <v>374</v>
+      <c r="A125" s="8" t="s">
+        <v>395</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>368</v>
+        <v>245</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>369</v>
+        <v>246</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E125" s="3"/>
     </row>
     <row r="126" spans="1:5">
-      <c r="A126" s="3" t="s">
-        <v>375</v>
+      <c r="A126" s="8" t="s">
+        <v>396</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>370</v>
+        <v>247</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>371</v>
+        <v>248</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E126" s="3"/>
     </row>
     <row r="127" spans="1:5" ht="150">
-      <c r="A127" s="3" t="s">
-        <v>376</v>
+      <c r="A127" s="8" t="s">
+        <v>397</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>372</v>
+        <v>249</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>373</v>
+        <v>250</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="E127" s="3"/>
     </row>

</xml_diff>